<commit_message>
Defined a minimal set of references and linked to side-data
</commit_message>
<xml_diff>
--- a/tabular/flavi-ncbi-refseqs-side-data.xlsx
+++ b/tabular/flavi-ncbi-refseqs-side-data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1504" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1505" uniqueCount="402">
   <si>
     <t>isolate</t>
   </si>
@@ -784,9 +784,6 @@
     <t>tick</t>
   </si>
   <si>
-    <t>DQ235149.1</t>
-  </si>
-  <si>
     <t>Turkish sheep encephalitis</t>
   </si>
   <si>
@@ -796,9 +793,6 @@
     <t>Primate</t>
   </si>
   <si>
-    <t>JF416960.1</t>
-  </si>
-  <si>
     <t>Bainyink virus</t>
   </si>
   <si>
@@ -814,9 +808,6 @@
     <t>unknown</t>
   </si>
   <si>
-    <t>KM408491.1</t>
-  </si>
-  <si>
     <t>La Tina</t>
   </si>
   <si>
@@ -826,279 +817,57 @@
     <t>Neoaves</t>
   </si>
   <si>
-    <t>NC_000943.1</t>
-  </si>
-  <si>
-    <t>NC_001437.1</t>
-  </si>
-  <si>
     <t>none</t>
   </si>
   <si>
-    <t>NC_001461.1</t>
-  </si>
-  <si>
-    <t>NC_001474.2</t>
-  </si>
-  <si>
-    <t>NC_001475.2</t>
-  </si>
-  <si>
-    <t>NC_001477.1</t>
-  </si>
-  <si>
-    <t>NC_001563.2</t>
-  </si>
-  <si>
     <t>Insect</t>
   </si>
   <si>
-    <t>NC_001564.2</t>
-  </si>
-  <si>
     <t>Rodent</t>
   </si>
   <si>
-    <t>NC_001672.1</t>
-  </si>
-  <si>
-    <t>NC_001710.1</t>
-  </si>
-  <si>
-    <t>NC_001809.1</t>
-  </si>
-  <si>
-    <t>NC_001837.1</t>
-  </si>
-  <si>
-    <t>NC_002031.1</t>
-  </si>
-  <si>
-    <t>NC_002032.1</t>
-  </si>
-  <si>
-    <t>NC_002640.1</t>
-  </si>
-  <si>
     <t>Suidae</t>
   </si>
   <si>
-    <t>NC_002657.1</t>
-  </si>
-  <si>
-    <t>NC_003635.1</t>
-  </si>
-  <si>
     <t>Vespbat</t>
   </si>
   <si>
-    <t>NC_003675.1</t>
-  </si>
-  <si>
-    <t>NC_003676.1</t>
-  </si>
-  <si>
     <t>Pestivirus Giraffe-1</t>
   </si>
   <si>
     <t>Giraffidae</t>
   </si>
   <si>
-    <t>NC_003678.1</t>
-  </si>
-  <si>
-    <t>NC_003679.1</t>
-  </si>
-  <si>
-    <t>NC_003687.1</t>
-  </si>
-  <si>
-    <t>NC_003690.1</t>
-  </si>
-  <si>
-    <t>NC_003996.1</t>
-  </si>
-  <si>
     <t>Hepatitis C virus</t>
   </si>
   <si>
-    <t>NC_004102.1</t>
-  </si>
-  <si>
-    <t>NC_004119.1</t>
-  </si>
-  <si>
-    <t>NC_004355.1</t>
-  </si>
-  <si>
-    <t>NC_005039.1</t>
-  </si>
-  <si>
-    <t>NC_005062.1</t>
-  </si>
-  <si>
-    <t>NC_005064.1</t>
-  </si>
-  <si>
-    <t>NC_006551.1</t>
-  </si>
-  <si>
-    <t>NC_006947.1</t>
-  </si>
-  <si>
     <t>St. Louis encephalitis virus</t>
   </si>
   <si>
-    <t>NC_007580.2</t>
-  </si>
-  <si>
-    <t>NC_008604.2</t>
-  </si>
-  <si>
-    <t>NC_008718.1</t>
-  </si>
-  <si>
-    <t>NC_008719.1</t>
-  </si>
-  <si>
-    <t>NC_009026.2</t>
-  </si>
-  <si>
-    <t>NC_009028.2</t>
-  </si>
-  <si>
-    <t>NC_012532.1</t>
-  </si>
-  <si>
-    <t>NC_012533.1</t>
-  </si>
-  <si>
     <t>Galloanserae</t>
   </si>
   <si>
-    <t>NC_012534.1</t>
-  </si>
-  <si>
-    <t>NC_012671.1</t>
-  </si>
-  <si>
-    <t>NC_012735.1</t>
-  </si>
-  <si>
     <t>Bovine viral diarrhea virus 3</t>
   </si>
   <si>
-    <t>NC_012812.1</t>
-  </si>
-  <si>
-    <t>NC_012932.1</t>
-  </si>
-  <si>
-    <t>NC_015843.2</t>
-  </si>
-  <si>
-    <t>NC_017086.1</t>
-  </si>
-  <si>
-    <t>NC_018705.3</t>
-  </si>
-  <si>
-    <t>NC_018713.1</t>
-  </si>
-  <si>
     <t>Perissodactyla</t>
   </si>
   <si>
-    <t>NC_020902.1</t>
-  </si>
-  <si>
-    <t>NC_021069.1</t>
-  </si>
-  <si>
-    <t>NC_021153.1</t>
-  </si>
-  <si>
-    <t>NC_021154.1</t>
-  </si>
-  <si>
-    <t>NC_023176.1</t>
-  </si>
-  <si>
-    <t>NC_023424.1</t>
-  </si>
-  <si>
-    <t>NC_023439.1</t>
-  </si>
-  <si>
     <t>Antilocapridae</t>
   </si>
   <si>
-    <t>NC_024018.2</t>
-  </si>
-  <si>
-    <t>NC_024377.1</t>
-  </si>
-  <si>
     <t>Illomantsi virus</t>
   </si>
   <si>
-    <t>NC_024889.1</t>
-  </si>
-  <si>
-    <t>NC_025672.1</t>
-  </si>
-  <si>
-    <t>NC_025673.1</t>
-  </si>
-  <si>
-    <t>NC_025677.1</t>
-  </si>
-  <si>
-    <t>NC_025679.1</t>
-  </si>
-  <si>
-    <t>NC_026620.1</t>
-  </si>
-  <si>
-    <t>NC_026623.1</t>
-  </si>
-  <si>
-    <t>NC_026624.1</t>
-  </si>
-  <si>
-    <t>NC_026797.1</t>
-  </si>
-  <si>
-    <t>NC_027709.1</t>
-  </si>
-  <si>
-    <t>NC_027817.1</t>
-  </si>
-  <si>
-    <t>NC_027819.1</t>
-  </si>
-  <si>
-    <t>NC_027998.2</t>
-  </si>
-  <si>
     <t>sandfly</t>
   </si>
   <si>
-    <t>NC_027999.1</t>
-  </si>
-  <si>
-    <t>NC_029055.1</t>
-  </si>
-  <si>
     <t>Kokobera virus</t>
   </si>
   <si>
     <t>Diprotodontia</t>
   </si>
   <si>
-    <t>NC_032088.1</t>
-  </si>
-  <si>
     <t>Boubou virus</t>
   </si>
   <si>
@@ -1219,20 +988,251 @@
     <t>Aedes aegypti</t>
   </si>
   <si>
-    <t>Accession</t>
-  </si>
-  <si>
     <t>Modoc county</t>
   </si>
   <si>
     <t>Ovis aries</t>
+  </si>
+  <si>
+    <t>sequenceID</t>
+  </si>
+  <si>
+    <t>DQ235149</t>
+  </si>
+  <si>
+    <t>JF416960</t>
+  </si>
+  <si>
+    <t>KM408491</t>
+  </si>
+  <si>
+    <t>NC_000943</t>
+  </si>
+  <si>
+    <t>NC_001437</t>
+  </si>
+  <si>
+    <t>NC_001461</t>
+  </si>
+  <si>
+    <t>NC_001477</t>
+  </si>
+  <si>
+    <t>NC_001672</t>
+  </si>
+  <si>
+    <t>NC_001710</t>
+  </si>
+  <si>
+    <t>NC_001809</t>
+  </si>
+  <si>
+    <t>NC_001837</t>
+  </si>
+  <si>
+    <t>NC_002031</t>
+  </si>
+  <si>
+    <t>NC_002032</t>
+  </si>
+  <si>
+    <t>NC_002640</t>
+  </si>
+  <si>
+    <t>NC_002657</t>
+  </si>
+  <si>
+    <t>NC_003635</t>
+  </si>
+  <si>
+    <t>NC_003675</t>
+  </si>
+  <si>
+    <t>NC_003676</t>
+  </si>
+  <si>
+    <t>NC_003678</t>
+  </si>
+  <si>
+    <t>NC_003679</t>
+  </si>
+  <si>
+    <t>NC_003687</t>
+  </si>
+  <si>
+    <t>NC_003690</t>
+  </si>
+  <si>
+    <t>NC_003996</t>
+  </si>
+  <si>
+    <t>NC_004102</t>
+  </si>
+  <si>
+    <t>NC_004119</t>
+  </si>
+  <si>
+    <t>NC_004355</t>
+  </si>
+  <si>
+    <t>NC_005039</t>
+  </si>
+  <si>
+    <t>NC_005062</t>
+  </si>
+  <si>
+    <t>NC_005064</t>
+  </si>
+  <si>
+    <t>NC_006551</t>
+  </si>
+  <si>
+    <t>NC_006947</t>
+  </si>
+  <si>
+    <t>NC_008718</t>
+  </si>
+  <si>
+    <t>NC_008719</t>
+  </si>
+  <si>
+    <t>NC_012532</t>
+  </si>
+  <si>
+    <t>NC_012533</t>
+  </si>
+  <si>
+    <t>NC_012534</t>
+  </si>
+  <si>
+    <t>NC_012671</t>
+  </si>
+  <si>
+    <t>NC_012735</t>
+  </si>
+  <si>
+    <t>NC_012812</t>
+  </si>
+  <si>
+    <t>NC_012932</t>
+  </si>
+  <si>
+    <t>NC_017086</t>
+  </si>
+  <si>
+    <t>NC_018713</t>
+  </si>
+  <si>
+    <t>NC_020902</t>
+  </si>
+  <si>
+    <t>NC_021069</t>
+  </si>
+  <si>
+    <t>NC_021153</t>
+  </si>
+  <si>
+    <t>NC_021154</t>
+  </si>
+  <si>
+    <t>NC_023176</t>
+  </si>
+  <si>
+    <t>NC_023424</t>
+  </si>
+  <si>
+    <t>NC_023439</t>
+  </si>
+  <si>
+    <t>NC_024377</t>
+  </si>
+  <si>
+    <t>NC_024889</t>
+  </si>
+  <si>
+    <t>NC_025672</t>
+  </si>
+  <si>
+    <t>NC_025673</t>
+  </si>
+  <si>
+    <t>NC_025677</t>
+  </si>
+  <si>
+    <t>NC_025679</t>
+  </si>
+  <si>
+    <t>NC_026620</t>
+  </si>
+  <si>
+    <t>NC_026623</t>
+  </si>
+  <si>
+    <t>NC_026624</t>
+  </si>
+  <si>
+    <t>NC_026797</t>
+  </si>
+  <si>
+    <t>NC_027709</t>
+  </si>
+  <si>
+    <t>NC_027817</t>
+  </si>
+  <si>
+    <t>NC_027819</t>
+  </si>
+  <si>
+    <t>NC_027999</t>
+  </si>
+  <si>
+    <t>NC_029055</t>
+  </si>
+  <si>
+    <t>NC_032088</t>
+  </si>
+  <si>
+    <t>NC_001474</t>
+  </si>
+  <si>
+    <t>NC_001475</t>
+  </si>
+  <si>
+    <t>NC_001563</t>
+  </si>
+  <si>
+    <t>NC_001564</t>
+  </si>
+  <si>
+    <t>NC_007580</t>
+  </si>
+  <si>
+    <t>NC_008604</t>
+  </si>
+  <si>
+    <t>NC_009026</t>
+  </si>
+  <si>
+    <t>NC_009028</t>
+  </si>
+  <si>
+    <t>NC_015843</t>
+  </si>
+  <si>
+    <t>NC_024018</t>
+  </si>
+  <si>
+    <t>NC_027998</t>
+  </si>
+  <si>
+    <t>NC_018705</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1248,6 +1248,22 @@
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1359,8 +1375,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1403,7 +1427,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1736,7 +1768,7 @@
   <dimension ref="A1:R111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:R111"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1755,7 +1787,7 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="2" t="s">
-        <v>399</v>
+        <v>324</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>109</v>
@@ -1770,22 +1802,22 @@
         <v>111</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>364</v>
+        <v>287</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>397</v>
+        <v>320</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>361</v>
+        <v>284</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>250</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>363</v>
+        <v>286</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>362</v>
+        <v>285</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>249</v>
@@ -1943,7 +1975,7 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" s="11" t="s">
-        <v>254</v>
+        <v>325</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>115</v>
@@ -1996,7 +2028,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>7</v>
@@ -2133,7 +2165,9 @@
       <c r="C9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="8"/>
+      <c r="D9" s="8" t="s">
+        <v>251</v>
+      </c>
       <c r="E9" s="8" t="s">
         <v>7</v>
       </c>
@@ -2236,7 +2270,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="K11" s="9"/>
       <c r="L11" s="8"/>
@@ -2264,7 +2298,7 @@
         <v>24</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>7</v>
@@ -2282,7 +2316,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
@@ -2290,10 +2324,10 @@
         <v>178</v>
       </c>
       <c r="N12" s="8" t="s">
-        <v>382</v>
+        <v>305</v>
       </c>
       <c r="O12" s="8" t="s">
-        <v>383</v>
+        <v>306</v>
       </c>
       <c r="P12" s="8" t="s">
         <v>7</v>
@@ -2307,7 +2341,7 @@
     </row>
     <row r="13" spans="1:18">
       <c r="A13" s="11" t="s">
-        <v>258</v>
+        <v>326</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>124</v>
@@ -2322,7 +2356,7 @@
         <v>7</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>125</v>
@@ -2540,7 +2574,7 @@
         <v>33</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>7</v>
@@ -2623,10 +2657,10 @@
     </row>
     <row r="20" spans="1:18">
       <c r="A20" s="11" t="s">
-        <v>264</v>
+        <v>327</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>7</v>
@@ -2638,7 +2672,7 @@
         <v>7</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>135</v>
@@ -2647,10 +2681,10 @@
         <v>135</v>
       </c>
       <c r="I20" s="13" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="K20" s="9"/>
       <c r="L20" s="13">
@@ -2707,7 +2741,7 @@
         <v>47</v>
       </c>
       <c r="O21" s="8" t="s">
-        <v>365</v>
+        <v>288</v>
       </c>
       <c r="P21" s="8">
         <v>2013</v>
@@ -2721,10 +2755,10 @@
     </row>
     <row r="22" spans="1:18">
       <c r="A22" s="6" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>7</v>
@@ -2748,10 +2782,10 @@
         <v>39</v>
       </c>
       <c r="N22" s="8" t="s">
-        <v>367</v>
+        <v>290</v>
       </c>
       <c r="O22" s="8" t="s">
-        <v>366</v>
+        <v>289</v>
       </c>
       <c r="P22" s="8">
         <v>1996</v>
@@ -2809,7 +2843,7 @@
     </row>
     <row r="24" spans="1:18">
       <c r="A24" s="11" t="s">
-        <v>268</v>
+        <v>328</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>141</v>
@@ -2824,7 +2858,7 @@
         <v>7</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>7</v>
@@ -2863,7 +2897,7 @@
     </row>
     <row r="25" spans="1:18">
       <c r="A25" s="11" t="s">
-        <v>269</v>
+        <v>329</v>
       </c>
       <c r="B25" s="12" t="s">
         <v>142</v>
@@ -2878,7 +2912,7 @@
         <v>7</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G25" s="8" t="s">
         <v>7</v>
@@ -2917,13 +2951,13 @@
     </row>
     <row r="26" spans="1:18">
       <c r="A26" s="11" t="s">
-        <v>271</v>
+        <v>330</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>143</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>384</v>
+        <v>307</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>251</v>
@@ -2932,7 +2966,7 @@
         <v>7</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G26" s="8" t="s">
         <v>7</v>
@@ -2944,7 +2978,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="12" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="K26" s="9"/>
       <c r="L26" s="13">
@@ -2971,13 +3005,13 @@
     </row>
     <row r="27" spans="1:18">
       <c r="A27" s="11" t="s">
-        <v>272</v>
+        <v>390</v>
       </c>
       <c r="B27" s="12" t="s">
         <v>144</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>385</v>
+        <v>308</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>251</v>
@@ -2986,7 +3020,7 @@
         <v>7</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G27" s="8" t="s">
         <v>7</v>
@@ -3025,13 +3059,13 @@
     </row>
     <row r="28" spans="1:18">
       <c r="A28" s="11" t="s">
-        <v>273</v>
+        <v>391</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>145</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>386</v>
+        <v>309</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>251</v>
@@ -3040,7 +3074,7 @@
         <v>7</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>7</v>
@@ -3079,13 +3113,13 @@
     </row>
     <row r="29" spans="1:18">
       <c r="A29" s="11" t="s">
-        <v>274</v>
+        <v>331</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>146</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>387</v>
+        <v>310</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>251</v>
@@ -3094,7 +3128,7 @@
         <v>7</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>7</v>
@@ -3133,13 +3167,13 @@
     </row>
     <row r="30" spans="1:18">
       <c r="A30" s="11" t="s">
-        <v>275</v>
+        <v>392</v>
       </c>
       <c r="B30" s="12" t="s">
         <v>147</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>388</v>
+        <v>311</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>251</v>
@@ -3148,7 +3182,7 @@
         <v>7</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>7</v>
@@ -3187,7 +3221,7 @@
     </row>
     <row r="31" spans="1:18">
       <c r="A31" s="11" t="s">
-        <v>277</v>
+        <v>393</v>
       </c>
       <c r="B31" s="12" t="s">
         <v>148</v>
@@ -3202,7 +3236,7 @@
         <v>7</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>149</v>
@@ -3215,7 +3249,7 @@
         <v>127</v>
       </c>
       <c r="K31" s="8" t="s">
-        <v>398</v>
+        <v>321</v>
       </c>
       <c r="L31" s="13">
         <v>31658</v>
@@ -3241,7 +3275,7 @@
     </row>
     <row r="32" spans="1:18">
       <c r="A32" s="11" t="s">
-        <v>279</v>
+        <v>332</v>
       </c>
       <c r="B32" s="12" t="s">
         <v>150</v>
@@ -3256,7 +3290,7 @@
         <v>7</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>7</v>
@@ -3295,7 +3329,7 @@
     </row>
     <row r="33" spans="1:18">
       <c r="A33" s="11" t="s">
-        <v>280</v>
+        <v>333</v>
       </c>
       <c r="B33" s="12" t="s">
         <v>151</v>
@@ -3310,7 +3344,7 @@
         <v>7</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>7</v>
@@ -3322,7 +3356,7 @@
         <v>0</v>
       </c>
       <c r="J33" s="12" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="K33" s="9"/>
       <c r="L33" s="13">
@@ -3349,13 +3383,13 @@
     </row>
     <row r="34" spans="1:18">
       <c r="A34" s="11" t="s">
-        <v>281</v>
+        <v>334</v>
       </c>
       <c r="B34" s="12" t="s">
         <v>152</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>389</v>
+        <v>312</v>
       </c>
       <c r="D34" s="8" t="s">
         <v>251</v>
@@ -3364,7 +3398,7 @@
         <v>7</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>7</v>
@@ -3403,7 +3437,7 @@
     </row>
     <row r="35" spans="1:18">
       <c r="A35" s="11" t="s">
-        <v>282</v>
+        <v>335</v>
       </c>
       <c r="B35" s="12" t="s">
         <v>153</v>
@@ -3418,7 +3452,7 @@
         <v>7</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>7</v>
@@ -3430,7 +3464,7 @@
         <v>0</v>
       </c>
       <c r="J35" s="12" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="K35" s="9"/>
       <c r="L35" s="13">
@@ -3457,13 +3491,13 @@
     </row>
     <row r="36" spans="1:18">
       <c r="A36" s="11" t="s">
-        <v>283</v>
+        <v>336</v>
       </c>
       <c r="B36" s="12" t="s">
         <v>154</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>390</v>
+        <v>313</v>
       </c>
       <c r="D36" s="8" t="s">
         <v>251</v>
@@ -3472,7 +3506,7 @@
         <v>7</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>7</v>
@@ -3511,7 +3545,7 @@
     </row>
     <row r="37" spans="1:18">
       <c r="A37" s="11" t="s">
-        <v>284</v>
+        <v>337</v>
       </c>
       <c r="B37" s="12" t="s">
         <v>155</v>
@@ -3526,7 +3560,7 @@
         <v>7</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>7</v>
@@ -3538,7 +3572,7 @@
         <v>0</v>
       </c>
       <c r="J37" s="12" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="K37" s="9"/>
       <c r="L37" s="13">
@@ -3565,13 +3599,13 @@
     </row>
     <row r="38" spans="1:18">
       <c r="A38" s="11" t="s">
-        <v>285</v>
+        <v>338</v>
       </c>
       <c r="B38" s="12" t="s">
         <v>156</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>391</v>
+        <v>314</v>
       </c>
       <c r="D38" s="8" t="s">
         <v>251</v>
@@ -3580,7 +3614,7 @@
         <v>7</v>
       </c>
       <c r="F38" s="12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>7</v>
@@ -3619,7 +3653,7 @@
     </row>
     <row r="39" spans="1:18">
       <c r="A39" s="11" t="s">
-        <v>287</v>
+        <v>339</v>
       </c>
       <c r="B39" s="12" t="s">
         <v>157</v>
@@ -3634,7 +3668,7 @@
         <v>7</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>286</v>
+        <v>268</v>
       </c>
       <c r="G39" s="8" t="s">
         <v>7</v>
@@ -3646,7 +3680,7 @@
         <v>0</v>
       </c>
       <c r="J39" s="12" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="K39" s="9"/>
       <c r="L39" s="13">
@@ -3673,7 +3707,7 @@
     </row>
     <row r="40" spans="1:18">
       <c r="A40" s="11" t="s">
-        <v>288</v>
+        <v>340</v>
       </c>
       <c r="B40" s="12" t="s">
         <v>158</v>
@@ -3688,7 +3722,7 @@
         <v>7</v>
       </c>
       <c r="F40" s="12" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="G40" s="8" t="s">
         <v>7</v>
@@ -3700,7 +3734,7 @@
         <v>0</v>
       </c>
       <c r="J40" s="12" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="K40" s="9"/>
       <c r="L40" s="13">
@@ -3713,7 +3747,7 @@
         <v>47</v>
       </c>
       <c r="O40" s="8" t="s">
-        <v>400</v>
+        <v>322</v>
       </c>
       <c r="P40" s="8" t="s">
         <v>7</v>
@@ -3727,7 +3761,7 @@
     </row>
     <row r="41" spans="1:18">
       <c r="A41" s="11" t="s">
-        <v>290</v>
+        <v>341</v>
       </c>
       <c r="B41" s="12" t="s">
         <v>159</v>
@@ -3742,7 +3776,7 @@
         <v>7</v>
       </c>
       <c r="F41" s="12" t="s">
-        <v>289</v>
+        <v>269</v>
       </c>
       <c r="G41" s="8" t="s">
         <v>7</v>
@@ -3754,7 +3788,7 @@
         <v>0</v>
       </c>
       <c r="J41" s="12" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="K41" s="9"/>
       <c r="L41" s="13">
@@ -3781,7 +3815,7 @@
     </row>
     <row r="42" spans="1:18">
       <c r="A42" s="11" t="s">
-        <v>291</v>
+        <v>342</v>
       </c>
       <c r="B42" s="12" t="s">
         <v>160</v>
@@ -3796,7 +3830,7 @@
         <v>7</v>
       </c>
       <c r="F42" s="12" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="G42" s="8" t="s">
         <v>7</v>
@@ -3808,7 +3842,7 @@
         <v>0</v>
       </c>
       <c r="J42" s="12" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="K42" s="9"/>
       <c r="L42" s="13">
@@ -3835,10 +3869,10 @@
     </row>
     <row r="43" spans="1:18">
       <c r="A43" s="11" t="s">
-        <v>294</v>
+        <v>343</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>292</v>
+        <v>270</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>7</v>
@@ -3850,7 +3884,7 @@
         <v>7</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>293</v>
+        <v>271</v>
       </c>
       <c r="G43" s="8" t="s">
         <v>161</v>
@@ -3862,7 +3896,7 @@
         <v>0</v>
       </c>
       <c r="J43" s="12" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="K43" s="9"/>
       <c r="L43" s="13">
@@ -3889,7 +3923,7 @@
     </row>
     <row r="44" spans="1:18">
       <c r="A44" s="11" t="s">
-        <v>295</v>
+        <v>344</v>
       </c>
       <c r="B44" s="12" t="s">
         <v>162</v>
@@ -3904,7 +3938,7 @@
         <v>7</v>
       </c>
       <c r="F44" s="12" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G44" s="8" t="s">
         <v>7</v>
@@ -3916,7 +3950,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="12" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="K44" s="9"/>
       <c r="L44" s="13">
@@ -3943,7 +3977,7 @@
     </row>
     <row r="45" spans="1:18">
       <c r="A45" s="11" t="s">
-        <v>296</v>
+        <v>345</v>
       </c>
       <c r="B45" s="12" t="s">
         <v>163</v>
@@ -3958,7 +3992,7 @@
         <v>7</v>
       </c>
       <c r="F45" s="12" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="G45" s="8" t="s">
         <v>7</v>
@@ -3997,7 +4031,7 @@
     </row>
     <row r="46" spans="1:18">
       <c r="A46" s="11" t="s">
-        <v>297</v>
+        <v>346</v>
       </c>
       <c r="B46" s="12" t="s">
         <v>164</v>
@@ -4051,7 +4085,7 @@
     </row>
     <row r="47" spans="1:18">
       <c r="A47" s="11" t="s">
-        <v>298</v>
+        <v>347</v>
       </c>
       <c r="B47" s="12" t="s">
         <v>165</v>
@@ -4066,7 +4100,7 @@
         <v>7</v>
       </c>
       <c r="F47" s="12" t="s">
-        <v>289</v>
+        <v>269</v>
       </c>
       <c r="G47" s="8" t="s">
         <v>166</v>
@@ -4078,7 +4112,7 @@
         <v>0</v>
       </c>
       <c r="J47" s="12" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="K47" s="9"/>
       <c r="L47" s="13">
@@ -4088,10 +4122,10 @@
         <v>7</v>
       </c>
       <c r="N47" s="8" t="s">
-        <v>369</v>
+        <v>292</v>
       </c>
       <c r="O47" s="8" t="s">
-        <v>368</v>
+        <v>291</v>
       </c>
       <c r="P47" s="8" t="s">
         <v>7</v>
@@ -4105,22 +4139,22 @@
     </row>
     <row r="48" spans="1:18">
       <c r="A48" s="11" t="s">
-        <v>300</v>
+        <v>348</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>299</v>
+        <v>272</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>392</v>
+        <v>315</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>251</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>393</v>
+        <v>316</v>
       </c>
       <c r="F48" s="12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G48" s="8" t="s">
         <v>7</v>
@@ -4132,7 +4166,7 @@
         <v>0</v>
       </c>
       <c r="J48" s="12" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="K48" s="9"/>
       <c r="L48" s="13">
@@ -4159,7 +4193,7 @@
     </row>
     <row r="49" spans="1:18">
       <c r="A49" s="11" t="s">
-        <v>301</v>
+        <v>349</v>
       </c>
       <c r="B49" s="12" t="s">
         <v>167</v>
@@ -4174,7 +4208,7 @@
         <v>7</v>
       </c>
       <c r="F49" s="12" t="s">
-        <v>289</v>
+        <v>269</v>
       </c>
       <c r="G49" s="8" t="s">
         <v>7</v>
@@ -4186,7 +4220,7 @@
         <v>0</v>
       </c>
       <c r="J49" s="12" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="K49" s="9"/>
       <c r="L49" s="13">
@@ -4199,7 +4233,7 @@
         <v>47</v>
       </c>
       <c r="O49" s="8" t="s">
-        <v>370</v>
+        <v>293</v>
       </c>
       <c r="P49" s="8" t="s">
         <v>7</v>
@@ -4213,7 +4247,7 @@
     </row>
     <row r="50" spans="1:18">
       <c r="A50" s="11" t="s">
-        <v>302</v>
+        <v>350</v>
       </c>
       <c r="B50" s="12" t="s">
         <v>168</v>
@@ -4267,7 +4301,7 @@
     </row>
     <row r="51" spans="1:18">
       <c r="A51" s="11" t="s">
-        <v>303</v>
+        <v>351</v>
       </c>
       <c r="B51" s="12" t="s">
         <v>170</v>
@@ -4282,7 +4316,7 @@
         <v>7</v>
       </c>
       <c r="F51" s="12" t="s">
-        <v>289</v>
+        <v>269</v>
       </c>
       <c r="G51" s="8" t="s">
         <v>7</v>
@@ -4291,10 +4325,10 @@
         <v>7</v>
       </c>
       <c r="I51" s="13" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="J51" s="12" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="K51" s="9"/>
       <c r="L51" s="13">
@@ -4321,13 +4355,13 @@
     </row>
     <row r="52" spans="1:18">
       <c r="A52" s="11" t="s">
-        <v>304</v>
+        <v>352</v>
       </c>
       <c r="B52" s="12" t="s">
         <v>171</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>394</v>
+        <v>317</v>
       </c>
       <c r="D52" s="8" t="s">
         <v>251</v>
@@ -4336,7 +4370,7 @@
         <v>7</v>
       </c>
       <c r="F52" s="12" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="G52" s="8" t="s">
         <v>7</v>
@@ -4375,13 +4409,13 @@
     </row>
     <row r="53" spans="1:18">
       <c r="A53" s="11" t="s">
-        <v>305</v>
+        <v>353</v>
       </c>
       <c r="B53" s="12" t="s">
         <v>172</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>395</v>
+        <v>318</v>
       </c>
       <c r="D53" s="8" t="s">
         <v>251</v>
@@ -4390,7 +4424,7 @@
         <v>7</v>
       </c>
       <c r="F53" s="12" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="G53" s="8" t="s">
         <v>7</v>
@@ -4429,7 +4463,7 @@
     </row>
     <row r="54" spans="1:18">
       <c r="A54" s="11" t="s">
-        <v>306</v>
+        <v>354</v>
       </c>
       <c r="B54" s="12" t="s">
         <v>173</v>
@@ -4444,7 +4478,7 @@
         <v>7</v>
       </c>
       <c r="F54" s="12" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G54" s="8" t="s">
         <v>7</v>
@@ -4483,7 +4517,7 @@
     </row>
     <row r="55" spans="1:18">
       <c r="A55" s="11" t="s">
-        <v>307</v>
+        <v>355</v>
       </c>
       <c r="B55" s="12" t="s">
         <v>174</v>
@@ -4537,10 +4571,10 @@
     </row>
     <row r="56" spans="1:18">
       <c r="A56" s="11" t="s">
-        <v>309</v>
+        <v>394</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>308</v>
+        <v>273</v>
       </c>
       <c r="C56" s="8" t="s">
         <v>7</v>
@@ -4552,7 +4586,7 @@
         <v>7</v>
       </c>
       <c r="F56" s="12" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G56" s="8" t="s">
         <v>7</v>
@@ -4591,7 +4625,7 @@
     </row>
     <row r="57" spans="1:18">
       <c r="A57" s="11" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="B57" s="12" t="s">
         <v>175</v>
@@ -4606,7 +4640,7 @@
         <v>7</v>
       </c>
       <c r="F57" s="12" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="G57" s="8" t="s">
         <v>7</v>
@@ -4631,7 +4665,7 @@
         <v>78</v>
       </c>
       <c r="O57" s="8" t="s">
-        <v>371</v>
+        <v>294</v>
       </c>
       <c r="P57" s="8">
         <v>2003</v>
@@ -4645,7 +4679,7 @@
     </row>
     <row r="58" spans="1:18">
       <c r="A58" s="11" t="s">
-        <v>311</v>
+        <v>356</v>
       </c>
       <c r="B58" s="12" t="s">
         <v>176</v>
@@ -4660,7 +4694,7 @@
         <v>7</v>
       </c>
       <c r="F58" s="12" t="s">
-        <v>289</v>
+        <v>269</v>
       </c>
       <c r="G58" s="8" t="s">
         <v>177</v>
@@ -4669,10 +4703,10 @@
         <v>177</v>
       </c>
       <c r="I58" s="13" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="J58" s="12" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="K58" s="9"/>
       <c r="L58" s="13">
@@ -4699,7 +4733,7 @@
     </row>
     <row r="59" spans="1:18">
       <c r="A59" s="11" t="s">
-        <v>312</v>
+        <v>357</v>
       </c>
       <c r="B59" s="12" t="s">
         <v>178</v>
@@ -4714,7 +4748,7 @@
         <v>7</v>
       </c>
       <c r="F59" s="12" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G59" s="8" t="s">
         <v>127</v>
@@ -4753,7 +4787,7 @@
     </row>
     <row r="60" spans="1:18">
       <c r="A60" s="11" t="s">
-        <v>313</v>
+        <v>396</v>
       </c>
       <c r="B60" s="12" t="s">
         <v>179</v>
@@ -4768,7 +4802,7 @@
         <v>7</v>
       </c>
       <c r="F60" s="12" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="G60" s="8" t="s">
         <v>7</v>
@@ -4807,7 +4841,7 @@
     </row>
     <row r="61" spans="1:18">
       <c r="A61" s="11" t="s">
-        <v>314</v>
+        <v>397</v>
       </c>
       <c r="B61" s="12" t="s">
         <v>180</v>
@@ -4822,7 +4856,7 @@
         <v>7</v>
       </c>
       <c r="F61" s="12" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G61" s="8" t="s">
         <v>7</v>
@@ -4861,7 +4895,7 @@
     </row>
     <row r="62" spans="1:18">
       <c r="A62" s="11" t="s">
-        <v>315</v>
+        <v>358</v>
       </c>
       <c r="B62" s="12" t="s">
         <v>181</v>
@@ -4915,7 +4949,7 @@
     </row>
     <row r="63" spans="1:18">
       <c r="A63" s="11" t="s">
-        <v>316</v>
+        <v>359</v>
       </c>
       <c r="B63" s="12" t="s">
         <v>183</v>
@@ -4967,7 +5001,7 @@
     </row>
     <row r="64" spans="1:18">
       <c r="A64" s="11" t="s">
-        <v>318</v>
+        <v>360</v>
       </c>
       <c r="B64" s="12" t="s">
         <v>184</v>
@@ -4982,7 +5016,7 @@
         <v>7</v>
       </c>
       <c r="F64" s="12" t="s">
-        <v>317</v>
+        <v>274</v>
       </c>
       <c r="G64" s="8" t="s">
         <v>127</v>
@@ -5019,7 +5053,7 @@
     </row>
     <row r="65" spans="1:18">
       <c r="A65" s="11" t="s">
-        <v>319</v>
+        <v>361</v>
       </c>
       <c r="B65" s="12" t="s">
         <v>185</v>
@@ -5034,7 +5068,7 @@
         <v>7</v>
       </c>
       <c r="F65" s="12" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="G65" s="8" t="s">
         <v>186</v>
@@ -5073,7 +5107,7 @@
     </row>
     <row r="66" spans="1:18">
       <c r="A66" s="11" t="s">
-        <v>320</v>
+        <v>362</v>
       </c>
       <c r="B66" s="12" t="s">
         <v>187</v>
@@ -5127,10 +5161,10 @@
     </row>
     <row r="67" spans="1:18">
       <c r="A67" s="11" t="s">
-        <v>322</v>
+        <v>363</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>321</v>
+        <v>275</v>
       </c>
       <c r="C67" s="8" t="s">
         <v>7</v>
@@ -5142,7 +5176,7 @@
         <v>7</v>
       </c>
       <c r="F67" s="12" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G67" s="8" t="s">
         <v>188</v>
@@ -5154,7 +5188,7 @@
         <v>0</v>
       </c>
       <c r="J67" s="12" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="K67" s="9"/>
       <c r="L67" s="13">
@@ -5181,7 +5215,7 @@
     </row>
     <row r="68" spans="1:18">
       <c r="A68" s="11" t="s">
-        <v>323</v>
+        <v>364</v>
       </c>
       <c r="B68" s="12" t="s">
         <v>189</v>
@@ -5196,7 +5230,7 @@
         <v>7</v>
       </c>
       <c r="F68" s="12" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="G68" s="8" t="s">
         <v>190</v>
@@ -5221,7 +5255,7 @@
         <v>78</v>
       </c>
       <c r="O68" s="8" t="s">
-        <v>372</v>
+        <v>295</v>
       </c>
       <c r="P68" s="8">
         <v>2003</v>
@@ -5235,7 +5269,7 @@
     </row>
     <row r="69" spans="1:18">
       <c r="A69" s="11" t="s">
-        <v>324</v>
+        <v>398</v>
       </c>
       <c r="B69" s="12" t="s">
         <v>191</v>
@@ -5333,7 +5367,7 @@
     </row>
     <row r="71" spans="1:18">
       <c r="A71" s="11" t="s">
-        <v>325</v>
+        <v>365</v>
       </c>
       <c r="B71" s="12" t="s">
         <v>194</v>
@@ -5348,7 +5382,7 @@
         <v>7</v>
       </c>
       <c r="F71" s="12" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="G71" s="8" t="s">
         <v>127</v>
@@ -5385,7 +5419,7 @@
     </row>
     <row r="72" spans="1:18">
       <c r="A72" s="11" t="s">
-        <v>326</v>
+        <v>401</v>
       </c>
       <c r="B72" s="12" t="s">
         <v>195</v>
@@ -5439,7 +5473,7 @@
     </row>
     <row r="73" spans="1:18">
       <c r="A73" s="11" t="s">
-        <v>327</v>
+        <v>366</v>
       </c>
       <c r="B73" s="12" t="s">
         <v>196</v>
@@ -5454,10 +5488,10 @@
         <v>7</v>
       </c>
       <c r="F73" s="12" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G73" s="8" t="s">
-        <v>401</v>
+        <v>323</v>
       </c>
       <c r="H73" s="8" t="s">
         <v>197</v>
@@ -5466,7 +5500,7 @@
         <v>0</v>
       </c>
       <c r="J73" s="12" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="K73" s="9"/>
       <c r="L73" s="13">
@@ -5493,7 +5527,7 @@
     </row>
     <row r="74" spans="1:18">
       <c r="A74" s="11" t="s">
-        <v>329</v>
+        <v>367</v>
       </c>
       <c r="B74" s="12" t="s">
         <v>198</v>
@@ -5508,7 +5542,7 @@
         <v>7</v>
       </c>
       <c r="F74" s="12" t="s">
-        <v>328</v>
+        <v>276</v>
       </c>
       <c r="G74" s="8" t="s">
         <v>221</v>
@@ -5520,7 +5554,7 @@
         <v>0</v>
       </c>
       <c r="J74" s="12" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="K74" s="9"/>
       <c r="L74" s="13">
@@ -5547,7 +5581,7 @@
     </row>
     <row r="75" spans="1:18">
       <c r="A75" s="11" t="s">
-        <v>330</v>
+        <v>368</v>
       </c>
       <c r="B75" s="12" t="s">
         <v>200</v>
@@ -5562,7 +5596,7 @@
         <v>7</v>
       </c>
       <c r="F75" s="12" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="G75" s="8" t="s">
         <v>201</v>
@@ -5601,7 +5635,7 @@
     </row>
     <row r="76" spans="1:18">
       <c r="A76" s="11" t="s">
-        <v>331</v>
+        <v>369</v>
       </c>
       <c r="B76" s="12" t="s">
         <v>202</v>
@@ -5616,7 +5650,7 @@
         <v>7</v>
       </c>
       <c r="F76" s="12" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="G76" s="8" t="s">
         <v>203</v>
@@ -5628,7 +5662,7 @@
         <v>0</v>
       </c>
       <c r="J76" s="12" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="K76" s="9"/>
       <c r="L76" s="13">
@@ -5655,7 +5689,7 @@
     </row>
     <row r="77" spans="1:18">
       <c r="A77" s="11" t="s">
-        <v>332</v>
+        <v>370</v>
       </c>
       <c r="B77" s="12" t="s">
         <v>204</v>
@@ -5670,7 +5704,7 @@
         <v>7</v>
       </c>
       <c r="F77" s="12" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="G77" s="8" t="s">
         <v>205</v>
@@ -5682,7 +5716,7 @@
         <v>0</v>
       </c>
       <c r="J77" s="12" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="K77" s="9"/>
       <c r="L77" s="13">
@@ -5709,7 +5743,7 @@
     </row>
     <row r="78" spans="1:18">
       <c r="A78" s="11" t="s">
-        <v>333</v>
+        <v>371</v>
       </c>
       <c r="B78" s="12" t="s">
         <v>206</v>
@@ -5736,7 +5770,7 @@
         <v>0</v>
       </c>
       <c r="J78" s="12" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="K78" s="9"/>
       <c r="L78" s="13">
@@ -5763,7 +5797,7 @@
     </row>
     <row r="79" spans="1:18">
       <c r="A79" s="11" t="s">
-        <v>334</v>
+        <v>372</v>
       </c>
       <c r="B79" s="12" t="s">
         <v>207</v>
@@ -5778,7 +5812,7 @@
         <v>7</v>
       </c>
       <c r="F79" s="12" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G79" s="8"/>
       <c r="H79" s="9"/>
@@ -5798,10 +5832,10 @@
         <v>7</v>
       </c>
       <c r="N79" s="8" t="s">
-        <v>374</v>
+        <v>297</v>
       </c>
       <c r="O79" s="8" t="s">
-        <v>373</v>
+        <v>296</v>
       </c>
       <c r="P79" s="8">
         <v>1969</v>
@@ -5815,7 +5849,7 @@
     </row>
     <row r="80" spans="1:18">
       <c r="A80" s="11" t="s">
-        <v>335</v>
+        <v>373</v>
       </c>
       <c r="B80" s="12" t="s">
         <v>209</v>
@@ -5830,7 +5864,7 @@
         <v>7</v>
       </c>
       <c r="F80" s="12" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G80" s="8"/>
       <c r="H80" s="9"/>
@@ -5850,10 +5884,10 @@
         <v>7</v>
       </c>
       <c r="N80" s="8" t="s">
-        <v>374</v>
+        <v>297</v>
       </c>
       <c r="O80" s="8" t="s">
-        <v>375</v>
+        <v>298</v>
       </c>
       <c r="P80" s="8">
         <v>1989</v>
@@ -5899,7 +5933,7 @@
         <v>86</v>
       </c>
       <c r="O81" s="8" t="s">
-        <v>376</v>
+        <v>299</v>
       </c>
       <c r="P81" s="8">
         <v>2010</v>
@@ -5913,7 +5947,7 @@
     </row>
     <row r="82" spans="1:18">
       <c r="A82" s="11" t="s">
-        <v>337</v>
+        <v>399</v>
       </c>
       <c r="B82" s="12" t="s">
         <v>213</v>
@@ -5926,7 +5960,7 @@
         <v>7</v>
       </c>
       <c r="F82" s="12" t="s">
-        <v>336</v>
+        <v>277</v>
       </c>
       <c r="G82" s="8" t="s">
         <v>214</v>
@@ -5938,7 +5972,7 @@
         <v>0</v>
       </c>
       <c r="J82" s="12" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="K82" s="9"/>
       <c r="L82" s="13">
@@ -6011,7 +6045,7 @@
     </row>
     <row r="84" spans="1:18">
       <c r="A84" s="11" t="s">
-        <v>338</v>
+        <v>374</v>
       </c>
       <c r="B84" s="12" t="s">
         <v>217</v>
@@ -6026,7 +6060,7 @@
         <v>7</v>
       </c>
       <c r="F84" s="12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G84" s="8" t="s">
         <v>218</v>
@@ -6038,7 +6072,7 @@
         <v>0</v>
       </c>
       <c r="J84" s="12" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="K84" s="9"/>
       <c r="L84" s="13">
@@ -6051,7 +6085,7 @@
         <v>23</v>
       </c>
       <c r="O84" s="8" t="s">
-        <v>377</v>
+        <v>300</v>
       </c>
       <c r="P84" s="8">
         <v>2010</v>
@@ -6068,7 +6102,7 @@
         <v>74</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>339</v>
+        <v>278</v>
       </c>
       <c r="C85" s="8" t="s">
         <v>7</v>
@@ -6149,7 +6183,7 @@
     </row>
     <row r="87" spans="1:18">
       <c r="A87" s="11" t="s">
-        <v>340</v>
+        <v>375</v>
       </c>
       <c r="B87" s="12" t="s">
         <v>220</v>
@@ -6162,7 +6196,7 @@
         <v>7</v>
       </c>
       <c r="F87" s="12" t="s">
-        <v>328</v>
+        <v>276</v>
       </c>
       <c r="G87" s="8" t="s">
         <v>221</v>
@@ -6174,7 +6208,7 @@
         <v>0</v>
       </c>
       <c r="J87" s="12" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="K87" s="9"/>
       <c r="L87" s="13">
@@ -6201,7 +6235,7 @@
     </row>
     <row r="88" spans="1:18">
       <c r="A88" s="11" t="s">
-        <v>341</v>
+        <v>376</v>
       </c>
       <c r="B88" s="12" t="s">
         <v>222</v>
@@ -6216,7 +6250,7 @@
         <v>7</v>
       </c>
       <c r="F88" s="12" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="G88" s="8" t="s">
         <v>223</v>
@@ -6228,7 +6262,7 @@
         <v>0</v>
       </c>
       <c r="J88" s="12" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="K88" s="9"/>
       <c r="L88" s="13">
@@ -6241,7 +6275,7 @@
         <v>47</v>
       </c>
       <c r="O88" s="8" t="s">
-        <v>381</v>
+        <v>304</v>
       </c>
       <c r="P88" s="8">
         <v>2013</v>
@@ -6255,7 +6289,7 @@
     </row>
     <row r="89" spans="1:18">
       <c r="A89" s="11" t="s">
-        <v>342</v>
+        <v>377</v>
       </c>
       <c r="B89" s="12" t="s">
         <v>224</v>
@@ -6270,7 +6304,7 @@
         <v>7</v>
       </c>
       <c r="F89" s="12" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="G89" s="8" t="s">
         <v>223</v>
@@ -6282,7 +6316,7 @@
         <v>0</v>
       </c>
       <c r="J89" s="12" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="K89" s="9"/>
       <c r="L89" s="13">
@@ -6295,7 +6329,7 @@
         <v>47</v>
       </c>
       <c r="O89" s="8" t="s">
-        <v>381</v>
+        <v>304</v>
       </c>
       <c r="P89" s="8">
         <v>2012</v>
@@ -6309,7 +6343,7 @@
     </row>
     <row r="90" spans="1:18">
       <c r="A90" s="11" t="s">
-        <v>343</v>
+        <v>378</v>
       </c>
       <c r="B90" s="12" t="s">
         <v>225</v>
@@ -6324,7 +6358,7 @@
         <v>7</v>
       </c>
       <c r="F90" s="12" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="G90" s="8" t="s">
         <v>223</v>
@@ -6336,7 +6370,7 @@
         <v>0</v>
       </c>
       <c r="J90" s="12" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="K90" s="9"/>
       <c r="L90" s="13">
@@ -6349,7 +6383,7 @@
         <v>47</v>
       </c>
       <c r="O90" s="8" t="s">
-        <v>381</v>
+        <v>304</v>
       </c>
       <c r="P90" s="8">
         <v>2013</v>
@@ -6363,7 +6397,7 @@
     </row>
     <row r="91" spans="1:18">
       <c r="A91" s="11" t="s">
-        <v>344</v>
+        <v>379</v>
       </c>
       <c r="B91" s="12" t="s">
         <v>226</v>
@@ -6378,7 +6412,7 @@
         <v>7</v>
       </c>
       <c r="F91" s="12" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="G91" s="8" t="s">
         <v>223</v>
@@ -6390,7 +6424,7 @@
         <v>0</v>
       </c>
       <c r="J91" s="12" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="K91" s="9"/>
       <c r="L91" s="13">
@@ -6403,7 +6437,7 @@
         <v>47</v>
       </c>
       <c r="O91" s="8" t="s">
-        <v>381</v>
+        <v>304</v>
       </c>
       <c r="P91" s="8">
         <v>2012</v>
@@ -6417,7 +6451,7 @@
     </row>
     <row r="92" spans="1:18">
       <c r="A92" s="11" t="s">
-        <v>345</v>
+        <v>380</v>
       </c>
       <c r="B92" s="12" t="s">
         <v>227</v>
@@ -6432,7 +6466,7 @@
         <v>7</v>
       </c>
       <c r="F92" s="12" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="G92" s="8" t="s">
         <v>228</v>
@@ -6444,7 +6478,7 @@
         <v>0</v>
       </c>
       <c r="J92" s="12" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="K92" s="9"/>
       <c r="L92" s="13">
@@ -6471,7 +6505,7 @@
     </row>
     <row r="93" spans="1:18">
       <c r="A93" s="11" t="s">
-        <v>346</v>
+        <v>381</v>
       </c>
       <c r="B93" s="12" t="s">
         <v>229</v>
@@ -6525,7 +6559,7 @@
     </row>
     <row r="94" spans="1:18">
       <c r="A94" s="11" t="s">
-        <v>347</v>
+        <v>382</v>
       </c>
       <c r="B94" s="12" t="s">
         <v>231</v>
@@ -6540,7 +6574,7 @@
         <v>7</v>
       </c>
       <c r="F94" s="12" t="s">
-        <v>289</v>
+        <v>269</v>
       </c>
       <c r="G94" s="8" t="s">
         <v>232</v>
@@ -6549,10 +6583,10 @@
         <v>232</v>
       </c>
       <c r="I94" s="13" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="J94" s="12" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="K94" s="9"/>
       <c r="L94" s="13">
@@ -6579,7 +6613,7 @@
     </row>
     <row r="95" spans="1:18">
       <c r="A95" s="11" t="s">
-        <v>348</v>
+        <v>383</v>
       </c>
       <c r="B95" s="12" t="s">
         <v>233</v>
@@ -6594,7 +6628,7 @@
         <v>7</v>
       </c>
       <c r="F95" s="12" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G95" s="8" t="s">
         <v>188</v>
@@ -6606,7 +6640,7 @@
         <v>0</v>
       </c>
       <c r="J95" s="12" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="K95" s="9"/>
       <c r="L95" s="13">
@@ -6633,7 +6667,7 @@
     </row>
     <row r="96" spans="1:18">
       <c r="A96" s="11" t="s">
-        <v>349</v>
+        <v>384</v>
       </c>
       <c r="B96" s="12" t="s">
         <v>234</v>
@@ -6687,7 +6721,7 @@
     </row>
     <row r="97" spans="1:18">
       <c r="A97" s="11" t="s">
-        <v>350</v>
+        <v>385</v>
       </c>
       <c r="B97" s="12" t="s">
         <v>236</v>
@@ -6702,7 +6736,7 @@
         <v>7</v>
       </c>
       <c r="F97" s="12" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="G97" s="8" t="s">
         <v>7</v>
@@ -6741,7 +6775,7 @@
     </row>
     <row r="98" spans="1:18">
       <c r="A98" s="11" t="s">
-        <v>351</v>
+        <v>386</v>
       </c>
       <c r="B98" s="12" t="s">
         <v>237</v>
@@ -6756,7 +6790,7 @@
         <v>7</v>
       </c>
       <c r="F98" s="12" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="G98" s="8" t="s">
         <v>216</v>
@@ -6795,7 +6829,7 @@
     </row>
     <row r="99" spans="1:18">
       <c r="A99" s="11" t="s">
-        <v>352</v>
+        <v>400</v>
       </c>
       <c r="B99" s="12" t="s">
         <v>238</v>
@@ -6810,7 +6844,7 @@
         <v>7</v>
       </c>
       <c r="F99" s="12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G99" s="8" t="s">
         <v>169</v>
@@ -6822,7 +6856,7 @@
         <v>0</v>
       </c>
       <c r="J99" s="12" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="K99" s="9"/>
       <c r="L99" s="13">
@@ -6849,7 +6883,7 @@
     </row>
     <row r="100" spans="1:18">
       <c r="A100" s="11" t="s">
-        <v>354</v>
+        <v>387</v>
       </c>
       <c r="B100" s="12" t="s">
         <v>239</v>
@@ -6864,7 +6898,7 @@
         <v>7</v>
       </c>
       <c r="F100" s="12" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="G100" s="8" t="s">
         <v>240</v>
@@ -6876,7 +6910,7 @@
         <v>0</v>
       </c>
       <c r="J100" s="12" t="s">
-        <v>353</v>
+        <v>279</v>
       </c>
       <c r="K100" s="9"/>
       <c r="L100" s="13">
@@ -6903,7 +6937,7 @@
     </row>
     <row r="101" spans="1:18">
       <c r="A101" s="11" t="s">
-        <v>355</v>
+        <v>388</v>
       </c>
       <c r="B101" s="12" t="s">
         <v>241</v>
@@ -7003,10 +7037,10 @@
     </row>
     <row r="103" spans="1:18">
       <c r="A103" s="11" t="s">
-        <v>358</v>
+        <v>389</v>
       </c>
       <c r="B103" s="12" t="s">
-        <v>356</v>
+        <v>280</v>
       </c>
       <c r="C103" s="8" t="s">
         <v>7</v>
@@ -7016,7 +7050,7 @@
         <v>7</v>
       </c>
       <c r="F103" s="12" t="s">
-        <v>357</v>
+        <v>281</v>
       </c>
       <c r="G103" s="8" t="s">
         <v>127</v>
@@ -7041,7 +7075,7 @@
         <v>10</v>
       </c>
       <c r="O103" s="8" t="s">
-        <v>380</v>
+        <v>303</v>
       </c>
       <c r="P103" s="8">
         <v>1998</v>
@@ -7058,7 +7092,7 @@
         <v>98</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>359</v>
+        <v>282</v>
       </c>
       <c r="C104" s="8" t="s">
         <v>7</v>
@@ -7307,7 +7341,7 @@
         <v>10</v>
       </c>
       <c r="O109" s="8" t="s">
-        <v>379</v>
+        <v>302</v>
       </c>
       <c r="P109" s="8" t="s">
         <v>7</v>
@@ -7368,7 +7402,7 @@
         <v>107</v>
       </c>
       <c r="B111" s="16" t="s">
-        <v>360</v>
+        <v>283</v>
       </c>
       <c r="C111" s="17" t="s">
         <v>7</v>
@@ -7379,10 +7413,10 @@
       </c>
       <c r="F111" s="16"/>
       <c r="G111" s="17" t="s">
-        <v>396</v>
+        <v>319</v>
       </c>
       <c r="H111" s="17" t="s">
-        <v>396</v>
+        <v>319</v>
       </c>
       <c r="I111" s="17"/>
       <c r="J111" s="16"/>
@@ -7395,7 +7429,7 @@
         <v>10</v>
       </c>
       <c r="O111" s="17" t="s">
-        <v>378</v>
+        <v>301</v>
       </c>
       <c r="P111" s="17" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
added SbCNV and GKaV accession numbers
</commit_message>
<xml_diff>
--- a/tabular/flavi-ncbi-refseqs-side-data.xlsx
+++ b/tabular/flavi-ncbi-refseqs-side-data.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11014"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus-group/Flaviviridae-GLUE/tabular/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF4836B-D38D-6844-B927-5E1E68307B1F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="0" windowWidth="32880" windowHeight="24940" tabRatio="500"/>
+    <workbookView xWindow="940" yWindow="460" windowWidth="27860" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="flavi.txt" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1467" uniqueCount="638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1542" uniqueCount="656">
   <si>
     <t>isolate</t>
   </si>
@@ -1933,12 +1939,66 @@
   </si>
   <si>
     <t>JEV</t>
+  </si>
+  <si>
+    <t>Africa/Southeast Asia</t>
+  </si>
+  <si>
+    <t>South America/Africa</t>
+  </si>
+  <si>
+    <t>Europe/Asia</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>Asia</t>
+  </si>
+  <si>
+    <t>Americas</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>Africa</t>
+  </si>
+  <si>
+    <t>Oceania</t>
+  </si>
+  <si>
+    <t>Africa/Asia</t>
+  </si>
+  <si>
+    <t>Africa/Americas</t>
+  </si>
+  <si>
+    <t>NC_020252</t>
+  </si>
+  <si>
+    <t>Pesti-like</t>
+  </si>
+  <si>
+    <t>Soybean cyst nematode virus</t>
+  </si>
+  <si>
+    <t>SbCNV-5</t>
+  </si>
+  <si>
+    <t>GKaV</t>
+  </si>
+  <si>
+    <t>gentian Kobu-sho-associated virus</t>
+  </si>
+  <si>
+    <t>NC_024077</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1951,10 +2011,12 @@
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -1981,6 +2043,7 @@
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -2258,7 +2321,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2345,6 +2408,9 @@
     <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="85">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2767,28 +2833,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R111"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.83203125" customWidth="1"/>
     <col min="2" max="2" width="35.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" style="1" customWidth="1"/>
-    <col min="7" max="8" width="36.5" customWidth="1"/>
-    <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="17.83203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5" customWidth="1"/>
-    <col min="13" max="13" width="18.1640625" customWidth="1"/>
-    <col min="14" max="14" width="23.6640625" customWidth="1"/>
-    <col min="18" max="18" width="20.6640625" customWidth="1"/>
+    <col min="6" max="6" width="5.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5" customWidth="1"/>
+    <col min="8" max="8" width="6.83203125" customWidth="1"/>
+    <col min="9" max="9" width="4.33203125" customWidth="1"/>
+    <col min="10" max="10" width="7.1640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="6.5" customWidth="1"/>
+    <col min="13" max="13" width="7.33203125" customWidth="1"/>
+    <col min="14" max="15" width="23.6640625" customWidth="1"/>
+    <col min="19" max="19" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>311</v>
       </c>
@@ -2832,19 +2900,22 @@
         <v>1</v>
       </c>
       <c r="O1" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>351</v>
       </c>
@@ -2886,19 +2957,22 @@
         <v>76</v>
       </c>
       <c r="O2" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="P2" s="8" t="s">
         <v>287</v>
       </c>
-      <c r="P2" s="8">
+      <c r="Q2" s="8">
         <v>2003</v>
       </c>
-      <c r="Q2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R2" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18">
+      <c r="R2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S2" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>380</v>
       </c>
@@ -2940,19 +3014,22 @@
         <v>46</v>
       </c>
       <c r="O3" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="P3" s="8" t="s">
         <v>463</v>
       </c>
-      <c r="P3" s="8">
+      <c r="Q3" s="8">
         <v>2012</v>
       </c>
-      <c r="Q3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R3" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18">
+      <c r="R3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S3" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>382</v>
       </c>
@@ -2994,19 +3071,22 @@
         <v>76</v>
       </c>
       <c r="O4" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="P4" s="8" t="s">
         <v>286</v>
       </c>
-      <c r="P4" s="8">
+      <c r="Q4" s="8">
         <v>2003</v>
       </c>
-      <c r="Q4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R4" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
+      <c r="R4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S4" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>24</v>
       </c>
@@ -3044,19 +3124,22 @@
         <v>297</v>
       </c>
       <c r="O5" s="8" t="s">
+        <v>644</v>
+      </c>
+      <c r="P5" s="8" t="s">
         <v>298</v>
       </c>
-      <c r="P5" s="8">
+      <c r="Q5" s="8">
         <v>2011</v>
       </c>
-      <c r="Q5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R5" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18">
+      <c r="R5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S5" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>26</v>
       </c>
@@ -3094,19 +3177,22 @@
         <v>27</v>
       </c>
       <c r="O6" s="8" t="s">
+        <v>644</v>
+      </c>
+      <c r="P6" s="8" t="s">
         <v>430</v>
       </c>
-      <c r="P6" s="8">
+      <c r="Q6" s="8">
         <v>2005</v>
       </c>
-      <c r="Q6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R6" s="10" t="s">
+      <c r="R6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S6" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>340</v>
       </c>
@@ -3148,19 +3234,22 @@
         <v>485</v>
       </c>
       <c r="O7" s="8" t="s">
+        <v>645</v>
+      </c>
+      <c r="P7" s="8" t="s">
         <v>507</v>
       </c>
-      <c r="P7" s="8">
+      <c r="Q7" s="8">
         <v>1999</v>
       </c>
-      <c r="Q7" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R7" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18">
+      <c r="R7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S7" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
         <v>373</v>
       </c>
@@ -3202,19 +3291,22 @@
         <v>91</v>
       </c>
       <c r="O8" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="P8" s="8" t="s">
         <v>585</v>
       </c>
-      <c r="P8" s="8">
+      <c r="Q8" s="8">
         <v>2011</v>
       </c>
-      <c r="Q8" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R8" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18">
+      <c r="R8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S8" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>355</v>
       </c>
@@ -3256,19 +3348,22 @@
         <v>56</v>
       </c>
       <c r="O9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="P9" s="8">
+        <v>642</v>
+      </c>
+      <c r="P9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q9" s="8">
         <v>2009</v>
       </c>
-      <c r="Q9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R9" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18">
+      <c r="R9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S9" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>22</v>
       </c>
@@ -3308,19 +3403,22 @@
         <v>23</v>
       </c>
       <c r="O10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="P10" s="8">
+        <v>645</v>
+      </c>
+      <c r="P10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q10" s="8">
         <v>2008</v>
       </c>
-      <c r="Q10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R10" s="10" t="s">
+      <c r="R10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S10" s="10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>68</v>
       </c>
@@ -3356,19 +3454,22 @@
         <v>21</v>
       </c>
       <c r="O11" s="8" t="s">
+        <v>645</v>
+      </c>
+      <c r="P11" s="8" t="s">
         <v>421</v>
       </c>
-      <c r="P11" s="8">
+      <c r="Q11" s="8">
         <v>2004</v>
       </c>
-      <c r="Q11" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R11" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18">
+      <c r="R11" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S11" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>31</v>
       </c>
@@ -3406,19 +3507,22 @@
         <v>10</v>
       </c>
       <c r="O12" s="8" t="s">
+        <v>646</v>
+      </c>
+      <c r="P12" s="8" t="s">
         <v>433</v>
       </c>
-      <c r="P12" s="8">
+      <c r="Q12" s="8">
         <v>2010</v>
       </c>
-      <c r="Q12" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R12" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18">
+      <c r="R12" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S12" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>372</v>
       </c>
@@ -3460,19 +3564,22 @@
         <v>10</v>
       </c>
       <c r="O13" s="8" t="s">
+        <v>646</v>
+      </c>
+      <c r="P13" s="8" t="s">
         <v>583</v>
       </c>
-      <c r="P13" s="8">
+      <c r="Q13" s="8">
         <v>2007</v>
       </c>
-      <c r="Q13" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R13" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18">
+      <c r="R13" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S13" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>348</v>
       </c>
@@ -3514,19 +3621,22 @@
         <v>55</v>
       </c>
       <c r="O14" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="P14" s="8">
+        <v>642</v>
+      </c>
+      <c r="P14" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q14" s="8">
         <v>2002</v>
       </c>
-      <c r="Q14" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R14" s="10" t="s">
+      <c r="R14" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S14" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>41</v>
       </c>
@@ -3564,19 +3674,22 @@
         <v>43</v>
       </c>
       <c r="O15" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="P15" s="8">
+        <v>644</v>
+      </c>
+      <c r="P15" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q15" s="8">
         <v>2007</v>
       </c>
-      <c r="Q15" s="8">
+      <c r="R15" s="8">
         <v>1</v>
       </c>
-      <c r="R15" s="10" t="s">
+      <c r="S15" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>374</v>
       </c>
@@ -3618,19 +3731,22 @@
         <v>94</v>
       </c>
       <c r="O16" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="P16" s="8" t="s">
         <v>588</v>
       </c>
-      <c r="P16" s="8">
+      <c r="Q16" s="8">
         <v>2012</v>
       </c>
-      <c r="Q16" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R16" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18">
+      <c r="R16" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S16" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>352</v>
       </c>
@@ -3670,19 +3786,22 @@
         <v>56</v>
       </c>
       <c r="O17" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="P17" s="8">
+        <v>642</v>
+      </c>
+      <c r="P17" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q17" s="8">
         <v>2010</v>
       </c>
-      <c r="Q17" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R17" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18">
+      <c r="R17" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S17" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>57</v>
       </c>
@@ -3718,19 +3837,22 @@
         <v>56</v>
       </c>
       <c r="O18" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="P18" s="8">
+        <v>642</v>
+      </c>
+      <c r="P18" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q18" s="8">
         <v>2009</v>
       </c>
-      <c r="Q18" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R18" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18">
+      <c r="R18" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S18" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>72</v>
       </c>
@@ -3764,19 +3886,22 @@
         <v>27</v>
       </c>
       <c r="O19" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="P19" s="8">
+        <v>644</v>
+      </c>
+      <c r="P19" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q19" s="8">
         <v>2007</v>
       </c>
-      <c r="Q19" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R19" s="10" t="s">
+      <c r="R19" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S19" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>74</v>
       </c>
@@ -3810,19 +3935,22 @@
         <v>27</v>
       </c>
       <c r="O20" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="P20" s="8">
+        <v>644</v>
+      </c>
+      <c r="P20" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q20" s="8">
         <v>2007</v>
       </c>
-      <c r="Q20" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R20" s="10" t="s">
+      <c r="R20" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S20" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>66</v>
       </c>
@@ -3860,19 +3988,22 @@
         <v>84</v>
       </c>
       <c r="O21" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="P21" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="P21" s="8">
+      <c r="Q21" s="8">
         <v>2010</v>
       </c>
-      <c r="Q21" s="8">
+      <c r="R21" s="8">
         <v>17</v>
       </c>
-      <c r="R21" s="10" t="s">
+      <c r="S21" s="10" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>20</v>
       </c>
@@ -3910,19 +4041,22 @@
         <v>21</v>
       </c>
       <c r="O22" s="8" t="s">
+        <v>645</v>
+      </c>
+      <c r="P22" s="8" t="s">
         <v>421</v>
       </c>
-      <c r="P22" s="8">
+      <c r="Q22" s="8">
         <v>2004</v>
       </c>
-      <c r="Q22" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R22" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18">
+      <c r="R22" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S22" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>9</v>
       </c>
@@ -3960,19 +4094,22 @@
         <v>10</v>
       </c>
       <c r="O23" s="8" t="s">
+        <v>646</v>
+      </c>
+      <c r="P23" s="8" t="s">
         <v>399</v>
       </c>
-      <c r="P23" s="8">
+      <c r="Q23" s="8">
         <v>1966</v>
       </c>
-      <c r="Q23" s="8">
+      <c r="R23" s="8">
         <v>4</v>
       </c>
-      <c r="R23" s="10" t="s">
+      <c r="S23" s="10" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>347</v>
       </c>
@@ -4012,19 +4149,22 @@
         <v>53</v>
       </c>
       <c r="O24" s="8" t="s">
+        <v>645</v>
+      </c>
+      <c r="P24" s="8" t="s">
         <v>543</v>
       </c>
-      <c r="P24" s="8">
+      <c r="Q24" s="8">
         <v>1966</v>
       </c>
-      <c r="Q24" s="8">
+      <c r="R24" s="8">
         <v>31</v>
       </c>
-      <c r="R24" s="10" t="s">
+      <c r="S24" s="10" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>33</v>
       </c>
@@ -4062,19 +4202,22 @@
         <v>34</v>
       </c>
       <c r="O25" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="P25" s="8">
+        <v>646</v>
+      </c>
+      <c r="P25" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q25" s="8">
         <v>1966</v>
       </c>
-      <c r="Q25" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R25" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18">
+      <c r="R25" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S25" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>14</v>
       </c>
@@ -4110,19 +4253,22 @@
         <v>15</v>
       </c>
       <c r="O26" s="8" t="s">
+        <v>645</v>
+      </c>
+      <c r="P26" s="8" t="s">
         <v>408</v>
       </c>
-      <c r="P26" s="8">
+      <c r="Q26" s="8">
         <v>1956</v>
       </c>
-      <c r="Q26" s="8">
+      <c r="R26" s="8">
         <v>28</v>
       </c>
-      <c r="R26" s="10" t="s">
+      <c r="S26" s="10" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>28</v>
       </c>
@@ -4160,19 +4306,22 @@
         <v>30</v>
       </c>
       <c r="O27" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="P27" s="8">
+        <v>642</v>
+      </c>
+      <c r="P27" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q27" s="8">
         <v>2011</v>
       </c>
-      <c r="Q27" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R27" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18">
+      <c r="R27" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S27" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>96</v>
       </c>
@@ -4208,19 +4357,22 @@
         <v>53</v>
       </c>
       <c r="O28" s="8" t="s">
+        <v>645</v>
+      </c>
+      <c r="P28" s="8" t="s">
         <v>603</v>
       </c>
-      <c r="P28" s="8">
+      <c r="Q28" s="8">
         <v>1967</v>
       </c>
-      <c r="Q28" s="8">
+      <c r="R28" s="8">
         <v>2</v>
       </c>
-      <c r="R28" s="10" t="s">
+      <c r="S28" s="10" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
         <v>383</v>
       </c>
@@ -4262,19 +4414,22 @@
         <v>84</v>
       </c>
       <c r="O29" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="P29" s="8">
+        <v>643</v>
+      </c>
+      <c r="P29" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q29" s="8">
         <v>1956</v>
       </c>
-      <c r="Q29" s="8">
+      <c r="R29" s="8">
         <v>2</v>
       </c>
-      <c r="R29" s="10" t="s">
+      <c r="S29" s="10" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
         <v>368</v>
       </c>
@@ -4316,19 +4471,22 @@
         <v>84</v>
       </c>
       <c r="O30" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="P30" s="8" t="s">
         <v>573</v>
       </c>
-      <c r="P30" s="8">
+      <c r="Q30" s="8">
         <v>1977</v>
       </c>
-      <c r="Q30" s="8">
+      <c r="R30" s="8">
         <v>28</v>
       </c>
-      <c r="R30" s="10" t="s">
+      <c r="S30" s="10" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
         <v>318</v>
       </c>
@@ -4367,10 +4525,10 @@
         <v>459</v>
       </c>
       <c r="N31" s="8" t="s">
-        <v>7</v>
+        <v>638</v>
       </c>
       <c r="O31" s="8" t="s">
-        <v>7</v>
+        <v>647</v>
       </c>
       <c r="P31" s="8" t="s">
         <v>7</v>
@@ -4378,11 +4536,14 @@
       <c r="Q31" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="R31" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18">
+      <c r="R31" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S31" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>377</v>
       </c>
@@ -4424,19 +4585,22 @@
         <v>44</v>
       </c>
       <c r="O32" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="P32" s="8" t="s">
         <v>454</v>
       </c>
-      <c r="P32" s="8">
+      <c r="Q32" s="8">
         <v>1964</v>
       </c>
-      <c r="Q32" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R32" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18">
+      <c r="R32" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S32" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
         <v>378</v>
       </c>
@@ -4478,19 +4642,22 @@
         <v>45</v>
       </c>
       <c r="O33" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="P33" s="8">
+        <v>642</v>
+      </c>
+      <c r="P33" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q33" s="8">
         <v>2000</v>
       </c>
-      <c r="Q33" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R33" s="10" t="s">
+      <c r="R33" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S33" s="10" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="34" spans="1:18">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
         <v>325</v>
       </c>
@@ -4529,10 +4696,10 @@
         <v>7</v>
       </c>
       <c r="N34" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="O34" s="8" t="s">
-        <v>7</v>
+        <v>638</v>
+      </c>
+      <c r="O34" s="18" t="s">
+        <v>647</v>
       </c>
       <c r="P34" s="8" t="s">
         <v>7</v>
@@ -4540,11 +4707,14 @@
       <c r="Q34" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="R34" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18">
+      <c r="R34" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S34" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>95</v>
       </c>
@@ -4582,19 +4752,22 @@
         <v>10</v>
       </c>
       <c r="O35" s="8" t="s">
+        <v>646</v>
+      </c>
+      <c r="P35" s="8" t="s">
         <v>595</v>
       </c>
-      <c r="P35" s="8">
+      <c r="Q35" s="8">
         <v>1969</v>
       </c>
-      <c r="Q35" s="8">
+      <c r="R35" s="8">
         <v>29</v>
       </c>
-      <c r="R35" s="10" t="s">
+      <c r="S35" s="10" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="36" spans="1:18">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>6</v>
       </c>
@@ -4632,19 +4805,22 @@
         <v>84</v>
       </c>
       <c r="O36" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="P36" s="8" t="s">
         <v>392</v>
       </c>
-      <c r="P36" s="8">
+      <c r="Q36" s="8">
         <v>1979</v>
       </c>
-      <c r="Q36" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R36" s="10" t="s">
+      <c r="R36" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S36" s="10" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="37" spans="1:18">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
         <v>384</v>
       </c>
@@ -4686,19 +4862,22 @@
         <v>84</v>
       </c>
       <c r="O37" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="P37" s="8" t="s">
         <v>532</v>
       </c>
-      <c r="P37" s="8">
+      <c r="Q37" s="8">
         <v>1944</v>
       </c>
-      <c r="Q37" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R37" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18">
+      <c r="R37" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S37" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
         <v>316</v>
       </c>
@@ -4740,19 +4919,22 @@
         <v>76</v>
       </c>
       <c r="O38" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="P38" s="8" t="s">
         <v>451</v>
       </c>
-      <c r="P38" s="8">
+      <c r="Q38" s="8">
         <v>1935</v>
       </c>
-      <c r="Q38" s="8">
+      <c r="R38" s="8">
         <v>21</v>
       </c>
-      <c r="R38" s="10" t="s">
+      <c r="S38" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:18">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>99</v>
       </c>
@@ -4788,19 +4970,22 @@
         <v>100</v>
       </c>
       <c r="O39" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="P39" s="8" t="s">
         <v>614</v>
       </c>
-      <c r="P39" s="8">
+      <c r="Q39" s="8">
         <v>1968</v>
       </c>
-      <c r="Q39" s="8">
+      <c r="R39" s="8">
         <v>11</v>
       </c>
-      <c r="R39" s="10" t="s">
+      <c r="S39" s="10" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="40" spans="1:18">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
         <v>346</v>
       </c>
@@ -4840,19 +5025,22 @@
         <v>19</v>
       </c>
       <c r="O40" s="8" t="s">
+        <v>645</v>
+      </c>
+      <c r="P40" s="8" t="s">
         <v>539</v>
       </c>
-      <c r="P40" s="8">
+      <c r="Q40" s="8">
         <v>1972</v>
       </c>
-      <c r="Q40" s="8">
+      <c r="R40" s="8">
         <v>26</v>
       </c>
-      <c r="R40" s="10" t="s">
+      <c r="S40" s="10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:18">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>18</v>
       </c>
@@ -4888,19 +5076,22 @@
         <v>19</v>
       </c>
       <c r="O41" s="8" t="s">
+        <v>645</v>
+      </c>
+      <c r="P41" s="8" t="s">
         <v>418</v>
       </c>
-      <c r="P41" s="8">
+      <c r="Q41" s="8">
         <v>1968</v>
       </c>
-      <c r="Q41" s="8">
+      <c r="R41" s="8">
         <v>24</v>
       </c>
-      <c r="R41" s="10" t="s">
+      <c r="S41" s="10" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="42" spans="1:18">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>257</v>
       </c>
@@ -4938,19 +5129,22 @@
         <v>282</v>
       </c>
       <c r="O42" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="P42" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="P42" s="8">
+      <c r="Q42" s="8">
         <v>1996</v>
       </c>
-      <c r="Q42" s="8">
+      <c r="R42" s="8">
         <v>22</v>
       </c>
-      <c r="R42" s="10" t="s">
+      <c r="S42" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:18">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
         <v>37</v>
       </c>
@@ -4988,19 +5182,22 @@
         <v>46</v>
       </c>
       <c r="O43" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="P43" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="P43" s="8">
+      <c r="Q43" s="8">
         <v>2013</v>
       </c>
-      <c r="Q43" s="8">
+      <c r="R43" s="8">
         <v>13</v>
       </c>
-      <c r="R43" s="10" t="s">
+      <c r="S43" s="10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:18">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
         <v>315</v>
       </c>
@@ -5044,19 +5241,22 @@
         <v>10</v>
       </c>
       <c r="O44" s="8" t="s">
+        <v>646</v>
+      </c>
+      <c r="P44" s="8" t="s">
         <v>450</v>
       </c>
-      <c r="P44" s="8">
+      <c r="Q44" s="8">
         <v>1951</v>
       </c>
-      <c r="Q44" s="8">
+      <c r="R44" s="8">
         <v>9</v>
       </c>
-      <c r="R44" s="10" t="s">
+      <c r="S44" s="10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="45" spans="1:18">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
         <v>376</v>
       </c>
@@ -5098,19 +5298,22 @@
         <v>10</v>
       </c>
       <c r="O45" s="8" t="s">
+        <v>646</v>
+      </c>
+      <c r="P45" s="8" t="s">
         <v>295</v>
       </c>
-      <c r="P45" s="8">
+      <c r="Q45" s="8">
         <v>1998</v>
       </c>
-      <c r="Q45" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R45" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18">
+      <c r="R45" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S45" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
         <v>388</v>
       </c>
@@ -5151,18 +5354,21 @@
       <c r="N46" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="O46" s="8"/>
-      <c r="P46" s="8">
+      <c r="O46" s="8" t="s">
+        <v>645</v>
+      </c>
+      <c r="P46" s="8"/>
+      <c r="Q46" s="8">
         <v>1966</v>
       </c>
-      <c r="Q46" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R46" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18">
+      <c r="R46" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S46" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
         <v>8</v>
       </c>
@@ -5199,20 +5405,23 @@
       <c r="N47" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="O47" s="18" t="s">
+      <c r="O47" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="P47" s="18" t="s">
         <v>392</v>
       </c>
-      <c r="P47" s="18">
+      <c r="Q47" s="18">
         <v>1975</v>
       </c>
-      <c r="Q47" s="8">
+      <c r="R47" s="8">
         <v>8</v>
       </c>
-      <c r="R47" s="10" t="s">
+      <c r="S47" s="10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="48" spans="1:18">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
         <v>97</v>
       </c>
@@ -5248,19 +5457,22 @@
         <v>19</v>
       </c>
       <c r="O48" s="8" t="s">
+        <v>645</v>
+      </c>
+      <c r="P48" s="8" t="s">
         <v>607</v>
       </c>
-      <c r="P48" s="8">
+      <c r="Q48" s="8">
         <v>1968</v>
       </c>
-      <c r="Q48" s="8">
+      <c r="R48" s="8">
         <v>22</v>
       </c>
-      <c r="R48" s="10" t="s">
+      <c r="S48" s="10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="49" spans="1:18">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A49" s="20" t="s">
         <v>344</v>
       </c>
@@ -5302,19 +5514,22 @@
         <v>34</v>
       </c>
       <c r="O49" s="8" t="s">
+        <v>646</v>
+      </c>
+      <c r="P49" s="8" t="s">
         <v>526</v>
       </c>
-      <c r="P49" s="8">
+      <c r="Q49" s="8">
         <v>1966</v>
       </c>
-      <c r="Q49" s="8">
+      <c r="R49" s="8">
         <v>21</v>
       </c>
-      <c r="R49" s="10" t="s">
+      <c r="S49" s="10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="1:18">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
         <v>375</v>
       </c>
@@ -5356,19 +5571,22 @@
         <v>15</v>
       </c>
       <c r="O50" s="8" t="s">
+        <v>645</v>
+      </c>
+      <c r="P50" s="8" t="s">
         <v>592</v>
       </c>
-      <c r="P50" s="8">
+      <c r="Q50" s="8">
         <v>1955</v>
       </c>
-      <c r="Q50" s="8">
+      <c r="R50" s="8">
         <v>2</v>
       </c>
-      <c r="R50" s="10" t="s">
+      <c r="S50" s="10" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="51" spans="1:18">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
         <v>381</v>
       </c>
@@ -5410,19 +5628,22 @@
         <v>46</v>
       </c>
       <c r="O51" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="P51" s="8" t="s">
         <v>516</v>
       </c>
-      <c r="P51" s="8" t="s">
-        <v>7</v>
-      </c>
       <c r="Q51" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="R51" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18">
+      <c r="R51" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S51" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>32</v>
       </c>
@@ -5460,19 +5681,22 @@
         <v>10</v>
       </c>
       <c r="O52" s="8" t="s">
+        <v>646</v>
+      </c>
+      <c r="P52" s="8" t="s">
         <v>437</v>
       </c>
-      <c r="P52" s="8">
+      <c r="Q52" s="8">
         <v>1961</v>
       </c>
-      <c r="Q52" s="8">
+      <c r="R52" s="8">
         <v>1</v>
       </c>
-      <c r="R52" s="10" t="s">
+      <c r="S52" s="10" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="53" spans="1:18">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
         <v>385</v>
       </c>
@@ -5516,19 +5740,22 @@
         <v>56</v>
       </c>
       <c r="O53" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="P53" s="8" t="s">
         <v>554</v>
       </c>
-      <c r="P53" s="8">
+      <c r="Q53" s="8">
         <v>2010</v>
       </c>
-      <c r="Q53" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R53" s="10" t="s">
+      <c r="R53" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S53" s="10" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="54" spans="1:18">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>35</v>
       </c>
@@ -5564,19 +5791,22 @@
         <v>10</v>
       </c>
       <c r="O54" s="8" t="s">
+        <v>646</v>
+      </c>
+      <c r="P54" s="8" t="s">
         <v>440</v>
       </c>
-      <c r="P54" s="8">
+      <c r="Q54" s="8">
         <v>2000</v>
       </c>
-      <c r="Q54" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R54" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="55" spans="1:18">
+      <c r="R54" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S54" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
         <v>98</v>
       </c>
@@ -5612,19 +5842,22 @@
         <v>23</v>
       </c>
       <c r="O55" s="8" t="s">
+        <v>645</v>
+      </c>
+      <c r="P55" s="8" t="s">
         <v>610</v>
       </c>
-      <c r="P55" s="8">
+      <c r="Q55" s="8">
         <v>1947</v>
       </c>
-      <c r="Q55" s="8">
+      <c r="R55" s="8">
         <v>27</v>
       </c>
-      <c r="R55" s="10" t="s">
+      <c r="S55" s="10" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="56" spans="1:18">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
         <v>341</v>
       </c>
@@ -5666,19 +5899,22 @@
         <v>15</v>
       </c>
       <c r="O56" s="8" t="s">
+        <v>645</v>
+      </c>
+      <c r="P56" s="8" t="s">
         <v>408</v>
       </c>
-      <c r="P56" s="8">
+      <c r="Q56" s="8">
         <v>1959</v>
       </c>
-      <c r="Q56" s="8">
+      <c r="R56" s="8">
         <v>30</v>
       </c>
-      <c r="R56" s="10" t="s">
+      <c r="S56" s="10" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="57" spans="1:18">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A57" s="11" t="s">
         <v>349</v>
       </c>
@@ -5720,19 +5956,22 @@
         <v>15</v>
       </c>
       <c r="O57" s="8" t="s">
+        <v>645</v>
+      </c>
+      <c r="P57" s="8" t="s">
         <v>548</v>
       </c>
-      <c r="P57" s="8">
+      <c r="Q57" s="8">
         <v>1955</v>
       </c>
-      <c r="Q57" s="8">
+      <c r="R57" s="8">
         <v>3</v>
       </c>
-      <c r="R57" s="10" t="s">
+      <c r="S57" s="10" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="58" spans="1:18">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
         <v>379</v>
       </c>
@@ -5774,19 +6013,22 @@
         <v>23</v>
       </c>
       <c r="O58" s="8" t="s">
+        <v>645</v>
+      </c>
+      <c r="P58" s="8" t="s">
         <v>461</v>
       </c>
-      <c r="P58" s="8">
+      <c r="Q58" s="8">
         <v>1937</v>
       </c>
-      <c r="Q58" s="8">
+      <c r="R58" s="8">
         <v>12</v>
       </c>
-      <c r="R58" s="10" t="s">
+      <c r="S58" s="10" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="59" spans="1:18">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
         <v>16</v>
       </c>
@@ -5822,19 +6064,22 @@
         <v>17</v>
       </c>
       <c r="O59" s="8" t="s">
+        <v>645</v>
+      </c>
+      <c r="P59" s="8" t="s">
         <v>413</v>
       </c>
-      <c r="P59" s="8">
+      <c r="Q59" s="8">
         <v>1968</v>
       </c>
-      <c r="Q59" s="8">
+      <c r="R59" s="8">
         <v>25</v>
       </c>
-      <c r="R59" s="10" t="s">
+      <c r="S59" s="10" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="60" spans="1:18">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
         <v>323</v>
       </c>
@@ -5873,10 +6118,10 @@
         <v>7</v>
       </c>
       <c r="N60" s="8" t="s">
-        <v>7</v>
+        <v>639</v>
       </c>
       <c r="O60" s="8" t="s">
-        <v>7</v>
+        <v>648</v>
       </c>
       <c r="P60" s="8" t="s">
         <v>7</v>
@@ -5884,11 +6129,14 @@
       <c r="Q60" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="R60" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="61" spans="1:18">
+      <c r="R60" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S60" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A61" s="11" t="s">
         <v>345</v>
       </c>
@@ -5929,20 +6177,23 @@
       <c r="N61" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="O61" s="8" t="s">
+      <c r="O61" s="18" t="s">
+        <v>645</v>
+      </c>
+      <c r="P61" s="8" t="s">
         <v>535</v>
       </c>
-      <c r="P61" s="8">
+      <c r="Q61" s="8">
         <v>1947</v>
       </c>
-      <c r="Q61" s="8">
+      <c r="R61" s="8">
         <v>20</v>
       </c>
-      <c r="R61" s="10" t="s">
+      <c r="S61" s="10" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="62" spans="1:18">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A62" s="11" t="s">
         <v>329</v>
       </c>
@@ -5984,19 +6235,22 @@
         <v>76</v>
       </c>
       <c r="O62" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="P62" s="8" t="s">
         <v>484</v>
       </c>
-      <c r="P62" s="8">
+      <c r="Q62" s="8">
         <v>1954</v>
       </c>
-      <c r="Q62" s="8">
+      <c r="R62" s="8">
         <v>9</v>
       </c>
-      <c r="R62" s="10" t="s">
+      <c r="S62" s="10" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="63" spans="1:18">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A63" s="11" t="s">
         <v>367</v>
       </c>
@@ -6038,19 +6292,22 @@
         <v>83</v>
       </c>
       <c r="O63" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="P63" s="8" t="s">
         <v>570</v>
       </c>
-      <c r="P63" s="8">
+      <c r="Q63" s="8">
         <v>1969</v>
       </c>
-      <c r="Q63" s="8">
+      <c r="R63" s="8">
         <v>8</v>
       </c>
-      <c r="R63" s="10" t="s">
+      <c r="S63" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="64" spans="1:18">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
         <v>327</v>
       </c>
@@ -6092,19 +6349,22 @@
         <v>46</v>
       </c>
       <c r="O64" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="P64" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="P64" s="8">
+      <c r="Q64" s="8">
         <v>1958</v>
       </c>
-      <c r="Q64" s="8">
-        <v>7</v>
-      </c>
-      <c r="R64" s="10" t="s">
+      <c r="R64" s="8">
+        <v>7</v>
+      </c>
+      <c r="S64" s="10" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="65" spans="1:18">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A65" s="11" t="s">
         <v>336</v>
       </c>
@@ -6146,19 +6406,22 @@
         <v>46</v>
       </c>
       <c r="O65" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="P65" s="8" t="s">
         <v>285</v>
       </c>
-      <c r="P65" s="8">
+      <c r="Q65" s="8">
         <v>1958</v>
       </c>
-      <c r="Q65" s="8">
+      <c r="R65" s="8">
         <v>29</v>
       </c>
-      <c r="R65" s="10" t="s">
+      <c r="S65" s="10" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="66" spans="1:18">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A66" s="11" t="s">
         <v>328</v>
       </c>
@@ -6200,19 +6463,22 @@
         <v>46</v>
       </c>
       <c r="O66" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="P66" s="8" t="s">
         <v>481</v>
       </c>
-      <c r="P66" s="8">
+      <c r="Q66" s="8">
         <v>1954</v>
       </c>
-      <c r="Q66" s="8">
+      <c r="R66" s="8">
         <v>10</v>
       </c>
-      <c r="R66" s="10" t="s">
+      <c r="S66" s="10" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="67" spans="1:18">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A67" s="11" t="s">
         <v>343</v>
       </c>
@@ -6253,20 +6519,23 @@
       <c r="N67" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="O67" s="8" t="s">
+      <c r="O67" s="18" t="s">
+        <v>645</v>
+      </c>
+      <c r="P67" s="8" t="s">
         <v>522</v>
       </c>
-      <c r="P67" s="8">
+      <c r="Q67" s="8">
         <v>1957</v>
       </c>
-      <c r="Q67" s="8">
+      <c r="R67" s="8">
         <v>4</v>
       </c>
-      <c r="R67" s="10" t="s">
+      <c r="S67" s="10" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="68" spans="1:18">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A68" s="11" t="s">
         <v>369</v>
       </c>
@@ -6308,19 +6577,22 @@
         <v>85</v>
       </c>
       <c r="O68" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="P68" s="8" t="s">
         <v>577</v>
       </c>
-      <c r="P68" s="8">
+      <c r="Q68" s="8">
         <v>1970</v>
       </c>
-      <c r="Q68" s="8">
+      <c r="R68" s="8">
         <v>8</v>
       </c>
-      <c r="R68" s="10" t="s">
+      <c r="S68" s="10" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="69" spans="1:18">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A69" s="11" t="s">
         <v>338</v>
       </c>
@@ -6362,19 +6634,22 @@
         <v>76</v>
       </c>
       <c r="O69" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="P69" s="8">
+        <v>642</v>
+      </c>
+      <c r="P69" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q69" s="8">
         <v>1971</v>
       </c>
-      <c r="Q69" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R69" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="70" spans="1:18">
+      <c r="R69" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S69" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A70" s="11" t="s">
         <v>334</v>
       </c>
@@ -6416,19 +6691,22 @@
         <v>284</v>
       </c>
       <c r="O70" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="P70" s="8" t="s">
         <v>283</v>
       </c>
-      <c r="P70" s="8">
+      <c r="Q70" s="8">
         <v>1974</v>
       </c>
-      <c r="Q70" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R70" s="10" t="s">
+      <c r="R70" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S70" s="10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="71" spans="1:18">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A71" s="11" t="s">
         <v>337</v>
       </c>
@@ -6470,19 +6748,22 @@
         <v>49</v>
       </c>
       <c r="O71" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="P71" s="8">
+        <v>642</v>
+      </c>
+      <c r="P71" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q71" s="8">
         <v>1995</v>
       </c>
-      <c r="Q71" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R71" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="72" spans="1:18">
+      <c r="R71" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S71" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A72" s="11" t="s">
         <v>103</v>
       </c>
@@ -6518,19 +6799,22 @@
         <v>10</v>
       </c>
       <c r="O72" s="8" t="s">
+        <v>646</v>
+      </c>
+      <c r="P72" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="P72" s="8">
+      <c r="Q72" s="8">
         <v>1976</v>
       </c>
-      <c r="Q72" s="8">
+      <c r="R72" s="8">
         <v>20</v>
       </c>
-      <c r="R72" s="10" t="s">
+      <c r="S72" s="10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="73" spans="1:18">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A73" s="11" t="s">
         <v>104</v>
       </c>
@@ -6565,20 +6849,23 @@
       <c r="N73" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="O73" s="8" t="s">
+      <c r="O73" s="18" t="s">
+        <v>645</v>
+      </c>
+      <c r="P73" s="8" t="s">
         <v>624</v>
       </c>
-      <c r="P73" s="8">
+      <c r="Q73" s="8">
         <v>1967</v>
       </c>
-      <c r="Q73" s="8">
+      <c r="R73" s="8">
         <v>8</v>
       </c>
-      <c r="R73" s="10" t="s">
+      <c r="S73" s="10" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="74" spans="1:18">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A74" s="11" t="s">
         <v>360</v>
       </c>
@@ -6620,19 +6907,22 @@
         <v>289</v>
       </c>
       <c r="O74" s="8" t="s">
+        <v>644</v>
+      </c>
+      <c r="P74" s="8" t="s">
         <v>290</v>
       </c>
-      <c r="P74" s="8">
+      <c r="Q74" s="8">
         <v>1989</v>
       </c>
-      <c r="Q74" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R74" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="75" spans="1:18">
+      <c r="R74" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S74" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A75" s="11" t="s">
         <v>342</v>
       </c>
@@ -6674,19 +6964,22 @@
         <v>51</v>
       </c>
       <c r="O75" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="P75" s="8" t="s">
         <v>514</v>
       </c>
-      <c r="P75" s="8">
+      <c r="Q75" s="8">
         <v>1972</v>
       </c>
-      <c r="Q75" s="8">
+      <c r="R75" s="8">
         <v>9</v>
       </c>
-      <c r="R75" s="10" t="s">
+      <c r="S75" s="10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="76" spans="1:18">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A76" s="11" t="s">
         <v>313</v>
       </c>
@@ -6728,19 +7021,22 @@
         <v>25</v>
       </c>
       <c r="O76" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="P76" s="8" t="s">
         <v>427</v>
       </c>
-      <c r="P76" s="8">
+      <c r="Q76" s="8">
         <v>1957</v>
       </c>
-      <c r="Q76" s="8">
+      <c r="R76" s="8">
         <v>27</v>
       </c>
-      <c r="R76" s="10" t="s">
+      <c r="S76" s="10" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="77" spans="1:18">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A77" s="11" t="s">
         <v>333</v>
       </c>
@@ -6782,19 +7078,22 @@
         <v>100</v>
       </c>
       <c r="O77" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="P77" s="8" t="s">
         <v>494</v>
       </c>
-      <c r="P77" s="8">
+      <c r="Q77" s="8">
         <v>1956</v>
       </c>
-      <c r="Q77" s="8">
+      <c r="R77" s="8">
         <v>17</v>
       </c>
-      <c r="R77" s="10" t="s">
+      <c r="S77" s="10" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="78" spans="1:18">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A78" s="11" t="s">
         <v>321</v>
       </c>
@@ -6836,19 +7135,22 @@
         <v>468</v>
       </c>
       <c r="O78" s="8" t="s">
+        <v>644</v>
+      </c>
+      <c r="P78" s="8" t="s">
         <v>469</v>
       </c>
-      <c r="P78" s="8">
+      <c r="Q78" s="8">
         <v>1929</v>
       </c>
-      <c r="Q78" s="8">
+      <c r="R78" s="8">
         <v>1</v>
       </c>
-      <c r="R78" s="10" t="s">
+      <c r="S78" s="10" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="79" spans="1:18">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A79" s="6" t="s">
         <v>101</v>
       </c>
@@ -6886,19 +7188,22 @@
         <v>102</v>
       </c>
       <c r="O79" s="8" t="s">
+        <v>644</v>
+      </c>
+      <c r="P79" s="8" t="s">
         <v>618</v>
       </c>
-      <c r="P79" s="8">
+      <c r="Q79" s="8">
         <v>1981</v>
       </c>
-      <c r="Q79" s="8">
+      <c r="R79" s="8">
         <v>3</v>
       </c>
-      <c r="R79" s="10" t="s">
+      <c r="S79" s="10" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="80" spans="1:18">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A80" s="11" t="s">
         <v>339</v>
       </c>
@@ -6940,19 +7245,22 @@
         <v>289</v>
       </c>
       <c r="O80" s="8" t="s">
+        <v>644</v>
+      </c>
+      <c r="P80" s="8" t="s">
         <v>505</v>
       </c>
-      <c r="P80" s="8">
+      <c r="Q80" s="8">
         <v>1947</v>
       </c>
-      <c r="Q80" s="8">
+      <c r="R80" s="8">
         <v>14</v>
       </c>
-      <c r="R80" s="10" t="s">
+      <c r="S80" s="10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="81" spans="1:18">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A81" s="11" t="s">
         <v>332</v>
       </c>
@@ -6994,19 +7302,22 @@
         <v>489</v>
       </c>
       <c r="O81" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="P81" s="8" t="s">
         <v>490</v>
       </c>
-      <c r="P81" s="8">
+      <c r="Q81" s="8">
         <v>1958</v>
       </c>
-      <c r="Q81" s="8">
+      <c r="R81" s="8">
         <v>23</v>
       </c>
-      <c r="R81" s="10" t="s">
+      <c r="S81" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="82" spans="1:18">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A82" s="11" t="s">
         <v>312</v>
       </c>
@@ -7046,19 +7357,22 @@
         <v>11</v>
       </c>
       <c r="O82" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="P82" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="P82" s="8">
+      <c r="Q82" s="8">
         <v>1968</v>
       </c>
-      <c r="Q82" s="8">
+      <c r="R82" s="8">
         <v>2</v>
       </c>
-      <c r="R82" s="10" t="s">
+      <c r="S82" s="10" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="83" spans="1:18">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
         <v>105</v>
       </c>
@@ -7094,19 +7408,22 @@
         <v>10</v>
       </c>
       <c r="O83" s="9" t="s">
+        <v>646</v>
+      </c>
+      <c r="P83" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="P83" s="9">
+      <c r="Q83" s="9">
         <v>1974</v>
       </c>
-      <c r="Q83" s="9">
+      <c r="R83" s="9">
         <v>26</v>
       </c>
-      <c r="R83" s="30" t="s">
+      <c r="S83" s="30" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="84" spans="1:18">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A84" s="11" t="s">
         <v>371</v>
       </c>
@@ -7148,19 +7465,22 @@
         <v>43</v>
       </c>
       <c r="O84" s="8" t="s">
+        <v>644</v>
+      </c>
+      <c r="P84" s="8" t="s">
         <v>580</v>
       </c>
-      <c r="P84" s="8">
+      <c r="Q84" s="8">
         <v>2011</v>
       </c>
-      <c r="Q84" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R84" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="85" spans="1:18">
+      <c r="R84" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S84" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A85" s="11" t="s">
         <v>319</v>
       </c>
@@ -7199,10 +7519,10 @@
         <v>465</v>
       </c>
       <c r="N85" s="8" t="s">
-        <v>7</v>
+        <v>640</v>
       </c>
       <c r="O85" s="8" t="s">
-        <v>7</v>
+        <v>644</v>
       </c>
       <c r="P85" s="8" t="s">
         <v>7</v>
@@ -7210,11 +7530,14 @@
       <c r="Q85" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="R85" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="86" spans="1:18">
+      <c r="R85" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S85" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A86" s="6" t="s">
         <v>12</v>
       </c>
@@ -7250,7 +7573,7 @@
         <v>13</v>
       </c>
       <c r="O86" s="8" t="s">
-        <v>7</v>
+        <v>642</v>
       </c>
       <c r="P86" s="8" t="s">
         <v>7</v>
@@ -7258,11 +7581,14 @@
       <c r="Q86" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="R86" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="87" spans="1:18">
+      <c r="R86" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S86" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A87" s="11" t="s">
         <v>359</v>
       </c>
@@ -7304,34 +7630,33 @@
         <v>289</v>
       </c>
       <c r="O87" s="8" t="s">
+        <v>644</v>
+      </c>
+      <c r="P87" s="8" t="s">
         <v>288</v>
       </c>
-      <c r="P87" s="8">
+      <c r="Q87" s="8">
         <v>1969</v>
       </c>
-      <c r="Q87" s="8">
+      <c r="R87" s="8">
         <v>18</v>
       </c>
-      <c r="R87" s="10" t="s">
+      <c r="S87" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="88" spans="1:18">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A88" s="11" t="s">
         <v>370</v>
       </c>
       <c r="B88" s="12" t="s">
         <v>227</v>
       </c>
-      <c r="C88" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="C88" s="8"/>
       <c r="D88" s="8" t="s">
         <v>497</v>
       </c>
-      <c r="E88" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="E88" s="8"/>
       <c r="F88" s="12" t="s">
         <v>253</v>
       </c>
@@ -7357,35 +7682,34 @@
       <c r="N88" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="O88" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="P88" s="8">
+      <c r="O88" s="18" t="s">
+        <v>645</v>
+      </c>
+      <c r="P88" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q88" s="8">
         <v>2011</v>
       </c>
-      <c r="Q88" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R88" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="89" spans="1:18">
+      <c r="R88" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S88" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A89" s="11" t="s">
         <v>362</v>
       </c>
       <c r="B89" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="C89" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="C89" s="8"/>
       <c r="D89" s="8" t="s">
         <v>497</v>
       </c>
-      <c r="E89" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="E89" s="8"/>
       <c r="F89" s="12" t="s">
         <v>270</v>
       </c>
@@ -7412,34 +7736,33 @@
         <v>76</v>
       </c>
       <c r="O89" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="P89" s="8">
+        <v>642</v>
+      </c>
+      <c r="P89" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q89" s="8">
         <v>2013</v>
       </c>
-      <c r="Q89" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R89" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="90" spans="1:18">
+      <c r="R89" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S89" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A90" s="11" t="s">
         <v>363</v>
       </c>
       <c r="B90" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="C90" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="C90" s="8"/>
       <c r="D90" s="8" t="s">
         <v>497</v>
       </c>
-      <c r="E90" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="E90" s="8"/>
       <c r="F90" s="12" t="s">
         <v>261</v>
       </c>
@@ -7466,34 +7789,33 @@
         <v>46</v>
       </c>
       <c r="O90" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="P90" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="P90" s="8">
+      <c r="Q90" s="8">
         <v>2013</v>
       </c>
-      <c r="Q90" s="8">
-        <v>7</v>
-      </c>
-      <c r="R90" s="10" t="s">
+      <c r="R90" s="8">
+        <v>7</v>
+      </c>
+      <c r="S90" s="10" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="91" spans="1:18">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A91" s="11" t="s">
         <v>364</v>
       </c>
       <c r="B91" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="C91" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="C91" s="8"/>
       <c r="D91" s="8" t="s">
         <v>497</v>
       </c>
-      <c r="E91" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="E91" s="8"/>
       <c r="F91" s="12" t="s">
         <v>261</v>
       </c>
@@ -7520,34 +7842,33 @@
         <v>46</v>
       </c>
       <c r="O91" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="P91" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="P91" s="8">
+      <c r="Q91" s="8">
         <v>2012</v>
       </c>
-      <c r="Q91" s="8">
+      <c r="R91" s="8">
         <v>20</v>
       </c>
-      <c r="R91" s="10" t="s">
+      <c r="S91" s="10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="92" spans="1:18">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A92" s="11" t="s">
         <v>366</v>
       </c>
       <c r="B92" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="C92" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="C92" s="8"/>
       <c r="D92" s="8" t="s">
         <v>497</v>
       </c>
-      <c r="E92" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="E92" s="8"/>
       <c r="F92" s="12" t="s">
         <v>261</v>
       </c>
@@ -7574,34 +7895,33 @@
         <v>46</v>
       </c>
       <c r="O92" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="P92" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="P92" s="8">
+      <c r="Q92" s="8">
         <v>2012</v>
       </c>
-      <c r="Q92" s="8">
+      <c r="R92" s="8">
         <v>2</v>
       </c>
-      <c r="R92" s="10" t="s">
+      <c r="S92" s="10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="93" spans="1:18">
+    <row r="93" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A93" s="11" t="s">
         <v>365</v>
       </c>
       <c r="B93" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="C93" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="C93" s="8"/>
       <c r="D93" s="8" t="s">
         <v>497</v>
       </c>
-      <c r="E93" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="E93" s="8"/>
       <c r="F93" s="12" t="s">
         <v>261</v>
       </c>
@@ -7628,34 +7948,33 @@
         <v>46</v>
       </c>
       <c r="O93" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="P93" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="P93" s="8">
+      <c r="Q93" s="8">
         <v>2013</v>
       </c>
-      <c r="Q93" s="8">
+      <c r="R93" s="8">
         <v>30</v>
       </c>
-      <c r="R93" s="10" t="s">
+      <c r="S93" s="10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="94" spans="1:18">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A94" s="11" t="s">
         <v>356</v>
       </c>
       <c r="B94" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="C94" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="C94" s="8"/>
       <c r="D94" s="8" t="s">
         <v>497</v>
       </c>
-      <c r="E94" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="E94" s="8"/>
       <c r="F94" s="12" t="s">
         <v>261</v>
       </c>
@@ -7682,19 +8001,22 @@
         <v>46</v>
       </c>
       <c r="O94" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="P94" s="8">
+        <v>643</v>
+      </c>
+      <c r="P94" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q94" s="8">
         <v>2008</v>
       </c>
-      <c r="Q94" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R94" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="95" spans="1:18">
+      <c r="R94" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S94" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A95" s="11" t="s">
         <v>335</v>
       </c>
@@ -7735,35 +8057,32 @@
       <c r="N95" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="O95" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="O95" s="8"/>
       <c r="P95" s="8" t="s">
         <v>7</v>
       </c>
       <c r="Q95" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="R95" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="96" spans="1:18">
+      <c r="R95" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S95" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A96" s="11" t="s">
         <v>354</v>
       </c>
       <c r="B96" s="12" t="s">
         <v>193</v>
       </c>
-      <c r="C96" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="C96" s="8"/>
       <c r="D96" s="8" t="s">
         <v>558</v>
       </c>
-      <c r="E96" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="E96" s="8"/>
       <c r="F96" s="12" t="s">
         <v>270</v>
       </c>
@@ -7790,19 +8109,22 @@
         <v>46</v>
       </c>
       <c r="O96" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="P96" s="8">
+        <v>643</v>
+      </c>
+      <c r="P96" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q96" s="8">
         <v>2011</v>
       </c>
-      <c r="Q96" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R96" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="97" spans="1:18">
+      <c r="R96" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S96" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="97" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A97" s="11" t="s">
         <v>320</v>
       </c>
@@ -7815,9 +8137,7 @@
       <c r="D97" s="12" t="s">
         <v>558</v>
       </c>
-      <c r="E97" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="E97" s="8"/>
       <c r="F97" s="12" t="s">
         <v>250</v>
       </c>
@@ -7843,20 +8163,21 @@
       <c r="N97" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="O97" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="O97" s="8"/>
       <c r="P97" s="8" t="s">
         <v>7</v>
       </c>
       <c r="Q97" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="R97" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="98" spans="1:18">
+      <c r="R97" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S97" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A98" s="11" t="s">
         <v>387</v>
       </c>
@@ -7869,9 +8190,7 @@
       <c r="D98" s="8" t="s">
         <v>558</v>
       </c>
-      <c r="E98" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="E98" s="8"/>
       <c r="F98" s="12" t="s">
         <v>250</v>
       </c>
@@ -7898,19 +8217,22 @@
         <v>46</v>
       </c>
       <c r="O98" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="P98" s="8">
+        <v>643</v>
+      </c>
+      <c r="P98" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q98" s="8">
         <v>2008</v>
       </c>
-      <c r="Q98" s="8">
+      <c r="R98" s="8">
         <v>28</v>
       </c>
-      <c r="R98" s="10" t="s">
+      <c r="S98" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="99" spans="1:18">
+    <row r="99" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A99" s="11" t="s">
         <v>322</v>
       </c>
@@ -7923,9 +8245,7 @@
       <c r="D99" s="12" t="s">
         <v>558</v>
       </c>
-      <c r="E99" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="E99" s="8"/>
       <c r="F99" s="12" t="s">
         <v>250</v>
       </c>
@@ -7951,35 +8271,32 @@
       <c r="N99" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="O99" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="O99" s="8"/>
       <c r="P99" s="8" t="s">
         <v>7</v>
       </c>
       <c r="Q99" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="R99" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="100" spans="1:18">
+      <c r="R99" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S99" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="100" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A100" s="11" t="s">
         <v>357</v>
       </c>
       <c r="B100" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="C100" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="C100" s="8"/>
       <c r="D100" s="8" t="s">
         <v>558</v>
       </c>
-      <c r="E100" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="E100" s="8"/>
       <c r="F100" s="12" t="s">
         <v>261</v>
       </c>
@@ -8006,34 +8323,33 @@
         <v>46</v>
       </c>
       <c r="O100" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="P100" s="8">
+        <v>643</v>
+      </c>
+      <c r="P100" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q100" s="8">
         <v>2008</v>
       </c>
-      <c r="Q100" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R100" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="101" spans="1:18">
+      <c r="R100" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S100" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="101" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A101" s="11" t="s">
         <v>361</v>
       </c>
       <c r="B101" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="C101" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="C101" s="8"/>
       <c r="D101" s="8" t="s">
         <v>558</v>
       </c>
-      <c r="E101" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="E101" s="8"/>
       <c r="F101" s="12" t="s">
         <v>250</v>
       </c>
@@ -8059,35 +8375,34 @@
       <c r="N101" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="O101" s="8" t="s">
+      <c r="O101" s="18" t="s">
+        <v>645</v>
+      </c>
+      <c r="P101" s="8" t="s">
         <v>292</v>
       </c>
-      <c r="P101" s="8">
+      <c r="Q101" s="8">
         <v>2010</v>
       </c>
-      <c r="Q101" s="8">
+      <c r="R101" s="8">
         <v>15</v>
       </c>
-      <c r="R101" s="10" t="s">
+      <c r="S101" s="10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="102" spans="1:18">
+    <row r="102" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A102" s="11" t="s">
         <v>331</v>
       </c>
       <c r="B102" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="C102" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="C102" s="8"/>
       <c r="D102" s="8" t="s">
         <v>441</v>
       </c>
-      <c r="E102" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="E102" s="8"/>
       <c r="F102" s="12" t="s">
         <v>253</v>
       </c>
@@ -8113,20 +8428,21 @@
       <c r="N102" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="O102" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="O102" s="8"/>
       <c r="P102" s="8" t="s">
         <v>7</v>
       </c>
       <c r="Q102" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="R102" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="103" spans="1:18">
+      <c r="R102" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S102" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="103" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A103" s="11" t="s">
         <v>317</v>
       </c>
@@ -8139,9 +8455,7 @@
       <c r="D103" s="8" t="s">
         <v>441</v>
       </c>
-      <c r="E103" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="E103" s="8"/>
       <c r="F103" s="12" t="s">
         <v>253</v>
       </c>
@@ -8167,20 +8481,21 @@
       <c r="N103" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="O103" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="O103" s="8"/>
       <c r="P103" s="8" t="s">
         <v>7</v>
       </c>
       <c r="Q103" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="R103" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="104" spans="1:18">
+      <c r="R103" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S103" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="104" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A104" s="11" t="s">
         <v>324</v>
       </c>
@@ -8193,9 +8508,7 @@
       <c r="D104" s="8" t="s">
         <v>441</v>
       </c>
-      <c r="E104" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="E104" s="8"/>
       <c r="F104" s="12" t="s">
         <v>253</v>
       </c>
@@ -8222,19 +8535,22 @@
         <v>46</v>
       </c>
       <c r="O104" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="P104" s="8" t="s">
         <v>473</v>
       </c>
-      <c r="P104" s="8" t="s">
-        <v>7</v>
-      </c>
       <c r="Q104" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="R104" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="105" spans="1:18">
+      <c r="R104" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S104" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="105" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A105" s="11" t="s">
         <v>350</v>
       </c>
@@ -8247,9 +8563,7 @@
       <c r="D105" s="8" t="s">
         <v>441</v>
       </c>
-      <c r="E105" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="E105" s="8"/>
       <c r="F105" s="12" t="s">
         <v>253</v>
       </c>
@@ -8276,19 +8590,22 @@
         <v>44</v>
       </c>
       <c r="O105" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="P105" s="8">
+        <v>642</v>
+      </c>
+      <c r="P105" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q105" s="8">
         <v>2004</v>
       </c>
-      <c r="Q105" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R105" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="106" spans="1:18">
+      <c r="R105" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S105" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="106" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A106" s="11" t="s">
         <v>326</v>
       </c>
@@ -8301,9 +8618,7 @@
       <c r="D106" s="8" t="s">
         <v>441</v>
       </c>
-      <c r="E106" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="E106" s="8"/>
       <c r="F106" s="12" t="s">
         <v>262</v>
       </c>
@@ -8329,35 +8644,32 @@
       <c r="N106" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="O106" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="O106" s="8"/>
       <c r="P106" s="8" t="s">
         <v>7</v>
       </c>
       <c r="Q106" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="R106" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="107" spans="1:18">
+      <c r="R106" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S106" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="107" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A107" s="11" t="s">
         <v>314</v>
       </c>
       <c r="B107" s="12" t="s">
         <v>252</v>
       </c>
-      <c r="C107" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="C107" s="8"/>
       <c r="D107" s="8" t="s">
         <v>441</v>
       </c>
-      <c r="E107" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="E107" s="8"/>
       <c r="F107" s="12" t="s">
         <v>253</v>
       </c>
@@ -8384,34 +8696,33 @@
         <v>13</v>
       </c>
       <c r="O107" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="P107" s="8">
+        <v>642</v>
+      </c>
+      <c r="P107" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q107" s="8">
         <v>2005</v>
       </c>
-      <c r="Q107" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R107" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="108" spans="1:18">
+      <c r="R107" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S107" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="108" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A108" s="11" t="s">
         <v>330</v>
       </c>
       <c r="B108" s="12" t="s">
         <v>264</v>
       </c>
-      <c r="C108" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="C108" s="8"/>
       <c r="D108" s="8" t="s">
         <v>441</v>
       </c>
-      <c r="E108" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="E108" s="8"/>
       <c r="F108" s="12" t="s">
         <v>265</v>
       </c>
@@ -8437,8 +8748,8 @@
       <c r="N108" s="8" t="s">
         <v>485</v>
       </c>
-      <c r="O108" s="8" t="s">
-        <v>7</v>
+      <c r="O108" s="18" t="s">
+        <v>645</v>
       </c>
       <c r="P108" s="8" t="s">
         <v>7</v>
@@ -8446,26 +8757,25 @@
       <c r="Q108" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="R108" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="109" spans="1:18">
+      <c r="R108" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S108" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="109" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A109" s="11" t="s">
         <v>353</v>
       </c>
       <c r="B109" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="C109" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="C109" s="8"/>
       <c r="D109" s="8" t="s">
         <v>441</v>
       </c>
-      <c r="E109" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="E109" s="8"/>
       <c r="F109" s="12" t="s">
         <v>253</v>
       </c>
@@ -8492,34 +8802,33 @@
         <v>13</v>
       </c>
       <c r="O109" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="P109" s="8">
+        <v>642</v>
+      </c>
+      <c r="P109" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q109" s="8">
         <v>2004</v>
       </c>
-      <c r="Q109" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="R109" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="110" spans="1:18">
+      <c r="R109" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S109" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="110" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A110" s="11" t="s">
         <v>358</v>
       </c>
       <c r="B110" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="C110" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="C110" s="8"/>
       <c r="D110" s="8" t="s">
         <v>441</v>
       </c>
-      <c r="E110" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="E110" s="8"/>
       <c r="F110" s="12" t="s">
         <v>246</v>
       </c>
@@ -8546,7 +8855,7 @@
         <v>10</v>
       </c>
       <c r="O110" s="8" t="s">
-        <v>7</v>
+        <v>646</v>
       </c>
       <c r="P110" s="8" t="s">
         <v>7</v>
@@ -8554,11 +8863,14 @@
       <c r="Q110" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="R110" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="111" spans="1:18">
+      <c r="R110" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S110" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="111" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A111" s="21" t="s">
         <v>386</v>
       </c>
@@ -8571,9 +8883,7 @@
       <c r="D111" s="24" t="s">
         <v>441</v>
       </c>
-      <c r="E111" s="24" t="s">
-        <v>7</v>
-      </c>
+      <c r="E111" s="24"/>
       <c r="F111" s="23" t="s">
         <v>271</v>
       </c>
@@ -8599,8 +8909,8 @@
       <c r="N111" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="O111" s="24" t="s">
-        <v>7</v>
+      <c r="O111" s="8" t="s">
+        <v>643</v>
       </c>
       <c r="P111" s="24" t="s">
         <v>7</v>
@@ -8608,12 +8918,43 @@
       <c r="Q111" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="R111" s="31" t="s">
-        <v>7</v>
+      <c r="R111" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="S111" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="112" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A112" s="11" t="s">
+        <v>655</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="C112" t="s">
+        <v>652</v>
+      </c>
+      <c r="D112" s="8" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" s="46" t="s">
+        <v>649</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="C113" t="s">
+        <v>653</v>
+      </c>
+      <c r="D113" s="8" t="s">
+        <v>650</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:R111">
+  <sortState ref="A2:S111">
     <sortCondition ref="D2:D111"/>
     <sortCondition ref="E2:E111"/>
     <sortCondition ref="B2:B111"/>

</xml_diff>

<commit_message>
Removed some info and added host groups
</commit_message>
<xml_diff>
--- a/tabular/flavi-ncbi-refseqs-side-data.xlsx
+++ b/tabular/flavi-ncbi-refseqs-side-data.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11014"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus-group/Flaviviridae-GLUE/tabular/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5CBA2A1-3C52-044A-874E-58238ABF65F7}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27700" yWindow="0" windowWidth="20920" windowHeight="24580" tabRatio="500"/>
+    <workbookView xWindow="1720" yWindow="460" windowWidth="20920" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="flavi.txt" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1553" uniqueCount="665">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1562" uniqueCount="674">
   <si>
     <t>isolate</t>
   </si>
@@ -2014,12 +2020,39 @@
   </si>
   <si>
     <t>Sus scrofa</t>
+  </si>
+  <si>
+    <t>MH716818</t>
+  </si>
+  <si>
+    <t>MG599986</t>
+  </si>
+  <si>
+    <t>MF776369</t>
+  </si>
+  <si>
+    <t>Eastern red scorpionfish flavivirus</t>
+  </si>
+  <si>
+    <t>Wenzhou shark flavivirus</t>
+  </si>
+  <si>
+    <t>Scoliodon macrorhynchos</t>
+  </si>
+  <si>
+    <t>Scorpaena jacksoniensis</t>
+  </si>
+  <si>
+    <t>Cyclopterus lumpus virus</t>
+  </si>
+  <si>
+    <t>Cyclopterus lumpus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2049,25 +2082,30 @@
       <sz val="14"/>
       <color theme="0"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="16">
@@ -2921,15 +2959,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S115"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E36" sqref="A31:E36"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F87" sqref="F87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="35.1640625" style="1" customWidth="1"/>
@@ -2944,7 +2982,7 @@
     <col min="19" max="19" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18">
+    <row r="1" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>310</v>
       </c>
@@ -3003,7 +3041,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="18">
+    <row r="2" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>330</v>
       </c>
@@ -3054,7 +3092,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="18">
+    <row r="3" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>316</v>
       </c>
@@ -3107,7 +3145,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="18">
+    <row r="4" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>323</v>
       </c>
@@ -3162,7 +3200,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="18">
+    <row r="5" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>349</v>
       </c>
@@ -3217,7 +3255,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="18">
+    <row r="6" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>325</v>
       </c>
@@ -3270,7 +3308,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="18">
+    <row r="7" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>313</v>
       </c>
@@ -3323,7 +3361,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="18">
+    <row r="8" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>329</v>
       </c>
@@ -3376,7 +3414,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="18">
+    <row r="9" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>352</v>
       </c>
@@ -3429,7 +3467,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="18">
+    <row r="10" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
         <v>357</v>
       </c>
@@ -3482,7 +3520,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="18">
+    <row r="11" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
         <v>385</v>
       </c>
@@ -3537,7 +3575,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="18">
+    <row r="12" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
         <v>652</v>
       </c>
@@ -3570,7 +3608,7 @@
       <c r="R12" s="12"/>
       <c r="S12" s="12"/>
     </row>
-    <row r="13" spans="1:19" ht="18">
+    <row r="13" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
         <v>647</v>
       </c>
@@ -3603,7 +3641,7 @@
       <c r="R13" s="12"/>
       <c r="S13" s="12"/>
     </row>
-    <row r="14" spans="1:19" ht="18">
+    <row r="14" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
         <v>654</v>
       </c>
@@ -3636,7 +3674,7 @@
       <c r="R14" s="12"/>
       <c r="S14" s="12"/>
     </row>
-    <row r="15" spans="1:19" ht="18">
+    <row r="15" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
         <v>655</v>
       </c>
@@ -3658,7 +3696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="18">
+    <row r="16" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
         <v>350</v>
       </c>
@@ -3715,7 +3753,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="18">
+    <row r="17" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" s="33" t="s">
         <v>379</v>
       </c>
@@ -3772,7 +3810,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="18">
+    <row r="18" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
         <v>381</v>
       </c>
@@ -3829,7 +3867,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="18">
+    <row r="19" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A19" s="36" t="s">
         <v>24</v>
       </c>
@@ -3882,7 +3920,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="18">
+    <row r="20" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" s="36" t="s">
         <v>26</v>
       </c>
@@ -3935,7 +3973,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="18">
+    <row r="21" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="33" t="s">
         <v>339</v>
       </c>
@@ -3992,7 +4030,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="18">
+    <row r="22" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A22" s="33" t="s">
         <v>372</v>
       </c>
@@ -4049,7 +4087,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="18">
+    <row r="23" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
         <v>354</v>
       </c>
@@ -4106,7 +4144,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="18">
+    <row r="24" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A24" s="36" t="s">
         <v>22</v>
       </c>
@@ -4161,7 +4199,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="18">
+    <row r="25" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A25" s="36" t="s">
         <v>68</v>
       </c>
@@ -4212,7 +4250,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="18">
+    <row r="26" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A26" s="36" t="s">
         <v>31</v>
       </c>
@@ -4265,7 +4303,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="18">
+    <row r="27" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
         <v>371</v>
       </c>
@@ -4322,7 +4360,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="18">
+    <row r="28" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A28" s="33" t="s">
         <v>347</v>
       </c>
@@ -4379,7 +4417,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="18">
+    <row r="29" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A29" s="43" t="s">
         <v>41</v>
       </c>
@@ -4432,7 +4470,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="18">
+    <row r="30" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A30" s="45" t="s">
         <v>373</v>
       </c>
@@ -4489,7 +4527,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="18">
+    <row r="31" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A31" s="38" t="s">
         <v>351</v>
       </c>
@@ -4544,7 +4582,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="18">
+    <row r="32" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A32" s="41" t="s">
         <v>57</v>
       </c>
@@ -4595,7 +4633,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="18">
+    <row r="33" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A33" s="41" t="s">
         <v>72</v>
       </c>
@@ -4644,7 +4682,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="18">
+    <row r="34" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A34" s="41" t="s">
         <v>74</v>
       </c>
@@ -4693,7 +4731,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="18">
+    <row r="35" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A35" s="41" t="s">
         <v>66</v>
       </c>
@@ -4746,7 +4784,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="18">
+    <row r="36" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A36" s="41" t="s">
         <v>20</v>
       </c>
@@ -4799,7 +4837,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="18">
+    <row r="37" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A37" s="47" t="s">
         <v>9</v>
       </c>
@@ -4852,7 +4890,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="18">
+    <row r="38" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A38" s="50" t="s">
         <v>346</v>
       </c>
@@ -4907,7 +4945,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="18">
+    <row r="39" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A39" s="47" t="s">
         <v>33</v>
       </c>
@@ -4960,7 +4998,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="18">
+    <row r="40" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A40" s="47" t="s">
         <v>14</v>
       </c>
@@ -5011,7 +5049,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="18">
+    <row r="41" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A41" s="47" t="s">
         <v>28</v>
       </c>
@@ -5064,7 +5102,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="18">
+    <row r="42" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A42" s="47" t="s">
         <v>96</v>
       </c>
@@ -5115,7 +5153,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="18">
+    <row r="43" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A43" s="50" t="s">
         <v>382</v>
       </c>
@@ -5172,7 +5210,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="18">
+    <row r="44" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A44" s="50" t="s">
         <v>367</v>
       </c>
@@ -5229,7 +5267,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="18">
+    <row r="45" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A45" s="50" t="s">
         <v>317</v>
       </c>
@@ -5286,7 +5324,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="18">
+    <row r="46" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A46" s="50" t="s">
         <v>376</v>
       </c>
@@ -5343,7 +5381,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="18">
+    <row r="47" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A47" s="50" t="s">
         <v>377</v>
       </c>
@@ -5400,7 +5438,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="18">
+    <row r="48" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A48" s="50" t="s">
         <v>324</v>
       </c>
@@ -5457,7 +5495,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="18">
+    <row r="49" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A49" s="47" t="s">
         <v>95</v>
       </c>
@@ -5510,7 +5548,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="18">
+    <row r="50" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A50" s="47" t="s">
         <v>6</v>
       </c>
@@ -5563,7 +5601,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="18">
+    <row r="51" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A51" s="50" t="s">
         <v>383</v>
       </c>
@@ -5620,7 +5658,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="18">
+    <row r="52" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A52" s="50" t="s">
         <v>315</v>
       </c>
@@ -5677,7 +5715,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="18">
+    <row r="53" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A53" s="47" t="s">
         <v>99</v>
       </c>
@@ -5728,7 +5766,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="18">
+    <row r="54" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A54" s="50" t="s">
         <v>345</v>
       </c>
@@ -5783,7 +5821,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="18">
+    <row r="55" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A55" s="47" t="s">
         <v>18</v>
       </c>
@@ -5834,7 +5872,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="18">
+    <row r="56" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A56" s="47" t="s">
         <v>257</v>
       </c>
@@ -5887,7 +5925,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="18">
+    <row r="57" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A57" s="47" t="s">
         <v>37</v>
       </c>
@@ -5940,7 +5978,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="18">
+    <row r="58" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A58" s="50" t="s">
         <v>314</v>
       </c>
@@ -5999,7 +6037,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="18">
+    <row r="59" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A59" s="50" t="s">
         <v>375</v>
       </c>
@@ -6056,7 +6094,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="18">
+    <row r="60" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A60" s="50" t="s">
         <v>387</v>
       </c>
@@ -6111,7 +6149,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="18">
+    <row r="61" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A61" s="47" t="s">
         <v>8</v>
       </c>
@@ -6164,7 +6202,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="18">
+    <row r="62" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A62" s="47" t="s">
         <v>97</v>
       </c>
@@ -6215,7 +6253,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="18">
+    <row r="63" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A63" s="50" t="s">
         <v>343</v>
       </c>
@@ -6272,7 +6310,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="18">
+    <row r="64" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A64" s="50" t="s">
         <v>374</v>
       </c>
@@ -6329,7 +6367,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="18">
+    <row r="65" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A65" s="50" t="s">
         <v>380</v>
       </c>
@@ -6386,7 +6424,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:19" ht="18">
+    <row r="66" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A66" s="47" t="s">
         <v>32</v>
       </c>
@@ -6439,7 +6477,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="67" spans="1:19" ht="18">
+    <row r="67" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A67" s="50" t="s">
         <v>384</v>
       </c>
@@ -6498,7 +6536,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="68" spans="1:19" ht="18">
+    <row r="68" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A68" s="47" t="s">
         <v>35</v>
       </c>
@@ -6549,7 +6587,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:19" ht="18">
+    <row r="69" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A69" s="47" t="s">
         <v>98</v>
       </c>
@@ -6600,7 +6638,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="70" spans="1:19" ht="18">
+    <row r="70" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A70" s="50" t="s">
         <v>340</v>
       </c>
@@ -6657,7 +6695,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="71" spans="1:19" ht="18">
+    <row r="71" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A71" s="50" t="s">
         <v>348</v>
       </c>
@@ -6714,7 +6752,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="72" spans="1:19" ht="18">
+    <row r="72" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A72" s="50" t="s">
         <v>378</v>
       </c>
@@ -6771,7 +6809,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="73" spans="1:19" ht="18">
+    <row r="73" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A73" s="47" t="s">
         <v>16</v>
       </c>
@@ -6822,7 +6860,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="74" spans="1:19" ht="18">
+    <row r="74" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A74" s="50" t="s">
         <v>322</v>
       </c>
@@ -6879,7 +6917,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:19" ht="18">
+    <row r="75" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A75" s="50" t="s">
         <v>344</v>
       </c>
@@ -6936,7 +6974,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="76" spans="1:19" ht="18">
+    <row r="76" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A76" s="18" t="s">
         <v>328</v>
       </c>
@@ -6993,7 +7031,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="77" spans="1:19" ht="18">
+    <row r="77" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A77" s="18" t="s">
         <v>366</v>
       </c>
@@ -7050,7 +7088,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="78" spans="1:19" ht="18">
+    <row r="78" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A78" s="18" t="s">
         <v>326</v>
       </c>
@@ -7107,7 +7145,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="79" spans="1:19" ht="18">
+    <row r="79" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A79" s="18" t="s">
         <v>335</v>
       </c>
@@ -7164,7 +7202,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="80" spans="1:19" ht="18">
+    <row r="80" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A80" s="18" t="s">
         <v>327</v>
       </c>
@@ -7221,7 +7259,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="81" spans="1:19" ht="18">
+    <row r="81" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A81" s="53" t="s">
         <v>342</v>
       </c>
@@ -7278,7 +7316,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="82" spans="1:19" ht="18">
+    <row r="82" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A82" s="53" t="s">
         <v>368</v>
       </c>
@@ -7335,7 +7373,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="83" spans="1:19" ht="18">
+    <row r="83" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A83" s="53" t="s">
         <v>337</v>
       </c>
@@ -7392,7 +7430,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:19" ht="18">
+    <row r="84" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A84" s="54" t="s">
         <v>333</v>
       </c>
@@ -7449,214 +7487,136 @@
         <v>80</v>
       </c>
     </row>
-    <row r="85" spans="1:19" ht="18">
-      <c r="A85" s="55" t="s">
+    <row r="85" spans="1:19" ht="19" x14ac:dyDescent="0.25">
+      <c r="A85" s="54" t="s">
+        <v>665</v>
+      </c>
+      <c r="B85" s="52" t="s">
+        <v>668</v>
+      </c>
+      <c r="C85" s="52"/>
+      <c r="D85" s="52"/>
+      <c r="E85" s="52"/>
+      <c r="F85" s="5"/>
+      <c r="G85" s="6" t="s">
+        <v>671</v>
+      </c>
+      <c r="H85" s="6"/>
+      <c r="I85" s="7"/>
+      <c r="J85" s="5"/>
+      <c r="K85" s="8"/>
+      <c r="L85" s="9"/>
+      <c r="M85" s="10"/>
+      <c r="N85" s="6"/>
+      <c r="O85" s="6"/>
+      <c r="P85" s="6"/>
+      <c r="Q85" s="6"/>
+      <c r="R85" s="6"/>
+      <c r="S85" s="6"/>
+    </row>
+    <row r="86" spans="1:19" ht="19" x14ac:dyDescent="0.25">
+      <c r="A86" s="54" t="s">
+        <v>666</v>
+      </c>
+      <c r="B86" s="52" t="s">
+        <v>669</v>
+      </c>
+      <c r="C86" s="52"/>
+      <c r="D86" s="52"/>
+      <c r="E86" s="52"/>
+      <c r="F86" s="5"/>
+      <c r="G86" s="6" t="s">
+        <v>670</v>
+      </c>
+      <c r="H86" s="6"/>
+      <c r="I86" s="7"/>
+      <c r="J86" s="5"/>
+      <c r="K86" s="8"/>
+      <c r="L86" s="9"/>
+      <c r="M86" s="10"/>
+      <c r="N86" s="6"/>
+      <c r="O86" s="6"/>
+      <c r="P86" s="6"/>
+      <c r="Q86" s="6"/>
+      <c r="R86" s="6"/>
+      <c r="S86" s="6"/>
+    </row>
+    <row r="87" spans="1:19" ht="19" x14ac:dyDescent="0.25">
+      <c r="A87" s="54" t="s">
+        <v>667</v>
+      </c>
+      <c r="B87" s="52" t="s">
+        <v>672</v>
+      </c>
+      <c r="C87" s="52"/>
+      <c r="D87" s="52"/>
+      <c r="E87" s="52"/>
+      <c r="F87" s="5"/>
+      <c r="G87" s="6" t="s">
+        <v>673</v>
+      </c>
+      <c r="H87" s="6"/>
+      <c r="I87" s="7"/>
+      <c r="J87" s="5"/>
+      <c r="K87" s="8"/>
+      <c r="L87" s="9"/>
+      <c r="M87" s="10"/>
+      <c r="N87" s="6"/>
+      <c r="O87" s="6"/>
+      <c r="P87" s="6"/>
+      <c r="Q87" s="6"/>
+      <c r="R87" s="6"/>
+      <c r="S87" s="6"/>
+    </row>
+    <row r="88" spans="1:19" ht="19" x14ac:dyDescent="0.25">
+      <c r="A88" s="55" t="s">
         <v>336</v>
       </c>
-      <c r="B85" s="20" t="s">
+      <c r="B88" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="C85" s="20" t="s">
+      <c r="C88" s="20" t="s">
         <v>499</v>
-      </c>
-      <c r="D85" s="20" t="s">
-        <v>245</v>
-      </c>
-      <c r="E85" s="20" t="s">
-        <v>630</v>
-      </c>
-      <c r="F85" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="G85" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="H85" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="I85" s="7">
-        <v>1</v>
-      </c>
-      <c r="J85" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="K85" s="8"/>
-      <c r="L85" s="9">
-        <v>172148</v>
-      </c>
-      <c r="M85" s="10">
-        <v>1176</v>
-      </c>
-      <c r="N85" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="O85" s="6" t="s">
-        <v>640</v>
-      </c>
-      <c r="P85" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q85" s="6">
-        <v>1995</v>
-      </c>
-      <c r="R85" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="S85" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="86" spans="1:19" ht="18">
-      <c r="A86" s="55" t="s">
-        <v>103</v>
-      </c>
-      <c r="B86" s="20" t="s">
-        <v>241</v>
-      </c>
-      <c r="C86" s="20" t="s">
-        <v>618</v>
-      </c>
-      <c r="D86" s="20" t="s">
-        <v>245</v>
-      </c>
-      <c r="E86" s="20" t="s">
-        <v>630</v>
-      </c>
-      <c r="F86" s="13"/>
-      <c r="G86" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="H86" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I86" s="6"/>
-      <c r="J86" s="13"/>
-      <c r="K86" s="8"/>
-      <c r="L86" s="14">
-        <v>64307</v>
-      </c>
-      <c r="M86" s="10" t="s">
-        <v>619</v>
-      </c>
-      <c r="N86" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="O86" s="6" t="s">
-        <v>644</v>
-      </c>
-      <c r="P86" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="Q86" s="6">
-        <v>1976</v>
-      </c>
-      <c r="R86" s="6">
-        <v>20</v>
-      </c>
-      <c r="S86" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="87" spans="1:19" ht="18">
-      <c r="A87" s="55" t="s">
-        <v>104</v>
-      </c>
-      <c r="B87" s="20" t="s">
-        <v>242</v>
-      </c>
-      <c r="C87" s="20" t="s">
-        <v>620</v>
-      </c>
-      <c r="D87" s="20" t="s">
-        <v>245</v>
-      </c>
-      <c r="E87" s="22" t="s">
-        <v>630</v>
-      </c>
-      <c r="F87" s="13"/>
-      <c r="G87" s="6" t="s">
-        <v>621</v>
-      </c>
-      <c r="H87" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I87" s="6"/>
-      <c r="J87" s="13"/>
-      <c r="K87" s="8"/>
-      <c r="L87" s="14">
-        <v>64310</v>
-      </c>
-      <c r="M87" s="10" t="s">
-        <v>622</v>
-      </c>
-      <c r="N87" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="O87" s="8" t="s">
-        <v>643</v>
-      </c>
-      <c r="P87" s="6" t="s">
-        <v>623</v>
-      </c>
-      <c r="Q87" s="6">
-        <v>1967</v>
-      </c>
-      <c r="R87" s="6">
-        <v>8</v>
-      </c>
-      <c r="S87" s="6" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="88" spans="1:19" ht="18">
-      <c r="A88" s="55" t="s">
-        <v>359</v>
-      </c>
-      <c r="B88" s="20" t="s">
-        <v>204</v>
-      </c>
-      <c r="C88" s="20" t="s">
-        <v>560</v>
       </c>
       <c r="D88" s="20" t="s">
         <v>245</v>
       </c>
-      <c r="E88" s="22" t="s">
+      <c r="E88" s="20" t="s">
         <v>630</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="H88" s="8"/>
+        <v>165</v>
+      </c>
+      <c r="H88" s="6" t="s">
+        <v>165</v>
+      </c>
       <c r="I88" s="7">
         <v>1</v>
       </c>
-      <c r="J88" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="K88" s="6" t="s">
-        <v>205</v>
-      </c>
+      <c r="J88" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="K88" s="8"/>
       <c r="L88" s="9">
-        <v>1456752</v>
-      </c>
-      <c r="M88" s="10" t="s">
-        <v>7</v>
+        <v>172148</v>
+      </c>
+      <c r="M88" s="10">
+        <v>1176</v>
       </c>
       <c r="N88" s="6" t="s">
-        <v>288</v>
+        <v>49</v>
       </c>
       <c r="O88" s="6" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="P88" s="6" t="s">
-        <v>289</v>
+        <v>7</v>
       </c>
       <c r="Q88" s="6">
-        <v>1989</v>
+        <v>1995</v>
       </c>
       <c r="R88" s="6" t="s">
         <v>7</v>
@@ -7665,15 +7625,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="1:19" ht="18">
+    <row r="89" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A89" s="55" t="s">
-        <v>341</v>
+        <v>103</v>
       </c>
       <c r="B89" s="20" t="s">
-        <v>170</v>
+        <v>241</v>
       </c>
       <c r="C89" s="20" t="s">
-        <v>510</v>
+        <v>618</v>
       </c>
       <c r="D89" s="20" t="s">
         <v>245</v>
@@ -7681,170 +7641,158 @@
       <c r="E89" s="20" t="s">
         <v>630</v>
       </c>
-      <c r="F89" s="5" t="s">
-        <v>246</v>
-      </c>
+      <c r="F89" s="13"/>
       <c r="G89" s="6" t="s">
-        <v>511</v>
+        <v>203</v>
       </c>
       <c r="H89" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I89" s="7">
-        <v>1</v>
-      </c>
-      <c r="J89" s="5" t="s">
-        <v>247</v>
-      </c>
+      <c r="I89" s="6"/>
+      <c r="J89" s="13"/>
       <c r="K89" s="8"/>
-      <c r="L89" s="9">
-        <v>64287</v>
+      <c r="L89" s="14">
+        <v>64307</v>
       </c>
       <c r="M89" s="10" t="s">
-        <v>512</v>
+        <v>619</v>
       </c>
       <c r="N89" s="6" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="O89" s="6" t="s">
-        <v>640</v>
+        <v>644</v>
       </c>
       <c r="P89" s="6" t="s">
-        <v>513</v>
+        <v>293</v>
       </c>
       <c r="Q89" s="6">
-        <v>1972</v>
+        <v>1976</v>
       </c>
       <c r="R89" s="6">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="S89" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="90" spans="1:19" ht="18">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A90" s="55" t="s">
-        <v>312</v>
+        <v>104</v>
       </c>
       <c r="B90" s="20" t="s">
-        <v>122</v>
+        <v>242</v>
       </c>
       <c r="C90" s="20" t="s">
-        <v>425</v>
+        <v>620</v>
       </c>
       <c r="D90" s="20" t="s">
         <v>245</v>
       </c>
-      <c r="E90" s="20" t="s">
+      <c r="E90" s="22" t="s">
         <v>630</v>
       </c>
-      <c r="F90" s="5" t="s">
-        <v>250</v>
-      </c>
+      <c r="F90" s="13"/>
       <c r="G90" s="6" t="s">
-        <v>123</v>
+        <v>621</v>
       </c>
       <c r="H90" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="I90" s="7">
-        <v>1</v>
-      </c>
-      <c r="J90" s="5" t="s">
-        <v>247</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="I90" s="6"/>
+      <c r="J90" s="13"/>
       <c r="K90" s="8"/>
-      <c r="L90" s="9">
-        <v>33743</v>
+      <c r="L90" s="14">
+        <v>64310</v>
       </c>
       <c r="M90" s="10" t="s">
-        <v>7</v>
+        <v>622</v>
       </c>
       <c r="N90" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="O90" s="6" t="s">
-        <v>640</v>
+        <v>23</v>
+      </c>
+      <c r="O90" s="8" t="s">
+        <v>643</v>
       </c>
       <c r="P90" s="6" t="s">
-        <v>426</v>
+        <v>623</v>
       </c>
       <c r="Q90" s="6">
-        <v>1957</v>
+        <v>1967</v>
       </c>
       <c r="R90" s="6">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="S90" s="6" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="91" spans="1:19" ht="18">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A91" s="55" t="s">
-        <v>332</v>
+        <v>359</v>
       </c>
       <c r="B91" s="20" t="s">
-        <v>160</v>
+        <v>204</v>
       </c>
       <c r="C91" s="20" t="s">
-        <v>490</v>
+        <v>560</v>
       </c>
       <c r="D91" s="20" t="s">
         <v>245</v>
       </c>
-      <c r="E91" s="20" t="s">
+      <c r="E91" s="22" t="s">
         <v>630</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>246</v>
+        <v>258</v>
       </c>
       <c r="G91" s="6" t="s">
-        <v>491</v>
-      </c>
-      <c r="H91" s="6" t="s">
-        <v>7</v>
-      </c>
+        <v>205</v>
+      </c>
+      <c r="H91" s="8"/>
       <c r="I91" s="7">
         <v>1</v>
       </c>
       <c r="J91" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="K91" s="8"/>
+      <c r="K91" s="6" t="s">
+        <v>205</v>
+      </c>
       <c r="L91" s="9">
-        <v>11085</v>
+        <v>1456752</v>
       </c>
       <c r="M91" s="10" t="s">
-        <v>492</v>
+        <v>7</v>
       </c>
       <c r="N91" s="6" t="s">
-        <v>100</v>
+        <v>288</v>
       </c>
       <c r="O91" s="6" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="P91" s="6" t="s">
-        <v>493</v>
+        <v>289</v>
       </c>
       <c r="Q91" s="6">
-        <v>1956</v>
-      </c>
-      <c r="R91" s="6">
-        <v>17</v>
+        <v>1989</v>
+      </c>
+      <c r="R91" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="S91" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="92" spans="1:19" ht="18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A92" s="55" t="s">
-        <v>320</v>
+        <v>341</v>
       </c>
       <c r="B92" s="20" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
       <c r="C92" s="20" t="s">
-        <v>299</v>
+        <v>510</v>
       </c>
       <c r="D92" s="20" t="s">
         <v>245</v>
@@ -7853,10 +7801,10 @@
         <v>630</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="G92" s="6" t="s">
-        <v>466</v>
+        <v>511</v>
       </c>
       <c r="H92" s="6" t="s">
         <v>7</v>
@@ -7869,92 +7817,96 @@
       </c>
       <c r="K92" s="8"/>
       <c r="L92" s="9">
-        <v>11086</v>
+        <v>64287</v>
       </c>
       <c r="M92" s="10" t="s">
-        <v>7</v>
+        <v>512</v>
       </c>
       <c r="N92" s="6" t="s">
-        <v>467</v>
+        <v>51</v>
       </c>
       <c r="O92" s="6" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="P92" s="6" t="s">
-        <v>468</v>
+        <v>513</v>
       </c>
       <c r="Q92" s="6">
-        <v>1929</v>
+        <v>1972</v>
       </c>
       <c r="R92" s="6">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="S92" s="6" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="93" spans="1:19" ht="18">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A93" s="55" t="s">
-        <v>101</v>
+        <v>312</v>
       </c>
       <c r="B93" s="20" t="s">
-        <v>240</v>
+        <v>122</v>
       </c>
       <c r="C93" s="20" t="s">
-        <v>614</v>
+        <v>425</v>
       </c>
       <c r="D93" s="20" t="s">
         <v>245</v>
       </c>
-      <c r="E93" s="22" t="s">
+      <c r="E93" s="20" t="s">
         <v>630</v>
       </c>
-      <c r="F93" s="13"/>
+      <c r="F93" s="5" t="s">
+        <v>250</v>
+      </c>
       <c r="G93" s="6" t="s">
-        <v>615</v>
+        <v>123</v>
       </c>
       <c r="H93" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I93" s="6"/>
+        <v>123</v>
+      </c>
+      <c r="I93" s="7">
+        <v>1</v>
+      </c>
       <c r="J93" s="5" t="s">
         <v>247</v>
       </c>
       <c r="K93" s="8"/>
-      <c r="L93" s="14">
-        <v>35279</v>
+      <c r="L93" s="9">
+        <v>33743</v>
       </c>
       <c r="M93" s="10" t="s">
-        <v>616</v>
+        <v>7</v>
       </c>
       <c r="N93" s="6" t="s">
-        <v>102</v>
+        <v>25</v>
       </c>
       <c r="O93" s="6" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="P93" s="6" t="s">
-        <v>617</v>
+        <v>426</v>
       </c>
       <c r="Q93" s="6">
-        <v>1981</v>
+        <v>1957</v>
       </c>
       <c r="R93" s="6">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="S93" s="6" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="94" spans="1:19" ht="18">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="94" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A94" s="55" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="B94" s="20" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C94" s="20" t="s">
-        <v>502</v>
+        <v>490</v>
       </c>
       <c r="D94" s="20" t="s">
         <v>245</v>
@@ -7963,10 +7915,10 @@
         <v>630</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="G94" s="6" t="s">
-        <v>165</v>
+        <v>491</v>
       </c>
       <c r="H94" s="6" t="s">
         <v>7</v>
@@ -7979,39 +7931,39 @@
       </c>
       <c r="K94" s="8"/>
       <c r="L94" s="9">
-        <v>12542</v>
+        <v>11085</v>
       </c>
       <c r="M94" s="10" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
       <c r="N94" s="6" t="s">
-        <v>288</v>
+        <v>100</v>
       </c>
       <c r="O94" s="6" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="P94" s="6" t="s">
-        <v>504</v>
+        <v>493</v>
       </c>
       <c r="Q94" s="6">
-        <v>1947</v>
+        <v>1956</v>
       </c>
       <c r="R94" s="6">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="S94" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="95" spans="1:19" ht="18">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A95" s="55" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="B95" s="20" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="C95" s="20" t="s">
-        <v>486</v>
+        <v>299</v>
       </c>
       <c r="D95" s="20" t="s">
         <v>245</v>
@@ -8020,10 +7972,10 @@
         <v>630</v>
       </c>
       <c r="F95" s="5" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="G95" s="6" t="s">
-        <v>165</v>
+        <v>466</v>
       </c>
       <c r="H95" s="6" t="s">
         <v>7</v>
@@ -8036,145 +7988,149 @@
       </c>
       <c r="K95" s="8"/>
       <c r="L95" s="9">
-        <v>11083</v>
+        <v>11086</v>
       </c>
       <c r="M95" s="10" t="s">
-        <v>487</v>
+        <v>7</v>
       </c>
       <c r="N95" s="6" t="s">
-        <v>488</v>
+        <v>467</v>
       </c>
       <c r="O95" s="6" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="P95" s="6" t="s">
-        <v>489</v>
+        <v>468</v>
       </c>
       <c r="Q95" s="6">
-        <v>1958</v>
+        <v>1929</v>
       </c>
       <c r="R95" s="6">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="S95" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="96" spans="1:19" ht="18">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A96" s="55" t="s">
-        <v>311</v>
+        <v>101</v>
       </c>
       <c r="B96" s="20" t="s">
-        <v>113</v>
+        <v>240</v>
       </c>
       <c r="C96" s="20" t="s">
-        <v>399</v>
+        <v>614</v>
       </c>
       <c r="D96" s="20" t="s">
         <v>245</v>
       </c>
-      <c r="E96" s="20" t="s">
+      <c r="E96" s="22" t="s">
         <v>630</v>
       </c>
-      <c r="F96" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="G96" s="5" t="s">
-        <v>400</v>
-      </c>
-      <c r="H96" s="7"/>
-      <c r="I96" s="7">
-        <v>1</v>
-      </c>
+      <c r="F96" s="13"/>
+      <c r="G96" s="6" t="s">
+        <v>615</v>
+      </c>
+      <c r="H96" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I96" s="6"/>
       <c r="J96" s="5" t="s">
         <v>247</v>
       </c>
       <c r="K96" s="8"/>
-      <c r="L96" s="9">
-        <v>64288</v>
+      <c r="L96" s="14">
+        <v>35279</v>
       </c>
       <c r="M96" s="10" t="s">
-        <v>401</v>
+        <v>616</v>
       </c>
       <c r="N96" s="6" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="O96" s="6" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="P96" s="6" t="s">
-        <v>402</v>
+        <v>617</v>
       </c>
       <c r="Q96" s="6">
-        <v>1968</v>
+        <v>1981</v>
       </c>
       <c r="R96" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S96" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="97" spans="1:19" ht="18">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="97" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A97" s="55" t="s">
-        <v>105</v>
+        <v>338</v>
       </c>
       <c r="B97" s="20" t="s">
-        <v>275</v>
+        <v>167</v>
       </c>
       <c r="C97" s="20" t="s">
-        <v>624</v>
+        <v>502</v>
       </c>
       <c r="D97" s="20" t="s">
         <v>245</v>
       </c>
-      <c r="E97" s="22" t="s">
+      <c r="E97" s="20" t="s">
         <v>630</v>
       </c>
-      <c r="F97" s="23"/>
-      <c r="G97" s="8" t="s">
-        <v>305</v>
-      </c>
-      <c r="H97" s="8" t="s">
-        <v>305</v>
-      </c>
-      <c r="I97" s="8"/>
-      <c r="J97" s="23"/>
+      <c r="F97" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="G97" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="H97" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I97" s="7">
+        <v>1</v>
+      </c>
+      <c r="J97" s="5" t="s">
+        <v>247</v>
+      </c>
       <c r="K97" s="8"/>
-      <c r="L97" s="24">
-        <v>40012</v>
-      </c>
-      <c r="M97" s="25" t="s">
-        <v>625</v>
-      </c>
-      <c r="N97" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="O97" s="8" t="s">
-        <v>644</v>
-      </c>
-      <c r="P97" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="Q97" s="8">
-        <v>1974</v>
-      </c>
-      <c r="R97" s="8">
-        <v>26</v>
-      </c>
-      <c r="S97" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="98" spans="1:19" ht="18">
+      <c r="L97" s="9">
+        <v>12542</v>
+      </c>
+      <c r="M97" s="10" t="s">
+        <v>503</v>
+      </c>
+      <c r="N97" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="O97" s="6" t="s">
+        <v>642</v>
+      </c>
+      <c r="P97" s="6" t="s">
+        <v>504</v>
+      </c>
+      <c r="Q97" s="6">
+        <v>1947</v>
+      </c>
+      <c r="R97" s="6">
+        <v>14</v>
+      </c>
+      <c r="S97" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="98" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A98" s="55" t="s">
-        <v>370</v>
+        <v>331</v>
       </c>
       <c r="B98" s="20" t="s">
-        <v>228</v>
+        <v>159</v>
       </c>
       <c r="C98" s="20" t="s">
-        <v>578</v>
+        <v>486</v>
       </c>
       <c r="D98" s="20" t="s">
         <v>245</v>
@@ -8183,13 +8139,13 @@
         <v>630</v>
       </c>
       <c r="F98" s="5" t="s">
-        <v>246</v>
+        <v>261</v>
       </c>
       <c r="G98" s="6" t="s">
-        <v>229</v>
+        <v>165</v>
       </c>
       <c r="H98" s="6" t="s">
-        <v>229</v>
+        <v>7</v>
       </c>
       <c r="I98" s="7">
         <v>1</v>
@@ -8199,39 +8155,39 @@
       </c>
       <c r="K98" s="8"/>
       <c r="L98" s="9">
-        <v>1691889</v>
+        <v>11083</v>
       </c>
       <c r="M98" s="10" t="s">
-        <v>88</v>
+        <v>487</v>
       </c>
       <c r="N98" s="6" t="s">
-        <v>43</v>
+        <v>488</v>
       </c>
       <c r="O98" s="6" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="P98" s="6" t="s">
-        <v>579</v>
+        <v>489</v>
       </c>
       <c r="Q98" s="6">
-        <v>2011</v>
-      </c>
-      <c r="R98" s="6" t="s">
-        <v>7</v>
+        <v>1958</v>
+      </c>
+      <c r="R98" s="6">
+        <v>23</v>
       </c>
       <c r="S98" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="99" spans="1:19" ht="18">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="99" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A99" s="55" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="B99" s="20" t="s">
-        <v>146</v>
+        <v>113</v>
       </c>
       <c r="C99" s="20" t="s">
-        <v>463</v>
+        <v>399</v>
       </c>
       <c r="D99" s="20" t="s">
         <v>245</v>
@@ -8240,14 +8196,12 @@
         <v>630</v>
       </c>
       <c r="F99" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="G99" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H99" s="6" t="s">
-        <v>7</v>
-      </c>
+        <v>246</v>
+      </c>
+      <c r="G99" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="H99" s="7"/>
       <c r="I99" s="7">
         <v>1</v>
       </c>
@@ -8256,183 +8210,187 @@
       </c>
       <c r="K99" s="8"/>
       <c r="L99" s="9">
-        <v>11084</v>
+        <v>64288</v>
       </c>
       <c r="M99" s="10" t="s">
-        <v>464</v>
+        <v>401</v>
       </c>
       <c r="N99" s="6" t="s">
-        <v>638</v>
+        <v>11</v>
       </c>
       <c r="O99" s="6" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="P99" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q99" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="R99" s="6" t="s">
-        <v>7</v>
+        <v>402</v>
+      </c>
+      <c r="Q99" s="6">
+        <v>1968</v>
+      </c>
+      <c r="R99" s="6">
+        <v>2</v>
       </c>
       <c r="S99" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="100" spans="1:19" ht="18">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="100" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A100" s="55" t="s">
-        <v>12</v>
+        <v>105</v>
       </c>
       <c r="B100" s="20" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="C100" s="20" t="s">
-        <v>403</v>
+        <v>624</v>
       </c>
       <c r="D100" s="20" t="s">
         <v>245</v>
       </c>
-      <c r="E100" s="20" t="s">
+      <c r="E100" s="22" t="s">
         <v>630</v>
       </c>
-      <c r="F100" s="13"/>
-      <c r="G100" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H100" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I100" s="6"/>
-      <c r="J100" s="13"/>
+      <c r="F100" s="23"/>
+      <c r="G100" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="H100" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="I100" s="8"/>
+      <c r="J100" s="23"/>
       <c r="K100" s="8"/>
-      <c r="L100" s="14">
-        <v>47300</v>
-      </c>
-      <c r="M100" s="10" t="s">
-        <v>404</v>
-      </c>
-      <c r="N100" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="O100" s="6" t="s">
-        <v>640</v>
-      </c>
-      <c r="P100" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q100" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="R100" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="S100" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="101" spans="1:19" ht="18">
+      <c r="L100" s="24">
+        <v>40012</v>
+      </c>
+      <c r="M100" s="25" t="s">
+        <v>625</v>
+      </c>
+      <c r="N100" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="O100" s="8" t="s">
+        <v>644</v>
+      </c>
+      <c r="P100" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="Q100" s="8">
+        <v>1974</v>
+      </c>
+      <c r="R100" s="8">
+        <v>26</v>
+      </c>
+      <c r="S100" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="101" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A101" s="55" t="s">
-        <v>358</v>
+        <v>370</v>
       </c>
       <c r="B101" s="20" t="s">
-        <v>202</v>
+        <v>228</v>
       </c>
       <c r="C101" s="20" t="s">
-        <v>558</v>
+        <v>578</v>
       </c>
       <c r="D101" s="20" t="s">
         <v>245</v>
       </c>
-      <c r="E101" s="22" t="s">
+      <c r="E101" s="20" t="s">
         <v>630</v>
       </c>
       <c r="F101" s="5" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="G101" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="H101" s="8"/>
+        <v>229</v>
+      </c>
+      <c r="H101" s="6" t="s">
+        <v>229</v>
+      </c>
       <c r="I101" s="7">
         <v>1</v>
       </c>
       <c r="J101" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="K101" s="6" t="s">
-        <v>203</v>
-      </c>
+      <c r="K101" s="8"/>
       <c r="L101" s="9">
-        <v>40004</v>
+        <v>1691889</v>
       </c>
       <c r="M101" s="10" t="s">
-        <v>559</v>
+        <v>88</v>
       </c>
       <c r="N101" s="6" t="s">
-        <v>288</v>
+        <v>43</v>
       </c>
       <c r="O101" s="6" t="s">
         <v>642</v>
       </c>
       <c r="P101" s="6" t="s">
-        <v>287</v>
+        <v>579</v>
       </c>
       <c r="Q101" s="6">
-        <v>1969</v>
-      </c>
-      <c r="R101" s="6">
-        <v>18</v>
+        <v>2011</v>
+      </c>
+      <c r="R101" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="S101" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="102" spans="1:19" ht="18">
-      <c r="A102" s="4" t="s">
-        <v>369</v>
-      </c>
-      <c r="B102" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="C102" s="6"/>
-      <c r="D102" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="E102" s="6"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:19" ht="19" x14ac:dyDescent="0.25">
+      <c r="A102" s="55" t="s">
+        <v>318</v>
+      </c>
+      <c r="B102" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="C102" s="20" t="s">
+        <v>463</v>
+      </c>
+      <c r="D102" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="E102" s="20" t="s">
+        <v>630</v>
+      </c>
       <c r="F102" s="5" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="G102" s="6" t="s">
-        <v>183</v>
+        <v>7</v>
       </c>
       <c r="H102" s="6" t="s">
-        <v>183</v>
+        <v>7</v>
       </c>
       <c r="I102" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J102" s="5" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="K102" s="8"/>
       <c r="L102" s="9">
-        <v>1633878</v>
+        <v>11084</v>
       </c>
       <c r="M102" s="10" t="s">
-        <v>86</v>
+        <v>464</v>
       </c>
       <c r="N102" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="O102" s="8" t="s">
-        <v>643</v>
+        <v>638</v>
+      </c>
+      <c r="O102" s="6" t="s">
+        <v>642</v>
       </c>
       <c r="P102" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="Q102" s="6">
-        <v>2011</v>
+      <c r="Q102" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="R102" s="6" t="s">
         <v>7</v>
@@ -8441,42 +8399,40 @@
         <v>7</v>
       </c>
     </row>
-    <row r="103" spans="1:19" ht="18">
-      <c r="A103" s="4" t="s">
-        <v>361</v>
-      </c>
-      <c r="B103" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="C103" s="6"/>
-      <c r="D103" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="E103" s="6"/>
-      <c r="F103" s="5" t="s">
-        <v>270</v>
-      </c>
+    <row r="103" spans="1:19" ht="19" x14ac:dyDescent="0.25">
+      <c r="A103" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="B103" s="20" t="s">
+        <v>248</v>
+      </c>
+      <c r="C103" s="20" t="s">
+        <v>403</v>
+      </c>
+      <c r="D103" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="E103" s="20" t="s">
+        <v>630</v>
+      </c>
+      <c r="F103" s="13"/>
       <c r="G103" s="6" t="s">
-        <v>216</v>
+        <v>7</v>
       </c>
       <c r="H103" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="I103" s="7">
-        <v>0</v>
-      </c>
-      <c r="J103" s="5" t="s">
-        <v>259</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="I103" s="6"/>
+      <c r="J103" s="13"/>
       <c r="K103" s="8"/>
-      <c r="L103" s="9">
-        <v>1416349</v>
+      <c r="L103" s="14">
+        <v>47300</v>
       </c>
       <c r="M103" s="10" t="s">
-        <v>7</v>
+        <v>404</v>
       </c>
       <c r="N103" s="6" t="s">
-        <v>76</v>
+        <v>13</v>
       </c>
       <c r="O103" s="6" t="s">
         <v>640</v>
@@ -8484,8 +8440,8 @@
       <c r="P103" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="Q103" s="6">
-        <v>2013</v>
+      <c r="Q103" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="R103" s="6" t="s">
         <v>7</v>
@@ -8494,65 +8450,69 @@
         <v>7</v>
       </c>
     </row>
-    <row r="104" spans="1:19" ht="18">
-      <c r="A104" s="4" t="s">
-        <v>362</v>
-      </c>
-      <c r="B104" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C104" s="6"/>
-      <c r="D104" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="E104" s="6"/>
+    <row r="104" spans="1:19" ht="19" x14ac:dyDescent="0.25">
+      <c r="A104" s="55" t="s">
+        <v>358</v>
+      </c>
+      <c r="B104" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="C104" s="20" t="s">
+        <v>558</v>
+      </c>
+      <c r="D104" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="E104" s="22" t="s">
+        <v>630</v>
+      </c>
       <c r="F104" s="5" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G104" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="H104" s="6" t="s">
-        <v>218</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="H104" s="8"/>
       <c r="I104" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J104" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="K104" s="8"/>
+        <v>247</v>
+      </c>
+      <c r="K104" s="6" t="s">
+        <v>203</v>
+      </c>
       <c r="L104" s="9">
-        <v>1562038</v>
+        <v>40004</v>
       </c>
       <c r="M104" s="10" t="s">
-        <v>77</v>
+        <v>559</v>
       </c>
       <c r="N104" s="6" t="s">
-        <v>46</v>
+        <v>288</v>
       </c>
       <c r="O104" s="6" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="P104" s="6" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="Q104" s="6">
-        <v>2013</v>
+        <v>1969</v>
       </c>
       <c r="R104" s="6">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="S104" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="105" spans="1:19" ht="18">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="105" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="C105" s="6"/>
       <c r="D105" s="6" t="s">
@@ -8560,13 +8520,13 @@
       </c>
       <c r="E105" s="6"/>
       <c r="F105" s="5" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="G105" s="6" t="s">
-        <v>218</v>
+        <v>183</v>
       </c>
       <c r="H105" s="6" t="s">
-        <v>218</v>
+        <v>183</v>
       </c>
       <c r="I105" s="7">
         <v>0</v>
@@ -8576,36 +8536,36 @@
       </c>
       <c r="K105" s="8"/>
       <c r="L105" s="9">
-        <v>1562039</v>
+        <v>1633878</v>
       </c>
       <c r="M105" s="10" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="N105" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="O105" s="6" t="s">
-        <v>641</v>
+        <v>87</v>
+      </c>
+      <c r="O105" s="8" t="s">
+        <v>643</v>
       </c>
       <c r="P105" s="6" t="s">
-        <v>295</v>
+        <v>7</v>
       </c>
       <c r="Q105" s="6">
-        <v>2012</v>
-      </c>
-      <c r="R105" s="6">
-        <v>20</v>
+        <v>2011</v>
+      </c>
+      <c r="R105" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="S105" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="106" spans="1:19" ht="18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="106" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="C106" s="6"/>
       <c r="D106" s="6" t="s">
@@ -8613,13 +8573,13 @@
       </c>
       <c r="E106" s="6"/>
       <c r="F106" s="5" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
       <c r="G106" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H106" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I106" s="7">
         <v>0</v>
@@ -8629,36 +8589,36 @@
       </c>
       <c r="K106" s="8"/>
       <c r="L106" s="9">
-        <v>1562065</v>
+        <v>1416349</v>
       </c>
       <c r="M106" s="10" t="s">
-        <v>82</v>
+        <v>7</v>
       </c>
       <c r="N106" s="6" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="O106" s="6" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="P106" s="6" t="s">
-        <v>295</v>
+        <v>7</v>
       </c>
       <c r="Q106" s="6">
-        <v>2012</v>
-      </c>
-      <c r="R106" s="6">
-        <v>2</v>
+        <v>2013</v>
+      </c>
+      <c r="R106" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="S106" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="107" spans="1:19" ht="18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="107" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C107" s="6"/>
       <c r="D107" s="6" t="s">
@@ -8682,10 +8642,10 @@
       </c>
       <c r="K107" s="8"/>
       <c r="L107" s="9">
-        <v>1562066</v>
+        <v>1562038</v>
       </c>
       <c r="M107" s="10" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="N107" s="6" t="s">
         <v>46</v>
@@ -8700,18 +8660,18 @@
         <v>2013</v>
       </c>
       <c r="R107" s="6">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="S107" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="108" spans="1:19" ht="18">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="108" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
-        <v>355</v>
+        <v>363</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>197</v>
+        <v>219</v>
       </c>
       <c r="C108" s="6"/>
       <c r="D108" s="6" t="s">
@@ -8722,10 +8682,10 @@
         <v>261</v>
       </c>
       <c r="G108" s="6" t="s">
-        <v>198</v>
+        <v>218</v>
       </c>
       <c r="H108" s="6" t="s">
-        <v>198</v>
+        <v>218</v>
       </c>
       <c r="I108" s="7">
         <v>0</v>
@@ -8735,10 +8695,10 @@
       </c>
       <c r="K108" s="8"/>
       <c r="L108" s="9">
-        <v>1281454</v>
+        <v>1562039</v>
       </c>
       <c r="M108" s="10" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="N108" s="6" t="s">
         <v>46</v>
@@ -8747,42 +8707,38 @@
         <v>641</v>
       </c>
       <c r="P108" s="6" t="s">
-        <v>7</v>
+        <v>295</v>
       </c>
       <c r="Q108" s="6">
-        <v>2008</v>
-      </c>
-      <c r="R108" s="6" t="s">
-        <v>7</v>
+        <v>2012</v>
+      </c>
+      <c r="R108" s="6">
+        <v>20</v>
       </c>
       <c r="S108" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="109" spans="1:19" ht="18">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="109" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
-        <v>334</v>
+        <v>365</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="C109" s="6" t="s">
-        <v>302</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="C109" s="6"/>
       <c r="D109" s="6" t="s">
         <v>496</v>
       </c>
-      <c r="E109" s="6" t="s">
-        <v>303</v>
-      </c>
+      <c r="E109" s="6"/>
       <c r="F109" s="5" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="G109" s="6" t="s">
-        <v>7</v>
+        <v>218</v>
       </c>
       <c r="H109" s="6" t="s">
-        <v>7</v>
+        <v>218</v>
       </c>
       <c r="I109" s="7">
         <v>0</v>
@@ -8792,48 +8748,50 @@
       </c>
       <c r="K109" s="8"/>
       <c r="L109" s="9">
-        <v>11103</v>
+        <v>1562065</v>
       </c>
       <c r="M109" s="10" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="N109" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="O109" s="6"/>
+        <v>46</v>
+      </c>
+      <c r="O109" s="6" t="s">
+        <v>641</v>
+      </c>
       <c r="P109" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q109" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="R109" s="6" t="s">
-        <v>7</v>
+        <v>295</v>
+      </c>
+      <c r="Q109" s="6">
+        <v>2012</v>
+      </c>
+      <c r="R109" s="6">
+        <v>2</v>
       </c>
       <c r="S109" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="110" spans="1:19" ht="18">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="110" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
-        <v>353</v>
+        <v>364</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>193</v>
+        <v>220</v>
       </c>
       <c r="C110" s="6"/>
       <c r="D110" s="6" t="s">
-        <v>557</v>
+        <v>496</v>
       </c>
       <c r="E110" s="6"/>
       <c r="F110" s="5" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="G110" s="6" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="H110" s="6" t="s">
-        <v>194</v>
+        <v>218</v>
       </c>
       <c r="I110" s="7">
         <v>0</v>
@@ -8843,10 +8801,10 @@
       </c>
       <c r="K110" s="8"/>
       <c r="L110" s="9">
-        <v>1307803</v>
+        <v>1562066</v>
       </c>
       <c r="M110" s="10" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="N110" s="6" t="s">
         <v>46</v>
@@ -8855,40 +8813,38 @@
         <v>641</v>
       </c>
       <c r="P110" s="6" t="s">
-        <v>7</v>
+        <v>295</v>
       </c>
       <c r="Q110" s="6">
-        <v>2011</v>
-      </c>
-      <c r="R110" s="6" t="s">
-        <v>7</v>
+        <v>2013</v>
+      </c>
+      <c r="R110" s="6">
+        <v>30</v>
       </c>
       <c r="S110" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="111" spans="1:19" ht="18">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="111" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
-        <v>319</v>
+        <v>355</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="C111" s="6" t="s">
-        <v>465</v>
-      </c>
-      <c r="D111" s="5" t="s">
-        <v>557</v>
+        <v>197</v>
+      </c>
+      <c r="C111" s="6"/>
+      <c r="D111" s="6" t="s">
+        <v>496</v>
       </c>
       <c r="E111" s="6"/>
       <c r="F111" s="5" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="G111" s="6" t="s">
-        <v>7</v>
+        <v>198</v>
       </c>
       <c r="H111" s="6" t="s">
-        <v>7</v>
+        <v>198</v>
       </c>
       <c r="I111" s="7">
         <v>0</v>
@@ -8898,20 +8854,22 @@
       </c>
       <c r="K111" s="8"/>
       <c r="L111" s="9">
-        <v>54290</v>
+        <v>1281454</v>
       </c>
       <c r="M111" s="10" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="N111" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="O111" s="6"/>
+        <v>46</v>
+      </c>
+      <c r="O111" s="6" t="s">
+        <v>641</v>
+      </c>
       <c r="P111" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="Q111" s="6" t="s">
-        <v>7</v>
+      <c r="Q111" s="6">
+        <v>2008</v>
       </c>
       <c r="R111" s="6" t="s">
         <v>7</v>
@@ -8920,28 +8878,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="112" spans="1:19" ht="18">
+    <row r="112" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
-        <v>386</v>
+        <v>334</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>232</v>
+        <v>266</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>585</v>
+        <v>302</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>557</v>
-      </c>
-      <c r="E112" s="6"/>
+        <v>496</v>
+      </c>
+      <c r="E112" s="6" t="s">
+        <v>303</v>
+      </c>
       <c r="F112" s="5" t="s">
         <v>250</v>
       </c>
       <c r="G112" s="6" t="s">
-        <v>165</v>
+        <v>7</v>
       </c>
       <c r="H112" s="6" t="s">
-        <v>165</v>
+        <v>7</v>
       </c>
       <c r="I112" s="7">
         <v>0</v>
@@ -8951,52 +8911,48 @@
       </c>
       <c r="K112" s="8"/>
       <c r="L112" s="9">
-        <v>1729141</v>
+        <v>11103</v>
       </c>
       <c r="M112" s="10" t="s">
-        <v>92</v>
+        <v>48</v>
       </c>
       <c r="N112" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="O112" s="6" t="s">
-        <v>641</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="O112" s="6"/>
       <c r="P112" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="Q112" s="6">
-        <v>2008</v>
-      </c>
-      <c r="R112" s="6">
-        <v>28</v>
+      <c r="Q112" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="R112" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="S112" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="113" spans="1:19" ht="18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="113" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
-        <v>321</v>
+        <v>353</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="C113" s="6" t="s">
-        <v>469</v>
-      </c>
-      <c r="D113" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C113" s="6"/>
+      <c r="D113" s="6" t="s">
         <v>557</v>
       </c>
       <c r="E113" s="6"/>
       <c r="F113" s="5" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="G113" s="6" t="s">
-        <v>7</v>
+        <v>216</v>
       </c>
       <c r="H113" s="6" t="s">
-        <v>7</v>
+        <v>194</v>
       </c>
       <c r="I113" s="7">
         <v>0</v>
@@ -9006,20 +8962,22 @@
       </c>
       <c r="K113" s="8"/>
       <c r="L113" s="9">
-        <v>1307800</v>
+        <v>1307803</v>
       </c>
       <c r="M113" s="10" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="N113" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="O113" s="6"/>
+        <v>46</v>
+      </c>
+      <c r="O113" s="6" t="s">
+        <v>641</v>
+      </c>
       <c r="P113" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="Q113" s="6" t="s">
-        <v>7</v>
+      <c r="Q113" s="6">
+        <v>2011</v>
       </c>
       <c r="R113" s="6" t="s">
         <v>7</v>
@@ -9028,26 +8986,28 @@
         <v>7</v>
       </c>
     </row>
-    <row r="114" spans="1:19" ht="18">
+    <row r="114" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
-        <v>356</v>
+        <v>319</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="C114" s="6"/>
-      <c r="D114" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C114" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="D114" s="5" t="s">
         <v>557</v>
       </c>
       <c r="E114" s="6"/>
       <c r="F114" s="5" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="G114" s="6" t="s">
-        <v>200</v>
+        <v>7</v>
       </c>
       <c r="H114" s="6" t="s">
-        <v>200</v>
+        <v>7</v>
       </c>
       <c r="I114" s="7">
         <v>0</v>
@@ -9057,22 +9017,20 @@
       </c>
       <c r="K114" s="8"/>
       <c r="L114" s="9">
-        <v>1321391</v>
+        <v>54290</v>
       </c>
       <c r="M114" s="10" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="N114" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="O114" s="6" t="s">
-        <v>641</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="O114" s="6"/>
       <c r="P114" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="Q114" s="6">
-        <v>2008</v>
+      <c r="Q114" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="R114" s="6" t="s">
         <v>7</v>
@@ -9081,14 +9039,16 @@
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="1:19" ht="18">
+    <row r="115" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
-        <v>360</v>
+        <v>386</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="C115" s="6"/>
+        <v>232</v>
+      </c>
+      <c r="C115" s="6" t="s">
+        <v>585</v>
+      </c>
       <c r="D115" s="6" t="s">
         <v>557</v>
       </c>
@@ -9097,10 +9057,10 @@
         <v>250</v>
       </c>
       <c r="G115" s="6" t="s">
-        <v>213</v>
+        <v>165</v>
       </c>
       <c r="H115" s="6" t="s">
-        <v>213</v>
+        <v>165</v>
       </c>
       <c r="I115" s="7">
         <v>0</v>
@@ -9110,35 +9070,194 @@
       </c>
       <c r="K115" s="8"/>
       <c r="L115" s="9">
+        <v>1729141</v>
+      </c>
+      <c r="M115" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="N115" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="O115" s="6" t="s">
+        <v>641</v>
+      </c>
+      <c r="P115" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q115" s="6">
+        <v>2008</v>
+      </c>
+      <c r="R115" s="6">
+        <v>28</v>
+      </c>
+      <c r="S115" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="116" spans="1:19" ht="19" x14ac:dyDescent="0.25">
+      <c r="A116" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C116" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="D116" s="5" t="s">
+        <v>557</v>
+      </c>
+      <c r="E116" s="6"/>
+      <c r="F116" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="G116" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H116" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I116" s="7">
+        <v>0</v>
+      </c>
+      <c r="J116" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="K116" s="8"/>
+      <c r="L116" s="9">
+        <v>1307800</v>
+      </c>
+      <c r="M116" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="N116" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="O116" s="6"/>
+      <c r="P116" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q116" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="R116" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="S116" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="117" spans="1:19" ht="19" x14ac:dyDescent="0.25">
+      <c r="A117" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C117" s="6"/>
+      <c r="D117" s="6" t="s">
+        <v>557</v>
+      </c>
+      <c r="E117" s="6"/>
+      <c r="F117" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="G117" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="H117" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="I117" s="7">
+        <v>0</v>
+      </c>
+      <c r="J117" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="K117" s="8"/>
+      <c r="L117" s="9">
+        <v>1321391</v>
+      </c>
+      <c r="M117" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="N117" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="O117" s="6" t="s">
+        <v>641</v>
+      </c>
+      <c r="P117" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q117" s="6">
+        <v>2008</v>
+      </c>
+      <c r="R117" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="S117" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="118" spans="1:19" ht="19" x14ac:dyDescent="0.25">
+      <c r="A118" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C118" s="6"/>
+      <c r="D118" s="6" t="s">
+        <v>557</v>
+      </c>
+      <c r="E118" s="6"/>
+      <c r="F118" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="G118" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="H118" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="I118" s="7">
+        <v>0</v>
+      </c>
+      <c r="J118" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="K118" s="8"/>
+      <c r="L118" s="9">
         <v>1454041</v>
       </c>
-      <c r="M115" s="10" t="s">
+      <c r="M118" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="N115" s="6" t="s">
+      <c r="N118" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O115" s="8" t="s">
+      <c r="O118" s="8" t="s">
         <v>643</v>
       </c>
-      <c r="P115" s="6" t="s">
+      <c r="P118" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="Q115" s="6">
+      <c r="Q118" s="6">
         <v>2010</v>
       </c>
-      <c r="R115" s="6">
+      <c r="R118" s="6">
         <v>15</v>
       </c>
-      <c r="S115" s="6" t="s">
+      <c r="S118" s="6" t="s">
         <v>71</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:S111">
-    <sortCondition ref="D2:D111"/>
-    <sortCondition ref="E2:E111"/>
-    <sortCondition ref="B2:B111"/>
+  <sortState ref="A2:S114">
+    <sortCondition ref="D2:D114"/>
+    <sortCondition ref="E2:E114"/>
+    <sortCondition ref="B2:B114"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Added 'whole_genome' feature locations
</commit_message>
<xml_diff>
--- a/tabular/flavi-ncbi-refseqs-side-data.xlsx
+++ b/tabular/flavi-ncbi-refseqs-side-data.xlsx
@@ -2326,8 +2326,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="615">
+  <cellStyleXfs count="619">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3105,7 +3109,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="615">
+  <cellStyles count="619">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3413,6 +3417,8 @@
     <cellStyle name="Followed Hyperlink" xfId="610" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="612" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="614" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="616" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="618" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3720,6 +3726,8 @@
     <cellStyle name="Hyperlink" xfId="609" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="611" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="613" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="615" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="617" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4061,7 +4069,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C62" sqref="C61:C62"/>
+      <selection pane="bottomLeft" activeCell="C54" sqref="A1:N132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
is the updated table
</commit_message>
<xml_diff>
--- a/tabular/flavi-ncbi-refseqs-side-data.xlsx
+++ b/tabular/flavi-ncbi-refseqs-side-data.xlsx
@@ -8,20 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus-group/Flaviviridae-GLUE/tabular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE974D10-2E3B-8945-888F-50DE06837702}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41BE6E6-DDE5-E64C-A071-96F84D007334}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1880" yWindow="1940" windowWidth="25620" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="flavi.txt" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">flavi.txt!$B$1:$M$112</definedName>
   </definedNames>
-  <calcPr calcId="140001"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -2091,7 +2097,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2191,6 +2197,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="20">
@@ -2309,7 +2321,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -2317,6 +2329,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="621">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2941,7 +2981,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3101,6 +3141,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="621">
@@ -3726,28 +3772,7 @@
     <cellStyle name="Hyperlink" xfId="619" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -4085,8 +4110,8 @@
   <dimension ref="A1:N132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I100" sqref="I100"/>
+      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C136" sqref="C136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9530,11 +9555,10 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N132">
-    <sortCondition ref="F2:F132"/>
-    <sortCondition ref="G2:G132"/>
-    <sortCondition ref="C2:C132"/>
-    <sortCondition ref="I2:I132"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N133">
+    <sortCondition ref="F2:F133"/>
+    <sortCondition ref="G2:G133"/>
+    <sortCondition ref="C2:C133"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -9547,6 +9571,102 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15435155-FEDC-4A4F-B6FC-9E903CB0280B}">
+  <dimension ref="A1:A16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="74">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="75">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="75">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="75">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="75">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="75">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="75">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="75">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="75">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="75">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="75">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="75">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="75">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="75">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <f>SUM(A1:A15)</f>
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L1"/>
   <sheetViews>

</xml_diff>

<commit_message>
removed sequences from wrong alignments
</commit_message>
<xml_diff>
--- a/tabular/flavi-ncbi-refseqs-side-data.xlsx
+++ b/tabular/flavi-ncbi-refseqs-side-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus-group/Flaviviridae-GLUE/tabular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41BE6E6-DDE5-E64C-A071-96F84D007334}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6E8196-3694-5D49-BA34-8A8851DF5735}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1880" yWindow="1940" windowWidth="25620" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11340" yWindow="460" windowWidth="18980" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="flavi.txt" sheetId="1" r:id="rId1"/>
@@ -4110,8 +4110,8 @@
   <dimension ref="A1:N132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C136" sqref="C136"/>
+      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B125" sqref="B125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4220,16 +4220,16 @@
     </row>
     <row r="3" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>646</v>
+        <v>280</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>647</v>
+        <v>99</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>675</v>
+        <v>343</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>676</v>
@@ -4242,7 +4242,7 @@
       </c>
       <c r="H3" s="13"/>
       <c r="I3" s="13" t="s">
-        <v>628</v>
+        <v>506</v>
       </c>
       <c r="J3" s="15" t="s">
         <v>197</v>
@@ -4250,22 +4250,28 @@
       <c r="K3" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="L3" s="16"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="17"/>
+      <c r="L3" s="16" t="s">
+        <v>344</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>477</v>
+      </c>
+      <c r="N3" s="17" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="4" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>99</v>
+        <v>125</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>343</v>
+        <v>385</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>676</v>
@@ -4278,7 +4284,7 @@
       </c>
       <c r="H4" s="13"/>
       <c r="I4" s="13" t="s">
-        <v>506</v>
+        <v>404</v>
       </c>
       <c r="J4" s="15" t="s">
         <v>197</v>
@@ -4287,27 +4293,27 @@
         <v>197</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="N4" s="17" t="s">
-        <v>211</v>
+        <v>386</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
-        <v>3</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>282</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>125</v>
+      <c r="A5" s="18">
+        <v>4</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>194</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>385</v>
+        <v>315</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>676</v>
@@ -4328,28 +4334,28 @@
       <c r="K5" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="L5" s="16" t="s">
-        <v>335</v>
+      <c r="L5" s="16">
+        <v>178</v>
       </c>
       <c r="M5" s="14" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="N5" s="17" t="s">
-        <v>386</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>194</v>
+        <v>79</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>676</v>
@@ -4362,7 +4368,7 @@
       </c>
       <c r="H6" s="13"/>
       <c r="I6" s="13" t="s">
-        <v>404</v>
+        <v>507</v>
       </c>
       <c r="J6" s="15" t="s">
         <v>197</v>
@@ -4370,28 +4376,28 @@
       <c r="K6" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="L6" s="16">
-        <v>178</v>
+      <c r="L6" s="16" t="s">
+        <v>1</v>
       </c>
       <c r="M6" s="14" t="s">
         <v>478</v>
       </c>
       <c r="N6" s="17" t="s">
-        <v>76</v>
+        <v>318</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18">
-        <v>5</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>79</v>
+      <c r="A7" s="11">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>122</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>317</v>
+        <v>209</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>676</v>
@@ -4404,7 +4410,7 @@
       </c>
       <c r="H7" s="13"/>
       <c r="I7" s="13" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="J7" s="15" t="s">
         <v>197</v>
@@ -4413,27 +4419,27 @@
         <v>197</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="M7" s="14" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="N7" s="17" t="s">
-        <v>318</v>
+        <v>377</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>240</v>
+        <v>273</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>122</v>
+        <v>179</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>209</v>
+        <v>437</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>676</v>
@@ -4446,7 +4452,7 @@
       </c>
       <c r="H8" s="13"/>
       <c r="I8" s="13" t="s">
-        <v>506</v>
+        <v>404</v>
       </c>
       <c r="J8" s="15" t="s">
         <v>197</v>
@@ -4455,27 +4461,27 @@
         <v>197</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="M8" s="14" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="N8" s="17" t="s">
-        <v>377</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>273</v>
+        <v>255</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>179</v>
+        <v>145</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>437</v>
+        <v>618</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>676</v>
@@ -4497,27 +4503,27 @@
         <v>197</v>
       </c>
       <c r="L9" s="16" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="M9" s="14" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="N9" s="17" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
-        <v>8</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>255</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>145</v>
+      <c r="A10" s="18">
+        <v>9</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>645</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>75</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>618</v>
+        <v>312</v>
       </c>
       <c r="E10" s="13" t="s">
         <v>676</v>
@@ -4530,7 +4536,7 @@
       </c>
       <c r="H10" s="13"/>
       <c r="I10" s="13" t="s">
-        <v>404</v>
+        <v>509</v>
       </c>
       <c r="J10" s="15" t="s">
         <v>197</v>
@@ -4539,27 +4545,27 @@
         <v>197</v>
       </c>
       <c r="L10" s="16" t="s">
-        <v>31</v>
+        <v>314</v>
       </c>
       <c r="M10" s="14" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="N10" s="17" t="s">
-        <v>146</v>
+        <v>313</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>645</v>
+        <v>36</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>75</v>
+        <v>159</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>312</v>
+        <v>424</v>
       </c>
       <c r="E11" s="13" t="s">
         <v>676</v>
@@ -4572,7 +4578,7 @@
       </c>
       <c r="H11" s="13"/>
       <c r="I11" s="13" t="s">
-        <v>509</v>
+        <v>404</v>
       </c>
       <c r="J11" s="15" t="s">
         <v>197</v>
@@ -4581,27 +4587,27 @@
         <v>197</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>314</v>
+        <v>37</v>
       </c>
       <c r="M11" s="14" t="s">
         <v>479</v>
       </c>
       <c r="N11" s="17" t="s">
-        <v>313</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>159</v>
+        <v>83</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>424</v>
+        <v>320</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>676</v>
@@ -4614,7 +4620,7 @@
       </c>
       <c r="H12" s="13"/>
       <c r="I12" s="13" t="s">
-        <v>404</v>
+        <v>508</v>
       </c>
       <c r="J12" s="15" t="s">
         <v>197</v>
@@ -4622,28 +4628,28 @@
       <c r="K12" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="L12" s="16" t="s">
-        <v>37</v>
+      <c r="L12" s="16">
+        <v>56</v>
       </c>
       <c r="M12" s="14" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="N12" s="17" t="s">
-        <v>160</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18">
-        <v>11</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>83</v>
+      <c r="A13" s="11">
+        <v>12</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>178</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>320</v>
+        <v>435</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>676</v>
@@ -4656,7 +4662,7 @@
       </c>
       <c r="H13" s="13"/>
       <c r="I13" s="13" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="J13" s="15" t="s">
         <v>197</v>
@@ -4664,28 +4670,28 @@
       <c r="K13" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="L13" s="16">
-        <v>56</v>
+      <c r="L13" s="16" t="s">
+        <v>49</v>
       </c>
       <c r="M13" s="14" t="s">
         <v>480</v>
       </c>
       <c r="N13" s="17" t="s">
-        <v>84</v>
+        <v>436</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>272</v>
+        <v>248</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>178</v>
+        <v>133</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>435</v>
+        <v>406</v>
       </c>
       <c r="E14" s="13" t="s">
         <v>676</v>
@@ -4698,7 +4704,7 @@
       </c>
       <c r="H14" s="13"/>
       <c r="I14" s="13" t="s">
-        <v>506</v>
+        <v>404</v>
       </c>
       <c r="J14" s="15" t="s">
         <v>197</v>
@@ -4707,27 +4713,27 @@
         <v>197</v>
       </c>
       <c r="L14" s="16" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="M14" s="14" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="N14" s="17" t="s">
-        <v>436</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>248</v>
+        <v>646</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>133</v>
+        <v>647</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>406</v>
+        <v>675</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>676</v>
@@ -4740,7 +4746,7 @@
       </c>
       <c r="H15" s="13"/>
       <c r="I15" s="13" t="s">
-        <v>404</v>
+        <v>628</v>
       </c>
       <c r="J15" s="15" t="s">
         <v>197</v>
@@ -4748,15 +4754,9 @@
       <c r="K15" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="L15" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="M15" s="14" t="s">
-        <v>476</v>
-      </c>
-      <c r="N15" s="17" t="s">
-        <v>134</v>
-      </c>
+      <c r="L15" s="16"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="17"/>
     </row>
     <row r="16" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
@@ -6774,16 +6774,16 @@
     </row>
     <row r="64" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="69">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B64" s="39" t="s">
-        <v>650</v>
+        <v>267</v>
       </c>
       <c r="C64" s="40" t="s">
-        <v>649</v>
+        <v>170</v>
       </c>
       <c r="D64" s="40" t="s">
-        <v>652</v>
+        <v>427</v>
       </c>
       <c r="E64" s="40" t="s">
         <v>676</v>
@@ -6796,30 +6796,36 @@
       </c>
       <c r="H64" s="40"/>
       <c r="I64" s="40" t="s">
-        <v>631</v>
+        <v>512</v>
       </c>
       <c r="J64" s="41" t="s">
         <v>631</v>
       </c>
       <c r="K64" s="40" t="s">
-        <v>631</v>
-      </c>
-      <c r="L64" s="16"/>
-      <c r="M64" s="14"/>
-      <c r="N64" s="17"/>
+        <v>629</v>
+      </c>
+      <c r="L64" s="16" t="s">
+        <v>428</v>
+      </c>
+      <c r="M64" s="14" t="s">
+        <v>477</v>
+      </c>
+      <c r="N64" s="17" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="65" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="69">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B65" s="39" t="s">
-        <v>267</v>
+        <v>228</v>
       </c>
       <c r="C65" s="40" t="s">
-        <v>170</v>
+        <v>108</v>
       </c>
       <c r="D65" s="40" t="s">
-        <v>427</v>
+        <v>354</v>
       </c>
       <c r="E65" s="40" t="s">
         <v>676</v>
@@ -6832,7 +6838,7 @@
       </c>
       <c r="H65" s="40"/>
       <c r="I65" s="40" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="J65" s="41" t="s">
         <v>631</v>
@@ -6841,27 +6847,27 @@
         <v>629</v>
       </c>
       <c r="L65" s="16" t="s">
-        <v>428</v>
+        <v>355</v>
       </c>
       <c r="M65" s="14" t="s">
         <v>477</v>
       </c>
       <c r="N65" s="17" t="s">
-        <v>171</v>
+        <v>148</v>
       </c>
     </row>
     <row r="66" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="69">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B66" s="39" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="C66" s="40" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="D66" s="40" t="s">
-        <v>354</v>
+        <v>370</v>
       </c>
       <c r="E66" s="40" t="s">
         <v>676</v>
@@ -6874,36 +6880,36 @@
       </c>
       <c r="H66" s="40"/>
       <c r="I66" s="40" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="J66" s="41" t="s">
         <v>631</v>
       </c>
       <c r="K66" s="40" t="s">
-        <v>629</v>
+        <v>654</v>
       </c>
       <c r="L66" s="16" t="s">
-        <v>355</v>
+        <v>1</v>
       </c>
       <c r="M66" s="14" t="s">
         <v>477</v>
       </c>
       <c r="N66" s="17" t="s">
-        <v>148</v>
+        <v>371</v>
       </c>
     </row>
     <row r="67" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="69">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B67" s="39" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="C67" s="40" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D67" s="40" t="s">
-        <v>370</v>
+        <v>356</v>
       </c>
       <c r="E67" s="40" t="s">
         <v>676</v>
@@ -6916,7 +6922,7 @@
       </c>
       <c r="H67" s="40"/>
       <c r="I67" s="40" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="J67" s="41" t="s">
         <v>631</v>
@@ -6925,27 +6931,27 @@
         <v>654</v>
       </c>
       <c r="L67" s="16" t="s">
-        <v>1</v>
+        <v>358</v>
       </c>
       <c r="M67" s="14" t="s">
         <v>477</v>
       </c>
       <c r="N67" s="17" t="s">
-        <v>371</v>
+        <v>357</v>
       </c>
     </row>
     <row r="68" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="69">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B68" s="39" t="s">
-        <v>229</v>
+        <v>650</v>
       </c>
       <c r="C68" s="40" t="s">
-        <v>109</v>
+        <v>649</v>
       </c>
       <c r="D68" s="40" t="s">
-        <v>356</v>
+        <v>652</v>
       </c>
       <c r="E68" s="40" t="s">
         <v>676</v>
@@ -6958,23 +6964,17 @@
       </c>
       <c r="H68" s="40"/>
       <c r="I68" s="40" t="s">
-        <v>515</v>
+        <v>631</v>
       </c>
       <c r="J68" s="41" t="s">
         <v>631</v>
       </c>
       <c r="K68" s="40" t="s">
-        <v>654</v>
-      </c>
-      <c r="L68" s="16" t="s">
-        <v>358</v>
-      </c>
-      <c r="M68" s="14" t="s">
-        <v>477</v>
-      </c>
-      <c r="N68" s="17" t="s">
-        <v>357</v>
-      </c>
+        <v>631</v>
+      </c>
+      <c r="L68" s="16"/>
+      <c r="M68" s="14"/>
+      <c r="N68" s="17"/>
     </row>
     <row r="69" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="70">
@@ -8098,16 +8098,16 @@
     </row>
     <row r="96" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A96" s="73">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B96" s="51" t="s">
-        <v>641</v>
+        <v>570</v>
       </c>
       <c r="C96" s="52" t="s">
-        <v>642</v>
+        <v>576</v>
       </c>
       <c r="D96" s="52" t="s">
-        <v>658</v>
+        <v>606</v>
       </c>
       <c r="E96" s="52" t="s">
         <v>676</v>
@@ -8122,7 +8122,7 @@
         <v>1</v>
       </c>
       <c r="I96" s="52" t="s">
-        <v>657</v>
+        <v>404</v>
       </c>
       <c r="J96" s="15" t="s">
         <v>197</v>
@@ -8130,22 +8130,26 @@
       <c r="K96" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="L96" s="16"/>
+      <c r="L96" s="16" t="s">
+        <v>670</v>
+      </c>
       <c r="M96" s="53"/>
-      <c r="N96" s="17"/>
+      <c r="N96" s="17" t="s">
+        <v>580</v>
+      </c>
     </row>
     <row r="97" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A97" s="73">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B97" s="51" t="s">
-        <v>570</v>
+        <v>667</v>
       </c>
       <c r="C97" s="52" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="D97" s="52" t="s">
-        <v>606</v>
+        <v>575</v>
       </c>
       <c r="E97" s="52" t="s">
         <v>676</v>
@@ -8160,7 +8164,7 @@
         <v>1</v>
       </c>
       <c r="I97" s="52" t="s">
-        <v>404</v>
+        <v>521</v>
       </c>
       <c r="J97" s="15" t="s">
         <v>197</v>
@@ -8169,25 +8173,25 @@
         <v>197</v>
       </c>
       <c r="L97" s="16" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="M97" s="53"/>
       <c r="N97" s="17" t="s">
-        <v>580</v>
+        <v>584</v>
       </c>
     </row>
     <row r="98" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A98" s="73">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B98" s="51" t="s">
-        <v>667</v>
+        <v>572</v>
       </c>
       <c r="C98" s="52" t="s">
-        <v>574</v>
+        <v>578</v>
       </c>
       <c r="D98" s="52" t="s">
-        <v>575</v>
+        <v>609</v>
       </c>
       <c r="E98" s="52" t="s">
         <v>676</v>
@@ -8202,7 +8206,7 @@
         <v>1</v>
       </c>
       <c r="I98" s="52" t="s">
-        <v>521</v>
+        <v>583</v>
       </c>
       <c r="J98" s="15" t="s">
         <v>197</v>
@@ -8210,26 +8214,24 @@
       <c r="K98" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="L98" s="16" t="s">
-        <v>669</v>
-      </c>
+      <c r="L98" s="16"/>
       <c r="M98" s="53"/>
       <c r="N98" s="17" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="99" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A99" s="73">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B99" s="51" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="C99" s="52" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="D99" s="52" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="E99" s="52" t="s">
         <v>676</v>
@@ -8244,7 +8246,7 @@
         <v>1</v>
       </c>
       <c r="I99" s="52" t="s">
-        <v>684</v>
+        <v>657</v>
       </c>
       <c r="J99" s="15" t="s">
         <v>197</v>
@@ -8258,16 +8260,16 @@
     </row>
     <row r="100" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A100" s="73">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B100" s="51" t="s">
-        <v>572</v>
+        <v>644</v>
       </c>
       <c r="C100" s="52" t="s">
-        <v>578</v>
+        <v>643</v>
       </c>
       <c r="D100" s="52" t="s">
-        <v>609</v>
+        <v>659</v>
       </c>
       <c r="E100" s="52" t="s">
         <v>676</v>
@@ -8282,7 +8284,7 @@
         <v>1</v>
       </c>
       <c r="I100" s="52" t="s">
-        <v>583</v>
+        <v>684</v>
       </c>
       <c r="J100" s="15" t="s">
         <v>197</v>
@@ -8292,9 +8294,7 @@
       </c>
       <c r="L100" s="16"/>
       <c r="M100" s="53"/>
-      <c r="N100" s="17" t="s">
-        <v>582</v>
-      </c>
+      <c r="N100" s="17"/>
     </row>
     <row r="101" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A101" s="73">
@@ -8804,16 +8804,16 @@
     </row>
     <row r="114" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A114" s="55">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B114" s="55" t="s">
-        <v>636</v>
+        <v>483</v>
       </c>
       <c r="C114" s="56" t="s">
-        <v>637</v>
+        <v>490</v>
       </c>
       <c r="D114" s="57" t="s">
-        <v>639</v>
+        <v>487</v>
       </c>
       <c r="E114" s="58" t="s">
         <v>676</v>
@@ -8826,7 +8826,7 @@
       </c>
       <c r="H114" s="57"/>
       <c r="I114" s="57" t="s">
-        <v>638</v>
+        <v>542</v>
       </c>
       <c r="J114" s="15" t="s">
         <v>197</v>
@@ -8836,20 +8836,22 @@
       </c>
       <c r="L114" s="62"/>
       <c r="M114" s="59"/>
-      <c r="N114" s="60"/>
+      <c r="N114" s="60" t="s">
+        <v>541</v>
+      </c>
     </row>
     <row r="115" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A115" s="55">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B115" s="55" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="C115" s="56" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="D115" s="57" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E115" s="58" t="s">
         <v>676</v>
@@ -8862,7 +8864,7 @@
       </c>
       <c r="H115" s="57"/>
       <c r="I115" s="57" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="J115" s="15" t="s">
         <v>197</v>
@@ -8873,21 +8875,21 @@
       <c r="L115" s="62"/>
       <c r="M115" s="59"/>
       <c r="N115" s="60" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="116" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A116" s="55">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B116" s="55" t="s">
-        <v>488</v>
+        <v>636</v>
       </c>
       <c r="C116" s="56" t="s">
-        <v>485</v>
+        <v>637</v>
       </c>
       <c r="D116" s="57" t="s">
-        <v>486</v>
+        <v>639</v>
       </c>
       <c r="E116" s="58" t="s">
         <v>676</v>
@@ -8900,7 +8902,7 @@
       </c>
       <c r="H116" s="57"/>
       <c r="I116" s="57" t="s">
-        <v>540</v>
+        <v>638</v>
       </c>
       <c r="J116" s="15" t="s">
         <v>197</v>
@@ -8910,9 +8912,7 @@
       </c>
       <c r="L116" s="62"/>
       <c r="M116" s="59"/>
-      <c r="N116" s="60" t="s">
-        <v>539</v>
-      </c>
+      <c r="N116" s="60"/>
     </row>
     <row r="117" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A117" s="63">
@@ -9555,10 +9555,10 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N133">
-    <sortCondition ref="F2:F133"/>
-    <sortCondition ref="G2:G133"/>
-    <sortCondition ref="C2:C133"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N135">
+    <sortCondition ref="F2:F135"/>
+    <sortCondition ref="G2:G135"/>
+    <sortCondition ref="A2:A135"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
split dISF1 clade into dISF1A and dISF1B
</commit_message>
<xml_diff>
--- a/tabular/flavi-ncbi-refseqs-side-data.xlsx
+++ b/tabular/flavi-ncbi-refseqs-side-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus-group/Flaviviridae-GLUE/tabular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6E8196-3694-5D49-BA34-8A8851DF5735}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF878A0-E93A-D840-AAA8-DE9921725439}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11340" yWindow="460" windowWidth="18980" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9820" yWindow="460" windowWidth="18980" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="flavi.txt" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="687">
   <si>
     <t>AY632538</t>
   </si>
@@ -2091,13 +2091,19 @@
   </si>
   <si>
     <t>Chrysopidae spp</t>
+  </si>
+  <si>
+    <t>dISF1A</t>
+  </si>
+  <si>
+    <t>dISF1B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2197,12 +2203,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="20">
@@ -2321,7 +2321,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -2329,34 +2329,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="621">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2981,7 +2953,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3141,12 +3113,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="621">
@@ -4110,8 +4076,8 @@
   <dimension ref="A1:N132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B125" sqref="B125"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16:G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4778,7 +4744,7 @@
         <v>191</v>
       </c>
       <c r="G16" s="21" t="s">
-        <v>472</v>
+        <v>685</v>
       </c>
       <c r="H16" s="21"/>
       <c r="I16" s="21" t="s">
@@ -4820,7 +4786,7 @@
         <v>191</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>472</v>
+        <v>686</v>
       </c>
       <c r="H17" s="24"/>
       <c r="I17" s="24" t="s">
@@ -4862,7 +4828,7 @@
         <v>191</v>
       </c>
       <c r="G18" s="21" t="s">
-        <v>472</v>
+        <v>686</v>
       </c>
       <c r="H18" s="21"/>
       <c r="I18" s="24" t="s">
@@ -4904,7 +4870,7 @@
         <v>191</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>472</v>
+        <v>686</v>
       </c>
       <c r="H19" s="24"/>
       <c r="I19" s="24" t="s">
@@ -4988,7 +4954,7 @@
         <v>191</v>
       </c>
       <c r="G21" s="24" t="s">
-        <v>472</v>
+        <v>686</v>
       </c>
       <c r="H21" s="24"/>
       <c r="I21" s="24" t="s">
@@ -5072,7 +5038,7 @@
         <v>191</v>
       </c>
       <c r="G23" s="24" t="s">
-        <v>472</v>
+        <v>685</v>
       </c>
       <c r="H23" s="24"/>
       <c r="I23" s="24" t="s">
@@ -9572,96 +9538,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15435155-FEDC-4A4F-B6FC-9E903CB0280B}">
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="74">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="75">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="75">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="75">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="75">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="75">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="75">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="75">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="75">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="75">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="75">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="75">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="75">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="75">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="75">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <f>SUM(A1:A15)</f>
-        <v>130</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Updated tabular data and brought into build
</commit_message>
<xml_diff>
--- a/tabular/flavi-ncbi-refseqs-side-data.xlsx
+++ b/tabular/flavi-ncbi-refseqs-side-data.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10414"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus-group/Flaviviridae-GLUE/tabular/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E79E737-A073-3A43-AB61-E36C02785796}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7480" yWindow="1020" windowWidth="40620" windowHeight="22420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="flavi.txt" sheetId="1" r:id="rId1"/>
@@ -20,16 +14,16 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">flavi.txt!$A$1:$M$112</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -2333,7 +2327,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2595,7 +2589,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="621">
+  <cellStyleXfs count="622">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3216,6 +3210,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="67">
@@ -3361,7 +3356,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="621">
+  <cellStyles count="622">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3672,6 +3667,7 @@
     <cellStyle name="Followed Hyperlink" xfId="616" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="618" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="620" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="621" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4318,15 +4314,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G115" sqref="G115"/>
+      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N150" sqref="A1:N150"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="48.33203125" style="1" customWidth="1"/>
@@ -4343,7 +4339,7 @@
     <col min="14" max="14" width="31.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="19">
       <c r="A1" s="9" t="s">
         <v>213</v>
       </c>
@@ -4387,7 +4383,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="18" customHeight="1">
       <c r="A2" s="10" t="s">
         <v>251</v>
       </c>
@@ -4429,7 +4425,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="18" customHeight="1">
       <c r="A3" s="10" t="s">
         <v>280</v>
       </c>
@@ -4471,7 +4467,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="18" customHeight="1">
       <c r="A4" s="10" t="s">
         <v>282</v>
       </c>
@@ -4513,7 +4509,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="18" customHeight="1">
       <c r="A5" s="17" t="s">
         <v>9</v>
       </c>
@@ -4555,7 +4551,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="18" customHeight="1">
       <c r="A6" s="17" t="s">
         <v>10</v>
       </c>
@@ -4597,7 +4593,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="18" customHeight="1">
       <c r="A7" s="10" t="s">
         <v>240</v>
       </c>
@@ -4639,7 +4635,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="18" customHeight="1">
       <c r="A8" s="10" t="s">
         <v>273</v>
       </c>
@@ -4681,7 +4677,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="18" customHeight="1">
       <c r="A9" s="10" t="s">
         <v>255</v>
       </c>
@@ -4723,7 +4719,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="18" customHeight="1">
       <c r="A10" s="17" t="s">
         <v>643</v>
       </c>
@@ -4765,7 +4761,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="18" customHeight="1">
       <c r="A11" s="17" t="s">
         <v>36</v>
       </c>
@@ -4807,7 +4803,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="18" customHeight="1">
       <c r="A12" s="17" t="s">
         <v>13</v>
       </c>
@@ -4849,7 +4845,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="18" customHeight="1">
       <c r="A13" s="10" t="s">
         <v>272</v>
       </c>
@@ -4891,7 +4887,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="18" customHeight="1">
       <c r="A14" s="10" t="s">
         <v>248</v>
       </c>
@@ -4933,7 +4929,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="18" customHeight="1">
       <c r="A15" s="10" t="s">
         <v>644</v>
       </c>
@@ -4975,7 +4971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="18" customHeight="1">
       <c r="A16" s="19" t="s">
         <v>196</v>
       </c>
@@ -5017,7 +5013,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="18" customHeight="1">
       <c r="A17" s="19" t="s">
         <v>17</v>
       </c>
@@ -5059,7 +5055,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="18" customHeight="1">
       <c r="A18" s="19" t="s">
         <v>11</v>
       </c>
@@ -5101,7 +5097,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="18" customHeight="1">
       <c r="A19" s="19" t="s">
         <v>35</v>
       </c>
@@ -5143,7 +5139,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="18" customHeight="1">
       <c r="A20" s="21" t="s">
         <v>252</v>
       </c>
@@ -5185,7 +5181,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="18" customHeight="1">
       <c r="A21" s="19" t="s">
         <v>26</v>
       </c>
@@ -5227,7 +5223,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="18" customHeight="1">
       <c r="A22" s="19" t="s">
         <v>39</v>
       </c>
@@ -5269,7 +5265,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="18" customHeight="1">
       <c r="A23" s="19" t="s">
         <v>41</v>
       </c>
@@ -5311,7 +5307,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="18" customHeight="1">
       <c r="A24" s="24" t="s">
         <v>19</v>
       </c>
@@ -5353,7 +5349,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="18" customHeight="1">
       <c r="A25" s="27" t="s">
         <v>274</v>
       </c>
@@ -5395,7 +5391,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="18" customHeight="1">
       <c r="A26" s="29" t="s">
         <v>3</v>
       </c>
@@ -5437,7 +5433,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="18" customHeight="1">
       <c r="A27" s="32" t="s">
         <v>247</v>
       </c>
@@ -5479,7 +5475,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="18" customHeight="1">
       <c r="A28" s="29" t="s">
         <v>15</v>
       </c>
@@ -5521,7 +5517,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="18" customHeight="1">
       <c r="A29" s="32" t="s">
         <v>283</v>
       </c>
@@ -5563,7 +5559,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="18" customHeight="1">
       <c r="A30" s="32" t="s">
         <v>268</v>
       </c>
@@ -5605,7 +5601,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="18" customHeight="1">
       <c r="A31" s="32" t="s">
         <v>219</v>
       </c>
@@ -5647,7 +5643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="18" customHeight="1">
       <c r="A32" s="32" t="s">
         <v>277</v>
       </c>
@@ -5689,7 +5685,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="18" customHeight="1">
       <c r="A33" s="32" t="s">
         <v>278</v>
       </c>
@@ -5731,7 +5727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="18" customHeight="1">
       <c r="A34" s="32" t="s">
         <v>226</v>
       </c>
@@ -5773,7 +5769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="18" customHeight="1">
       <c r="A35" s="29" t="s">
         <v>0</v>
       </c>
@@ -5815,7 +5811,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="18" customHeight="1">
       <c r="A36" s="32" t="s">
         <v>284</v>
       </c>
@@ -5857,7 +5853,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="18" customHeight="1">
       <c r="A37" s="32" t="s">
         <v>217</v>
       </c>
@@ -5897,7 +5893,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" ht="18" customHeight="1">
       <c r="A38" s="32" t="s">
         <v>246</v>
       </c>
@@ -5939,7 +5935,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" ht="18" customHeight="1">
       <c r="A39" s="29" t="s">
         <v>7</v>
       </c>
@@ -5981,7 +5977,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" ht="18" customHeight="1">
       <c r="A40" s="32" t="s">
         <v>216</v>
       </c>
@@ -6023,7 +6019,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" ht="18" customHeight="1">
       <c r="A41" s="32" t="s">
         <v>276</v>
       </c>
@@ -6065,7 +6061,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" ht="18" customHeight="1">
       <c r="A42" s="29" t="s">
         <v>8</v>
       </c>
@@ -6107,7 +6103,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="18" customHeight="1">
       <c r="A43" s="32" t="s">
         <v>288</v>
       </c>
@@ -6149,7 +6145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" ht="18" customHeight="1">
       <c r="A44" s="29" t="s">
         <v>2</v>
       </c>
@@ -6191,7 +6187,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" ht="18" customHeight="1">
       <c r="A45" s="32" t="s">
         <v>275</v>
       </c>
@@ -6233,7 +6229,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" ht="18" customHeight="1">
       <c r="A46" s="32" t="s">
         <v>281</v>
       </c>
@@ -6275,7 +6271,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" ht="18" customHeight="1">
       <c r="A47" s="29" t="s">
         <v>14</v>
       </c>
@@ -6317,7 +6313,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" ht="18" customHeight="1">
       <c r="A48" s="32" t="s">
         <v>285</v>
       </c>
@@ -6359,7 +6355,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="18" customHeight="1">
       <c r="A49" s="29" t="s">
         <v>16</v>
       </c>
@@ -6401,7 +6397,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" ht="18" customHeight="1">
       <c r="A50" s="32" t="s">
         <v>241</v>
       </c>
@@ -6443,7 +6439,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" ht="18" customHeight="1">
       <c r="A51" s="32" t="s">
         <v>279</v>
       </c>
@@ -6485,7 +6481,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" ht="18" customHeight="1">
       <c r="A52" s="29" t="s">
         <v>6</v>
       </c>
@@ -6527,7 +6523,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" ht="18" customHeight="1">
       <c r="A53" s="32" t="s">
         <v>245</v>
       </c>
@@ -6569,7 +6565,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" ht="18" customHeight="1">
       <c r="A54" s="32" t="s">
         <v>692</v>
       </c>
@@ -6611,7 +6607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" ht="18" customHeight="1">
       <c r="A55" s="32" t="s">
         <v>693</v>
       </c>
@@ -6653,7 +6649,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" ht="18" customHeight="1">
       <c r="A56" s="32" t="s">
         <v>694</v>
       </c>
@@ -6695,7 +6691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" ht="18" customHeight="1">
       <c r="A57" s="32" t="s">
         <v>695</v>
       </c>
@@ -6737,7 +6733,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" ht="18" customHeight="1">
       <c r="A58" s="32" t="s">
         <v>696</v>
       </c>
@@ -6779,7 +6775,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" ht="18" customHeight="1">
       <c r="A59" s="32" t="s">
         <v>697</v>
       </c>
@@ -6821,7 +6817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" ht="18" customHeight="1">
       <c r="A60" s="32" t="s">
         <v>699</v>
       </c>
@@ -6863,7 +6859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" ht="18" customHeight="1">
       <c r="A61" s="35" t="s">
         <v>5</v>
       </c>
@@ -6905,7 +6901,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" ht="18" customHeight="1">
       <c r="A62" s="35" t="s">
         <v>54</v>
       </c>
@@ -6947,7 +6943,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" ht="18" customHeight="1">
       <c r="A63" s="35" t="s">
         <v>53</v>
       </c>
@@ -6989,7 +6985,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" ht="18" customHeight="1">
       <c r="A64" s="35" t="s">
         <v>57</v>
       </c>
@@ -7031,7 +7027,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" ht="18" customHeight="1">
       <c r="A65" s="35" t="s">
         <v>55</v>
       </c>
@@ -7073,7 +7069,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" ht="18" customHeight="1">
       <c r="A66" s="35" t="s">
         <v>244</v>
       </c>
@@ -7115,7 +7111,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" ht="18" customHeight="1">
       <c r="A67" s="35" t="s">
         <v>56</v>
       </c>
@@ -7157,7 +7153,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" ht="18" customHeight="1">
       <c r="A68" s="35" t="s">
         <v>249</v>
       </c>
@@ -7199,7 +7195,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" ht="18" customHeight="1">
       <c r="A69" s="35" t="s">
         <v>224</v>
       </c>
@@ -7241,7 +7237,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" ht="18" customHeight="1">
       <c r="A70" s="35" t="s">
         <v>698</v>
       </c>
@@ -7283,7 +7279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" ht="18" customHeight="1">
       <c r="A71" s="37" t="s">
         <v>230</v>
       </c>
@@ -7325,7 +7321,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" ht="18" customHeight="1">
       <c r="A72" s="37" t="s">
         <v>267</v>
       </c>
@@ -7367,7 +7363,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" ht="18" customHeight="1">
       <c r="A73" s="37" t="s">
         <v>228</v>
       </c>
@@ -7409,7 +7405,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" ht="18" customHeight="1">
       <c r="A74" s="37" t="s">
         <v>237</v>
       </c>
@@ -7451,7 +7447,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" ht="18" customHeight="1">
       <c r="A75" s="37" t="s">
         <v>229</v>
       </c>
@@ -7493,7 +7489,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" ht="18" customHeight="1">
       <c r="A76" s="37" t="s">
         <v>648</v>
       </c>
@@ -7535,7 +7531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" ht="18" customHeight="1">
       <c r="A77" s="40" t="s">
         <v>243</v>
       </c>
@@ -7577,7 +7573,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" ht="18" customHeight="1">
       <c r="A78" s="40" t="s">
         <v>269</v>
       </c>
@@ -7619,7 +7615,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" ht="18" customHeight="1">
       <c r="A79" s="40" t="s">
         <v>238</v>
       </c>
@@ -7661,7 +7657,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" ht="18" customHeight="1">
       <c r="A80" s="42" t="s">
         <v>59</v>
       </c>
@@ -7703,7 +7699,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" ht="18" customHeight="1">
       <c r="A81" s="42" t="s">
         <v>60</v>
       </c>
@@ -7745,7 +7741,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="82" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" ht="19">
       <c r="A82" s="42" t="s">
         <v>260</v>
       </c>
@@ -7787,7 +7783,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" ht="19">
       <c r="A83" s="42" t="s">
         <v>242</v>
       </c>
@@ -7829,7 +7825,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="84" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" ht="19">
       <c r="A84" s="42" t="s">
         <v>215</v>
       </c>
@@ -7871,7 +7867,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" ht="19">
       <c r="A85" s="42" t="s">
         <v>234</v>
       </c>
@@ -7913,7 +7909,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="86" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" ht="19">
       <c r="A86" s="42" t="s">
         <v>222</v>
       </c>
@@ -7955,7 +7951,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="87" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" ht="19">
       <c r="A87" s="42" t="s">
         <v>58</v>
       </c>
@@ -7997,7 +7993,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" ht="18" customHeight="1">
       <c r="A88" s="42" t="s">
         <v>239</v>
       </c>
@@ -8039,7 +8035,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="89" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" ht="18" customHeight="1">
       <c r="A89" s="42" t="s">
         <v>233</v>
       </c>
@@ -8081,7 +8077,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="90" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" ht="18" customHeight="1">
       <c r="A90" s="42" t="s">
         <v>214</v>
       </c>
@@ -8123,7 +8119,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="91" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" ht="18" customHeight="1">
       <c r="A91" s="42" t="s">
         <v>61</v>
       </c>
@@ -8165,7 +8161,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="92" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" ht="19">
       <c r="A92" s="42" t="s">
         <v>271</v>
       </c>
@@ -8207,7 +8203,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="93" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" ht="19">
       <c r="A93" s="42" t="s">
         <v>220</v>
       </c>
@@ -8249,7 +8245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" ht="19">
       <c r="A94" s="42" t="s">
         <v>4</v>
       </c>
@@ -8291,7 +8287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" ht="19">
       <c r="A95" s="42" t="s">
         <v>259</v>
       </c>
@@ -8333,7 +8329,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="96" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" ht="19">
       <c r="A96" s="52" t="s">
         <v>618</v>
       </c>
@@ -8375,7 +8371,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="97" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" ht="19">
       <c r="A97" s="57" t="s">
         <v>557</v>
       </c>
@@ -8417,7 +8413,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="98" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" ht="19">
       <c r="A98" s="52" t="s">
         <v>619</v>
       </c>
@@ -8459,7 +8455,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="99" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" ht="19">
       <c r="A99" s="57" t="s">
         <v>556</v>
       </c>
@@ -8501,7 +8497,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="100" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" ht="19">
       <c r="A100" s="57" t="s">
         <v>555</v>
       </c>
@@ -8543,7 +8539,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="101" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" ht="19">
       <c r="A101" s="52" t="s">
         <v>482</v>
       </c>
@@ -8585,7 +8581,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="102" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" ht="19">
       <c r="A102" s="52" t="s">
         <v>487</v>
       </c>
@@ -8627,7 +8623,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="103" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" ht="19">
       <c r="A103" s="52" t="s">
         <v>634</v>
       </c>
@@ -8667,7 +8663,7 @@
       </c>
       <c r="N103" s="56"/>
     </row>
-    <row r="104" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" ht="19">
       <c r="A104" s="58" t="s">
         <v>218</v>
       </c>
@@ -8709,7 +8705,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="105" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" ht="19">
       <c r="A105" s="58" t="s">
         <v>225</v>
       </c>
@@ -8751,7 +8747,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="106" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" ht="19">
       <c r="A106" s="58" t="s">
         <v>227</v>
       </c>
@@ -8793,7 +8789,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="107" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" ht="19">
       <c r="A107" s="58" t="s">
         <v>232</v>
       </c>
@@ -8835,7 +8831,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="108" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" ht="19">
       <c r="A108" s="58" t="s">
         <v>286</v>
       </c>
@@ -8877,7 +8873,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="109" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" ht="19">
       <c r="A109" s="58" t="s">
         <v>258</v>
       </c>
@@ -8919,7 +8915,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="110" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" ht="19">
       <c r="A110" s="58" t="s">
         <v>231</v>
       </c>
@@ -8961,7 +8957,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="111" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" ht="19">
       <c r="A111" s="58" t="s">
         <v>250</v>
       </c>
@@ -9003,7 +8999,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="112" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:14" ht="19">
       <c r="A112" s="58" t="s">
         <v>253</v>
       </c>
@@ -9045,7 +9041,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="113" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:14" ht="19">
       <c r="A113" s="58" t="s">
         <v>265</v>
       </c>
@@ -9087,7 +9083,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="114" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:14" ht="19">
       <c r="A114" s="58" t="s">
         <v>659</v>
       </c>
@@ -9129,7 +9125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:14" ht="19">
       <c r="A115" s="58" t="s">
         <v>671</v>
       </c>
@@ -9169,7 +9165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:14" ht="19">
       <c r="A116" s="47" t="s">
         <v>497</v>
       </c>
@@ -9211,7 +9207,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="117" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:14" ht="19">
       <c r="A117" s="47" t="s">
         <v>495</v>
       </c>
@@ -9253,7 +9249,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="118" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:14" ht="19">
       <c r="A118" s="47" t="s">
         <v>235</v>
       </c>
@@ -9295,7 +9291,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="119" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:14" ht="19">
       <c r="A119" s="47" t="s">
         <v>496</v>
       </c>
@@ -9337,7 +9333,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="120" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:14" ht="19">
       <c r="A120" s="27" t="s">
         <v>236</v>
       </c>
@@ -9377,7 +9373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:14" ht="19">
       <c r="A121" s="27" t="s">
         <v>270</v>
       </c>
@@ -9417,7 +9413,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="122" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:14" ht="19">
       <c r="A122" s="27" t="s">
         <v>262</v>
       </c>
@@ -9457,7 +9453,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="123" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:14" ht="19">
       <c r="A123" s="27" t="s">
         <v>263</v>
       </c>
@@ -9497,7 +9493,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="124" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:14" ht="19">
       <c r="A124" s="27" t="s">
         <v>264</v>
       </c>
@@ -9537,7 +9533,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="125" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:14" ht="19">
       <c r="A125" s="27" t="s">
         <v>256</v>
       </c>
@@ -9577,7 +9573,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="126" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:14" ht="19">
       <c r="A126" s="27" t="s">
         <v>682</v>
       </c>
@@ -9614,7 +9610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:14" ht="19">
       <c r="A127" s="27" t="s">
         <v>683</v>
       </c>
@@ -9651,7 +9647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:14" ht="19">
       <c r="A128" s="27" t="s">
         <v>684</v>
       </c>
@@ -9688,7 +9684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:14" ht="19">
       <c r="A129" s="27" t="s">
         <v>685</v>
       </c>
@@ -9725,7 +9721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:14" ht="19">
       <c r="A130" s="27" t="s">
         <v>686</v>
       </c>
@@ -9762,7 +9758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:14" ht="19">
       <c r="A131" s="27" t="s">
         <v>687</v>
       </c>
@@ -9799,7 +9795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:14" ht="19">
       <c r="A132" s="27" t="s">
         <v>688</v>
       </c>
@@ -9836,7 +9832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:14" ht="19">
       <c r="A133" s="27" t="s">
         <v>691</v>
       </c>
@@ -9873,7 +9869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:14" ht="19">
       <c r="A134" s="61" t="s">
         <v>254</v>
       </c>
@@ -9913,7 +9909,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="135" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:14" ht="19">
       <c r="A135" s="61" t="s">
         <v>221</v>
       </c>
@@ -9953,7 +9949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:14" ht="19">
       <c r="A136" s="61" t="s">
         <v>287</v>
       </c>
@@ -9993,7 +9989,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="137" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:14" ht="19">
       <c r="A137" s="61" t="s">
         <v>266</v>
       </c>
@@ -10033,7 +10029,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="138" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:14" ht="19">
       <c r="A138" s="61" t="s">
         <v>223</v>
       </c>
@@ -10073,7 +10069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:14" ht="19">
       <c r="A139" s="61" t="s">
         <v>257</v>
       </c>
@@ -10113,7 +10109,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="140" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:14" ht="19">
       <c r="A140" s="61" t="s">
         <v>261</v>
       </c>
@@ -10153,7 +10149,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="141" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:14" ht="19">
       <c r="A141" s="61" t="s">
         <v>689</v>
       </c>
@@ -10193,7 +10189,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="142" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:14" ht="19">
       <c r="A142" s="61" t="s">
         <v>690</v>
       </c>
@@ -10233,7 +10229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:14" ht="19">
       <c r="A143" s="49" t="s">
         <v>572</v>
       </c>
@@ -10277,7 +10273,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="144" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:14" ht="19">
       <c r="A144" s="49" t="s">
         <v>570</v>
       </c>
@@ -10321,7 +10317,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="145" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:14" ht="19">
       <c r="A145" s="49" t="s">
         <v>569</v>
       </c>
@@ -10365,7 +10361,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="146" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:14" ht="19">
       <c r="A146" s="49" t="s">
         <v>665</v>
       </c>
@@ -10409,7 +10405,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="147" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:14" ht="19">
       <c r="A147" s="49" t="s">
         <v>571</v>
       </c>
@@ -10453,7 +10449,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="148" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:14" ht="19">
       <c r="A148" s="49" t="s">
         <v>639</v>
       </c>
@@ -10497,7 +10493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:14" ht="19">
       <c r="A149" s="49" t="s">
         <v>642</v>
       </c>
@@ -10541,7 +10537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:14" ht="19">
       <c r="A150" s="49" t="s">
         <v>666</v>
       </c>
@@ -10585,7 +10581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:14" ht="19">
       <c r="F151" s="65"/>
       <c r="G151" s="65"/>
       <c r="H151" s="65"/>
@@ -10594,7 +10590,7 @@
       <c r="K151" s="65"/>
       <c r="L151" s="65"/>
     </row>
-    <row r="152" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:14" ht="19">
       <c r="F152" s="65"/>
       <c r="G152" s="65"/>
       <c r="H152" s="65"/>
@@ -10603,7 +10599,7 @@
       <c r="K152" s="65"/>
       <c r="L152" s="65"/>
     </row>
-    <row r="153" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:14" ht="19">
       <c r="F153" s="65"/>
       <c r="G153" s="65"/>
       <c r="H153" s="65"/>
@@ -10613,14 +10609,14 @@
       <c r="L153" s="65"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N153">
+  <sortState ref="A2:N153">
     <sortCondition ref="D2:D153"/>
     <sortCondition ref="E2:E153"/>
     <sortCondition ref="F2:F153"/>
     <sortCondition ref="G2:G153"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B57" r:id="rId1" display="https://it.wikipedia.org/wiki/Baiyangdian_virus" xr:uid="{58752D86-BFC4-4544-AB22-E17E33BA2CF7}"/>
+    <hyperlink ref="B57" r:id="rId1" display="https://it.wikipedia.org/wiki/Baiyangdian_virus"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -10633,91 +10629,91 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="17" thickBot="1">
       <c r="A1" s="63">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="17" thickBot="1">
       <c r="A2" s="64">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="17" thickBot="1">
       <c r="A3" s="64">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="17" thickBot="1">
       <c r="A4" s="64">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="17" thickBot="1">
       <c r="A5" s="64">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="17" thickBot="1">
       <c r="A6" s="64">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="17" thickBot="1">
       <c r="A7" s="64">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" ht="17" thickBot="1">
       <c r="A8" s="64">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" ht="17" thickBot="1">
       <c r="A9" s="64">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" ht="17" thickBot="1">
       <c r="A10" s="64">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" ht="17" thickBot="1">
       <c r="A11" s="64">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" ht="17" thickBot="1">
       <c r="A12" s="64">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" ht="17" thickBot="1">
       <c r="A13" s="64">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" ht="17" thickBot="1">
       <c r="A14" s="64">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" ht="17" thickBot="1">
       <c r="A15" s="64">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1">
       <c r="A16">
         <f>SUM(A1:A15)</f>
         <v>130</v>
@@ -10734,16 +10730,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="18" customHeight="1">
       <c r="A1" s="5">
         <v>69</v>
       </c>

</xml_diff>

<commit_message>
Updated alignment tree select statements to match updates in tabular data
</commit_message>
<xml_diff>
--- a/tabular/flavi-ncbi-refseqs-side-data.xlsx
+++ b/tabular/flavi-ncbi-refseqs-side-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7480" yWindow="1020" windowWidth="40620" windowHeight="22420" tabRatio="500"/>
+    <workbookView xWindow="3220" yWindow="700" windowWidth="40620" windowHeight="22420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="flavi.txt" sheetId="1" r:id="rId1"/>
@@ -2589,7 +2589,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="622">
+  <cellStyleXfs count="623">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3210,6 +3210,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -3356,7 +3357,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="622">
+  <cellStyles count="623">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3668,6 +3669,7 @@
     <cellStyle name="Followed Hyperlink" xfId="618" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="620" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="621" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="622" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4317,9 +4319,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N150" sqref="A1:N150"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="F17:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4339,7 +4341,7 @@
     <col min="14" max="14" width="31.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="19">
+    <row r="1" spans="1:14" ht="18">
       <c r="A1" s="9" t="s">
         <v>213</v>
       </c>
@@ -7741,7 +7743,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="82" spans="1:14" ht="19">
+    <row r="82" spans="1:14" ht="18">
       <c r="A82" s="42" t="s">
         <v>260</v>
       </c>
@@ -7783,7 +7785,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="19">
+    <row r="83" spans="1:14" ht="18">
       <c r="A83" s="42" t="s">
         <v>242</v>
       </c>
@@ -7825,7 +7827,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="84" spans="1:14" ht="19">
+    <row r="84" spans="1:14" ht="18">
       <c r="A84" s="42" t="s">
         <v>215</v>
       </c>
@@ -7867,7 +7869,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="19">
+    <row r="85" spans="1:14" ht="18">
       <c r="A85" s="42" t="s">
         <v>234</v>
       </c>
@@ -7909,7 +7911,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="86" spans="1:14" ht="19">
+    <row r="86" spans="1:14" ht="18">
       <c r="A86" s="42" t="s">
         <v>222</v>
       </c>
@@ -7951,7 +7953,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="87" spans="1:14" ht="19">
+    <row r="87" spans="1:14" ht="18">
       <c r="A87" s="42" t="s">
         <v>58</v>
       </c>
@@ -8161,7 +8163,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="92" spans="1:14" ht="19">
+    <row r="92" spans="1:14" ht="18">
       <c r="A92" s="42" t="s">
         <v>271</v>
       </c>
@@ -8203,7 +8205,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="93" spans="1:14" ht="19">
+    <row r="93" spans="1:14" ht="18">
       <c r="A93" s="42" t="s">
         <v>220</v>
       </c>
@@ -8245,7 +8247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:14" ht="19">
+    <row r="94" spans="1:14" ht="18">
       <c r="A94" s="42" t="s">
         <v>4</v>
       </c>
@@ -8287,7 +8289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:14" ht="19">
+    <row r="95" spans="1:14" ht="18">
       <c r="A95" s="42" t="s">
         <v>259</v>
       </c>
@@ -8329,7 +8331,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="96" spans="1:14" ht="19">
+    <row r="96" spans="1:14" ht="18">
       <c r="A96" s="52" t="s">
         <v>618</v>
       </c>
@@ -8371,7 +8373,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="97" spans="1:14" ht="19">
+    <row r="97" spans="1:14" ht="18">
       <c r="A97" s="57" t="s">
         <v>557</v>
       </c>
@@ -8413,7 +8415,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="98" spans="1:14" ht="19">
+    <row r="98" spans="1:14" ht="18">
       <c r="A98" s="52" t="s">
         <v>619</v>
       </c>
@@ -8455,7 +8457,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="99" spans="1:14" ht="19">
+    <row r="99" spans="1:14" ht="18">
       <c r="A99" s="57" t="s">
         <v>556</v>
       </c>
@@ -8497,7 +8499,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="100" spans="1:14" ht="19">
+    <row r="100" spans="1:14" ht="18">
       <c r="A100" s="57" t="s">
         <v>555</v>
       </c>
@@ -8539,7 +8541,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="101" spans="1:14" ht="19">
+    <row r="101" spans="1:14" ht="18">
       <c r="A101" s="52" t="s">
         <v>482</v>
       </c>
@@ -8581,7 +8583,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="102" spans="1:14" ht="19">
+    <row r="102" spans="1:14" ht="18">
       <c r="A102" s="52" t="s">
         <v>487</v>
       </c>
@@ -8623,7 +8625,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="103" spans="1:14" ht="19">
+    <row r="103" spans="1:14" ht="18">
       <c r="A103" s="52" t="s">
         <v>634</v>
       </c>
@@ -8663,7 +8665,7 @@
       </c>
       <c r="N103" s="56"/>
     </row>
-    <row r="104" spans="1:14" ht="19">
+    <row r="104" spans="1:14" ht="18">
       <c r="A104" s="58" t="s">
         <v>218</v>
       </c>
@@ -8705,7 +8707,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="105" spans="1:14" ht="19">
+    <row r="105" spans="1:14" ht="18">
       <c r="A105" s="58" t="s">
         <v>225</v>
       </c>
@@ -8747,7 +8749,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="106" spans="1:14" ht="19">
+    <row r="106" spans="1:14" ht="18">
       <c r="A106" s="58" t="s">
         <v>227</v>
       </c>
@@ -8789,7 +8791,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="107" spans="1:14" ht="19">
+    <row r="107" spans="1:14" ht="18">
       <c r="A107" s="58" t="s">
         <v>232</v>
       </c>
@@ -8831,7 +8833,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="108" spans="1:14" ht="19">
+    <row r="108" spans="1:14" ht="18">
       <c r="A108" s="58" t="s">
         <v>286</v>
       </c>
@@ -8873,7 +8875,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="109" spans="1:14" ht="19">
+    <row r="109" spans="1:14" ht="18">
       <c r="A109" s="58" t="s">
         <v>258</v>
       </c>
@@ -8915,7 +8917,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="110" spans="1:14" ht="19">
+    <row r="110" spans="1:14" ht="18">
       <c r="A110" s="58" t="s">
         <v>231</v>
       </c>
@@ -8957,7 +8959,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="111" spans="1:14" ht="19">
+    <row r="111" spans="1:14" ht="18">
       <c r="A111" s="58" t="s">
         <v>250</v>
       </c>
@@ -8999,7 +9001,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="112" spans="1:14" ht="19">
+    <row r="112" spans="1:14" ht="18">
       <c r="A112" s="58" t="s">
         <v>253</v>
       </c>
@@ -9041,7 +9043,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="113" spans="1:14" ht="19">
+    <row r="113" spans="1:14" ht="18">
       <c r="A113" s="58" t="s">
         <v>265</v>
       </c>
@@ -9083,7 +9085,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="114" spans="1:14" ht="19">
+    <row r="114" spans="1:14" ht="18">
       <c r="A114" s="58" t="s">
         <v>659</v>
       </c>
@@ -9125,7 +9127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:14" ht="19">
+    <row r="115" spans="1:14" ht="18">
       <c r="A115" s="58" t="s">
         <v>671</v>
       </c>
@@ -9165,7 +9167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:14" ht="19">
+    <row r="116" spans="1:14" ht="18">
       <c r="A116" s="47" t="s">
         <v>497</v>
       </c>
@@ -9207,7 +9209,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="117" spans="1:14" ht="19">
+    <row r="117" spans="1:14" ht="18">
       <c r="A117" s="47" t="s">
         <v>495</v>
       </c>
@@ -9249,7 +9251,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="118" spans="1:14" ht="19">
+    <row r="118" spans="1:14" ht="18">
       <c r="A118" s="47" t="s">
         <v>235</v>
       </c>
@@ -9291,7 +9293,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="119" spans="1:14" ht="19">
+    <row r="119" spans="1:14" ht="18">
       <c r="A119" s="47" t="s">
         <v>496</v>
       </c>
@@ -9333,7 +9335,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="120" spans="1:14" ht="19">
+    <row r="120" spans="1:14" ht="18">
       <c r="A120" s="27" t="s">
         <v>236</v>
       </c>
@@ -9373,7 +9375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:14" ht="19">
+    <row r="121" spans="1:14" ht="18">
       <c r="A121" s="27" t="s">
         <v>270</v>
       </c>
@@ -9413,7 +9415,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="122" spans="1:14" ht="19">
+    <row r="122" spans="1:14" ht="18">
       <c r="A122" s="27" t="s">
         <v>262</v>
       </c>
@@ -9453,7 +9455,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="123" spans="1:14" ht="19">
+    <row r="123" spans="1:14" ht="18">
       <c r="A123" s="27" t="s">
         <v>263</v>
       </c>
@@ -9493,7 +9495,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="124" spans="1:14" ht="19">
+    <row r="124" spans="1:14" ht="18">
       <c r="A124" s="27" t="s">
         <v>264</v>
       </c>
@@ -9533,7 +9535,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="125" spans="1:14" ht="19">
+    <row r="125" spans="1:14" ht="18">
       <c r="A125" s="27" t="s">
         <v>256</v>
       </c>
@@ -9573,7 +9575,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="126" spans="1:14" ht="19">
+    <row r="126" spans="1:14" ht="18">
       <c r="A126" s="27" t="s">
         <v>682</v>
       </c>
@@ -9610,7 +9612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:14" ht="19">
+    <row r="127" spans="1:14" ht="18">
       <c r="A127" s="27" t="s">
         <v>683</v>
       </c>
@@ -9647,7 +9649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:14" ht="19">
+    <row r="128" spans="1:14" ht="18">
       <c r="A128" s="27" t="s">
         <v>684</v>
       </c>
@@ -9684,7 +9686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:14" ht="19">
+    <row r="129" spans="1:14" ht="18">
       <c r="A129" s="27" t="s">
         <v>685</v>
       </c>
@@ -9721,7 +9723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:14" ht="19">
+    <row r="130" spans="1:14" ht="18">
       <c r="A130" s="27" t="s">
         <v>686</v>
       </c>
@@ -9758,7 +9760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:14" ht="19">
+    <row r="131" spans="1:14" ht="18">
       <c r="A131" s="27" t="s">
         <v>687</v>
       </c>
@@ -9795,7 +9797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:14" ht="19">
+    <row r="132" spans="1:14" ht="18">
       <c r="A132" s="27" t="s">
         <v>688</v>
       </c>
@@ -9832,7 +9834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:14" ht="19">
+    <row r="133" spans="1:14" ht="18">
       <c r="A133" s="27" t="s">
         <v>691</v>
       </c>
@@ -9869,7 +9871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:14" ht="19">
+    <row r="134" spans="1:14" ht="18">
       <c r="A134" s="61" t="s">
         <v>254</v>
       </c>
@@ -9909,7 +9911,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="135" spans="1:14" ht="19">
+    <row r="135" spans="1:14" ht="18">
       <c r="A135" s="61" t="s">
         <v>221</v>
       </c>
@@ -9949,7 +9951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:14" ht="19">
+    <row r="136" spans="1:14" ht="18">
       <c r="A136" s="61" t="s">
         <v>287</v>
       </c>
@@ -9989,7 +9991,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="137" spans="1:14" ht="19">
+    <row r="137" spans="1:14" ht="18">
       <c r="A137" s="61" t="s">
         <v>266</v>
       </c>
@@ -10029,7 +10031,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="138" spans="1:14" ht="19">
+    <row r="138" spans="1:14" ht="18">
       <c r="A138" s="61" t="s">
         <v>223</v>
       </c>
@@ -10069,7 +10071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:14" ht="19">
+    <row r="139" spans="1:14" ht="18">
       <c r="A139" s="61" t="s">
         <v>257</v>
       </c>
@@ -10109,7 +10111,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="140" spans="1:14" ht="19">
+    <row r="140" spans="1:14" ht="18">
       <c r="A140" s="61" t="s">
         <v>261</v>
       </c>
@@ -10149,7 +10151,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="141" spans="1:14" ht="19">
+    <row r="141" spans="1:14" ht="18">
       <c r="A141" s="61" t="s">
         <v>689</v>
       </c>
@@ -10189,7 +10191,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="142" spans="1:14" ht="19">
+    <row r="142" spans="1:14" ht="18">
       <c r="A142" s="61" t="s">
         <v>690</v>
       </c>
@@ -10229,7 +10231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:14" ht="19">
+    <row r="143" spans="1:14" ht="18">
       <c r="A143" s="49" t="s">
         <v>572</v>
       </c>
@@ -10273,7 +10275,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="144" spans="1:14" ht="19">
+    <row r="144" spans="1:14" ht="18">
       <c r="A144" s="49" t="s">
         <v>570</v>
       </c>
@@ -10317,7 +10319,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="145" spans="1:14" ht="19">
+    <row r="145" spans="1:14" ht="18">
       <c r="A145" s="49" t="s">
         <v>569</v>
       </c>
@@ -10361,7 +10363,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="146" spans="1:14" ht="19">
+    <row r="146" spans="1:14" ht="18">
       <c r="A146" s="49" t="s">
         <v>665</v>
       </c>
@@ -10405,7 +10407,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="147" spans="1:14" ht="19">
+    <row r="147" spans="1:14" ht="18">
       <c r="A147" s="49" t="s">
         <v>571</v>
       </c>
@@ -10449,7 +10451,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="148" spans="1:14" ht="19">
+    <row r="148" spans="1:14" ht="18">
       <c r="A148" s="49" t="s">
         <v>639</v>
       </c>
@@ -10493,7 +10495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:14" ht="19">
+    <row r="149" spans="1:14" ht="18">
       <c r="A149" s="49" t="s">
         <v>642</v>
       </c>
@@ -10537,7 +10539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:14" ht="19">
+    <row r="150" spans="1:14" ht="18">
       <c r="A150" s="49" t="s">
         <v>666</v>
       </c>
@@ -10581,7 +10583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:14" ht="19">
+    <row r="151" spans="1:14" ht="18">
       <c r="F151" s="65"/>
       <c r="G151" s="65"/>
       <c r="H151" s="65"/>
@@ -10590,7 +10592,7 @@
       <c r="K151" s="65"/>
       <c r="L151" s="65"/>
     </row>
-    <row r="152" spans="1:14" ht="19">
+    <row r="152" spans="1:14" ht="18">
       <c r="F152" s="65"/>
       <c r="G152" s="65"/>
       <c r="H152" s="65"/>
@@ -10599,7 +10601,7 @@
       <c r="K152" s="65"/>
       <c r="L152" s="65"/>
     </row>
-    <row r="153" spans="1:14" ht="19">
+    <row r="153" spans="1:14" ht="18">
       <c r="F153" s="65"/>
       <c r="G153" s="65"/>
       <c r="H153" s="65"/>
@@ -10638,77 +10640,77 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="17" thickBot="1">
+    <row r="1" spans="1:1" ht="16" thickBot="1">
       <c r="A1" s="63">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="17" thickBot="1">
+    <row r="2" spans="1:1" ht="16" thickBot="1">
       <c r="A2" s="64">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="17" thickBot="1">
+    <row r="3" spans="1:1" ht="16" thickBot="1">
       <c r="A3" s="64">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="17" thickBot="1">
+    <row r="4" spans="1:1" ht="16" thickBot="1">
       <c r="A4" s="64">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="17" thickBot="1">
+    <row r="5" spans="1:1" ht="16" thickBot="1">
       <c r="A5" s="64">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="17" thickBot="1">
+    <row r="6" spans="1:1" ht="16" thickBot="1">
       <c r="A6" s="64">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="17" thickBot="1">
+    <row r="7" spans="1:1" ht="16" thickBot="1">
       <c r="A7" s="64">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="17" thickBot="1">
+    <row r="8" spans="1:1" ht="16" thickBot="1">
       <c r="A8" s="64">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="17" thickBot="1">
+    <row r="9" spans="1:1" ht="16" thickBot="1">
       <c r="A9" s="64">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="17" thickBot="1">
+    <row r="10" spans="1:1" ht="16" thickBot="1">
       <c r="A10" s="64">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="17" thickBot="1">
+    <row r="11" spans="1:1" ht="16" thickBot="1">
       <c r="A11" s="64">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="17" thickBot="1">
+    <row r="12" spans="1:1" ht="16" thickBot="1">
       <c r="A12" s="64">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="17" thickBot="1">
+    <row r="13" spans="1:1" ht="16" thickBot="1">
       <c r="A13" s="64">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="17" thickBot="1">
+    <row r="14" spans="1:1" ht="16" thickBot="1">
       <c r="A14" s="64">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="17" thickBot="1">
+    <row r="15" spans="1:1" ht="16" thickBot="1">
       <c r="A15" s="64">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Added missing Jingmen taxa
</commit_message>
<xml_diff>
--- a/tabular/flavi-ncbi-refseqs-side-data.xlsx
+++ b/tabular/flavi-ncbi-refseqs-side-data.xlsx
@@ -2589,7 +2589,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="623">
+  <cellStyleXfs count="625">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3210,6 +3210,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3357,7 +3359,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="623">
+  <cellStyles count="625">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3670,6 +3672,8 @@
     <cellStyle name="Followed Hyperlink" xfId="620" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="621" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="622" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="623" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="624" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4319,9 +4323,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="F17:G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A146" sqref="A146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Updating alignments, alignment tree - creating correct structure
</commit_message>
<xml_diff>
--- a/tabular/flavi-ncbi-refseqs-side-data.xlsx
+++ b/tabular/flavi-ncbi-refseqs-side-data.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7160" yWindow="500" windowWidth="38100" windowHeight="24900" tabRatio="500"/>
+    <workbookView xWindow="6280" yWindow="500" windowWidth="29780" windowHeight="17980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="flavi.txt" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
+    <sheet name="removed" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">flavi.txt!$A$1:$M$112</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">flavi.txt!$A$1:$M$111</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1922" uniqueCount="764">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1922" uniqueCount="766">
   <si>
     <t>AY632538</t>
   </si>
@@ -2322,6 +2322,12 @@
   </si>
   <si>
     <t>LayV</t>
+  </si>
+  <si>
+    <t>HepaPegi</t>
+  </si>
+  <si>
+    <t>Hepegivirus</t>
   </si>
 </sst>
 </file>
@@ -2547,13 +2553,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FF330000"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF330000"/>
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -2595,7 +2601,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="625">
+  <cellStyleXfs count="637">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3216,6 +3222,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3350,9 +3368,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3364,12 +3379,15 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="625">
+  <cellStyles count="637">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3684,6 +3702,18 @@
     <cellStyle name="Followed Hyperlink" xfId="622" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="623" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="624" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="625" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="626" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="627" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="628" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="629" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="630" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="631" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="632" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="633" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="634" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="635" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="636" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4331,11 +4361,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N153"/>
+  <dimension ref="A1:N152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4389,13 +4419,13 @@
       <c r="K1" s="8" t="s">
         <v>623</v>
       </c>
-      <c r="L1" s="67" t="s">
+      <c r="L1" s="66" t="s">
         <v>504</v>
       </c>
-      <c r="M1" s="68" t="s">
+      <c r="M1" s="67" t="s">
         <v>474</v>
       </c>
-      <c r="N1" s="68" t="s">
+      <c r="N1" s="67" t="s">
         <v>615</v>
       </c>
     </row>
@@ -6607,13 +6637,13 @@
       <c r="I54" s="33" t="s">
         <v>403</v>
       </c>
-      <c r="J54" s="65" t="s">
+      <c r="J54" s="64" t="s">
         <v>80</v>
       </c>
-      <c r="K54" s="65" t="s">
+      <c r="K54" s="64" t="s">
         <v>632</v>
       </c>
-      <c r="L54" s="65" t="s">
+      <c r="L54" s="64" t="s">
         <v>737</v>
       </c>
       <c r="M54" s="13" t="s">
@@ -6649,19 +6679,19 @@
       <c r="I55" s="33" t="s">
         <v>403</v>
       </c>
-      <c r="J55" s="65" t="s">
+      <c r="J55" s="64" t="s">
         <v>80</v>
       </c>
-      <c r="K55" s="65" t="s">
+      <c r="K55" s="64" t="s">
         <v>632</v>
       </c>
-      <c r="L55" s="65" t="s">
+      <c r="L55" s="64" t="s">
         <v>738</v>
       </c>
       <c r="M55" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="N55" s="65" t="s">
+      <c r="N55" s="64" t="s">
         <v>745</v>
       </c>
     </row>
@@ -6691,19 +6721,19 @@
       <c r="I56" s="33" t="s">
         <v>403</v>
       </c>
-      <c r="J56" s="65" t="s">
+      <c r="J56" s="64" t="s">
         <v>80</v>
       </c>
-      <c r="K56" s="65" t="s">
+      <c r="K56" s="64" t="s">
         <v>632</v>
       </c>
-      <c r="L56" s="65" t="s">
+      <c r="L56" s="64" t="s">
         <v>1</v>
       </c>
       <c r="M56" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="N56" s="65" t="s">
+      <c r="N56" s="64" t="s">
         <v>1</v>
       </c>
     </row>
@@ -6733,19 +6763,19 @@
       <c r="I57" s="33" t="s">
         <v>403</v>
       </c>
-      <c r="J57" s="65" t="s">
+      <c r="J57" s="64" t="s">
         <v>80</v>
       </c>
-      <c r="K57" s="65" t="s">
+      <c r="K57" s="64" t="s">
         <v>632</v>
       </c>
-      <c r="L57" s="65" t="s">
+      <c r="L57" s="64" t="s">
         <v>1</v>
       </c>
       <c r="M57" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="N57" s="65" t="s">
+      <c r="N57" s="64" t="s">
         <v>746</v>
       </c>
     </row>
@@ -6775,19 +6805,19 @@
       <c r="I58" s="33" t="s">
         <v>403</v>
       </c>
-      <c r="J58" s="65" t="s">
+      <c r="J58" s="64" t="s">
         <v>80</v>
       </c>
-      <c r="K58" s="65" t="s">
+      <c r="K58" s="64" t="s">
         <v>633</v>
       </c>
-      <c r="L58" s="66">
+      <c r="L58" s="65">
         <v>25008</v>
       </c>
       <c r="M58" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="N58" s="65" t="s">
+      <c r="N58" s="64" t="s">
         <v>747</v>
       </c>
     </row>
@@ -6817,19 +6847,19 @@
       <c r="I59" s="33" t="s">
         <v>403</v>
       </c>
-      <c r="J59" s="65" t="s">
+      <c r="J59" s="64" t="s">
         <v>80</v>
       </c>
-      <c r="K59" s="65" t="s">
+      <c r="K59" s="64" t="s">
         <v>633</v>
       </c>
-      <c r="L59" s="65" t="s">
+      <c r="L59" s="64" t="s">
         <v>741</v>
       </c>
       <c r="M59" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="N59" s="65" t="s">
+      <c r="N59" s="64" t="s">
         <v>1</v>
       </c>
     </row>
@@ -6859,19 +6889,19 @@
       <c r="I60" s="33" t="s">
         <v>403</v>
       </c>
-      <c r="J60" s="65" t="s">
+      <c r="J60" s="64" t="s">
         <v>80</v>
       </c>
-      <c r="K60" s="65" t="s">
+      <c r="K60" s="64" t="s">
         <v>632</v>
       </c>
-      <c r="L60" s="65" t="s">
+      <c r="L60" s="64" t="s">
         <v>744</v>
       </c>
       <c r="M60" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="N60" s="65" t="s">
+      <c r="N60" s="64" t="s">
         <v>1</v>
       </c>
     </row>
@@ -7279,19 +7309,19 @@
       <c r="I70" s="36" t="s">
         <v>505</v>
       </c>
-      <c r="J70" s="65" t="s">
+      <c r="J70" s="64" t="s">
         <v>80</v>
       </c>
-      <c r="K70" s="65" t="s">
+      <c r="K70" s="64" t="s">
         <v>633</v>
       </c>
-      <c r="L70" s="65" t="s">
+      <c r="L70" s="64" t="s">
         <v>743</v>
       </c>
       <c r="M70" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="N70" s="65" t="s">
+      <c r="N70" s="64" t="s">
         <v>1</v>
       </c>
     </row>
@@ -7801,13 +7831,13 @@
     </row>
     <row r="83" spans="1:14" ht="18">
       <c r="A83" s="42" t="s">
-        <v>242</v>
+        <v>215</v>
       </c>
       <c r="B83" s="43" t="s">
-        <v>124</v>
+        <v>77</v>
       </c>
       <c r="C83" s="43" t="s">
-        <v>380</v>
+        <v>315</v>
       </c>
       <c r="D83" s="43" t="s">
         <v>753</v>
@@ -7823,33 +7853,33 @@
       </c>
       <c r="H83" s="43"/>
       <c r="I83" s="43" t="s">
-        <v>630</v>
+        <v>653</v>
       </c>
       <c r="J83" s="44" t="s">
         <v>192</v>
       </c>
       <c r="K83" s="44" t="s">
-        <v>632</v>
+        <v>624</v>
       </c>
       <c r="L83" s="15" t="s">
-        <v>382</v>
+        <v>1</v>
       </c>
       <c r="M83" s="13" t="s">
         <v>475</v>
       </c>
       <c r="N83" s="16" t="s">
-        <v>381</v>
+        <v>78</v>
       </c>
     </row>
     <row r="84" spans="1:14" ht="18">
       <c r="A84" s="42" t="s">
-        <v>215</v>
+        <v>234</v>
       </c>
       <c r="B84" s="43" t="s">
-        <v>77</v>
+        <v>114</v>
       </c>
       <c r="C84" s="43" t="s">
-        <v>315</v>
+        <v>363</v>
       </c>
       <c r="D84" s="43" t="s">
         <v>753</v>
@@ -7865,7 +7895,7 @@
       </c>
       <c r="H84" s="43"/>
       <c r="I84" s="43" t="s">
-        <v>653</v>
+        <v>519</v>
       </c>
       <c r="J84" s="44" t="s">
         <v>192</v>
@@ -7874,24 +7904,24 @@
         <v>624</v>
       </c>
       <c r="L84" s="15" t="s">
-        <v>1</v>
+        <v>365</v>
       </c>
       <c r="M84" s="13" t="s">
         <v>475</v>
       </c>
       <c r="N84" s="16" t="s">
-        <v>78</v>
+        <v>364</v>
       </c>
     </row>
     <row r="85" spans="1:14" ht="18">
       <c r="A85" s="42" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="B85" s="43" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="C85" s="43" t="s">
-        <v>363</v>
+        <v>204</v>
       </c>
       <c r="D85" s="43" t="s">
         <v>753</v>
@@ -7913,27 +7943,27 @@
         <v>192</v>
       </c>
       <c r="K85" s="44" t="s">
-        <v>624</v>
+        <v>654</v>
       </c>
       <c r="L85" s="15" t="s">
-        <v>365</v>
+        <v>1</v>
       </c>
       <c r="M85" s="13" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="N85" s="16" t="s">
-        <v>364</v>
+        <v>347</v>
       </c>
     </row>
     <row r="86" spans="1:14" ht="18">
       <c r="A86" s="42" t="s">
-        <v>222</v>
+        <v>58</v>
       </c>
       <c r="B86" s="43" t="s">
-        <v>102</v>
+        <v>188</v>
       </c>
       <c r="C86" s="43" t="s">
-        <v>204</v>
+        <v>458</v>
       </c>
       <c r="D86" s="43" t="s">
         <v>753</v>
@@ -7949,33 +7979,33 @@
       </c>
       <c r="H86" s="43"/>
       <c r="I86" s="43" t="s">
-        <v>519</v>
+        <v>630</v>
       </c>
       <c r="J86" s="44" t="s">
         <v>192</v>
       </c>
       <c r="K86" s="44" t="s">
-        <v>654</v>
+        <v>632</v>
       </c>
       <c r="L86" s="15" t="s">
-        <v>1</v>
+        <v>460</v>
       </c>
       <c r="M86" s="13" t="s">
         <v>477</v>
       </c>
       <c r="N86" s="16" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="87" spans="1:14" ht="18">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" ht="18" customHeight="1">
       <c r="A87" s="42" t="s">
-        <v>58</v>
+        <v>239</v>
       </c>
       <c r="B87" s="43" t="s">
-        <v>188</v>
+        <v>121</v>
       </c>
       <c r="C87" s="43" t="s">
-        <v>458</v>
+        <v>374</v>
       </c>
       <c r="D87" s="43" t="s">
         <v>753</v>
@@ -7991,33 +8021,33 @@
       </c>
       <c r="H87" s="43"/>
       <c r="I87" s="43" t="s">
-        <v>630</v>
+        <v>564</v>
       </c>
       <c r="J87" s="44" t="s">
         <v>192</v>
       </c>
       <c r="K87" s="44" t="s">
-        <v>632</v>
+        <v>624</v>
       </c>
       <c r="L87" s="15" t="s">
-        <v>460</v>
+        <v>375</v>
       </c>
       <c r="M87" s="13" t="s">
         <v>477</v>
       </c>
       <c r="N87" s="16" t="s">
-        <v>459</v>
+        <v>119</v>
       </c>
     </row>
     <row r="88" spans="1:14" ht="18" customHeight="1">
       <c r="A88" s="42" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B88" s="43" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C88" s="43" t="s">
-        <v>374</v>
+        <v>361</v>
       </c>
       <c r="D88" s="43" t="s">
         <v>753</v>
@@ -8033,7 +8063,7 @@
       </c>
       <c r="H88" s="43"/>
       <c r="I88" s="43" t="s">
-        <v>564</v>
+        <v>519</v>
       </c>
       <c r="J88" s="44" t="s">
         <v>192</v>
@@ -8042,10 +8072,10 @@
         <v>624</v>
       </c>
       <c r="L88" s="15" t="s">
-        <v>375</v>
+        <v>362</v>
       </c>
       <c r="M88" s="13" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="N88" s="16" t="s">
         <v>119</v>
@@ -8053,13 +8083,13 @@
     </row>
     <row r="89" spans="1:14" ht="18" customHeight="1">
       <c r="A89" s="42" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
       <c r="B89" s="43" t="s">
-        <v>113</v>
+        <v>69</v>
       </c>
       <c r="C89" s="43" t="s">
-        <v>361</v>
+        <v>296</v>
       </c>
       <c r="D89" s="43" t="s">
         <v>753</v>
@@ -8075,33 +8105,33 @@
       </c>
       <c r="H89" s="43"/>
       <c r="I89" s="43" t="s">
-        <v>519</v>
+        <v>631</v>
       </c>
       <c r="J89" s="44" t="s">
         <v>192</v>
       </c>
       <c r="K89" s="44" t="s">
-        <v>624</v>
+        <v>633</v>
       </c>
       <c r="L89" s="15" t="s">
-        <v>362</v>
+        <v>298</v>
       </c>
       <c r="M89" s="13" t="s">
-        <v>476</v>
-      </c>
-      <c r="N89" s="16" t="s">
-        <v>119</v>
+        <v>475</v>
+      </c>
+      <c r="N89" s="45" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="90" spans="1:14" ht="18" customHeight="1">
       <c r="A90" s="42" t="s">
-        <v>214</v>
+        <v>61</v>
       </c>
       <c r="B90" s="43" t="s">
-        <v>69</v>
+        <v>202</v>
       </c>
       <c r="C90" s="43" t="s">
-        <v>296</v>
+        <v>466</v>
       </c>
       <c r="D90" s="43" t="s">
         <v>753</v>
@@ -8117,33 +8147,33 @@
       </c>
       <c r="H90" s="43"/>
       <c r="I90" s="43" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="J90" s="44" t="s">
         <v>192</v>
       </c>
       <c r="K90" s="44" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="L90" s="15" t="s">
-        <v>298</v>
+        <v>467</v>
       </c>
       <c r="M90" s="13" t="s">
-        <v>475</v>
-      </c>
-      <c r="N90" s="45" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="91" spans="1:14" ht="18" customHeight="1">
+        <v>479</v>
+      </c>
+      <c r="N90" s="16" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" ht="18">
       <c r="A91" s="42" t="s">
-        <v>61</v>
+        <v>271</v>
       </c>
       <c r="B91" s="43" t="s">
-        <v>202</v>
+        <v>176</v>
       </c>
       <c r="C91" s="43" t="s">
-        <v>466</v>
+        <v>433</v>
       </c>
       <c r="D91" s="43" t="s">
         <v>753</v>
@@ -8159,33 +8189,33 @@
       </c>
       <c r="H91" s="43"/>
       <c r="I91" s="43" t="s">
-        <v>630</v>
+        <v>519</v>
       </c>
       <c r="J91" s="44" t="s">
         <v>192</v>
       </c>
       <c r="K91" s="44" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="L91" s="15" t="s">
-        <v>467</v>
+        <v>48</v>
       </c>
       <c r="M91" s="13" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="N91" s="16" t="s">
-        <v>210</v>
+        <v>177</v>
       </c>
     </row>
     <row r="92" spans="1:14" ht="18">
       <c r="A92" s="42" t="s">
-        <v>271</v>
+        <v>220</v>
       </c>
       <c r="B92" s="43" t="s">
-        <v>176</v>
+        <v>100</v>
       </c>
       <c r="C92" s="43" t="s">
-        <v>433</v>
+        <v>344</v>
       </c>
       <c r="D92" s="43" t="s">
         <v>753</v>
@@ -8207,27 +8237,27 @@
         <v>192</v>
       </c>
       <c r="K92" s="44" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="L92" s="15" t="s">
-        <v>48</v>
+        <v>345</v>
       </c>
       <c r="M92" s="13" t="s">
         <v>477</v>
       </c>
       <c r="N92" s="16" t="s">
-        <v>177</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:14" ht="18">
       <c r="A93" s="42" t="s">
-        <v>220</v>
+        <v>4</v>
       </c>
       <c r="B93" s="43" t="s">
-        <v>100</v>
+        <v>193</v>
       </c>
       <c r="C93" s="43" t="s">
-        <v>344</v>
+        <v>299</v>
       </c>
       <c r="D93" s="43" t="s">
         <v>753</v>
@@ -8245,17 +8275,17 @@
       <c r="I93" s="43" t="s">
         <v>519</v>
       </c>
-      <c r="J93" s="44" t="s">
+      <c r="J93" s="46" t="s">
         <v>192</v>
       </c>
       <c r="K93" s="44" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="L93" s="15" t="s">
-        <v>345</v>
+        <v>300</v>
       </c>
       <c r="M93" s="13" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="N93" s="16" t="s">
         <v>1</v>
@@ -8263,13 +8293,13 @@
     </row>
     <row r="94" spans="1:14" ht="18">
       <c r="A94" s="42" t="s">
-        <v>4</v>
+        <v>259</v>
       </c>
       <c r="B94" s="43" t="s">
-        <v>193</v>
+        <v>152</v>
       </c>
       <c r="C94" s="43" t="s">
-        <v>299</v>
+        <v>417</v>
       </c>
       <c r="D94" s="43" t="s">
         <v>753</v>
@@ -8287,73 +8317,73 @@
       <c r="I94" s="43" t="s">
         <v>519</v>
       </c>
-      <c r="J94" s="46" t="s">
+      <c r="J94" s="44" t="s">
         <v>192</v>
       </c>
       <c r="K94" s="44" t="s">
-        <v>628</v>
+        <v>632</v>
       </c>
       <c r="L94" s="15" t="s">
-        <v>300</v>
+        <v>418</v>
       </c>
       <c r="M94" s="13" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="N94" s="16" t="s">
-        <v>1</v>
+        <v>153</v>
       </c>
     </row>
     <row r="95" spans="1:14" ht="18">
-      <c r="A95" s="42" t="s">
-        <v>259</v>
-      </c>
-      <c r="B95" s="43" t="s">
-        <v>152</v>
-      </c>
-      <c r="C95" s="43" t="s">
-        <v>417</v>
-      </c>
-      <c r="D95" s="43" t="s">
-        <v>753</v>
-      </c>
-      <c r="E95" s="43" t="s">
-        <v>674</v>
-      </c>
-      <c r="F95" s="43" t="s">
-        <v>191</v>
-      </c>
-      <c r="G95" s="43" t="s">
-        <v>586</v>
-      </c>
-      <c r="H95" s="43"/>
-      <c r="I95" s="43" t="s">
-        <v>519</v>
-      </c>
-      <c r="J95" s="44" t="s">
-        <v>192</v>
-      </c>
-      <c r="K95" s="44" t="s">
-        <v>632</v>
+      <c r="A95" s="52" t="s">
+        <v>618</v>
+      </c>
+      <c r="B95" s="53" t="s">
+        <v>488</v>
+      </c>
+      <c r="C95" s="54" t="s">
+        <v>613</v>
+      </c>
+      <c r="D95" s="54" t="s">
+        <v>753</v>
+      </c>
+      <c r="E95" s="55" t="s">
+        <v>674</v>
+      </c>
+      <c r="F95" s="55" t="s">
+        <v>483</v>
+      </c>
+      <c r="G95" s="54" t="s">
+        <v>554</v>
+      </c>
+      <c r="H95" s="54"/>
+      <c r="I95" s="54" t="s">
+        <v>530</v>
+      </c>
+      <c r="J95" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="K95" s="14" t="s">
+        <v>197</v>
       </c>
       <c r="L95" s="15" t="s">
-        <v>418</v>
-      </c>
-      <c r="M95" s="13" t="s">
-        <v>477</v>
-      </c>
-      <c r="N95" s="16" t="s">
-        <v>153</v>
+        <v>1</v>
+      </c>
+      <c r="M95" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="N95" s="56" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="96" spans="1:14" ht="18">
-      <c r="A96" s="52" t="s">
-        <v>618</v>
+      <c r="A96" s="57" t="s">
+        <v>557</v>
       </c>
       <c r="B96" s="53" t="s">
-        <v>488</v>
-      </c>
-      <c r="C96" s="54" t="s">
-        <v>613</v>
+        <v>558</v>
+      </c>
+      <c r="C96" s="53" t="s">
+        <v>614</v>
       </c>
       <c r="D96" s="54" t="s">
         <v>753</v>
@@ -8364,12 +8394,12 @@
       <c r="F96" s="55" t="s">
         <v>483</v>
       </c>
-      <c r="G96" s="54" t="s">
+      <c r="G96" s="53" t="s">
         <v>554</v>
       </c>
-      <c r="H96" s="54"/>
-      <c r="I96" s="54" t="s">
-        <v>530</v>
+      <c r="H96" s="53"/>
+      <c r="I96" s="53" t="s">
+        <v>566</v>
       </c>
       <c r="J96" s="14" t="s">
         <v>197</v>
@@ -8383,19 +8413,19 @@
       <c r="M96" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="N96" s="56" t="s">
-        <v>491</v>
+      <c r="N96" s="16" t="s">
+        <v>565</v>
       </c>
     </row>
     <row r="97" spans="1:14" ht="18">
-      <c r="A97" s="57" t="s">
-        <v>557</v>
+      <c r="A97" s="52" t="s">
+        <v>619</v>
       </c>
       <c r="B97" s="53" t="s">
-        <v>558</v>
+        <v>490</v>
       </c>
       <c r="C97" s="53" t="s">
-        <v>614</v>
+        <v>675</v>
       </c>
       <c r="D97" s="54" t="s">
         <v>753</v>
@@ -8406,12 +8436,12 @@
       <c r="F97" s="55" t="s">
         <v>483</v>
       </c>
-      <c r="G97" s="53" t="s">
+      <c r="G97" s="54" t="s">
         <v>554</v>
       </c>
-      <c r="H97" s="53"/>
-      <c r="I97" s="53" t="s">
-        <v>566</v>
+      <c r="H97" s="54"/>
+      <c r="I97" s="54" t="s">
+        <v>531</v>
       </c>
       <c r="J97" s="14" t="s">
         <v>197</v>
@@ -8425,19 +8455,19 @@
       <c r="M97" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="N97" s="16" t="s">
-        <v>565</v>
+      <c r="N97" s="56" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="98" spans="1:14" ht="18">
-      <c r="A98" s="52" t="s">
-        <v>619</v>
+      <c r="A98" s="57" t="s">
+        <v>556</v>
       </c>
       <c r="B98" s="53" t="s">
-        <v>490</v>
+        <v>559</v>
       </c>
       <c r="C98" s="53" t="s">
-        <v>675</v>
+        <v>612</v>
       </c>
       <c r="D98" s="54" t="s">
         <v>753</v>
@@ -8448,12 +8478,12 @@
       <c r="F98" s="55" t="s">
         <v>483</v>
       </c>
-      <c r="G98" s="54" t="s">
+      <c r="G98" s="53" t="s">
         <v>554</v>
       </c>
-      <c r="H98" s="54"/>
-      <c r="I98" s="54" t="s">
-        <v>531</v>
+      <c r="H98" s="53"/>
+      <c r="I98" s="53" t="s">
+        <v>564</v>
       </c>
       <c r="J98" s="14" t="s">
         <v>197</v>
@@ -8467,19 +8497,19 @@
       <c r="M98" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="N98" s="56" t="s">
-        <v>492</v>
+      <c r="N98" s="16" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="99" spans="1:14" ht="18">
       <c r="A99" s="57" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B99" s="53" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="C99" s="53" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D99" s="54" t="s">
         <v>753</v>
@@ -8495,7 +8525,7 @@
       </c>
       <c r="H99" s="53"/>
       <c r="I99" s="53" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="J99" s="14" t="s">
         <v>197</v>
@@ -8510,18 +8540,18 @@
         <v>1</v>
       </c>
       <c r="N99" s="16" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="100" spans="1:14" ht="18">
-      <c r="A100" s="57" t="s">
-        <v>555</v>
+      <c r="A100" s="52" t="s">
+        <v>482</v>
       </c>
       <c r="B100" s="53" t="s">
-        <v>560</v>
-      </c>
-      <c r="C100" s="53" t="s">
-        <v>611</v>
+        <v>489</v>
+      </c>
+      <c r="C100" s="54" t="s">
+        <v>486</v>
       </c>
       <c r="D100" s="54" t="s">
         <v>753</v>
@@ -8532,12 +8562,12 @@
       <c r="F100" s="55" t="s">
         <v>483</v>
       </c>
-      <c r="G100" s="53" t="s">
-        <v>554</v>
-      </c>
-      <c r="H100" s="53"/>
-      <c r="I100" s="53" t="s">
-        <v>562</v>
+      <c r="G100" s="54" t="s">
+        <v>553</v>
+      </c>
+      <c r="H100" s="54"/>
+      <c r="I100" s="54" t="s">
+        <v>541</v>
       </c>
       <c r="J100" s="14" t="s">
         <v>197</v>
@@ -8551,19 +8581,19 @@
       <c r="M100" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="N100" s="16" t="s">
-        <v>561</v>
+      <c r="N100" s="56" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="101" spans="1:14" ht="18">
       <c r="A101" s="52" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
       <c r="B101" s="53" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="C101" s="54" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D101" s="54" t="s">
         <v>753</v>
@@ -8579,7 +8609,7 @@
       </c>
       <c r="H101" s="54"/>
       <c r="I101" s="54" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="J101" s="14" t="s">
         <v>197</v>
@@ -8594,18 +8624,18 @@
         <v>1</v>
       </c>
       <c r="N101" s="56" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="102" spans="1:14" ht="18">
       <c r="A102" s="52" t="s">
-        <v>487</v>
+        <v>634</v>
       </c>
       <c r="B102" s="53" t="s">
-        <v>484</v>
+        <v>635</v>
       </c>
       <c r="C102" s="54" t="s">
-        <v>485</v>
+        <v>637</v>
       </c>
       <c r="D102" s="54" t="s">
         <v>753</v>
@@ -8621,7 +8651,7 @@
       </c>
       <c r="H102" s="54"/>
       <c r="I102" s="54" t="s">
-        <v>539</v>
+        <v>636</v>
       </c>
       <c r="J102" s="14" t="s">
         <v>197</v>
@@ -8635,35 +8665,33 @@
       <c r="M102" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="N102" s="56" t="s">
-        <v>538</v>
-      </c>
+      <c r="N102" s="56"/>
     </row>
     <row r="103" spans="1:14" ht="18">
-      <c r="A103" s="52" t="s">
-        <v>634</v>
-      </c>
-      <c r="B103" s="53" t="s">
-        <v>635</v>
-      </c>
-      <c r="C103" s="54" t="s">
-        <v>637</v>
-      </c>
-      <c r="D103" s="54" t="s">
-        <v>753</v>
-      </c>
-      <c r="E103" s="55" t="s">
-        <v>674</v>
-      </c>
-      <c r="F103" s="55" t="s">
-        <v>483</v>
-      </c>
-      <c r="G103" s="54" t="s">
-        <v>553</v>
-      </c>
-      <c r="H103" s="54"/>
-      <c r="I103" s="54" t="s">
-        <v>636</v>
+      <c r="A103" s="58" t="s">
+        <v>218</v>
+      </c>
+      <c r="B103" s="59" t="s">
+        <v>94</v>
+      </c>
+      <c r="C103" s="60" t="s">
+        <v>335</v>
+      </c>
+      <c r="D103" s="60" t="s">
+        <v>753</v>
+      </c>
+      <c r="E103" s="60" t="s">
+        <v>674</v>
+      </c>
+      <c r="F103" s="60" t="s">
+        <v>325</v>
+      </c>
+      <c r="G103" s="60" t="s">
+        <v>545</v>
+      </c>
+      <c r="H103" s="60"/>
+      <c r="I103" s="60" t="s">
+        <v>522</v>
       </c>
       <c r="J103" s="14" t="s">
         <v>197</v>
@@ -8677,17 +8705,19 @@
       <c r="M103" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="N103" s="56"/>
+      <c r="N103" s="16" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="104" spans="1:14" ht="18">
       <c r="A104" s="58" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="B104" s="59" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="C104" s="60" t="s">
-        <v>335</v>
+        <v>349</v>
       </c>
       <c r="D104" s="60" t="s">
         <v>753</v>
@@ -8699,7 +8729,7 @@
         <v>325</v>
       </c>
       <c r="G104" s="60" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="H104" s="60"/>
       <c r="I104" s="60" t="s">
@@ -8712,10 +8742,10 @@
         <v>197</v>
       </c>
       <c r="L104" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M104" s="15" t="s">
-        <v>1</v>
+        <v>350</v>
+      </c>
+      <c r="M104" s="13" t="s">
+        <v>476</v>
       </c>
       <c r="N104" s="16" t="s">
         <v>136</v>
@@ -8723,13 +8753,13 @@
     </row>
     <row r="105" spans="1:14" ht="18">
       <c r="A105" s="58" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B105" s="59" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C105" s="60" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="D105" s="60" t="s">
         <v>753</v>
@@ -8741,11 +8771,11 @@
         <v>325</v>
       </c>
       <c r="G105" s="60" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="H105" s="60"/>
       <c r="I105" s="60" t="s">
-        <v>522</v>
+        <v>527</v>
       </c>
       <c r="J105" s="14" t="s">
         <v>197</v>
@@ -8754,24 +8784,24 @@
         <v>197</v>
       </c>
       <c r="L105" s="15" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="M105" s="13" t="s">
-        <v>476</v>
+        <v>1</v>
       </c>
       <c r="N105" s="16" t="s">
-        <v>136</v>
+        <v>494</v>
       </c>
     </row>
     <row r="106" spans="1:14" ht="18">
       <c r="A106" s="58" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="B106" s="59" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C106" s="60" t="s">
-        <v>351</v>
+        <v>596</v>
       </c>
       <c r="D106" s="60" t="s">
         <v>753</v>
@@ -8783,11 +8813,11 @@
         <v>325</v>
       </c>
       <c r="G106" s="60" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="H106" s="60"/>
       <c r="I106" s="60" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="J106" s="14" t="s">
         <v>197</v>
@@ -8796,24 +8826,24 @@
         <v>197</v>
       </c>
       <c r="L106" s="15" t="s">
-        <v>352</v>
+        <v>360</v>
       </c>
       <c r="M106" s="13" t="s">
         <v>1</v>
       </c>
       <c r="N106" s="16" t="s">
-        <v>494</v>
+        <v>212</v>
       </c>
     </row>
     <row r="107" spans="1:14" ht="18">
       <c r="A107" s="58" t="s">
-        <v>232</v>
+        <v>286</v>
       </c>
       <c r="B107" s="59" t="s">
-        <v>112</v>
+        <v>158</v>
       </c>
       <c r="C107" s="60" t="s">
-        <v>596</v>
+        <v>422</v>
       </c>
       <c r="D107" s="60" t="s">
         <v>753</v>
@@ -8825,11 +8855,11 @@
         <v>325</v>
       </c>
       <c r="G107" s="60" t="s">
-        <v>544</v>
+        <v>552</v>
       </c>
       <c r="H107" s="60"/>
       <c r="I107" s="60" t="s">
-        <v>521</v>
+        <v>529</v>
       </c>
       <c r="J107" s="14" t="s">
         <v>197</v>
@@ -8838,24 +8868,24 @@
         <v>197</v>
       </c>
       <c r="L107" s="15" t="s">
-        <v>360</v>
+        <v>1</v>
       </c>
       <c r="M107" s="13" t="s">
-        <v>1</v>
+        <v>476</v>
       </c>
       <c r="N107" s="16" t="s">
-        <v>212</v>
+        <v>493</v>
       </c>
     </row>
     <row r="108" spans="1:14" ht="18">
       <c r="A108" s="58" t="s">
-        <v>286</v>
+        <v>258</v>
       </c>
       <c r="B108" s="59" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="C108" s="60" t="s">
-        <v>422</v>
+        <v>597</v>
       </c>
       <c r="D108" s="60" t="s">
         <v>753</v>
@@ -8867,11 +8897,11 @@
         <v>325</v>
       </c>
       <c r="G108" s="60" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="H108" s="60"/>
       <c r="I108" s="60" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="J108" s="14" t="s">
         <v>197</v>
@@ -8880,24 +8910,24 @@
         <v>197</v>
       </c>
       <c r="L108" s="15" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="M108" s="13" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="N108" s="16" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="109" spans="1:14" ht="18">
       <c r="A109" s="58" t="s">
-        <v>258</v>
+        <v>231</v>
       </c>
       <c r="B109" s="59" t="s">
-        <v>151</v>
+        <v>198</v>
       </c>
       <c r="C109" s="60" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
       <c r="D109" s="60" t="s">
         <v>753</v>
@@ -8909,11 +8939,11 @@
         <v>325</v>
       </c>
       <c r="G109" s="60" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="H109" s="60"/>
       <c r="I109" s="60" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="J109" s="14" t="s">
         <v>197</v>
@@ -8922,24 +8952,24 @@
         <v>197</v>
       </c>
       <c r="L109" s="15" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="M109" s="13" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="N109" s="16" t="s">
-        <v>494</v>
+        <v>111</v>
       </c>
     </row>
     <row r="110" spans="1:14" ht="18">
       <c r="A110" s="58" t="s">
-        <v>231</v>
+        <v>250</v>
       </c>
       <c r="B110" s="59" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C110" s="60" t="s">
-        <v>600</v>
+        <v>409</v>
       </c>
       <c r="D110" s="60" t="s">
         <v>753</v>
@@ -8951,11 +8981,11 @@
         <v>325</v>
       </c>
       <c r="G110" s="60" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="H110" s="60"/>
       <c r="I110" s="60" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="J110" s="14" t="s">
         <v>197</v>
@@ -8964,24 +8994,24 @@
         <v>197</v>
       </c>
       <c r="L110" s="15" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="M110" s="13" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="N110" s="16" t="s">
-        <v>111</v>
+        <v>136</v>
       </c>
     </row>
     <row r="111" spans="1:14" ht="18">
       <c r="A111" s="58" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B111" s="59" t="s">
-        <v>201</v>
+        <v>143</v>
       </c>
       <c r="C111" s="60" t="s">
-        <v>409</v>
+        <v>598</v>
       </c>
       <c r="D111" s="60" t="s">
         <v>753</v>
@@ -8993,11 +9023,11 @@
         <v>325</v>
       </c>
       <c r="G111" s="60" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="H111" s="60"/>
       <c r="I111" s="60" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="J111" s="14" t="s">
         <v>197</v>
@@ -9012,18 +9042,18 @@
         <v>475</v>
       </c>
       <c r="N111" s="16" t="s">
-        <v>136</v>
+        <v>212</v>
       </c>
     </row>
     <row r="112" spans="1:14" ht="18">
       <c r="A112" s="58" t="s">
-        <v>253</v>
-      </c>
-      <c r="B112" s="59" t="s">
-        <v>143</v>
+        <v>265</v>
+      </c>
+      <c r="B112" s="60" t="s">
+        <v>168</v>
       </c>
       <c r="C112" s="60" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="D112" s="60" t="s">
         <v>753</v>
@@ -9035,11 +9065,11 @@
         <v>325</v>
       </c>
       <c r="G112" s="60" t="s">
-        <v>550</v>
+        <v>658</v>
       </c>
       <c r="H112" s="60"/>
       <c r="I112" s="60" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="J112" s="14" t="s">
         <v>197</v>
@@ -9048,24 +9078,24 @@
         <v>197</v>
       </c>
       <c r="L112" s="15" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="M112" s="13" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="N112" s="16" t="s">
-        <v>212</v>
+        <v>166</v>
       </c>
     </row>
     <row r="113" spans="1:14" ht="18">
       <c r="A113" s="58" t="s">
-        <v>265</v>
+        <v>659</v>
       </c>
       <c r="B113" s="60" t="s">
-        <v>168</v>
+        <v>660</v>
       </c>
       <c r="C113" s="60" t="s">
-        <v>599</v>
+        <v>661</v>
       </c>
       <c r="D113" s="60" t="s">
         <v>753</v>
@@ -9077,11 +9107,11 @@
         <v>325</v>
       </c>
       <c r="G113" s="60" t="s">
-        <v>658</v>
+        <v>662</v>
       </c>
       <c r="H113" s="60"/>
       <c r="I113" s="60" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="J113" s="14" t="s">
         <v>197</v>
@@ -9090,24 +9120,24 @@
         <v>197</v>
       </c>
       <c r="L113" s="15" t="s">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="M113" s="13" t="s">
-        <v>476</v>
+        <v>1</v>
       </c>
       <c r="N113" s="16" t="s">
-        <v>166</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:14" ht="18">
       <c r="A114" s="58" t="s">
-        <v>659</v>
+        <v>671</v>
       </c>
       <c r="B114" s="60" t="s">
-        <v>660</v>
+        <v>638</v>
       </c>
       <c r="C114" s="60" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="D114" s="60" t="s">
         <v>753</v>
@@ -9118,12 +9148,10 @@
       <c r="F114" s="60" t="s">
         <v>325</v>
       </c>
-      <c r="G114" s="60" t="s">
-        <v>662</v>
-      </c>
+      <c r="G114" s="60"/>
       <c r="H114" s="60"/>
       <c r="I114" s="60" t="s">
-        <v>527</v>
+        <v>629</v>
       </c>
       <c r="J114" s="14" t="s">
         <v>197</v>
@@ -9142,28 +9170,30 @@
       </c>
     </row>
     <row r="115" spans="1:14" ht="18">
-      <c r="A115" s="58" t="s">
-        <v>671</v>
-      </c>
-      <c r="B115" s="60" t="s">
-        <v>638</v>
-      </c>
-      <c r="C115" s="60" t="s">
-        <v>663</v>
-      </c>
-      <c r="D115" s="60" t="s">
-        <v>753</v>
-      </c>
-      <c r="E115" s="60" t="s">
-        <v>674</v>
-      </c>
-      <c r="F115" s="60" t="s">
-        <v>325</v>
-      </c>
-      <c r="G115" s="60"/>
-      <c r="H115" s="60"/>
-      <c r="I115" s="60" t="s">
-        <v>629</v>
+      <c r="A115" s="47" t="s">
+        <v>497</v>
+      </c>
+      <c r="B115" s="48" t="s">
+        <v>502</v>
+      </c>
+      <c r="C115" s="48" t="s">
+        <v>609</v>
+      </c>
+      <c r="D115" s="48" t="s">
+        <v>753</v>
+      </c>
+      <c r="E115" s="48" t="s">
+        <v>674</v>
+      </c>
+      <c r="F115" s="48" t="s">
+        <v>621</v>
+      </c>
+      <c r="G115" s="48" t="s">
+        <v>366</v>
+      </c>
+      <c r="H115" s="48"/>
+      <c r="I115" s="48" t="s">
+        <v>518</v>
       </c>
       <c r="J115" s="14" t="s">
         <v>197</v>
@@ -9178,18 +9208,18 @@
         <v>1</v>
       </c>
       <c r="N115" s="16" t="s">
-        <v>1</v>
+        <v>503</v>
       </c>
     </row>
     <row r="116" spans="1:14" ht="18">
       <c r="A116" s="47" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B116" s="48" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="C116" s="48" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="D116" s="48" t="s">
         <v>753</v>
@@ -9205,7 +9235,7 @@
       </c>
       <c r="H116" s="48"/>
       <c r="I116" s="48" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="J116" s="14" t="s">
         <v>197</v>
@@ -9220,18 +9250,18 @@
         <v>1</v>
       </c>
       <c r="N116" s="16" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="117" spans="1:14" ht="18">
       <c r="A117" s="47" t="s">
-        <v>495</v>
+        <v>235</v>
       </c>
       <c r="B117" s="48" t="s">
-        <v>498</v>
+        <v>115</v>
       </c>
       <c r="C117" s="48" t="s">
-        <v>610</v>
+        <v>366</v>
       </c>
       <c r="D117" s="48" t="s">
         <v>753</v>
@@ -9247,7 +9277,7 @@
       </c>
       <c r="H117" s="48"/>
       <c r="I117" s="48" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="J117" s="14" t="s">
         <v>197</v>
@@ -9256,24 +9286,24 @@
         <v>197</v>
       </c>
       <c r="L117" s="15" t="s">
-        <v>1</v>
+        <v>367</v>
       </c>
       <c r="M117" s="13" t="s">
-        <v>1</v>
+        <v>476</v>
       </c>
       <c r="N117" s="16" t="s">
-        <v>501</v>
+        <v>116</v>
       </c>
     </row>
     <row r="118" spans="1:14" ht="18">
       <c r="A118" s="47" t="s">
-        <v>235</v>
+        <v>496</v>
       </c>
       <c r="B118" s="48" t="s">
-        <v>115</v>
+        <v>499</v>
       </c>
       <c r="C118" s="48" t="s">
-        <v>366</v>
+        <v>610</v>
       </c>
       <c r="D118" s="48" t="s">
         <v>753</v>
@@ -9289,7 +9319,7 @@
       </c>
       <c r="H118" s="48"/>
       <c r="I118" s="48" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="J118" s="14" t="s">
         <v>197</v>
@@ -9298,40 +9328,40 @@
         <v>197</v>
       </c>
       <c r="L118" s="15" t="s">
-        <v>367</v>
+        <v>1</v>
       </c>
       <c r="M118" s="13" t="s">
-        <v>476</v>
+        <v>1</v>
       </c>
       <c r="N118" s="16" t="s">
-        <v>116</v>
+        <v>500</v>
       </c>
     </row>
     <row r="119" spans="1:14" ht="18">
-      <c r="A119" s="47" t="s">
-        <v>496</v>
-      </c>
-      <c r="B119" s="48" t="s">
-        <v>499</v>
-      </c>
-      <c r="C119" s="48" t="s">
-        <v>610</v>
-      </c>
-      <c r="D119" s="48" t="s">
-        <v>753</v>
-      </c>
-      <c r="E119" s="48" t="s">
-        <v>674</v>
-      </c>
-      <c r="F119" s="48" t="s">
-        <v>621</v>
-      </c>
-      <c r="G119" s="48" t="s">
-        <v>366</v>
-      </c>
-      <c r="H119" s="48"/>
-      <c r="I119" s="48" t="s">
-        <v>517</v>
+      <c r="A119" s="27" t="s">
+        <v>236</v>
+      </c>
+      <c r="B119" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="C119" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="D119" s="26" t="s">
+        <v>753</v>
+      </c>
+      <c r="E119" s="26" t="s">
+        <v>764</v>
+      </c>
+      <c r="F119" s="26" t="s">
+        <v>368</v>
+      </c>
+      <c r="G119" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="H119" s="26"/>
+      <c r="I119" s="26" t="s">
+        <v>625</v>
       </c>
       <c r="J119" s="14" t="s">
         <v>197</v>
@@ -9340,40 +9370,36 @@
         <v>197</v>
       </c>
       <c r="L119" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M119" s="13" t="s">
-        <v>1</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="M119" s="13"/>
       <c r="N119" s="16" t="s">
-        <v>500</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:14" ht="18">
       <c r="A120" s="27" t="s">
-        <v>236</v>
+        <v>270</v>
       </c>
       <c r="B120" s="28" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="C120" s="26" t="s">
-        <v>207</v>
+        <v>592</v>
       </c>
       <c r="D120" s="26" t="s">
         <v>753</v>
       </c>
       <c r="E120" s="26" t="s">
-        <v>368</v>
+        <v>764</v>
       </c>
       <c r="F120" s="26" t="s">
         <v>368</v>
       </c>
-      <c r="G120" s="26" t="s">
-        <v>208</v>
-      </c>
+      <c r="G120" s="26"/>
       <c r="H120" s="26"/>
       <c r="I120" s="26" t="s">
-        <v>625</v>
+        <v>522</v>
       </c>
       <c r="J120" s="14" t="s">
         <v>197</v>
@@ -9382,28 +9408,30 @@
         <v>197</v>
       </c>
       <c r="L120" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="M120" s="13"/>
+        <v>47</v>
+      </c>
+      <c r="M120" s="13" t="s">
+        <v>478</v>
+      </c>
       <c r="N120" s="16" t="s">
-        <v>1</v>
+        <v>136</v>
       </c>
     </row>
     <row r="121" spans="1:14" ht="18">
       <c r="A121" s="27" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="B121" s="28" t="s">
-        <v>175</v>
+        <v>616</v>
       </c>
       <c r="C121" s="26" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="D121" s="26" t="s">
         <v>753</v>
       </c>
       <c r="E121" s="26" t="s">
-        <v>368</v>
+        <v>764</v>
       </c>
       <c r="F121" s="26" t="s">
         <v>368</v>
@@ -9411,7 +9439,7 @@
       <c r="G121" s="26"/>
       <c r="H121" s="26"/>
       <c r="I121" s="26" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="J121" s="14" t="s">
         <v>197</v>
@@ -9420,30 +9448,30 @@
         <v>197</v>
       </c>
       <c r="L121" s="15" t="s">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="M121" s="13" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="N121" s="16" t="s">
-        <v>136</v>
+        <v>164</v>
       </c>
     </row>
     <row r="122" spans="1:14" ht="18">
       <c r="A122" s="27" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B122" s="28" t="s">
-        <v>616</v>
+        <v>165</v>
       </c>
       <c r="C122" s="26" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="D122" s="26" t="s">
         <v>753</v>
       </c>
       <c r="E122" s="26" t="s">
-        <v>368</v>
+        <v>764</v>
       </c>
       <c r="F122" s="26" t="s">
         <v>368</v>
@@ -9451,7 +9479,7 @@
       <c r="G122" s="26"/>
       <c r="H122" s="26"/>
       <c r="I122" s="26" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="J122" s="14" t="s">
         <v>197</v>
@@ -9460,30 +9488,30 @@
         <v>197</v>
       </c>
       <c r="L122" s="15" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="M122" s="13" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="N122" s="16" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="123" spans="1:14" ht="18">
       <c r="A123" s="27" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B123" s="28" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C123" s="26" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="D123" s="26" t="s">
         <v>753</v>
       </c>
       <c r="E123" s="26" t="s">
-        <v>368</v>
+        <v>764</v>
       </c>
       <c r="F123" s="26" t="s">
         <v>368</v>
@@ -9500,7 +9528,7 @@
         <v>197</v>
       </c>
       <c r="L123" s="15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M123" s="13" t="s">
         <v>476</v>
@@ -9511,19 +9539,19 @@
     </row>
     <row r="124" spans="1:14" ht="18">
       <c r="A124" s="27" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="B124" s="28" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="C124" s="26" t="s">
-        <v>595</v>
+        <v>32</v>
       </c>
       <c r="D124" s="26" t="s">
         <v>753</v>
       </c>
       <c r="E124" s="26" t="s">
-        <v>368</v>
+        <v>764</v>
       </c>
       <c r="F124" s="26" t="s">
         <v>368</v>
@@ -9531,7 +9559,7 @@
       <c r="G124" s="26"/>
       <c r="H124" s="26"/>
       <c r="I124" s="26" t="s">
-        <v>524</v>
+        <v>512</v>
       </c>
       <c r="J124" s="14" t="s">
         <v>197</v>
@@ -9540,38 +9568,38 @@
         <v>197</v>
       </c>
       <c r="L124" s="15" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="M124" s="13" t="s">
         <v>476</v>
       </c>
       <c r="N124" s="16" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
     </row>
     <row r="125" spans="1:14" ht="18">
       <c r="A125" s="27" t="s">
-        <v>256</v>
+        <v>682</v>
       </c>
       <c r="B125" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="C125" s="26" t="s">
-        <v>32</v>
+      <c r="C125" s="28" t="s">
+        <v>676</v>
       </c>
       <c r="D125" s="26" t="s">
         <v>753</v>
       </c>
       <c r="E125" s="26" t="s">
+        <v>764</v>
+      </c>
+      <c r="F125" s="28" t="s">
         <v>368</v>
       </c>
-      <c r="F125" s="26" t="s">
-        <v>368</v>
-      </c>
-      <c r="G125" s="26"/>
-      <c r="H125" s="26"/>
-      <c r="I125" s="26" t="s">
-        <v>512</v>
+      <c r="G125" s="28"/>
+      <c r="H125" s="28"/>
+      <c r="I125" s="28" t="s">
+        <v>729</v>
       </c>
       <c r="J125" s="14" t="s">
         <v>197</v>
@@ -9579,31 +9607,28 @@
       <c r="K125" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="L125" s="15" t="s">
-        <v>32</v>
+      <c r="L125" s="64" t="s">
+        <v>728</v>
       </c>
       <c r="M125" s="13" t="s">
-        <v>476</v>
-      </c>
-      <c r="N125" s="16" t="s">
-        <v>148</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126" spans="1:14" ht="18">
       <c r="A126" s="27" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="B126" s="28" t="s">
-        <v>147</v>
+        <v>726</v>
       </c>
       <c r="C126" s="28" t="s">
-        <v>676</v>
+        <v>754</v>
       </c>
       <c r="D126" s="26" t="s">
         <v>753</v>
       </c>
       <c r="E126" s="26" t="s">
-        <v>368</v>
+        <v>764</v>
       </c>
       <c r="F126" s="28" t="s">
         <v>368</v>
@@ -9611,7 +9636,7 @@
       <c r="G126" s="28"/>
       <c r="H126" s="28"/>
       <c r="I126" s="28" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="J126" s="14" t="s">
         <v>197</v>
@@ -9619,8 +9644,8 @@
       <c r="K126" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="L126" s="65" t="s">
-        <v>728</v>
+      <c r="L126" s="64" t="s">
+        <v>727</v>
       </c>
       <c r="M126" s="13" t="s">
         <v>1</v>
@@ -9628,19 +9653,19 @@
     </row>
     <row r="127" spans="1:14" ht="18">
       <c r="A127" s="27" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="B127" s="28" t="s">
-        <v>726</v>
+        <v>713</v>
       </c>
       <c r="C127" s="28" t="s">
-        <v>754</v>
+        <v>762</v>
       </c>
       <c r="D127" s="26" t="s">
         <v>753</v>
       </c>
       <c r="E127" s="26" t="s">
-        <v>368</v>
+        <v>764</v>
       </c>
       <c r="F127" s="28" t="s">
         <v>368</v>
@@ -9648,7 +9673,7 @@
       <c r="G127" s="28"/>
       <c r="H127" s="28"/>
       <c r="I127" s="28" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="J127" s="14" t="s">
         <v>197</v>
@@ -9656,8 +9681,8 @@
       <c r="K127" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="L127" s="65" t="s">
-        <v>727</v>
+      <c r="L127" s="64" t="s">
+        <v>732</v>
       </c>
       <c r="M127" s="13" t="s">
         <v>1</v>
@@ -9665,19 +9690,19 @@
     </row>
     <row r="128" spans="1:14" ht="18">
       <c r="A128" s="27" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="B128" s="28" t="s">
-        <v>713</v>
+        <v>733</v>
       </c>
       <c r="C128" s="28" t="s">
-        <v>762</v>
+        <v>755</v>
       </c>
       <c r="D128" s="26" t="s">
         <v>753</v>
       </c>
       <c r="E128" s="26" t="s">
-        <v>368</v>
+        <v>764</v>
       </c>
       <c r="F128" s="28" t="s">
         <v>368</v>
@@ -9685,7 +9710,7 @@
       <c r="G128" s="28"/>
       <c r="H128" s="28"/>
       <c r="I128" s="28" t="s">
-        <v>731</v>
+        <v>714</v>
       </c>
       <c r="J128" s="14" t="s">
         <v>197</v>
@@ -9693,8 +9718,8 @@
       <c r="K128" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="L128" s="65" t="s">
-        <v>732</v>
+      <c r="L128" s="64" t="s">
+        <v>1</v>
       </c>
       <c r="M128" s="13" t="s">
         <v>1</v>
@@ -9702,19 +9727,19 @@
     </row>
     <row r="129" spans="1:14" ht="18">
       <c r="A129" s="27" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="B129" s="28" t="s">
-        <v>733</v>
+        <v>715</v>
       </c>
       <c r="C129" s="28" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="D129" s="26" t="s">
         <v>753</v>
       </c>
       <c r="E129" s="26" t="s">
-        <v>368</v>
+        <v>764</v>
       </c>
       <c r="F129" s="28" t="s">
         <v>368</v>
@@ -9722,7 +9747,7 @@
       <c r="G129" s="28"/>
       <c r="H129" s="28"/>
       <c r="I129" s="28" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="J129" s="14" t="s">
         <v>197</v>
@@ -9730,8 +9755,8 @@
       <c r="K129" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="L129" s="65" t="s">
-        <v>1</v>
+      <c r="L129" s="64" t="s">
+        <v>734</v>
       </c>
       <c r="M129" s="13" t="s">
         <v>1</v>
@@ -9739,19 +9764,19 @@
     </row>
     <row r="130" spans="1:14" ht="18">
       <c r="A130" s="27" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="B130" s="28" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="C130" s="28" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="D130" s="26" t="s">
         <v>753</v>
       </c>
       <c r="E130" s="26" t="s">
-        <v>368</v>
+        <v>764</v>
       </c>
       <c r="F130" s="28" t="s">
         <v>368</v>
@@ -9759,7 +9784,7 @@
       <c r="G130" s="28"/>
       <c r="H130" s="28"/>
       <c r="I130" s="28" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="J130" s="14" t="s">
         <v>197</v>
@@ -9767,8 +9792,8 @@
       <c r="K130" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="L130" s="65" t="s">
-        <v>734</v>
+      <c r="L130" s="64" t="s">
+        <v>735</v>
       </c>
       <c r="M130" s="13" t="s">
         <v>1</v>
@@ -9776,19 +9801,19 @@
     </row>
     <row r="131" spans="1:14" ht="18">
       <c r="A131" s="27" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="B131" s="28" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="C131" s="28" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="D131" s="26" t="s">
         <v>753</v>
       </c>
       <c r="E131" s="26" t="s">
-        <v>368</v>
+        <v>764</v>
       </c>
       <c r="F131" s="28" t="s">
         <v>368</v>
@@ -9796,7 +9821,7 @@
       <c r="G131" s="28"/>
       <c r="H131" s="28"/>
       <c r="I131" s="28" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="J131" s="14" t="s">
         <v>197</v>
@@ -9804,8 +9829,8 @@
       <c r="K131" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="L131" s="65" t="s">
-        <v>735</v>
+      <c r="L131" s="64" t="s">
+        <v>736</v>
       </c>
       <c r="M131" s="13" t="s">
         <v>1</v>
@@ -9813,19 +9838,19 @@
     </row>
     <row r="132" spans="1:14" ht="18">
       <c r="A132" s="27" t="s">
-        <v>688</v>
+        <v>691</v>
       </c>
       <c r="B132" s="28" t="s">
-        <v>719</v>
+        <v>724</v>
       </c>
       <c r="C132" s="28" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="D132" s="26" t="s">
         <v>753</v>
       </c>
       <c r="E132" s="26" t="s">
-        <v>368</v>
+        <v>764</v>
       </c>
       <c r="F132" s="28" t="s">
         <v>368</v>
@@ -9833,7 +9858,7 @@
       <c r="G132" s="28"/>
       <c r="H132" s="28"/>
       <c r="I132" s="28" t="s">
-        <v>720</v>
+        <v>750</v>
       </c>
       <c r="J132" s="14" t="s">
         <v>197</v>
@@ -9841,8 +9866,8 @@
       <c r="K132" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="L132" s="65" t="s">
-        <v>736</v>
+      <c r="L132" s="64" t="s">
+        <v>725</v>
       </c>
       <c r="M132" s="13" t="s">
         <v>1</v>
@@ -9850,256 +9875,259 @@
     </row>
     <row r="133" spans="1:14" ht="18">
       <c r="A133" s="27" t="s">
-        <v>691</v>
+        <v>254</v>
       </c>
       <c r="B133" s="28" t="s">
-        <v>724</v>
+        <v>144</v>
       </c>
       <c r="C133" s="28" t="s">
-        <v>759</v>
+        <v>604</v>
       </c>
       <c r="D133" s="26" t="s">
         <v>753</v>
       </c>
       <c r="E133" s="26" t="s">
-        <v>368</v>
-      </c>
-      <c r="F133" s="28" t="s">
-        <v>368</v>
-      </c>
-      <c r="G133" s="28"/>
-      <c r="H133" s="28"/>
-      <c r="I133" s="28" t="s">
-        <v>750</v>
-      </c>
-      <c r="J133" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="K133" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="L133" s="65" t="s">
-        <v>725</v>
-      </c>
-      <c r="M133" s="13" t="s">
-        <v>1</v>
+        <v>764</v>
+      </c>
+      <c r="F133" s="61" t="s">
+        <v>416</v>
+      </c>
+      <c r="G133" s="61"/>
+      <c r="H133" s="61"/>
+      <c r="I133" s="61" t="s">
+        <v>523</v>
+      </c>
+      <c r="J133" s="61" t="s">
+        <v>197</v>
+      </c>
+      <c r="K133" s="61" t="s">
+        <v>197</v>
+      </c>
+      <c r="L133" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="M133" s="61" t="s">
+        <v>476</v>
+      </c>
+      <c r="N133" s="16" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="134" spans="1:14" ht="18">
-      <c r="A134" s="61" t="s">
-        <v>254</v>
-      </c>
-      <c r="B134" s="39" t="s">
-        <v>144</v>
-      </c>
-      <c r="C134" s="62" t="s">
-        <v>604</v>
-      </c>
-      <c r="D134" s="62" t="s">
-        <v>753</v>
-      </c>
-      <c r="E134" s="62" t="s">
+      <c r="A134" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="B134" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="C134" s="28" t="s">
+        <v>346</v>
+      </c>
+      <c r="D134" s="26" t="s">
+        <v>753</v>
+      </c>
+      <c r="E134" s="26" t="s">
+        <v>764</v>
+      </c>
+      <c r="F134" s="39" t="s">
         <v>416</v>
       </c>
-      <c r="F134" s="62" t="s">
+      <c r="G134" s="61"/>
+      <c r="H134" s="61"/>
+      <c r="I134" s="61" t="s">
+        <v>588</v>
+      </c>
+      <c r="J134" s="61" t="s">
+        <v>197</v>
+      </c>
+      <c r="K134" s="61" t="s">
+        <v>197</v>
+      </c>
+      <c r="L134" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="M134" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="N134" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:14" ht="18">
+      <c r="A135" s="27" t="s">
+        <v>287</v>
+      </c>
+      <c r="B135" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="C135" s="28" t="s">
+        <v>437</v>
+      </c>
+      <c r="D135" s="26" t="s">
+        <v>753</v>
+      </c>
+      <c r="E135" s="26" t="s">
+        <v>764</v>
+      </c>
+      <c r="F135" s="61" t="s">
         <v>416</v>
       </c>
-      <c r="G134" s="62"/>
-      <c r="H134" s="62"/>
-      <c r="I134" s="62" t="s">
-        <v>523</v>
-      </c>
-      <c r="J134" s="62" t="s">
-        <v>197</v>
-      </c>
-      <c r="K134" s="62" t="s">
-        <v>197</v>
-      </c>
-      <c r="L134" s="62" t="s">
-        <v>30</v>
-      </c>
-      <c r="M134" s="62" t="s">
+      <c r="G135" s="61"/>
+      <c r="H135" s="61"/>
+      <c r="I135" s="61" t="s">
+        <v>588</v>
+      </c>
+      <c r="J135" s="61" t="s">
+        <v>197</v>
+      </c>
+      <c r="K135" s="61" t="s">
+        <v>197</v>
+      </c>
+      <c r="L135" s="61" t="s">
+        <v>51</v>
+      </c>
+      <c r="M135" s="61" t="s">
         <v>476</v>
       </c>
-      <c r="N134" s="16" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="135" spans="1:14" ht="18">
-      <c r="A135" s="61" t="s">
-        <v>221</v>
-      </c>
-      <c r="B135" s="39" t="s">
-        <v>101</v>
-      </c>
-      <c r="C135" s="62" t="s">
-        <v>346</v>
-      </c>
-      <c r="D135" s="62" t="s">
-        <v>753</v>
-      </c>
-      <c r="E135" s="39" t="s">
+      <c r="N135" s="16" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="136" spans="1:14" ht="18">
+      <c r="A136" s="27" t="s">
+        <v>266</v>
+      </c>
+      <c r="B136" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="C136" s="28" t="s">
+        <v>603</v>
+      </c>
+      <c r="D136" s="26" t="s">
+        <v>753</v>
+      </c>
+      <c r="E136" s="26" t="s">
+        <v>764</v>
+      </c>
+      <c r="F136" s="39" t="s">
         <v>416</v>
       </c>
-      <c r="F135" s="39" t="s">
-        <v>416</v>
-      </c>
-      <c r="G135" s="62"/>
-      <c r="H135" s="62"/>
-      <c r="I135" s="62" t="s">
-        <v>588</v>
-      </c>
-      <c r="J135" s="62" t="s">
-        <v>197</v>
-      </c>
-      <c r="K135" s="62" t="s">
-        <v>197</v>
-      </c>
-      <c r="L135" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="M135" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="N135" s="16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="136" spans="1:14" ht="18">
-      <c r="A136" s="61" t="s">
-        <v>287</v>
-      </c>
-      <c r="B136" s="39" t="s">
-        <v>180</v>
-      </c>
-      <c r="C136" s="62" t="s">
-        <v>437</v>
-      </c>
-      <c r="D136" s="62" t="s">
-        <v>753</v>
-      </c>
-      <c r="E136" s="62" t="s">
-        <v>416</v>
-      </c>
-      <c r="F136" s="62" t="s">
-        <v>416</v>
-      </c>
-      <c r="G136" s="62"/>
-      <c r="H136" s="62"/>
-      <c r="I136" s="62" t="s">
-        <v>588</v>
-      </c>
-      <c r="J136" s="62" t="s">
-        <v>197</v>
-      </c>
-      <c r="K136" s="62" t="s">
-        <v>197</v>
-      </c>
-      <c r="L136" s="62" t="s">
-        <v>51</v>
-      </c>
-      <c r="M136" s="62" t="s">
+      <c r="G136" s="61"/>
+      <c r="H136" s="61"/>
+      <c r="I136" s="61" t="s">
+        <v>524</v>
+      </c>
+      <c r="J136" s="61" t="s">
+        <v>197</v>
+      </c>
+      <c r="K136" s="61" t="s">
+        <v>197</v>
+      </c>
+      <c r="L136" s="61" t="s">
+        <v>46</v>
+      </c>
+      <c r="M136" s="61" t="s">
         <v>476</v>
       </c>
       <c r="N136" s="16" t="s">
-        <v>119</v>
+        <v>166</v>
       </c>
     </row>
     <row r="137" spans="1:14" ht="18">
-      <c r="A137" s="61" t="s">
-        <v>266</v>
-      </c>
-      <c r="B137" s="39" t="s">
-        <v>169</v>
-      </c>
-      <c r="C137" s="62" t="s">
-        <v>603</v>
-      </c>
-      <c r="D137" s="62" t="s">
-        <v>753</v>
-      </c>
-      <c r="E137" s="39" t="s">
-        <v>416</v>
+      <c r="A137" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="B137" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="C137" s="28" t="s">
+        <v>348</v>
+      </c>
+      <c r="D137" s="26" t="s">
+        <v>753</v>
+      </c>
+      <c r="E137" s="26" t="s">
+        <v>764</v>
       </c>
       <c r="F137" s="39" t="s">
         <v>416</v>
       </c>
-      <c r="G137" s="62"/>
-      <c r="H137" s="62"/>
-      <c r="I137" s="62" t="s">
-        <v>524</v>
-      </c>
-      <c r="J137" s="62" t="s">
-        <v>197</v>
-      </c>
-      <c r="K137" s="62" t="s">
-        <v>197</v>
-      </c>
-      <c r="L137" s="62" t="s">
-        <v>46</v>
-      </c>
-      <c r="M137" s="62" t="s">
-        <v>476</v>
+      <c r="G137" s="61"/>
+      <c r="H137" s="61"/>
+      <c r="I137" s="61" t="s">
+        <v>588</v>
+      </c>
+      <c r="J137" s="61" t="s">
+        <v>197</v>
+      </c>
+      <c r="K137" s="61" t="s">
+        <v>197</v>
+      </c>
+      <c r="L137" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="M137" s="61" t="s">
+        <v>1</v>
       </c>
       <c r="N137" s="16" t="s">
-        <v>166</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:14" ht="18">
-      <c r="A138" s="61" t="s">
-        <v>223</v>
-      </c>
-      <c r="B138" s="39" t="s">
-        <v>103</v>
-      </c>
-      <c r="C138" s="62" t="s">
-        <v>348</v>
-      </c>
-      <c r="D138" s="62" t="s">
-        <v>753</v>
-      </c>
-      <c r="E138" s="39" t="s">
-        <v>416</v>
+      <c r="A138" s="27" t="s">
+        <v>257</v>
+      </c>
+      <c r="B138" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="C138" s="28" t="s">
+        <v>602</v>
+      </c>
+      <c r="D138" s="26" t="s">
+        <v>753</v>
+      </c>
+      <c r="E138" s="26" t="s">
+        <v>764</v>
       </c>
       <c r="F138" s="39" t="s">
         <v>416</v>
       </c>
-      <c r="G138" s="62"/>
-      <c r="H138" s="62"/>
-      <c r="I138" s="62" t="s">
-        <v>588</v>
-      </c>
-      <c r="J138" s="62" t="s">
-        <v>197</v>
-      </c>
-      <c r="K138" s="62" t="s">
-        <v>197</v>
-      </c>
-      <c r="L138" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="M138" s="62" t="s">
-        <v>1</v>
+      <c r="G138" s="39"/>
+      <c r="H138" s="39"/>
+      <c r="I138" s="39" t="s">
+        <v>525</v>
+      </c>
+      <c r="J138" s="39" t="s">
+        <v>197</v>
+      </c>
+      <c r="K138" s="39" t="s">
+        <v>197</v>
+      </c>
+      <c r="L138" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M138" s="61" t="s">
+        <v>476</v>
       </c>
       <c r="N138" s="16" t="s">
-        <v>1</v>
+        <v>150</v>
       </c>
     </row>
     <row r="139" spans="1:14" ht="18">
-      <c r="A139" s="61" t="s">
-        <v>257</v>
-      </c>
-      <c r="B139" s="39" t="s">
-        <v>149</v>
-      </c>
-      <c r="C139" s="39" t="s">
-        <v>602</v>
-      </c>
-      <c r="D139" s="62" t="s">
-        <v>753</v>
-      </c>
-      <c r="E139" s="39" t="s">
-        <v>416</v>
+      <c r="A139" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="B139" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="C139" s="28" t="s">
+        <v>601</v>
+      </c>
+      <c r="D139" s="26" t="s">
+        <v>753</v>
+      </c>
+      <c r="E139" s="26" t="s">
+        <v>764</v>
       </c>
       <c r="F139" s="39" t="s">
         <v>416</v>
@@ -10107,7 +10135,7 @@
       <c r="G139" s="39"/>
       <c r="H139" s="39"/>
       <c r="I139" s="39" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="J139" s="39" t="s">
         <v>197</v>
@@ -10115,31 +10143,31 @@
       <c r="K139" s="39" t="s">
         <v>197</v>
       </c>
-      <c r="L139" s="62" t="s">
-        <v>33</v>
-      </c>
-      <c r="M139" s="62" t="s">
-        <v>476</v>
+      <c r="L139" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="M139" s="61" t="s">
+        <v>478</v>
       </c>
       <c r="N139" s="16" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
     </row>
     <row r="140" spans="1:14" ht="18">
-      <c r="A140" s="61" t="s">
-        <v>261</v>
-      </c>
-      <c r="B140" s="39" t="s">
-        <v>161</v>
-      </c>
-      <c r="C140" s="39" t="s">
-        <v>601</v>
-      </c>
-      <c r="D140" s="62" t="s">
-        <v>753</v>
-      </c>
-      <c r="E140" s="39" t="s">
-        <v>416</v>
+      <c r="A140" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="B140" s="28" t="s">
+        <v>721</v>
+      </c>
+      <c r="C140" s="28" t="s">
+        <v>760</v>
+      </c>
+      <c r="D140" s="26" t="s">
+        <v>753</v>
+      </c>
+      <c r="E140" s="26" t="s">
+        <v>764</v>
       </c>
       <c r="F140" s="39" t="s">
         <v>416</v>
@@ -10147,7 +10175,7 @@
       <c r="G140" s="39"/>
       <c r="H140" s="39"/>
       <c r="I140" s="39" t="s">
-        <v>526</v>
+        <v>749</v>
       </c>
       <c r="J140" s="39" t="s">
         <v>197</v>
@@ -10155,39 +10183,39 @@
       <c r="K140" s="39" t="s">
         <v>197</v>
       </c>
-      <c r="L140" s="62" t="s">
-        <v>38</v>
-      </c>
-      <c r="M140" s="62" t="s">
-        <v>478</v>
+      <c r="L140" s="64" t="s">
+        <v>1</v>
+      </c>
+      <c r="M140" s="61" t="s">
+        <v>1</v>
       </c>
       <c r="N140" s="16" t="s">
-        <v>162</v>
+        <v>749</v>
       </c>
     </row>
     <row r="141" spans="1:14" ht="18">
-      <c r="A141" s="61" t="s">
-        <v>689</v>
-      </c>
-      <c r="B141" s="39" t="s">
-        <v>721</v>
-      </c>
-      <c r="C141" s="39" t="s">
-        <v>760</v>
-      </c>
-      <c r="D141" s="62" t="s">
-        <v>753</v>
-      </c>
-      <c r="E141" s="39" t="s">
-        <v>416</v>
-      </c>
-      <c r="F141" s="39" t="s">
-        <v>416</v>
-      </c>
-      <c r="G141" s="39"/>
-      <c r="H141" s="39"/>
-      <c r="I141" s="39" t="s">
-        <v>749</v>
+      <c r="A141" s="27" t="s">
+        <v>690</v>
+      </c>
+      <c r="B141" s="28" t="s">
+        <v>722</v>
+      </c>
+      <c r="C141" s="28" t="s">
+        <v>761</v>
+      </c>
+      <c r="D141" s="26" t="s">
+        <v>753</v>
+      </c>
+      <c r="E141" s="26" t="s">
+        <v>764</v>
+      </c>
+      <c r="F141" s="68" t="s">
+        <v>765</v>
+      </c>
+      <c r="G141" s="68"/>
+      <c r="H141" s="68"/>
+      <c r="I141" s="68" t="s">
+        <v>119</v>
       </c>
       <c r="J141" s="39" t="s">
         <v>197</v>
@@ -10195,71 +10223,75 @@
       <c r="K141" s="39" t="s">
         <v>197</v>
       </c>
-      <c r="L141" s="65" t="s">
-        <v>1</v>
-      </c>
-      <c r="M141" s="62" t="s">
+      <c r="L141" s="64" t="s">
+        <v>723</v>
+      </c>
+      <c r="M141" s="61" t="s">
         <v>1</v>
       </c>
       <c r="N141" s="16" t="s">
-        <v>749</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:14" ht="18">
-      <c r="A142" s="61" t="s">
-        <v>690</v>
-      </c>
-      <c r="B142" s="39" t="s">
-        <v>722</v>
-      </c>
-      <c r="C142" s="39" t="s">
-        <v>761</v>
-      </c>
-      <c r="D142" s="62" t="s">
-        <v>753</v>
-      </c>
-      <c r="E142" s="39" t="s">
-        <v>416</v>
-      </c>
-      <c r="F142" s="39" t="s">
-        <v>416</v>
-      </c>
-      <c r="G142" s="39"/>
-      <c r="H142" s="39"/>
-      <c r="I142" s="39" t="s">
-        <v>119</v>
-      </c>
-      <c r="J142" s="39" t="s">
-        <v>197</v>
-      </c>
-      <c r="K142" s="39" t="s">
-        <v>197</v>
-      </c>
-      <c r="L142" s="65" t="s">
-        <v>723</v>
-      </c>
-      <c r="M142" s="62" t="s">
+      <c r="A142" s="49" t="s">
+        <v>572</v>
+      </c>
+      <c r="B142" s="50" t="s">
+        <v>578</v>
+      </c>
+      <c r="C142" s="50" t="s">
+        <v>607</v>
+      </c>
+      <c r="D142" s="50" t="s">
+        <v>679</v>
+      </c>
+      <c r="E142" s="50" t="s">
+        <v>674</v>
+      </c>
+      <c r="F142" s="50" t="s">
+        <v>679</v>
+      </c>
+      <c r="G142" s="50" t="s">
+        <v>677</v>
+      </c>
+      <c r="H142" s="50">
+        <v>1</v>
+      </c>
+      <c r="I142" s="50" t="s">
+        <v>519</v>
+      </c>
+      <c r="J142" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="K142" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="L142" s="15" t="s">
+        <v>670</v>
+      </c>
+      <c r="M142" s="13" t="s">
         <v>1</v>
       </c>
       <c r="N142" s="16" t="s">
-        <v>1</v>
+        <v>585</v>
       </c>
     </row>
     <row r="143" spans="1:14" ht="18">
       <c r="A143" s="49" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="B143" s="50" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C143" s="50" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D143" s="50" t="s">
         <v>679</v>
       </c>
       <c r="E143" s="50" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="F143" s="50" t="s">
         <v>679</v>
@@ -10271,7 +10303,7 @@
         <v>1</v>
       </c>
       <c r="I143" s="50" t="s">
-        <v>519</v>
+        <v>580</v>
       </c>
       <c r="J143" s="14" t="s">
         <v>197</v>
@@ -10280,30 +10312,30 @@
         <v>197</v>
       </c>
       <c r="L143" s="15" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="M143" s="13" t="s">
         <v>1</v>
       </c>
       <c r="N143" s="16" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="144" spans="1:14" ht="18">
       <c r="A144" s="49" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B144" s="50" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C144" s="50" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D144" s="50" t="s">
         <v>679</v>
       </c>
       <c r="E144" s="50" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="F144" s="50" t="s">
         <v>679</v>
@@ -10315,7 +10347,7 @@
         <v>1</v>
       </c>
       <c r="I144" s="50" t="s">
-        <v>580</v>
+        <v>403</v>
       </c>
       <c r="J144" s="14" t="s">
         <v>197</v>
@@ -10324,30 +10356,30 @@
         <v>197</v>
       </c>
       <c r="L144" s="15" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="M144" s="13" t="s">
         <v>1</v>
       </c>
       <c r="N144" s="16" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
     </row>
     <row r="145" spans="1:14" ht="18">
       <c r="A145" s="49" t="s">
-        <v>569</v>
+        <v>665</v>
       </c>
       <c r="B145" s="50" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C145" s="50" t="s">
-        <v>605</v>
+        <v>574</v>
       </c>
       <c r="D145" s="50" t="s">
         <v>679</v>
       </c>
       <c r="E145" s="50" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="F145" s="50" t="s">
         <v>679</v>
@@ -10359,7 +10391,7 @@
         <v>1</v>
       </c>
       <c r="I145" s="50" t="s">
-        <v>403</v>
+        <v>520</v>
       </c>
       <c r="J145" s="14" t="s">
         <v>197</v>
@@ -10368,30 +10400,30 @@
         <v>197</v>
       </c>
       <c r="L145" s="15" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="M145" s="13" t="s">
         <v>1</v>
       </c>
       <c r="N145" s="16" t="s">
-        <v>579</v>
+        <v>583</v>
       </c>
     </row>
     <row r="146" spans="1:14" ht="18">
       <c r="A146" s="49" t="s">
-        <v>665</v>
+        <v>571</v>
       </c>
       <c r="B146" s="50" t="s">
-        <v>573</v>
+        <v>577</v>
       </c>
       <c r="C146" s="50" t="s">
-        <v>574</v>
+        <v>608</v>
       </c>
       <c r="D146" s="50" t="s">
         <v>679</v>
       </c>
       <c r="E146" s="50" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="F146" s="50" t="s">
         <v>679</v>
@@ -10403,7 +10435,7 @@
         <v>1</v>
       </c>
       <c r="I146" s="50" t="s">
-        <v>520</v>
+        <v>582</v>
       </c>
       <c r="J146" s="14" t="s">
         <v>197</v>
@@ -10412,30 +10444,30 @@
         <v>197</v>
       </c>
       <c r="L146" s="15" t="s">
-        <v>667</v>
+        <v>1</v>
       </c>
       <c r="M146" s="13" t="s">
         <v>1</v>
       </c>
       <c r="N146" s="16" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="147" spans="1:14" ht="18">
       <c r="A147" s="49" t="s">
-        <v>571</v>
+        <v>639</v>
       </c>
       <c r="B147" s="50" t="s">
-        <v>577</v>
+        <v>640</v>
       </c>
       <c r="C147" s="50" t="s">
-        <v>608</v>
+        <v>656</v>
       </c>
       <c r="D147" s="50" t="s">
         <v>679</v>
       </c>
       <c r="E147" s="50" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="F147" s="50" t="s">
         <v>679</v>
@@ -10447,7 +10479,7 @@
         <v>1</v>
       </c>
       <c r="I147" s="50" t="s">
-        <v>582</v>
+        <v>655</v>
       </c>
       <c r="J147" s="14" t="s">
         <v>197</v>
@@ -10462,24 +10494,24 @@
         <v>1</v>
       </c>
       <c r="N147" s="16" t="s">
-        <v>581</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148" spans="1:14" ht="18">
       <c r="A148" s="49" t="s">
-        <v>639</v>
+        <v>642</v>
       </c>
       <c r="B148" s="50" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="C148" s="50" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="D148" s="50" t="s">
         <v>679</v>
       </c>
       <c r="E148" s="50" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="F148" s="50" t="s">
         <v>679</v>
@@ -10491,7 +10523,7 @@
         <v>1</v>
       </c>
       <c r="I148" s="50" t="s">
-        <v>655</v>
+        <v>681</v>
       </c>
       <c r="J148" s="14" t="s">
         <v>197</v>
@@ -10511,31 +10543,31 @@
     </row>
     <row r="149" spans="1:14" ht="18">
       <c r="A149" s="49" t="s">
-        <v>642</v>
+        <v>666</v>
       </c>
       <c r="B149" s="50" t="s">
-        <v>641</v>
+        <v>573</v>
       </c>
       <c r="C149" s="50" t="s">
-        <v>657</v>
+        <v>574</v>
       </c>
       <c r="D149" s="50" t="s">
         <v>679</v>
       </c>
       <c r="E149" s="50" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="F149" s="50" t="s">
         <v>679</v>
       </c>
       <c r="G149" s="50" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="H149" s="50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I149" s="50" t="s">
-        <v>681</v>
+        <v>520</v>
       </c>
       <c r="J149" s="14" t="s">
         <v>197</v>
@@ -10544,9 +10576,9 @@
         <v>197</v>
       </c>
       <c r="L149" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M149" s="13" t="s">
+        <v>667</v>
+      </c>
+      <c r="M149" s="51" t="s">
         <v>1</v>
       </c>
       <c r="N149" s="16" t="s">
@@ -10554,75 +10586,31 @@
       </c>
     </row>
     <row r="150" spans="1:14" ht="18">
-      <c r="A150" s="49" t="s">
-        <v>666</v>
-      </c>
-      <c r="B150" s="50" t="s">
-        <v>573</v>
-      </c>
-      <c r="C150" s="50" t="s">
-        <v>574</v>
-      </c>
-      <c r="D150" s="50" t="s">
-        <v>679</v>
-      </c>
-      <c r="E150" s="50" t="s">
-        <v>679</v>
-      </c>
-      <c r="F150" s="50" t="s">
-        <v>679</v>
-      </c>
-      <c r="G150" s="50" t="s">
-        <v>678</v>
-      </c>
-      <c r="H150" s="50">
-        <v>3</v>
-      </c>
-      <c r="I150" s="50" t="s">
-        <v>520</v>
-      </c>
-      <c r="J150" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="K150" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="L150" s="15" t="s">
-        <v>667</v>
-      </c>
-      <c r="M150" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="N150" s="16" t="s">
-        <v>1</v>
-      </c>
+      <c r="F150" s="64"/>
+      <c r="G150" s="64"/>
+      <c r="H150" s="64"/>
+      <c r="I150" s="64"/>
+      <c r="J150" s="64"/>
+      <c r="K150" s="64"/>
+      <c r="L150" s="64"/>
     </row>
     <row r="151" spans="1:14" ht="18">
-      <c r="F151" s="65"/>
-      <c r="G151" s="65"/>
-      <c r="H151" s="65"/>
-      <c r="I151" s="65"/>
-      <c r="J151" s="65"/>
-      <c r="K151" s="65"/>
-      <c r="L151" s="65"/>
+      <c r="F151" s="64"/>
+      <c r="G151" s="64"/>
+      <c r="H151" s="64"/>
+      <c r="I151" s="64"/>
+      <c r="J151" s="64"/>
+      <c r="K151" s="64"/>
+      <c r="L151" s="64"/>
     </row>
     <row r="152" spans="1:14" ht="18">
-      <c r="F152" s="65"/>
-      <c r="G152" s="65"/>
-      <c r="H152" s="65"/>
-      <c r="I152" s="65"/>
-      <c r="J152" s="65"/>
-      <c r="K152" s="65"/>
-      <c r="L152" s="65"/>
-    </row>
-    <row r="153" spans="1:14" ht="18">
-      <c r="F153" s="65"/>
-      <c r="G153" s="65"/>
-      <c r="H153" s="65"/>
-      <c r="I153" s="65"/>
-      <c r="J153" s="65"/>
-      <c r="K153" s="65"/>
-      <c r="L153" s="65"/>
+      <c r="F152" s="64"/>
+      <c r="G152" s="64"/>
+      <c r="H152" s="64"/>
+      <c r="I152" s="64"/>
+      <c r="J152" s="64"/>
+      <c r="K152" s="64"/>
+      <c r="L152" s="64"/>
     </row>
   </sheetData>
   <sortState ref="A2:N153">
@@ -10655,77 +10643,77 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:1" ht="16" thickBot="1">
-      <c r="A1" s="63">
+      <c r="A1" s="62">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="16" thickBot="1">
-      <c r="A2" s="64">
+      <c r="A2" s="63">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="16" thickBot="1">
-      <c r="A3" s="64">
+      <c r="A3" s="63">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="16" thickBot="1">
-      <c r="A4" s="64">
+      <c r="A4" s="63">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="16" thickBot="1">
-      <c r="A5" s="64">
+      <c r="A5" s="63">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="16" thickBot="1">
-      <c r="A6" s="64">
+      <c r="A6" s="63">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="16" thickBot="1">
-      <c r="A7" s="64">
+      <c r="A7" s="63">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="16" thickBot="1">
-      <c r="A8" s="64">
+      <c r="A8" s="63">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="16" thickBot="1">
-      <c r="A9" s="64">
+      <c r="A9" s="63">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="16" thickBot="1">
-      <c r="A10" s="64">
+      <c r="A10" s="63">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="16" thickBot="1">
-      <c r="A11" s="64">
+      <c r="A11" s="63">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="16" thickBot="1">
-      <c r="A12" s="64">
+      <c r="A12" s="63">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="16" thickBot="1">
-      <c r="A13" s="64">
+      <c r="A13" s="63">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="16" thickBot="1">
-      <c r="A14" s="64">
+      <c r="A14" s="63">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="16" thickBot="1">
-      <c r="A15" s="64">
+      <c r="A15" s="63">
         <v>6</v>
       </c>
     </row>
@@ -10747,51 +10735,91 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="18" customHeight="1">
-      <c r="A1" s="5">
-        <v>69</v>
-      </c>
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="1:14" ht="18" customHeight="1">
+      <c r="A1" s="6" t="s">
         <v>620</v>
       </c>
+      <c r="B1" s="5" t="s">
+        <v>118</v>
+      </c>
       <c r="C1" s="5" t="s">
-        <v>118</v>
+        <v>371</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>371</v>
+        <v>191</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>586</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="I1" s="4">
+        <v>1176</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="18">
+      <c r="A2" s="42" t="s">
+        <v>242</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="43" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2" s="43" t="s">
+        <v>753</v>
+      </c>
+      <c r="E2" s="43" t="s">
+        <v>674</v>
+      </c>
+      <c r="F2" s="43" t="s">
         <v>191</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G2" s="43" t="s">
         <v>586</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="H2" s="43"/>
+      <c r="I2" s="43" t="s">
+        <v>630</v>
+      </c>
+      <c r="J2" s="44" t="s">
         <v>192</v>
       </c>
-      <c r="J1" s="4">
-        <v>1176</v>
-      </c>
-      <c r="K1" s="3" t="s">
+      <c r="K2" s="44" t="s">
+        <v>632</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>382</v>
+      </c>
+      <c r="M2" s="13" t="s">
         <v>475</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>568</v>
+      <c r="N2" s="16" t="s">
+        <v>381</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Added invertebrate sequences from Parry et al (2019)
</commit_message>
<xml_diff>
--- a/tabular/flavi-ncbi-refseqs-side-data.xlsx
+++ b/tabular/flavi-ncbi-refseqs-side-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6280" yWindow="500" windowWidth="29780" windowHeight="17980" tabRatio="500"/>
+    <workbookView xWindow="1120" yWindow="1000" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="flavi.txt" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="removed" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">flavi.txt!$A$1:$M$111</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">flavi.txt!$A$1:$M$114</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1922" uniqueCount="766">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1973" uniqueCount="789">
   <si>
     <t>AY632538</t>
   </si>
@@ -2328,6 +2328,75 @@
   </si>
   <si>
     <t>Hepegivirus</t>
+  </si>
+  <si>
+    <t>Gammarus chevreuxi flavivirus</t>
+  </si>
+  <si>
+    <t>MK473875</t>
+  </si>
+  <si>
+    <t>MK473877</t>
+  </si>
+  <si>
+    <t>MK473878</t>
+  </si>
+  <si>
+    <t>MK473880</t>
+  </si>
+  <si>
+    <t>MK473881</t>
+  </si>
+  <si>
+    <t>Southern pygmy squid flavivirus</t>
+  </si>
+  <si>
+    <t>Crangon crangon flavivirus</t>
+  </si>
+  <si>
+    <t>Firefly squid flavivirus</t>
+  </si>
+  <si>
+    <t>Gammarus pulex flavivirus</t>
+  </si>
+  <si>
+    <t>SpsFV</t>
+  </si>
+  <si>
+    <t>FfsFV</t>
+  </si>
+  <si>
+    <t>GcFV</t>
+  </si>
+  <si>
+    <t>CcFV</t>
+  </si>
+  <si>
+    <t>GpFV</t>
+  </si>
+  <si>
+    <t>Crustacean</t>
+  </si>
+  <si>
+    <t>Gammarus</t>
+  </si>
+  <si>
+    <t>Crangon</t>
+  </si>
+  <si>
+    <t>crustacean</t>
+  </si>
+  <si>
+    <t>Gammarus chevreuxi</t>
+  </si>
+  <si>
+    <t>Crangon crangon</t>
+  </si>
+  <si>
+    <t>Gammarus pulex</t>
+  </si>
+  <si>
+    <t>Squid</t>
   </si>
 </sst>
 </file>
@@ -2442,7 +2511,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="21">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2563,6 +2632,18 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -2601,7 +2682,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="638">
+  <cellStyleXfs count="664">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3240,8 +3321,34 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3387,8 +3494,12 @@
     <xf numFmtId="0" fontId="5" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="638">
+  <cellStyles count="664">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3716,6 +3827,32 @@
     <cellStyle name="Followed Hyperlink" xfId="635" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="636" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="637" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="638" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="639" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="640" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="641" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="642" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="643" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="644" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="645" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="646" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="647" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="648" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="649" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="650" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="651" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="652" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="653" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="654" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="655" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="656" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="657" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="658" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="659" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="660" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="661" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="662" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="663" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4363,11 +4500,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N152"/>
+  <dimension ref="A1:N154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A114" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A134" sqref="A134"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:N154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8336,140 +8473,134 @@
       </c>
     </row>
     <row r="95" spans="1:14" ht="18">
-      <c r="A95" s="52" t="s">
+      <c r="A95" s="69" t="s">
+        <v>768</v>
+      </c>
+      <c r="B95" s="70" t="s">
+        <v>766</v>
+      </c>
+      <c r="C95" s="70" t="s">
+        <v>778</v>
+      </c>
+      <c r="D95" s="70" t="s">
+        <v>753</v>
+      </c>
+      <c r="E95" s="70" t="s">
+        <v>674</v>
+      </c>
+      <c r="F95" s="70" t="s">
+        <v>191</v>
+      </c>
+      <c r="G95" s="70" t="s">
+        <v>781</v>
+      </c>
+      <c r="H95" s="70"/>
+      <c r="I95" s="70" t="s">
+        <v>782</v>
+      </c>
+      <c r="J95" s="70" t="s">
+        <v>784</v>
+      </c>
+      <c r="K95" s="70"/>
+      <c r="L95" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M95" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="N95" s="16" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" ht="18">
+      <c r="A96" s="69" t="s">
+        <v>769</v>
+      </c>
+      <c r="B96" s="70" t="s">
+        <v>773</v>
+      </c>
+      <c r="C96" s="70" t="s">
+        <v>779</v>
+      </c>
+      <c r="D96" s="70" t="s">
+        <v>753</v>
+      </c>
+      <c r="E96" s="70" t="s">
+        <v>674</v>
+      </c>
+      <c r="F96" s="70" t="s">
+        <v>191</v>
+      </c>
+      <c r="G96" s="70" t="s">
+        <v>781</v>
+      </c>
+      <c r="H96" s="70"/>
+      <c r="I96" s="70" t="s">
+        <v>783</v>
+      </c>
+      <c r="J96" s="70" t="s">
+        <v>784</v>
+      </c>
+      <c r="K96" s="70"/>
+      <c r="L96" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M96" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="N96" s="16" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" ht="18">
+      <c r="A97" s="69" t="s">
+        <v>771</v>
+      </c>
+      <c r="B97" s="70" t="s">
+        <v>775</v>
+      </c>
+      <c r="C97" s="70" t="s">
+        <v>780</v>
+      </c>
+      <c r="D97" s="70" t="s">
+        <v>753</v>
+      </c>
+      <c r="E97" s="70" t="s">
+        <v>674</v>
+      </c>
+      <c r="F97" s="70" t="s">
+        <v>191</v>
+      </c>
+      <c r="G97" s="70" t="s">
+        <v>781</v>
+      </c>
+      <c r="H97" s="70"/>
+      <c r="I97" s="70" t="s">
+        <v>782</v>
+      </c>
+      <c r="J97" s="70" t="s">
+        <v>784</v>
+      </c>
+      <c r="K97" s="70"/>
+      <c r="L97" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M97" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="N97" s="16" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" ht="18">
+      <c r="A98" s="52" t="s">
         <v>618</v>
       </c>
-      <c r="B95" s="53" t="s">
+      <c r="B98" s="53" t="s">
         <v>488</v>
       </c>
-      <c r="C95" s="54" t="s">
+      <c r="C98" s="54" t="s">
         <v>613</v>
-      </c>
-      <c r="D95" s="54" t="s">
-        <v>753</v>
-      </c>
-      <c r="E95" s="55" t="s">
-        <v>674</v>
-      </c>
-      <c r="F95" s="55" t="s">
-        <v>483</v>
-      </c>
-      <c r="G95" s="54" t="s">
-        <v>554</v>
-      </c>
-      <c r="H95" s="54"/>
-      <c r="I95" s="54" t="s">
-        <v>530</v>
-      </c>
-      <c r="J95" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="K95" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="L95" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M95" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="N95" s="56" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="96" spans="1:14" ht="18">
-      <c r="A96" s="57" t="s">
-        <v>557</v>
-      </c>
-      <c r="B96" s="53" t="s">
-        <v>558</v>
-      </c>
-      <c r="C96" s="53" t="s">
-        <v>614</v>
-      </c>
-      <c r="D96" s="54" t="s">
-        <v>753</v>
-      </c>
-      <c r="E96" s="55" t="s">
-        <v>674</v>
-      </c>
-      <c r="F96" s="55" t="s">
-        <v>483</v>
-      </c>
-      <c r="G96" s="53" t="s">
-        <v>554</v>
-      </c>
-      <c r="H96" s="53"/>
-      <c r="I96" s="53" t="s">
-        <v>566</v>
-      </c>
-      <c r="J96" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="K96" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="L96" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M96" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="N96" s="16" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="97" spans="1:14" ht="18">
-      <c r="A97" s="52" t="s">
-        <v>619</v>
-      </c>
-      <c r="B97" s="53" t="s">
-        <v>490</v>
-      </c>
-      <c r="C97" s="53" t="s">
-        <v>675</v>
-      </c>
-      <c r="D97" s="54" t="s">
-        <v>753</v>
-      </c>
-      <c r="E97" s="55" t="s">
-        <v>674</v>
-      </c>
-      <c r="F97" s="55" t="s">
-        <v>483</v>
-      </c>
-      <c r="G97" s="54" t="s">
-        <v>554</v>
-      </c>
-      <c r="H97" s="54"/>
-      <c r="I97" s="54" t="s">
-        <v>531</v>
-      </c>
-      <c r="J97" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="K97" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="L97" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M97" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="N97" s="56" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="98" spans="1:14" ht="18">
-      <c r="A98" s="57" t="s">
-        <v>556</v>
-      </c>
-      <c r="B98" s="53" t="s">
-        <v>559</v>
-      </c>
-      <c r="C98" s="53" t="s">
-        <v>612</v>
       </c>
       <c r="D98" s="54" t="s">
         <v>753</v>
@@ -8480,12 +8611,12 @@
       <c r="F98" s="55" t="s">
         <v>483</v>
       </c>
-      <c r="G98" s="53" t="s">
+      <c r="G98" s="54" t="s">
         <v>554</v>
       </c>
-      <c r="H98" s="53"/>
-      <c r="I98" s="53" t="s">
-        <v>564</v>
+      <c r="H98" s="54"/>
+      <c r="I98" s="54" t="s">
+        <v>530</v>
       </c>
       <c r="J98" s="14" t="s">
         <v>197</v>
@@ -8499,19 +8630,19 @@
       <c r="M98" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="N98" s="16" t="s">
-        <v>563</v>
+      <c r="N98" s="56" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="99" spans="1:14" ht="18">
       <c r="A99" s="57" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="B99" s="53" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C99" s="53" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="D99" s="54" t="s">
         <v>753</v>
@@ -8527,7 +8658,7 @@
       </c>
       <c r="H99" s="53"/>
       <c r="I99" s="53" t="s">
-        <v>562</v>
+        <v>566</v>
       </c>
       <c r="J99" s="14" t="s">
         <v>197</v>
@@ -8542,18 +8673,18 @@
         <v>1</v>
       </c>
       <c r="N99" s="16" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
     </row>
     <row r="100" spans="1:14" ht="18">
       <c r="A100" s="52" t="s">
-        <v>482</v>
+        <v>619</v>
       </c>
       <c r="B100" s="53" t="s">
-        <v>489</v>
-      </c>
-      <c r="C100" s="54" t="s">
-        <v>486</v>
+        <v>490</v>
+      </c>
+      <c r="C100" s="53" t="s">
+        <v>675</v>
       </c>
       <c r="D100" s="54" t="s">
         <v>753</v>
@@ -8565,11 +8696,11 @@
         <v>483</v>
       </c>
       <c r="G100" s="54" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="H100" s="54"/>
       <c r="I100" s="54" t="s">
-        <v>541</v>
+        <v>531</v>
       </c>
       <c r="J100" s="14" t="s">
         <v>197</v>
@@ -8584,18 +8715,18 @@
         <v>1</v>
       </c>
       <c r="N100" s="56" t="s">
-        <v>540</v>
+        <v>492</v>
       </c>
     </row>
     <row r="101" spans="1:14" ht="18">
-      <c r="A101" s="52" t="s">
-        <v>487</v>
+      <c r="A101" s="57" t="s">
+        <v>556</v>
       </c>
       <c r="B101" s="53" t="s">
-        <v>484</v>
-      </c>
-      <c r="C101" s="54" t="s">
-        <v>485</v>
+        <v>559</v>
+      </c>
+      <c r="C101" s="53" t="s">
+        <v>612</v>
       </c>
       <c r="D101" s="54" t="s">
         <v>753</v>
@@ -8606,12 +8737,12 @@
       <c r="F101" s="55" t="s">
         <v>483</v>
       </c>
-      <c r="G101" s="54" t="s">
-        <v>553</v>
-      </c>
-      <c r="H101" s="54"/>
-      <c r="I101" s="54" t="s">
-        <v>539</v>
+      <c r="G101" s="53" t="s">
+        <v>554</v>
+      </c>
+      <c r="H101" s="53"/>
+      <c r="I101" s="53" t="s">
+        <v>564</v>
       </c>
       <c r="J101" s="14" t="s">
         <v>197</v>
@@ -8625,19 +8756,19 @@
       <c r="M101" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="N101" s="56" t="s">
-        <v>538</v>
+      <c r="N101" s="16" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="102" spans="1:14" ht="18">
-      <c r="A102" s="52" t="s">
-        <v>634</v>
+      <c r="A102" s="57" t="s">
+        <v>555</v>
       </c>
       <c r="B102" s="53" t="s">
-        <v>635</v>
-      </c>
-      <c r="C102" s="54" t="s">
-        <v>637</v>
+        <v>560</v>
+      </c>
+      <c r="C102" s="53" t="s">
+        <v>611</v>
       </c>
       <c r="D102" s="54" t="s">
         <v>753</v>
@@ -8648,137 +8779,139 @@
       <c r="F102" s="55" t="s">
         <v>483</v>
       </c>
-      <c r="G102" s="54" t="s">
+      <c r="G102" s="53" t="s">
+        <v>554</v>
+      </c>
+      <c r="H102" s="53"/>
+      <c r="I102" s="53" t="s">
+        <v>562</v>
+      </c>
+      <c r="J102" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="K102" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="L102" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M102" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="N102" s="16" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" ht="18">
+      <c r="A103" s="52" t="s">
+        <v>482</v>
+      </c>
+      <c r="B103" s="53" t="s">
+        <v>489</v>
+      </c>
+      <c r="C103" s="54" t="s">
+        <v>486</v>
+      </c>
+      <c r="D103" s="54" t="s">
+        <v>753</v>
+      </c>
+      <c r="E103" s="55" t="s">
+        <v>674</v>
+      </c>
+      <c r="F103" s="55" t="s">
+        <v>483</v>
+      </c>
+      <c r="G103" s="54" t="s">
         <v>553</v>
       </c>
-      <c r="H102" s="54"/>
-      <c r="I102" s="54" t="s">
+      <c r="H103" s="54"/>
+      <c r="I103" s="54" t="s">
+        <v>541</v>
+      </c>
+      <c r="J103" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="K103" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="L103" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M103" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="N103" s="56" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" ht="18">
+      <c r="A104" s="52" t="s">
+        <v>487</v>
+      </c>
+      <c r="B104" s="53" t="s">
+        <v>484</v>
+      </c>
+      <c r="C104" s="54" t="s">
+        <v>485</v>
+      </c>
+      <c r="D104" s="54" t="s">
+        <v>753</v>
+      </c>
+      <c r="E104" s="55" t="s">
+        <v>674</v>
+      </c>
+      <c r="F104" s="55" t="s">
+        <v>483</v>
+      </c>
+      <c r="G104" s="54" t="s">
+        <v>553</v>
+      </c>
+      <c r="H104" s="54"/>
+      <c r="I104" s="54" t="s">
+        <v>539</v>
+      </c>
+      <c r="J104" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="K104" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="L104" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M104" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="N104" s="56" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" ht="18">
+      <c r="A105" s="52" t="s">
+        <v>634</v>
+      </c>
+      <c r="B105" s="53" t="s">
+        <v>635</v>
+      </c>
+      <c r="C105" s="54" t="s">
+        <v>637</v>
+      </c>
+      <c r="D105" s="54" t="s">
+        <v>753</v>
+      </c>
+      <c r="E105" s="55" t="s">
+        <v>674</v>
+      </c>
+      <c r="F105" s="55" t="s">
+        <v>483</v>
+      </c>
+      <c r="G105" s="54" t="s">
+        <v>553</v>
+      </c>
+      <c r="H105" s="54"/>
+      <c r="I105" s="54" t="s">
         <v>636</v>
       </c>
-      <c r="J102" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="K102" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="L102" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M102" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="N102" s="56"/>
-    </row>
-    <row r="103" spans="1:14" ht="18">
-      <c r="A103" s="58" t="s">
-        <v>218</v>
-      </c>
-      <c r="B103" s="59" t="s">
-        <v>94</v>
-      </c>
-      <c r="C103" s="60" t="s">
-        <v>335</v>
-      </c>
-      <c r="D103" s="60" t="s">
-        <v>753</v>
-      </c>
-      <c r="E103" s="60" t="s">
-        <v>674</v>
-      </c>
-      <c r="F103" s="60" t="s">
-        <v>325</v>
-      </c>
-      <c r="G103" s="60" t="s">
-        <v>545</v>
-      </c>
-      <c r="H103" s="60"/>
-      <c r="I103" s="60" t="s">
-        <v>522</v>
-      </c>
-      <c r="J103" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="K103" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="L103" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M103" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="N103" s="16" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="104" spans="1:14" ht="18">
-      <c r="A104" s="58" t="s">
-        <v>225</v>
-      </c>
-      <c r="B104" s="59" t="s">
-        <v>105</v>
-      </c>
-      <c r="C104" s="60" t="s">
-        <v>349</v>
-      </c>
-      <c r="D104" s="60" t="s">
-        <v>753</v>
-      </c>
-      <c r="E104" s="60" t="s">
-        <v>674</v>
-      </c>
-      <c r="F104" s="60" t="s">
-        <v>325</v>
-      </c>
-      <c r="G104" s="60" t="s">
-        <v>546</v>
-      </c>
-      <c r="H104" s="60"/>
-      <c r="I104" s="60" t="s">
-        <v>522</v>
-      </c>
-      <c r="J104" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="K104" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="L104" s="15" t="s">
-        <v>350</v>
-      </c>
-      <c r="M104" s="13" t="s">
-        <v>476</v>
-      </c>
-      <c r="N104" s="16" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="105" spans="1:14" ht="18">
-      <c r="A105" s="58" t="s">
-        <v>227</v>
-      </c>
-      <c r="B105" s="59" t="s">
-        <v>107</v>
-      </c>
-      <c r="C105" s="60" t="s">
-        <v>351</v>
-      </c>
-      <c r="D105" s="60" t="s">
-        <v>753</v>
-      </c>
-      <c r="E105" s="60" t="s">
-        <v>674</v>
-      </c>
-      <c r="F105" s="60" t="s">
-        <v>325</v>
-      </c>
-      <c r="G105" s="60" t="s">
-        <v>548</v>
-      </c>
-      <c r="H105" s="60"/>
-      <c r="I105" s="60" t="s">
-        <v>527</v>
-      </c>
       <c r="J105" s="14" t="s">
         <v>197</v>
       </c>
@@ -8786,24 +8919,22 @@
         <v>197</v>
       </c>
       <c r="L105" s="15" t="s">
-        <v>352</v>
-      </c>
-      <c r="M105" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="N105" s="16" t="s">
-        <v>494</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="M105" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="N105" s="56"/>
     </row>
     <row r="106" spans="1:14" ht="18">
       <c r="A106" s="58" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="B106" s="59" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="C106" s="60" t="s">
-        <v>596</v>
+        <v>335</v>
       </c>
       <c r="D106" s="60" t="s">
         <v>753</v>
@@ -8815,11 +8946,11 @@
         <v>325</v>
       </c>
       <c r="G106" s="60" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="H106" s="60"/>
       <c r="I106" s="60" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="J106" s="14" t="s">
         <v>197</v>
@@ -8828,24 +8959,24 @@
         <v>197</v>
       </c>
       <c r="L106" s="15" t="s">
-        <v>360</v>
-      </c>
-      <c r="M106" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="M106" s="15" t="s">
         <v>1</v>
       </c>
       <c r="N106" s="16" t="s">
-        <v>212</v>
+        <v>136</v>
       </c>
     </row>
     <row r="107" spans="1:14" ht="18">
       <c r="A107" s="58" t="s">
-        <v>286</v>
+        <v>225</v>
       </c>
       <c r="B107" s="59" t="s">
-        <v>158</v>
+        <v>105</v>
       </c>
       <c r="C107" s="60" t="s">
-        <v>422</v>
+        <v>349</v>
       </c>
       <c r="D107" s="60" t="s">
         <v>753</v>
@@ -8857,11 +8988,11 @@
         <v>325</v>
       </c>
       <c r="G107" s="60" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
       <c r="H107" s="60"/>
       <c r="I107" s="60" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
       <c r="J107" s="14" t="s">
         <v>197</v>
@@ -8870,24 +9001,24 @@
         <v>197</v>
       </c>
       <c r="L107" s="15" t="s">
-        <v>1</v>
+        <v>350</v>
       </c>
       <c r="M107" s="13" t="s">
         <v>476</v>
       </c>
       <c r="N107" s="16" t="s">
-        <v>493</v>
+        <v>136</v>
       </c>
     </row>
     <row r="108" spans="1:14" ht="18">
       <c r="A108" s="58" t="s">
-        <v>258</v>
+        <v>227</v>
       </c>
       <c r="B108" s="59" t="s">
-        <v>151</v>
+        <v>107</v>
       </c>
       <c r="C108" s="60" t="s">
-        <v>597</v>
+        <v>351</v>
       </c>
       <c r="D108" s="60" t="s">
         <v>753</v>
@@ -8899,7 +9030,7 @@
         <v>325</v>
       </c>
       <c r="G108" s="60" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="H108" s="60"/>
       <c r="I108" s="60" t="s">
@@ -8912,10 +9043,10 @@
         <v>197</v>
       </c>
       <c r="L108" s="15" t="s">
-        <v>34</v>
+        <v>352</v>
       </c>
       <c r="M108" s="13" t="s">
-        <v>479</v>
+        <v>1</v>
       </c>
       <c r="N108" s="16" t="s">
         <v>494</v>
@@ -8923,13 +9054,13 @@
     </row>
     <row r="109" spans="1:14" ht="18">
       <c r="A109" s="58" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B109" s="59" t="s">
-        <v>198</v>
+        <v>112</v>
       </c>
       <c r="C109" s="60" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="D109" s="60" t="s">
         <v>753</v>
@@ -8941,11 +9072,11 @@
         <v>325</v>
       </c>
       <c r="G109" s="60" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="H109" s="60"/>
       <c r="I109" s="60" t="s">
-        <v>528</v>
+        <v>521</v>
       </c>
       <c r="J109" s="14" t="s">
         <v>197</v>
@@ -8954,24 +9085,24 @@
         <v>197</v>
       </c>
       <c r="L109" s="15" t="s">
-        <v>21</v>
+        <v>360</v>
       </c>
       <c r="M109" s="13" t="s">
-        <v>478</v>
+        <v>1</v>
       </c>
       <c r="N109" s="16" t="s">
-        <v>111</v>
+        <v>212</v>
       </c>
     </row>
     <row r="110" spans="1:14" ht="18">
       <c r="A110" s="58" t="s">
-        <v>250</v>
+        <v>286</v>
       </c>
       <c r="B110" s="59" t="s">
-        <v>201</v>
+        <v>158</v>
       </c>
       <c r="C110" s="60" t="s">
-        <v>409</v>
+        <v>422</v>
       </c>
       <c r="D110" s="60" t="s">
         <v>753</v>
@@ -8983,11 +9114,11 @@
         <v>325</v>
       </c>
       <c r="G110" s="60" t="s">
-        <v>547</v>
+        <v>552</v>
       </c>
       <c r="H110" s="60"/>
       <c r="I110" s="60" t="s">
-        <v>522</v>
+        <v>529</v>
       </c>
       <c r="J110" s="14" t="s">
         <v>197</v>
@@ -8999,21 +9130,21 @@
         <v>1</v>
       </c>
       <c r="M110" s="13" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="N110" s="16" t="s">
-        <v>136</v>
+        <v>493</v>
       </c>
     </row>
     <row r="111" spans="1:14" ht="18">
       <c r="A111" s="58" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="B111" s="59" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="C111" s="60" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D111" s="60" t="s">
         <v>753</v>
@@ -9025,11 +9156,11 @@
         <v>325</v>
       </c>
       <c r="G111" s="60" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="H111" s="60"/>
       <c r="I111" s="60" t="s">
-        <v>521</v>
+        <v>527</v>
       </c>
       <c r="J111" s="14" t="s">
         <v>197</v>
@@ -9038,24 +9169,24 @@
         <v>197</v>
       </c>
       <c r="L111" s="15" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="M111" s="13" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
       <c r="N111" s="16" t="s">
-        <v>212</v>
+        <v>494</v>
       </c>
     </row>
     <row r="112" spans="1:14" ht="18">
       <c r="A112" s="58" t="s">
-        <v>265</v>
-      </c>
-      <c r="B112" s="60" t="s">
-        <v>168</v>
+        <v>231</v>
+      </c>
+      <c r="B112" s="59" t="s">
+        <v>198</v>
       </c>
       <c r="C112" s="60" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="D112" s="60" t="s">
         <v>753</v>
@@ -9067,11 +9198,11 @@
         <v>325</v>
       </c>
       <c r="G112" s="60" t="s">
-        <v>658</v>
+        <v>549</v>
       </c>
       <c r="H112" s="60"/>
       <c r="I112" s="60" t="s">
-        <v>524</v>
+        <v>528</v>
       </c>
       <c r="J112" s="14" t="s">
         <v>197</v>
@@ -9080,24 +9211,24 @@
         <v>197</v>
       </c>
       <c r="L112" s="15" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="M112" s="13" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="N112" s="16" t="s">
-        <v>166</v>
+        <v>111</v>
       </c>
     </row>
     <row r="113" spans="1:14" ht="18">
       <c r="A113" s="58" t="s">
-        <v>659</v>
-      </c>
-      <c r="B113" s="60" t="s">
-        <v>660</v>
+        <v>250</v>
+      </c>
+      <c r="B113" s="59" t="s">
+        <v>201</v>
       </c>
       <c r="C113" s="60" t="s">
-        <v>661</v>
+        <v>409</v>
       </c>
       <c r="D113" s="60" t="s">
         <v>753</v>
@@ -9109,11 +9240,11 @@
         <v>325</v>
       </c>
       <c r="G113" s="60" t="s">
-        <v>662</v>
+        <v>547</v>
       </c>
       <c r="H113" s="60"/>
       <c r="I113" s="60" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="J113" s="14" t="s">
         <v>197</v>
@@ -9125,21 +9256,21 @@
         <v>1</v>
       </c>
       <c r="M113" s="13" t="s">
-        <v>1</v>
+        <v>475</v>
       </c>
       <c r="N113" s="16" t="s">
-        <v>1</v>
+        <v>136</v>
       </c>
     </row>
     <row r="114" spans="1:14" ht="18">
       <c r="A114" s="58" t="s">
-        <v>671</v>
-      </c>
-      <c r="B114" s="60" t="s">
-        <v>638</v>
+        <v>253</v>
+      </c>
+      <c r="B114" s="59" t="s">
+        <v>143</v>
       </c>
       <c r="C114" s="60" t="s">
-        <v>663</v>
+        <v>598</v>
       </c>
       <c r="D114" s="60" t="s">
         <v>753</v>
@@ -9150,137 +9281,137 @@
       <c r="F114" s="60" t="s">
         <v>325</v>
       </c>
-      <c r="G114" s="60"/>
+      <c r="G114" s="60" t="s">
+        <v>550</v>
+      </c>
       <c r="H114" s="60"/>
       <c r="I114" s="60" t="s">
+        <v>521</v>
+      </c>
+      <c r="J114" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="K114" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="L114" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M114" s="13" t="s">
+        <v>475</v>
+      </c>
+      <c r="N114" s="16" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14" ht="18">
+      <c r="A115" s="58" t="s">
+        <v>265</v>
+      </c>
+      <c r="B115" s="60" t="s">
+        <v>168</v>
+      </c>
+      <c r="C115" s="60" t="s">
+        <v>599</v>
+      </c>
+      <c r="D115" s="60" t="s">
+        <v>753</v>
+      </c>
+      <c r="E115" s="60" t="s">
+        <v>674</v>
+      </c>
+      <c r="F115" s="60" t="s">
+        <v>325</v>
+      </c>
+      <c r="G115" s="60" t="s">
+        <v>658</v>
+      </c>
+      <c r="H115" s="60"/>
+      <c r="I115" s="60" t="s">
+        <v>524</v>
+      </c>
+      <c r="J115" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="K115" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="L115" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="M115" s="13" t="s">
+        <v>476</v>
+      </c>
+      <c r="N115" s="16" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" ht="18">
+      <c r="A116" s="58" t="s">
+        <v>659</v>
+      </c>
+      <c r="B116" s="60" t="s">
+        <v>660</v>
+      </c>
+      <c r="C116" s="60" t="s">
+        <v>661</v>
+      </c>
+      <c r="D116" s="60" t="s">
+        <v>753</v>
+      </c>
+      <c r="E116" s="60" t="s">
+        <v>674</v>
+      </c>
+      <c r="F116" s="60" t="s">
+        <v>325</v>
+      </c>
+      <c r="G116" s="60" t="s">
+        <v>662</v>
+      </c>
+      <c r="H116" s="60"/>
+      <c r="I116" s="60" t="s">
+        <v>527</v>
+      </c>
+      <c r="J116" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="K116" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="L116" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M116" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="N116" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:14" ht="18">
+      <c r="A117" s="58" t="s">
+        <v>671</v>
+      </c>
+      <c r="B117" s="60" t="s">
+        <v>638</v>
+      </c>
+      <c r="C117" s="60" t="s">
+        <v>663</v>
+      </c>
+      <c r="D117" s="60" t="s">
+        <v>753</v>
+      </c>
+      <c r="E117" s="60" t="s">
+        <v>674</v>
+      </c>
+      <c r="F117" s="60" t="s">
+        <v>325</v>
+      </c>
+      <c r="G117" s="60"/>
+      <c r="H117" s="60"/>
+      <c r="I117" s="60" t="s">
         <v>629</v>
       </c>
-      <c r="J114" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="K114" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="L114" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M114" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="N114" s="16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="115" spans="1:14" ht="18">
-      <c r="A115" s="47" t="s">
-        <v>497</v>
-      </c>
-      <c r="B115" s="48" t="s">
-        <v>502</v>
-      </c>
-      <c r="C115" s="48" t="s">
-        <v>609</v>
-      </c>
-      <c r="D115" s="48" t="s">
-        <v>753</v>
-      </c>
-      <c r="E115" s="48" t="s">
-        <v>674</v>
-      </c>
-      <c r="F115" s="48" t="s">
-        <v>621</v>
-      </c>
-      <c r="G115" s="48" t="s">
-        <v>366</v>
-      </c>
-      <c r="H115" s="48"/>
-      <c r="I115" s="48" t="s">
-        <v>518</v>
-      </c>
-      <c r="J115" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="K115" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="L115" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M115" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="N115" s="16" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="116" spans="1:14" ht="18">
-      <c r="A116" s="47" t="s">
-        <v>495</v>
-      </c>
-      <c r="B116" s="48" t="s">
-        <v>498</v>
-      </c>
-      <c r="C116" s="48" t="s">
-        <v>610</v>
-      </c>
-      <c r="D116" s="48" t="s">
-        <v>753</v>
-      </c>
-      <c r="E116" s="48" t="s">
-        <v>674</v>
-      </c>
-      <c r="F116" s="48" t="s">
-        <v>621</v>
-      </c>
-      <c r="G116" s="48" t="s">
-        <v>366</v>
-      </c>
-      <c r="H116" s="48"/>
-      <c r="I116" s="48" t="s">
-        <v>516</v>
-      </c>
-      <c r="J116" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="K116" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="L116" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M116" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="N116" s="16" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="117" spans="1:14" ht="18">
-      <c r="A117" s="47" t="s">
-        <v>235</v>
-      </c>
-      <c r="B117" s="48" t="s">
-        <v>115</v>
-      </c>
-      <c r="C117" s="48" t="s">
-        <v>366</v>
-      </c>
-      <c r="D117" s="48" t="s">
-        <v>753</v>
-      </c>
-      <c r="E117" s="48" t="s">
-        <v>674</v>
-      </c>
-      <c r="F117" s="48" t="s">
-        <v>621</v>
-      </c>
-      <c r="G117" s="48" t="s">
-        <v>366</v>
-      </c>
-      <c r="H117" s="48"/>
-      <c r="I117" s="48" t="s">
-        <v>515</v>
-      </c>
       <c r="J117" s="14" t="s">
         <v>197</v>
       </c>
@@ -9288,24 +9419,24 @@
         <v>197</v>
       </c>
       <c r="L117" s="15" t="s">
-        <v>367</v>
+        <v>1</v>
       </c>
       <c r="M117" s="13" t="s">
-        <v>476</v>
+        <v>1</v>
       </c>
       <c r="N117" s="16" t="s">
-        <v>116</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:14" ht="18">
       <c r="A118" s="47" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B118" s="48" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="C118" s="48" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D118" s="48" t="s">
         <v>753</v>
@@ -9316,238 +9447,221 @@
       <c r="F118" s="48" t="s">
         <v>621</v>
       </c>
-      <c r="G118" s="48" t="s">
-        <v>366</v>
-      </c>
+      <c r="G118" s="48"/>
       <c r="H118" s="48"/>
       <c r="I118" s="48" t="s">
+        <v>518</v>
+      </c>
+      <c r="J118" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="K118" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="L118" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M118" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="N118" s="16" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="119" spans="1:14" ht="18">
+      <c r="A119" s="47" t="s">
+        <v>495</v>
+      </c>
+      <c r="B119" s="48" t="s">
+        <v>498</v>
+      </c>
+      <c r="C119" s="48" t="s">
+        <v>610</v>
+      </c>
+      <c r="D119" s="48" t="s">
+        <v>753</v>
+      </c>
+      <c r="E119" s="48" t="s">
+        <v>674</v>
+      </c>
+      <c r="F119" s="48" t="s">
+        <v>621</v>
+      </c>
+      <c r="G119" s="48"/>
+      <c r="H119" s="48"/>
+      <c r="I119" s="48" t="s">
+        <v>516</v>
+      </c>
+      <c r="J119" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="K119" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="L119" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M119" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="N119" s="16" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="120" spans="1:14" ht="18">
+      <c r="A120" s="47" t="s">
+        <v>235</v>
+      </c>
+      <c r="B120" s="48" t="s">
+        <v>115</v>
+      </c>
+      <c r="C120" s="48" t="s">
+        <v>366</v>
+      </c>
+      <c r="D120" s="48" t="s">
+        <v>753</v>
+      </c>
+      <c r="E120" s="48" t="s">
+        <v>674</v>
+      </c>
+      <c r="F120" s="48" t="s">
+        <v>621</v>
+      </c>
+      <c r="G120" s="48" t="s">
+        <v>366</v>
+      </c>
+      <c r="H120" s="48"/>
+      <c r="I120" s="48" t="s">
+        <v>515</v>
+      </c>
+      <c r="J120" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="K120" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="L120" s="15" t="s">
+        <v>367</v>
+      </c>
+      <c r="M120" s="13" t="s">
+        <v>476</v>
+      </c>
+      <c r="N120" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="121" spans="1:14" ht="18">
+      <c r="A121" s="47" t="s">
+        <v>767</v>
+      </c>
+      <c r="B121" s="48" t="s">
+        <v>772</v>
+      </c>
+      <c r="C121" s="48" t="s">
+        <v>776</v>
+      </c>
+      <c r="D121" s="48" t="s">
+        <v>753</v>
+      </c>
+      <c r="E121" s="48" t="s">
+        <v>674</v>
+      </c>
+      <c r="F121" s="48" t="s">
+        <v>621</v>
+      </c>
+      <c r="G121" s="48" t="s">
+        <v>788</v>
+      </c>
+      <c r="H121" s="48"/>
+      <c r="I121" s="48"/>
+      <c r="J121" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="K121" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="L121" s="64"/>
+    </row>
+    <row r="122" spans="1:14" ht="18">
+      <c r="A122" s="47" t="s">
+        <v>770</v>
+      </c>
+      <c r="B122" s="48" t="s">
+        <v>774</v>
+      </c>
+      <c r="C122" s="48" t="s">
+        <v>777</v>
+      </c>
+      <c r="D122" s="48" t="s">
+        <v>753</v>
+      </c>
+      <c r="E122" s="48" t="s">
+        <v>674</v>
+      </c>
+      <c r="F122" s="48" t="s">
+        <v>621</v>
+      </c>
+      <c r="G122" s="48" t="s">
+        <v>788</v>
+      </c>
+      <c r="H122" s="48"/>
+      <c r="I122" s="48"/>
+      <c r="J122" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="K122" s="14" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="123" spans="1:14" ht="18">
+      <c r="A123" s="47" t="s">
+        <v>496</v>
+      </c>
+      <c r="B123" s="48" t="s">
+        <v>499</v>
+      </c>
+      <c r="C123" s="48" t="s">
+        <v>610</v>
+      </c>
+      <c r="D123" s="48" t="s">
+        <v>753</v>
+      </c>
+      <c r="E123" s="48" t="s">
+        <v>674</v>
+      </c>
+      <c r="F123" s="48" t="s">
+        <v>621</v>
+      </c>
+      <c r="G123" s="48"/>
+      <c r="H123" s="48"/>
+      <c r="I123" s="48" t="s">
         <v>517</v>
       </c>
-      <c r="J118" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="K118" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="L118" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M118" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="N118" s="16" t="s">
+      <c r="J123" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="K123" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="L123" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M123" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="N123" s="16" t="s">
         <v>500</v>
-      </c>
-    </row>
-    <row r="119" spans="1:14" ht="18">
-      <c r="A119" s="27" t="s">
-        <v>236</v>
-      </c>
-      <c r="B119" s="28" t="s">
-        <v>199</v>
-      </c>
-      <c r="C119" s="26" t="s">
-        <v>207</v>
-      </c>
-      <c r="D119" s="26" t="s">
-        <v>753</v>
-      </c>
-      <c r="E119" s="26" t="s">
-        <v>764</v>
-      </c>
-      <c r="F119" s="26" t="s">
-        <v>368</v>
-      </c>
-      <c r="G119" s="26" t="s">
-        <v>208</v>
-      </c>
-      <c r="H119" s="26"/>
-      <c r="I119" s="26" t="s">
-        <v>625</v>
-      </c>
-      <c r="J119" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="K119" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="L119" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="M119" s="13"/>
-      <c r="N119" s="16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120" spans="1:14" ht="18">
-      <c r="A120" s="27" t="s">
-        <v>270</v>
-      </c>
-      <c r="B120" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="C120" s="26" t="s">
-        <v>592</v>
-      </c>
-      <c r="D120" s="26" t="s">
-        <v>753</v>
-      </c>
-      <c r="E120" s="26" t="s">
-        <v>764</v>
-      </c>
-      <c r="F120" s="26" t="s">
-        <v>368</v>
-      </c>
-      <c r="G120" s="26"/>
-      <c r="H120" s="26"/>
-      <c r="I120" s="26" t="s">
-        <v>522</v>
-      </c>
-      <c r="J120" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="K120" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="L120" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="M120" s="13" t="s">
-        <v>478</v>
-      </c>
-      <c r="N120" s="16" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="121" spans="1:14" ht="18">
-      <c r="A121" s="27" t="s">
-        <v>262</v>
-      </c>
-      <c r="B121" s="28" t="s">
-        <v>616</v>
-      </c>
-      <c r="C121" s="26" t="s">
-        <v>593</v>
-      </c>
-      <c r="D121" s="26" t="s">
-        <v>753</v>
-      </c>
-      <c r="E121" s="26" t="s">
-        <v>764</v>
-      </c>
-      <c r="F121" s="26" t="s">
-        <v>368</v>
-      </c>
-      <c r="G121" s="26"/>
-      <c r="H121" s="26"/>
-      <c r="I121" s="26" t="s">
-        <v>523</v>
-      </c>
-      <c r="J121" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="K121" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="L121" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M121" s="13" t="s">
-        <v>475</v>
-      </c>
-      <c r="N121" s="16" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="122" spans="1:14" ht="18">
-      <c r="A122" s="27" t="s">
-        <v>263</v>
-      </c>
-      <c r="B122" s="28" t="s">
-        <v>165</v>
-      </c>
-      <c r="C122" s="26" t="s">
-        <v>594</v>
-      </c>
-      <c r="D122" s="26" t="s">
-        <v>753</v>
-      </c>
-      <c r="E122" s="26" t="s">
-        <v>764</v>
-      </c>
-      <c r="F122" s="26" t="s">
-        <v>368</v>
-      </c>
-      <c r="G122" s="26"/>
-      <c r="H122" s="26"/>
-      <c r="I122" s="26" t="s">
-        <v>524</v>
-      </c>
-      <c r="J122" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="K122" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="L122" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="M122" s="13" t="s">
-        <v>476</v>
-      </c>
-      <c r="N122" s="16" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="123" spans="1:14" ht="18">
-      <c r="A123" s="27" t="s">
-        <v>264</v>
-      </c>
-      <c r="B123" s="28" t="s">
-        <v>167</v>
-      </c>
-      <c r="C123" s="26" t="s">
-        <v>595</v>
-      </c>
-      <c r="D123" s="26" t="s">
-        <v>753</v>
-      </c>
-      <c r="E123" s="26" t="s">
-        <v>764</v>
-      </c>
-      <c r="F123" s="26" t="s">
-        <v>368</v>
-      </c>
-      <c r="G123" s="26"/>
-      <c r="H123" s="26"/>
-      <c r="I123" s="26" t="s">
-        <v>524</v>
-      </c>
-      <c r="J123" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="K123" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="L123" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="M123" s="13" t="s">
-        <v>476</v>
-      </c>
-      <c r="N123" s="16" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="124" spans="1:14" ht="18">
       <c r="A124" s="27" t="s">
-        <v>256</v>
+        <v>236</v>
       </c>
       <c r="B124" s="28" t="s">
-        <v>147</v>
+        <v>199</v>
       </c>
       <c r="C124" s="26" t="s">
-        <v>32</v>
+        <v>207</v>
       </c>
       <c r="D124" s="26" t="s">
         <v>753</v>
@@ -9558,10 +9672,12 @@
       <c r="F124" s="26" t="s">
         <v>368</v>
       </c>
-      <c r="G124" s="26"/>
+      <c r="G124" s="26" t="s">
+        <v>208</v>
+      </c>
       <c r="H124" s="26"/>
       <c r="I124" s="26" t="s">
-        <v>512</v>
+        <v>625</v>
       </c>
       <c r="J124" s="14" t="s">
         <v>197</v>
@@ -9570,24 +9686,22 @@
         <v>197</v>
       </c>
       <c r="L124" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="M124" s="13" t="s">
-        <v>476</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="M124" s="13"/>
       <c r="N124" s="16" t="s">
-        <v>148</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:14" ht="18">
       <c r="A125" s="27" t="s">
-        <v>682</v>
+        <v>270</v>
       </c>
       <c r="B125" s="28" t="s">
-        <v>147</v>
-      </c>
-      <c r="C125" s="28" t="s">
-        <v>676</v>
+        <v>175</v>
+      </c>
+      <c r="C125" s="26" t="s">
+        <v>592</v>
       </c>
       <c r="D125" s="26" t="s">
         <v>753</v>
@@ -9595,13 +9709,13 @@
       <c r="E125" s="26" t="s">
         <v>764</v>
       </c>
-      <c r="F125" s="28" t="s">
+      <c r="F125" s="26" t="s">
         <v>368</v>
       </c>
-      <c r="G125" s="28"/>
-      <c r="H125" s="28"/>
-      <c r="I125" s="28" t="s">
-        <v>729</v>
+      <c r="G125" s="26"/>
+      <c r="H125" s="26"/>
+      <c r="I125" s="26" t="s">
+        <v>522</v>
       </c>
       <c r="J125" s="14" t="s">
         <v>197</v>
@@ -9609,22 +9723,25 @@
       <c r="K125" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="L125" s="64" t="s">
-        <v>728</v>
+      <c r="L125" s="15" t="s">
+        <v>47</v>
       </c>
       <c r="M125" s="13" t="s">
-        <v>1</v>
+        <v>478</v>
+      </c>
+      <c r="N125" s="16" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="126" spans="1:14" ht="18">
       <c r="A126" s="27" t="s">
-        <v>683</v>
+        <v>262</v>
       </c>
       <c r="B126" s="28" t="s">
-        <v>726</v>
-      </c>
-      <c r="C126" s="28" t="s">
-        <v>754</v>
+        <v>616</v>
+      </c>
+      <c r="C126" s="26" t="s">
+        <v>593</v>
       </c>
       <c r="D126" s="26" t="s">
         <v>753</v>
@@ -9632,13 +9749,13 @@
       <c r="E126" s="26" t="s">
         <v>764</v>
       </c>
-      <c r="F126" s="28" t="s">
+      <c r="F126" s="26" t="s">
         <v>368</v>
       </c>
-      <c r="G126" s="28"/>
-      <c r="H126" s="28"/>
-      <c r="I126" s="28" t="s">
-        <v>730</v>
+      <c r="G126" s="26"/>
+      <c r="H126" s="26"/>
+      <c r="I126" s="26" t="s">
+        <v>523</v>
       </c>
       <c r="J126" s="14" t="s">
         <v>197</v>
@@ -9646,22 +9763,25 @@
       <c r="K126" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="L126" s="64" t="s">
-        <v>727</v>
+      <c r="L126" s="15" t="s">
+        <v>1</v>
       </c>
       <c r="M126" s="13" t="s">
-        <v>1</v>
+        <v>475</v>
+      </c>
+      <c r="N126" s="16" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="127" spans="1:14" ht="18">
       <c r="A127" s="27" t="s">
-        <v>684</v>
+        <v>263</v>
       </c>
       <c r="B127" s="28" t="s">
-        <v>713</v>
-      </c>
-      <c r="C127" s="28" t="s">
-        <v>762</v>
+        <v>165</v>
+      </c>
+      <c r="C127" s="26" t="s">
+        <v>594</v>
       </c>
       <c r="D127" s="26" t="s">
         <v>753</v>
@@ -9669,13 +9789,13 @@
       <c r="E127" s="26" t="s">
         <v>764</v>
       </c>
-      <c r="F127" s="28" t="s">
+      <c r="F127" s="26" t="s">
         <v>368</v>
       </c>
-      <c r="G127" s="28"/>
-      <c r="H127" s="28"/>
-      <c r="I127" s="28" t="s">
-        <v>731</v>
+      <c r="G127" s="26"/>
+      <c r="H127" s="26"/>
+      <c r="I127" s="26" t="s">
+        <v>524</v>
       </c>
       <c r="J127" s="14" t="s">
         <v>197</v>
@@ -9683,22 +9803,25 @@
       <c r="K127" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="L127" s="64" t="s">
-        <v>732</v>
+      <c r="L127" s="15" t="s">
+        <v>43</v>
       </c>
       <c r="M127" s="13" t="s">
-        <v>1</v>
+        <v>476</v>
+      </c>
+      <c r="N127" s="16" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="128" spans="1:14" ht="18">
       <c r="A128" s="27" t="s">
-        <v>685</v>
+        <v>264</v>
       </c>
       <c r="B128" s="28" t="s">
-        <v>733</v>
-      </c>
-      <c r="C128" s="28" t="s">
-        <v>755</v>
+        <v>167</v>
+      </c>
+      <c r="C128" s="26" t="s">
+        <v>595</v>
       </c>
       <c r="D128" s="26" t="s">
         <v>753</v>
@@ -9706,13 +9829,13 @@
       <c r="E128" s="26" t="s">
         <v>764</v>
       </c>
-      <c r="F128" s="28" t="s">
+      <c r="F128" s="26" t="s">
         <v>368</v>
       </c>
-      <c r="G128" s="28"/>
-      <c r="H128" s="28"/>
-      <c r="I128" s="28" t="s">
-        <v>714</v>
+      <c r="G128" s="26"/>
+      <c r="H128" s="26"/>
+      <c r="I128" s="26" t="s">
+        <v>524</v>
       </c>
       <c r="J128" s="14" t="s">
         <v>197</v>
@@ -9720,22 +9843,25 @@
       <c r="K128" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="L128" s="64" t="s">
-        <v>1</v>
+      <c r="L128" s="15" t="s">
+        <v>44</v>
       </c>
       <c r="M128" s="13" t="s">
-        <v>1</v>
+        <v>476</v>
+      </c>
+      <c r="N128" s="16" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="129" spans="1:14" ht="18">
       <c r="A129" s="27" t="s">
-        <v>686</v>
+        <v>256</v>
       </c>
       <c r="B129" s="28" t="s">
-        <v>715</v>
-      </c>
-      <c r="C129" s="28" t="s">
-        <v>756</v>
+        <v>147</v>
+      </c>
+      <c r="C129" s="26" t="s">
+        <v>32</v>
       </c>
       <c r="D129" s="26" t="s">
         <v>753</v>
@@ -9743,13 +9869,13 @@
       <c r="E129" s="26" t="s">
         <v>764</v>
       </c>
-      <c r="F129" s="28" t="s">
+      <c r="F129" s="26" t="s">
         <v>368</v>
       </c>
-      <c r="G129" s="28"/>
-      <c r="H129" s="28"/>
-      <c r="I129" s="28" t="s">
-        <v>716</v>
+      <c r="G129" s="26"/>
+      <c r="H129" s="26"/>
+      <c r="I129" s="26" t="s">
+        <v>512</v>
       </c>
       <c r="J129" s="14" t="s">
         <v>197</v>
@@ -9757,22 +9883,25 @@
       <c r="K129" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="L129" s="64" t="s">
-        <v>734</v>
+      <c r="L129" s="15" t="s">
+        <v>32</v>
       </c>
       <c r="M129" s="13" t="s">
-        <v>1</v>
+        <v>476</v>
+      </c>
+      <c r="N129" s="16" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="130" spans="1:14" ht="18">
       <c r="A130" s="27" t="s">
-        <v>687</v>
+        <v>682</v>
       </c>
       <c r="B130" s="28" t="s">
-        <v>717</v>
+        <v>147</v>
       </c>
       <c r="C130" s="28" t="s">
-        <v>757</v>
+        <v>676</v>
       </c>
       <c r="D130" s="26" t="s">
         <v>753</v>
@@ -9786,7 +9915,7 @@
       <c r="G130" s="28"/>
       <c r="H130" s="28"/>
       <c r="I130" s="28" t="s">
-        <v>718</v>
+        <v>729</v>
       </c>
       <c r="J130" s="14" t="s">
         <v>197</v>
@@ -9795,7 +9924,7 @@
         <v>197</v>
       </c>
       <c r="L130" s="64" t="s">
-        <v>735</v>
+        <v>728</v>
       </c>
       <c r="M130" s="13" t="s">
         <v>1</v>
@@ -9803,13 +9932,13 @@
     </row>
     <row r="131" spans="1:14" ht="18">
       <c r="A131" s="27" t="s">
-        <v>688</v>
+        <v>683</v>
       </c>
       <c r="B131" s="28" t="s">
-        <v>719</v>
+        <v>726</v>
       </c>
       <c r="C131" s="28" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
       <c r="D131" s="26" t="s">
         <v>753</v>
@@ -9823,7 +9952,7 @@
       <c r="G131" s="28"/>
       <c r="H131" s="28"/>
       <c r="I131" s="28" t="s">
-        <v>720</v>
+        <v>730</v>
       </c>
       <c r="J131" s="14" t="s">
         <v>197</v>
@@ -9832,7 +9961,7 @@
         <v>197</v>
       </c>
       <c r="L131" s="64" t="s">
-        <v>736</v>
+        <v>727</v>
       </c>
       <c r="M131" s="13" t="s">
         <v>1</v>
@@ -9840,13 +9969,13 @@
     </row>
     <row r="132" spans="1:14" ht="18">
       <c r="A132" s="27" t="s">
-        <v>691</v>
+        <v>684</v>
       </c>
       <c r="B132" s="28" t="s">
-        <v>724</v>
+        <v>713</v>
       </c>
       <c r="C132" s="28" t="s">
-        <v>759</v>
+        <v>762</v>
       </c>
       <c r="D132" s="26" t="s">
         <v>753</v>
@@ -9860,7 +9989,7 @@
       <c r="G132" s="28"/>
       <c r="H132" s="28"/>
       <c r="I132" s="28" t="s">
-        <v>750</v>
+        <v>731</v>
       </c>
       <c r="J132" s="14" t="s">
         <v>197</v>
@@ -9869,7 +9998,7 @@
         <v>197</v>
       </c>
       <c r="L132" s="64" t="s">
-        <v>725</v>
+        <v>732</v>
       </c>
       <c r="M132" s="13" t="s">
         <v>1</v>
@@ -9877,13 +10006,13 @@
     </row>
     <row r="133" spans="1:14" ht="18">
       <c r="A133" s="27" t="s">
-        <v>254</v>
+        <v>685</v>
       </c>
       <c r="B133" s="28" t="s">
-        <v>144</v>
+        <v>733</v>
       </c>
       <c r="C133" s="28" t="s">
-        <v>604</v>
+        <v>755</v>
       </c>
       <c r="D133" s="26" t="s">
         <v>753</v>
@@ -9891,39 +10020,36 @@
       <c r="E133" s="26" t="s">
         <v>764</v>
       </c>
-      <c r="F133" s="61" t="s">
-        <v>416</v>
-      </c>
-      <c r="G133" s="61"/>
-      <c r="H133" s="61"/>
-      <c r="I133" s="61" t="s">
-        <v>523</v>
-      </c>
-      <c r="J133" s="61" t="s">
-        <v>197</v>
-      </c>
-      <c r="K133" s="61" t="s">
-        <v>197</v>
-      </c>
-      <c r="L133" s="61" t="s">
-        <v>30</v>
-      </c>
-      <c r="M133" s="61" t="s">
-        <v>476</v>
-      </c>
-      <c r="N133" s="16" t="s">
-        <v>164</v>
+      <c r="F133" s="28" t="s">
+        <v>368</v>
+      </c>
+      <c r="G133" s="28"/>
+      <c r="H133" s="28"/>
+      <c r="I133" s="28" t="s">
+        <v>714</v>
+      </c>
+      <c r="J133" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="K133" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="L133" s="64" t="s">
+        <v>1</v>
+      </c>
+      <c r="M133" s="13" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:14" ht="18">
       <c r="A134" s="27" t="s">
-        <v>221</v>
+        <v>686</v>
       </c>
       <c r="B134" s="28" t="s">
-        <v>101</v>
+        <v>715</v>
       </c>
       <c r="C134" s="28" t="s">
-        <v>346</v>
+        <v>756</v>
       </c>
       <c r="D134" s="26" t="s">
         <v>753</v>
@@ -9931,39 +10057,36 @@
       <c r="E134" s="26" t="s">
         <v>764</v>
       </c>
-      <c r="F134" s="39" t="s">
-        <v>416</v>
-      </c>
-      <c r="G134" s="61"/>
-      <c r="H134" s="61"/>
-      <c r="I134" s="61" t="s">
-        <v>588</v>
-      </c>
-      <c r="J134" s="61" t="s">
-        <v>197</v>
-      </c>
-      <c r="K134" s="61" t="s">
-        <v>197</v>
-      </c>
-      <c r="L134" s="61" t="s">
-        <v>1</v>
-      </c>
-      <c r="M134" s="61" t="s">
-        <v>1</v>
-      </c>
-      <c r="N134" s="16" t="s">
+      <c r="F134" s="28" t="s">
+        <v>368</v>
+      </c>
+      <c r="G134" s="28"/>
+      <c r="H134" s="28"/>
+      <c r="I134" s="28" t="s">
+        <v>716</v>
+      </c>
+      <c r="J134" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="K134" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="L134" s="64" t="s">
+        <v>734</v>
+      </c>
+      <c r="M134" s="13" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:14" ht="18">
       <c r="A135" s="27" t="s">
-        <v>287</v>
+        <v>687</v>
       </c>
       <c r="B135" s="28" t="s">
-        <v>180</v>
+        <v>717</v>
       </c>
       <c r="C135" s="28" t="s">
-        <v>437</v>
+        <v>757</v>
       </c>
       <c r="D135" s="26" t="s">
         <v>753</v>
@@ -9971,39 +10094,36 @@
       <c r="E135" s="26" t="s">
         <v>764</v>
       </c>
-      <c r="F135" s="61" t="s">
-        <v>416</v>
-      </c>
-      <c r="G135" s="61"/>
-      <c r="H135" s="61"/>
-      <c r="I135" s="61" t="s">
-        <v>588</v>
-      </c>
-      <c r="J135" s="61" t="s">
-        <v>197</v>
-      </c>
-      <c r="K135" s="61" t="s">
-        <v>197</v>
-      </c>
-      <c r="L135" s="61" t="s">
-        <v>51</v>
-      </c>
-      <c r="M135" s="61" t="s">
-        <v>476</v>
-      </c>
-      <c r="N135" s="16" t="s">
-        <v>119</v>
+      <c r="F135" s="28" t="s">
+        <v>368</v>
+      </c>
+      <c r="G135" s="28"/>
+      <c r="H135" s="28"/>
+      <c r="I135" s="28" t="s">
+        <v>718</v>
+      </c>
+      <c r="J135" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="K135" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="L135" s="64" t="s">
+        <v>735</v>
+      </c>
+      <c r="M135" s="13" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:14" ht="18">
       <c r="A136" s="27" t="s">
-        <v>266</v>
+        <v>688</v>
       </c>
       <c r="B136" s="28" t="s">
-        <v>169</v>
+        <v>719</v>
       </c>
       <c r="C136" s="28" t="s">
-        <v>603</v>
+        <v>758</v>
       </c>
       <c r="D136" s="26" t="s">
         <v>753</v>
@@ -10011,39 +10131,36 @@
       <c r="E136" s="26" t="s">
         <v>764</v>
       </c>
-      <c r="F136" s="39" t="s">
-        <v>416</v>
-      </c>
-      <c r="G136" s="61"/>
-      <c r="H136" s="61"/>
-      <c r="I136" s="61" t="s">
-        <v>524</v>
-      </c>
-      <c r="J136" s="61" t="s">
-        <v>197</v>
-      </c>
-      <c r="K136" s="61" t="s">
-        <v>197</v>
-      </c>
-      <c r="L136" s="61" t="s">
-        <v>46</v>
-      </c>
-      <c r="M136" s="61" t="s">
-        <v>476</v>
-      </c>
-      <c r="N136" s="16" t="s">
-        <v>166</v>
+      <c r="F136" s="28" t="s">
+        <v>368</v>
+      </c>
+      <c r="G136" s="28"/>
+      <c r="H136" s="28"/>
+      <c r="I136" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="J136" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="K136" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="L136" s="64" t="s">
+        <v>736</v>
+      </c>
+      <c r="M136" s="13" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:14" ht="18">
       <c r="A137" s="27" t="s">
-        <v>223</v>
+        <v>691</v>
       </c>
       <c r="B137" s="28" t="s">
-        <v>103</v>
+        <v>724</v>
       </c>
       <c r="C137" s="28" t="s">
-        <v>348</v>
+        <v>759</v>
       </c>
       <c r="D137" s="26" t="s">
         <v>753</v>
@@ -10051,39 +10168,36 @@
       <c r="E137" s="26" t="s">
         <v>764</v>
       </c>
-      <c r="F137" s="39" t="s">
-        <v>416</v>
-      </c>
-      <c r="G137" s="61"/>
-      <c r="H137" s="61"/>
-      <c r="I137" s="61" t="s">
-        <v>588</v>
-      </c>
-      <c r="J137" s="61" t="s">
-        <v>197</v>
-      </c>
-      <c r="K137" s="61" t="s">
-        <v>197</v>
-      </c>
-      <c r="L137" s="61" t="s">
-        <v>1</v>
-      </c>
-      <c r="M137" s="61" t="s">
-        <v>1</v>
-      </c>
-      <c r="N137" s="16" t="s">
+      <c r="F137" s="28" t="s">
+        <v>368</v>
+      </c>
+      <c r="G137" s="28"/>
+      <c r="H137" s="28"/>
+      <c r="I137" s="28" t="s">
+        <v>750</v>
+      </c>
+      <c r="J137" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="K137" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="L137" s="64" t="s">
+        <v>725</v>
+      </c>
+      <c r="M137" s="13" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:14" ht="18">
       <c r="A138" s="27" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B138" s="28" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C138" s="28" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="D138" s="26" t="s">
         <v>753</v>
@@ -10091,39 +10205,39 @@
       <c r="E138" s="26" t="s">
         <v>764</v>
       </c>
-      <c r="F138" s="39" t="s">
+      <c r="F138" s="61" t="s">
         <v>416</v>
       </c>
-      <c r="G138" s="39"/>
-      <c r="H138" s="39"/>
-      <c r="I138" s="39" t="s">
-        <v>525</v>
-      </c>
-      <c r="J138" s="39" t="s">
-        <v>197</v>
-      </c>
-      <c r="K138" s="39" t="s">
+      <c r="G138" s="61"/>
+      <c r="H138" s="61"/>
+      <c r="I138" s="61" t="s">
+        <v>523</v>
+      </c>
+      <c r="J138" s="61" t="s">
+        <v>197</v>
+      </c>
+      <c r="K138" s="61" t="s">
         <v>197</v>
       </c>
       <c r="L138" s="61" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="M138" s="61" t="s">
         <v>476</v>
       </c>
       <c r="N138" s="16" t="s">
-        <v>150</v>
+        <v>164</v>
       </c>
     </row>
     <row r="139" spans="1:14" ht="18">
       <c r="A139" s="27" t="s">
-        <v>261</v>
+        <v>221</v>
       </c>
       <c r="B139" s="28" t="s">
-        <v>161</v>
+        <v>101</v>
       </c>
       <c r="C139" s="28" t="s">
-        <v>601</v>
+        <v>346</v>
       </c>
       <c r="D139" s="26" t="s">
         <v>753</v>
@@ -10134,36 +10248,36 @@
       <c r="F139" s="39" t="s">
         <v>416</v>
       </c>
-      <c r="G139" s="39"/>
-      <c r="H139" s="39"/>
-      <c r="I139" s="39" t="s">
-        <v>526</v>
-      </c>
-      <c r="J139" s="39" t="s">
-        <v>197</v>
-      </c>
-      <c r="K139" s="39" t="s">
+      <c r="G139" s="61"/>
+      <c r="H139" s="61"/>
+      <c r="I139" s="61" t="s">
+        <v>588</v>
+      </c>
+      <c r="J139" s="61" t="s">
+        <v>197</v>
+      </c>
+      <c r="K139" s="61" t="s">
         <v>197</v>
       </c>
       <c r="L139" s="61" t="s">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="M139" s="61" t="s">
-        <v>478</v>
+        <v>1</v>
       </c>
       <c r="N139" s="16" t="s">
-        <v>162</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:14" ht="18">
       <c r="A140" s="27" t="s">
-        <v>689</v>
+        <v>287</v>
       </c>
       <c r="B140" s="28" t="s">
-        <v>721</v>
+        <v>180</v>
       </c>
       <c r="C140" s="28" t="s">
-        <v>760</v>
+        <v>437</v>
       </c>
       <c r="D140" s="26" t="s">
         <v>753</v>
@@ -10171,39 +10285,39 @@
       <c r="E140" s="26" t="s">
         <v>764</v>
       </c>
-      <c r="F140" s="39" t="s">
+      <c r="F140" s="61" t="s">
         <v>416</v>
       </c>
-      <c r="G140" s="39"/>
-      <c r="H140" s="39"/>
-      <c r="I140" s="39" t="s">
-        <v>749</v>
-      </c>
-      <c r="J140" s="39" t="s">
-        <v>197</v>
-      </c>
-      <c r="K140" s="39" t="s">
-        <v>197</v>
-      </c>
-      <c r="L140" s="64" t="s">
-        <v>1</v>
+      <c r="G140" s="61"/>
+      <c r="H140" s="61"/>
+      <c r="I140" s="61" t="s">
+        <v>588</v>
+      </c>
+      <c r="J140" s="61" t="s">
+        <v>197</v>
+      </c>
+      <c r="K140" s="61" t="s">
+        <v>197</v>
+      </c>
+      <c r="L140" s="61" t="s">
+        <v>51</v>
       </c>
       <c r="M140" s="61" t="s">
-        <v>1</v>
+        <v>476</v>
       </c>
       <c r="N140" s="16" t="s">
-        <v>749</v>
+        <v>119</v>
       </c>
     </row>
     <row r="141" spans="1:14" ht="18">
       <c r="A141" s="27" t="s">
-        <v>690</v>
+        <v>266</v>
       </c>
       <c r="B141" s="28" t="s">
-        <v>722</v>
+        <v>169</v>
       </c>
       <c r="C141" s="28" t="s">
-        <v>761</v>
+        <v>603</v>
       </c>
       <c r="D141" s="26" t="s">
         <v>753</v>
@@ -10211,259 +10325,239 @@
       <c r="E141" s="26" t="s">
         <v>764</v>
       </c>
-      <c r="F141" s="68" t="s">
+      <c r="F141" s="39" t="s">
+        <v>416</v>
+      </c>
+      <c r="G141" s="61"/>
+      <c r="H141" s="61"/>
+      <c r="I141" s="61" t="s">
+        <v>524</v>
+      </c>
+      <c r="J141" s="61" t="s">
+        <v>197</v>
+      </c>
+      <c r="K141" s="61" t="s">
+        <v>197</v>
+      </c>
+      <c r="L141" s="61" t="s">
+        <v>46</v>
+      </c>
+      <c r="M141" s="61" t="s">
+        <v>476</v>
+      </c>
+      <c r="N141" s="16" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="142" spans="1:14" ht="18">
+      <c r="A142" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="B142" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="C142" s="28" t="s">
+        <v>348</v>
+      </c>
+      <c r="D142" s="26" t="s">
+        <v>753</v>
+      </c>
+      <c r="E142" s="26" t="s">
+        <v>764</v>
+      </c>
+      <c r="F142" s="39" t="s">
+        <v>416</v>
+      </c>
+      <c r="G142" s="61"/>
+      <c r="H142" s="61"/>
+      <c r="I142" s="61" t="s">
+        <v>588</v>
+      </c>
+      <c r="J142" s="61" t="s">
+        <v>197</v>
+      </c>
+      <c r="K142" s="61" t="s">
+        <v>197</v>
+      </c>
+      <c r="L142" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="M142" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="N142" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:14" ht="18">
+      <c r="A143" s="27" t="s">
+        <v>257</v>
+      </c>
+      <c r="B143" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="C143" s="28" t="s">
+        <v>602</v>
+      </c>
+      <c r="D143" s="26" t="s">
+        <v>753</v>
+      </c>
+      <c r="E143" s="26" t="s">
+        <v>764</v>
+      </c>
+      <c r="F143" s="39" t="s">
+        <v>416</v>
+      </c>
+      <c r="G143" s="39"/>
+      <c r="H143" s="39"/>
+      <c r="I143" s="39" t="s">
+        <v>525</v>
+      </c>
+      <c r="J143" s="39" t="s">
+        <v>197</v>
+      </c>
+      <c r="K143" s="39" t="s">
+        <v>197</v>
+      </c>
+      <c r="L143" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M143" s="61" t="s">
+        <v>476</v>
+      </c>
+      <c r="N143" s="16" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="144" spans="1:14" ht="18">
+      <c r="A144" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="B144" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="C144" s="28" t="s">
+        <v>601</v>
+      </c>
+      <c r="D144" s="26" t="s">
+        <v>753</v>
+      </c>
+      <c r="E144" s="26" t="s">
+        <v>764</v>
+      </c>
+      <c r="F144" s="39" t="s">
+        <v>416</v>
+      </c>
+      <c r="G144" s="39"/>
+      <c r="H144" s="39"/>
+      <c r="I144" s="39" t="s">
+        <v>526</v>
+      </c>
+      <c r="J144" s="39" t="s">
+        <v>197</v>
+      </c>
+      <c r="K144" s="39" t="s">
+        <v>197</v>
+      </c>
+      <c r="L144" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="M144" s="61" t="s">
+        <v>478</v>
+      </c>
+      <c r="N144" s="16" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="145" spans="1:14" ht="18">
+      <c r="A145" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="B145" s="28" t="s">
+        <v>721</v>
+      </c>
+      <c r="C145" s="28" t="s">
+        <v>760</v>
+      </c>
+      <c r="D145" s="26" t="s">
+        <v>753</v>
+      </c>
+      <c r="E145" s="26" t="s">
+        <v>764</v>
+      </c>
+      <c r="F145" s="39" t="s">
+        <v>416</v>
+      </c>
+      <c r="G145" s="39"/>
+      <c r="H145" s="39"/>
+      <c r="I145" s="39" t="s">
+        <v>749</v>
+      </c>
+      <c r="J145" s="39" t="s">
+        <v>197</v>
+      </c>
+      <c r="K145" s="39" t="s">
+        <v>197</v>
+      </c>
+      <c r="L145" s="64" t="s">
+        <v>1</v>
+      </c>
+      <c r="M145" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="N145" s="16" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="146" spans="1:14" ht="18">
+      <c r="A146" s="27" t="s">
+        <v>690</v>
+      </c>
+      <c r="B146" s="28" t="s">
+        <v>722</v>
+      </c>
+      <c r="C146" s="28" t="s">
+        <v>761</v>
+      </c>
+      <c r="D146" s="26" t="s">
+        <v>753</v>
+      </c>
+      <c r="E146" s="26" t="s">
+        <v>764</v>
+      </c>
+      <c r="F146" s="68" t="s">
         <v>765</v>
       </c>
-      <c r="G141" s="68"/>
-      <c r="H141" s="68"/>
-      <c r="I141" s="68" t="s">
+      <c r="G146" s="68"/>
+      <c r="H146" s="68"/>
+      <c r="I146" s="68" t="s">
         <v>119</v>
       </c>
-      <c r="J141" s="39" t="s">
-        <v>197</v>
-      </c>
-      <c r="K141" s="39" t="s">
-        <v>197</v>
-      </c>
-      <c r="L141" s="64" t="s">
+      <c r="J146" s="39" t="s">
+        <v>197</v>
+      </c>
+      <c r="K146" s="39" t="s">
+        <v>197</v>
+      </c>
+      <c r="L146" s="64" t="s">
         <v>723</v>
       </c>
-      <c r="M141" s="61" t="s">
-        <v>1</v>
-      </c>
-      <c r="N141" s="16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="142" spans="1:14" ht="18">
-      <c r="A142" s="49" t="s">
-        <v>572</v>
-      </c>
-      <c r="B142" s="50" t="s">
-        <v>578</v>
-      </c>
-      <c r="C142" s="50" t="s">
-        <v>607</v>
-      </c>
-      <c r="D142" s="50" t="s">
-        <v>679</v>
-      </c>
-      <c r="E142" s="50" t="s">
-        <v>674</v>
-      </c>
-      <c r="F142" s="50" t="s">
-        <v>679</v>
-      </c>
-      <c r="G142" s="50" t="s">
-        <v>677</v>
-      </c>
-      <c r="H142" s="50">
-        <v>1</v>
-      </c>
-      <c r="I142" s="50" t="s">
-        <v>519</v>
-      </c>
-      <c r="J142" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="K142" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="L142" s="15" t="s">
-        <v>670</v>
-      </c>
-      <c r="M142" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="N142" s="16" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="143" spans="1:14" ht="18">
-      <c r="A143" s="49" t="s">
-        <v>570</v>
-      </c>
-      <c r="B143" s="50" t="s">
-        <v>576</v>
-      </c>
-      <c r="C143" s="50" t="s">
-        <v>606</v>
-      </c>
-      <c r="D143" s="50" t="s">
-        <v>679</v>
-      </c>
-      <c r="E143" s="50" t="s">
-        <v>674</v>
-      </c>
-      <c r="F143" s="50" t="s">
-        <v>679</v>
-      </c>
-      <c r="G143" s="50" t="s">
-        <v>677</v>
-      </c>
-      <c r="H143" s="50">
-        <v>1</v>
-      </c>
-      <c r="I143" s="50" t="s">
-        <v>580</v>
-      </c>
-      <c r="J143" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="K143" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="L143" s="15" t="s">
-        <v>669</v>
-      </c>
-      <c r="M143" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="N143" s="16" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="144" spans="1:14" ht="18">
-      <c r="A144" s="49" t="s">
-        <v>569</v>
-      </c>
-      <c r="B144" s="50" t="s">
-        <v>575</v>
-      </c>
-      <c r="C144" s="50" t="s">
-        <v>605</v>
-      </c>
-      <c r="D144" s="50" t="s">
-        <v>679</v>
-      </c>
-      <c r="E144" s="50" t="s">
-        <v>674</v>
-      </c>
-      <c r="F144" s="50" t="s">
-        <v>679</v>
-      </c>
-      <c r="G144" s="50" t="s">
-        <v>677</v>
-      </c>
-      <c r="H144" s="50">
-        <v>1</v>
-      </c>
-      <c r="I144" s="50" t="s">
-        <v>403</v>
-      </c>
-      <c r="J144" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="K144" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="L144" s="15" t="s">
-        <v>668</v>
-      </c>
-      <c r="M144" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="N144" s="16" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="145" spans="1:14" ht="18">
-      <c r="A145" s="49" t="s">
-        <v>665</v>
-      </c>
-      <c r="B145" s="50" t="s">
-        <v>573</v>
-      </c>
-      <c r="C145" s="50" t="s">
-        <v>574</v>
-      </c>
-      <c r="D145" s="50" t="s">
-        <v>679</v>
-      </c>
-      <c r="E145" s="50" t="s">
-        <v>674</v>
-      </c>
-      <c r="F145" s="50" t="s">
-        <v>679</v>
-      </c>
-      <c r="G145" s="50" t="s">
-        <v>677</v>
-      </c>
-      <c r="H145" s="50">
-        <v>1</v>
-      </c>
-      <c r="I145" s="50" t="s">
-        <v>520</v>
-      </c>
-      <c r="J145" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="K145" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="L145" s="15" t="s">
-        <v>667</v>
-      </c>
-      <c r="M145" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="N145" s="16" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="146" spans="1:14" ht="18">
-      <c r="A146" s="49" t="s">
-        <v>571</v>
-      </c>
-      <c r="B146" s="50" t="s">
-        <v>577</v>
-      </c>
-      <c r="C146" s="50" t="s">
-        <v>608</v>
-      </c>
-      <c r="D146" s="50" t="s">
-        <v>679</v>
-      </c>
-      <c r="E146" s="50" t="s">
-        <v>674</v>
-      </c>
-      <c r="F146" s="50" t="s">
-        <v>679</v>
-      </c>
-      <c r="G146" s="50" t="s">
-        <v>677</v>
-      </c>
-      <c r="H146" s="50">
-        <v>1</v>
-      </c>
-      <c r="I146" s="50" t="s">
-        <v>582</v>
-      </c>
-      <c r="J146" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="K146" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="L146" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M146" s="13" t="s">
+      <c r="M146" s="61" t="s">
         <v>1</v>
       </c>
       <c r="N146" s="16" t="s">
-        <v>581</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:14" ht="18">
       <c r="A147" s="49" t="s">
-        <v>639</v>
+        <v>572</v>
       </c>
       <c r="B147" s="50" t="s">
-        <v>640</v>
+        <v>578</v>
       </c>
       <c r="C147" s="50" t="s">
-        <v>656</v>
+        <v>607</v>
       </c>
       <c r="D147" s="50" t="s">
         <v>679</v>
@@ -10481,7 +10575,7 @@
         <v>1</v>
       </c>
       <c r="I147" s="50" t="s">
-        <v>655</v>
+        <v>519</v>
       </c>
       <c r="J147" s="14" t="s">
         <v>197</v>
@@ -10490,24 +10584,24 @@
         <v>197</v>
       </c>
       <c r="L147" s="15" t="s">
-        <v>1</v>
+        <v>670</v>
       </c>
       <c r="M147" s="13" t="s">
         <v>1</v>
       </c>
       <c r="N147" s="16" t="s">
-        <v>1</v>
+        <v>585</v>
       </c>
     </row>
     <row r="148" spans="1:14" ht="18">
       <c r="A148" s="49" t="s">
-        <v>642</v>
+        <v>570</v>
       </c>
       <c r="B148" s="50" t="s">
-        <v>641</v>
+        <v>576</v>
       </c>
       <c r="C148" s="50" t="s">
-        <v>657</v>
+        <v>606</v>
       </c>
       <c r="D148" s="50" t="s">
         <v>679</v>
@@ -10525,7 +10619,7 @@
         <v>1</v>
       </c>
       <c r="I148" s="50" t="s">
-        <v>681</v>
+        <v>580</v>
       </c>
       <c r="J148" s="14" t="s">
         <v>197</v>
@@ -10534,24 +10628,24 @@
         <v>197</v>
       </c>
       <c r="L148" s="15" t="s">
-        <v>1</v>
+        <v>669</v>
       </c>
       <c r="M148" s="13" t="s">
         <v>1</v>
       </c>
       <c r="N148" s="16" t="s">
-        <v>1</v>
+        <v>584</v>
       </c>
     </row>
     <row r="149" spans="1:14" ht="18">
       <c r="A149" s="49" t="s">
-        <v>666</v>
+        <v>569</v>
       </c>
       <c r="B149" s="50" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="C149" s="50" t="s">
-        <v>574</v>
+        <v>605</v>
       </c>
       <c r="D149" s="50" t="s">
         <v>679</v>
@@ -10563,56 +10657,249 @@
         <v>679</v>
       </c>
       <c r="G149" s="50" t="s">
+        <v>677</v>
+      </c>
+      <c r="H149" s="50">
+        <v>1</v>
+      </c>
+      <c r="I149" s="50" t="s">
+        <v>403</v>
+      </c>
+      <c r="J149" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="K149" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="L149" s="15" t="s">
+        <v>668</v>
+      </c>
+      <c r="M149" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="N149" s="16" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="150" spans="1:14" ht="18">
+      <c r="A150" s="49" t="s">
+        <v>665</v>
+      </c>
+      <c r="B150" s="50" t="s">
+        <v>573</v>
+      </c>
+      <c r="C150" s="50" t="s">
+        <v>574</v>
+      </c>
+      <c r="D150" s="50" t="s">
+        <v>679</v>
+      </c>
+      <c r="E150" s="50" t="s">
+        <v>674</v>
+      </c>
+      <c r="F150" s="50" t="s">
+        <v>679</v>
+      </c>
+      <c r="G150" s="50" t="s">
+        <v>677</v>
+      </c>
+      <c r="H150" s="50">
+        <v>1</v>
+      </c>
+      <c r="I150" s="50" t="s">
+        <v>520</v>
+      </c>
+      <c r="J150" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="K150" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="L150" s="15" t="s">
+        <v>667</v>
+      </c>
+      <c r="M150" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="N150" s="16" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="151" spans="1:14" ht="18">
+      <c r="A151" s="49" t="s">
+        <v>571</v>
+      </c>
+      <c r="B151" s="50" t="s">
+        <v>577</v>
+      </c>
+      <c r="C151" s="50" t="s">
+        <v>608</v>
+      </c>
+      <c r="D151" s="50" t="s">
+        <v>679</v>
+      </c>
+      <c r="E151" s="50" t="s">
+        <v>674</v>
+      </c>
+      <c r="F151" s="50" t="s">
+        <v>679</v>
+      </c>
+      <c r="G151" s="50" t="s">
+        <v>677</v>
+      </c>
+      <c r="H151" s="50">
+        <v>1</v>
+      </c>
+      <c r="I151" s="50" t="s">
+        <v>582</v>
+      </c>
+      <c r="J151" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="K151" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="L151" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M151" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="N151" s="16" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="152" spans="1:14" ht="18">
+      <c r="A152" s="49" t="s">
+        <v>639</v>
+      </c>
+      <c r="B152" s="50" t="s">
+        <v>640</v>
+      </c>
+      <c r="C152" s="50" t="s">
+        <v>656</v>
+      </c>
+      <c r="D152" s="50" t="s">
+        <v>679</v>
+      </c>
+      <c r="E152" s="50" t="s">
+        <v>674</v>
+      </c>
+      <c r="F152" s="50" t="s">
+        <v>679</v>
+      </c>
+      <c r="G152" s="50" t="s">
+        <v>677</v>
+      </c>
+      <c r="H152" s="50">
+        <v>1</v>
+      </c>
+      <c r="I152" s="50" t="s">
+        <v>655</v>
+      </c>
+      <c r="J152" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="K152" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="L152" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M152" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="N152" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:14" ht="18">
+      <c r="A153" s="49" t="s">
+        <v>642</v>
+      </c>
+      <c r="B153" s="50" t="s">
+        <v>641</v>
+      </c>
+      <c r="C153" s="50" t="s">
+        <v>657</v>
+      </c>
+      <c r="D153" s="50" t="s">
+        <v>679</v>
+      </c>
+      <c r="E153" s="50" t="s">
+        <v>674</v>
+      </c>
+      <c r="F153" s="50" t="s">
+        <v>679</v>
+      </c>
+      <c r="G153" s="50" t="s">
+        <v>677</v>
+      </c>
+      <c r="H153" s="50">
+        <v>1</v>
+      </c>
+      <c r="I153" s="50" t="s">
+        <v>681</v>
+      </c>
+      <c r="J153" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="K153" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="L153" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M153" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="N153" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:14" ht="18">
+      <c r="A154" s="49" t="s">
+        <v>666</v>
+      </c>
+      <c r="B154" s="50" t="s">
+        <v>573</v>
+      </c>
+      <c r="C154" s="50" t="s">
+        <v>574</v>
+      </c>
+      <c r="D154" s="50" t="s">
+        <v>679</v>
+      </c>
+      <c r="E154" s="50" t="s">
+        <v>674</v>
+      </c>
+      <c r="F154" s="50" t="s">
+        <v>679</v>
+      </c>
+      <c r="G154" s="50" t="s">
         <v>678</v>
       </c>
-      <c r="H149" s="50">
+      <c r="H154" s="50">
         <v>3</v>
       </c>
-      <c r="I149" s="50" t="s">
+      <c r="I154" s="50" t="s">
         <v>520</v>
       </c>
-      <c r="J149" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="K149" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="L149" s="15" t="s">
+      <c r="J154" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="K154" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="L154" s="15" t="s">
         <v>667</v>
       </c>
-      <c r="M149" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="N149" s="16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="150" spans="1:14" ht="18">
-      <c r="F150" s="64"/>
-      <c r="G150" s="64"/>
-      <c r="H150" s="64"/>
-      <c r="I150" s="64"/>
-      <c r="J150" s="64"/>
-      <c r="K150" s="64"/>
-      <c r="L150" s="64"/>
-    </row>
-    <row r="151" spans="1:14" ht="18">
-      <c r="F151" s="64"/>
-      <c r="G151" s="64"/>
-      <c r="H151" s="64"/>
-      <c r="I151" s="64"/>
-      <c r="J151" s="64"/>
-      <c r="K151" s="64"/>
-      <c r="L151" s="64"/>
-    </row>
-    <row r="152" spans="1:14" ht="18">
-      <c r="F152" s="64"/>
-      <c r="G152" s="64"/>
-      <c r="H152" s="64"/>
-      <c r="I152" s="64"/>
-      <c r="J152" s="64"/>
-      <c r="K152" s="64"/>
-      <c r="L152" s="64"/>
+      <c r="M154" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="N154" s="16" t="s">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:N153">

</xml_diff>

<commit_message>
Made Shungao Lacewing Virus 2 the main reference for the Pestinsect group
</commit_message>
<xml_diff>
--- a/tabular/flavi-ncbi-refseqs-side-data.xlsx
+++ b/tabular/flavi-ncbi-refseqs-side-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="1000" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="12040" yWindow="5500" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="flavi.txt" sheetId="1" r:id="rId1"/>
@@ -2682,7 +2682,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="664">
+  <cellStyleXfs count="668">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3303,6 +3303,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3499,7 +3503,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="664">
+  <cellStyles count="668">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3853,6 +3857,10 @@
     <cellStyle name="Followed Hyperlink" xfId="661" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="662" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="663" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="664" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="665" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="666" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="667" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4503,8 +4511,8 @@
   <dimension ref="A1:N154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:N154"/>
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Creating reference sequence summary script
</commit_message>
<xml_diff>
--- a/tabular/flavi-ncbi-refseqs-side-data.xlsx
+++ b/tabular/flavi-ncbi-refseqs-side-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12040" yWindow="5500" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="7720" yWindow="10700" windowWidth="34420" windowHeight="17220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="flavi.txt" sheetId="1" r:id="rId1"/>
@@ -2682,7 +2682,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="668">
+  <cellStyleXfs count="678">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3303,6 +3303,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3503,7 +3513,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="668">
+  <cellStyles count="678">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3861,6 +3871,16 @@
     <cellStyle name="Followed Hyperlink" xfId="665" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="666" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="667" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="668" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="669" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="670" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="671" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="672" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="673" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="674" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="675" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="676" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="677" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4511,8 +4531,8 @@
   <dimension ref="A1:N154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A100" sqref="A100"/>
+      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G120" sqref="G120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Updated alignments and metadata
</commit_message>
<xml_diff>
--- a/tabular/flavi-ncbi-refseqs-side-data.xlsx
+++ b/tabular/flavi-ncbi-refseqs-side-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="0" windowWidth="35180" windowHeight="23040" tabRatio="500"/>
+    <workbookView xWindow="4420" yWindow="500" windowWidth="35180" windowHeight="23040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="flavi.txt" sheetId="1" r:id="rId1"/>
@@ -2725,7 +2725,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="714">
+  <cellStyleXfs count="718">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3346,6 +3346,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3592,7 +3596,7 @@
     <xf numFmtId="0" fontId="10" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="714">
+  <cellStyles count="718">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3996,6 +4000,10 @@
     <cellStyle name="Followed Hyperlink" xfId="711" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="712" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="713" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="714" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="715" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="716" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="717" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4646,8 +4654,8 @@
   <dimension ref="A1:N160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="A1:XFD1048576"/>
+      <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G132" sqref="G132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>